<commit_message>
updated after episode 602
</commit_message>
<xml_diff>
--- a/SGU_Science_or_Fiction.xlsx
+++ b/SGU_Science_or_Fiction.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xwhx\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xwhx\Documents\SGU_Science_or_Fiction\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6135" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6135"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>Episode</t>
   </si>
@@ -92,6 +92,21 @@
   </si>
   <si>
     <t>The Hubble Space Telescope has discovered a probable new exoplanet using a unique method – by imaging a shadow cast upon a ring of dust surrounding the parent star. https://www.nasa.gov/feature/goddard/2017/hubble-captures-shadow-play-caused-by-possible-planet</t>
+  </si>
+  <si>
+    <t>Global warming</t>
+  </si>
+  <si>
+    <t>Carl Sagan was the first scientist to publicly warn about the possibility of manmade global warming from greenhouse gas emissions, in a 1980 essay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The 15 hottest years on record since 1880 have all been since 1998. </t>
+  </si>
+  <si>
+    <t>Climate models show that even if CO2 emissions were stopped entirely, global temperatures would continue to rise for at least a century</t>
+  </si>
+  <si>
+    <t>Overall % Wins</t>
   </si>
 </sst>
 </file>
@@ -443,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,6 +607,445 @@
         <f>NA()</f>
         <v>#N/A</v>
       </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>602</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="1">
+        <v>2</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1">
+        <v>1</v>
+      </c>
+      <c r="L4" s="1">
+        <v>1</v>
+      </c>
+      <c r="M4" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N4" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+    </row>
+    <row r="18" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+    </row>
+    <row r="19" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+    </row>
+    <row r="20" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+    </row>
+    <row r="21" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+    </row>
+    <row r="22" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+    </row>
+    <row r="23" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+    </row>
+    <row r="24" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+    </row>
+    <row r="25" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+    </row>
+    <row r="26" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+    </row>
+    <row r="27" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+    </row>
+    <row r="28" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+    </row>
+    <row r="29" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+    </row>
+    <row r="30" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+    </row>
+    <row r="31" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+    </row>
+    <row r="32" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+    </row>
+    <row r="33" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+    </row>
+    <row r="34" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+    </row>
+    <row r="35" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+    </row>
+    <row r="36" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+    </row>
+    <row r="37" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+    </row>
+    <row r="38" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+    </row>
+    <row r="39" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+    </row>
+    <row r="40" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+    </row>
+    <row r="41" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+    </row>
+    <row r="42" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+    </row>
+    <row r="43" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+      <c r="L43" s="1"/>
+    </row>
+    <row r="44" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
+      <c r="L44" s="1"/>
+    </row>
+    <row r="45" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+      <c r="L45" s="1"/>
+    </row>
+    <row r="46" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+      <c r="L46" s="1"/>
+    </row>
+    <row r="47" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="1"/>
+    </row>
+    <row r="48" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
+      <c r="L48" s="1"/>
+    </row>
+    <row r="49" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
+      <c r="L49" s="1"/>
+    </row>
+    <row r="50" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+      <c r="L50" s="1"/>
+    </row>
+    <row r="51" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+      <c r="L51" s="1"/>
+    </row>
+    <row r="52" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
+      <c r="L52" s="1"/>
+    </row>
+    <row r="53" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
+      <c r="L53" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -604,7 +1058,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A4" sqref="A4:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -735,7 +1189,46 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D4" s="1"/>
+      <c r="A4" s="3">
+        <f>Data!A4</f>
+        <v>602</v>
+      </c>
+      <c r="B4" s="4" t="str">
+        <f>Data!B4</f>
+        <v>Global warming</v>
+      </c>
+      <c r="C4" s="5" t="str">
+        <f>Data!H4</f>
+        <v>Steve</v>
+      </c>
+      <c r="D4" s="1">
+        <f>IF(Data!I4=Data!$G4,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <f>IF(Data!J4=Data!$G4,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <f>IF(Data!K4=Data!$G4,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <f>IF(Data!L4=Data!$G4,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H4" s="1" t="e">
+        <f>IF(Data!M4=Data!$G4,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I4" s="1" t="e">
+        <f>IF(Data!N4=Data!$G4,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J4" s="1">
+        <f>IF(SUMIF(D4:I4,"&lt;&gt;#N/A")=0, 1, 0)</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -745,62 +1238,68 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="str">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="str">
         <f>Results!D1</f>
         <v>Bob</v>
       </c>
-      <c r="B1" s="2" t="str">
+      <c r="C1" s="2" t="str">
         <f>Results!E1</f>
         <v>Kara</v>
       </c>
-      <c r="C1" s="2" t="str">
+      <c r="D1" s="2" t="str">
         <f>Results!F1</f>
         <v>Jay</v>
       </c>
-      <c r="D1" s="2" t="str">
+      <c r="E1" s="2" t="str">
         <f>Results!G1</f>
         <v>Evan</v>
       </c>
-      <c r="E1" s="2" t="str">
+      <c r="F1" s="2" t="str">
         <f>Results!H1</f>
         <v>George</v>
       </c>
-      <c r="F1" s="2" t="str">
+      <c r="G1" s="2" t="str">
         <f>Results!I1</f>
         <v>Steve</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="6">
         <f>SUMIF(Results!D2:D52,"&lt;&gt;#N/A")/COUNTIFS(Results!D2:D52,"&lt;&gt;#N/A",Results!D2:D52,"&lt;&gt;")</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C2" s="6">
+        <f>SUMIF(Results!E2:E52,"&lt;&gt;#N/A")/COUNTIFS(Results!E2:E52,"&lt;&gt;#N/A",Results!E2:E52,"&lt;&gt;")</f>
         <v>0.5</v>
       </c>
-      <c r="B2" s="6">
-        <f>SUMIF(Results!E2:E52,"&lt;&gt;#N/A")/COUNTIFS(Results!E2:E52,"&lt;&gt;#N/A",Results!E2:E52,"&lt;&gt;")</f>
-        <v>0</v>
-      </c>
-      <c r="C2" s="6">
+      <c r="D2" s="6">
         <f>SUMIF(Results!F2:F52,"&lt;&gt;#N/A")/COUNTIFS(Results!F2:F52,"&lt;&gt;#N/A",Results!F2:F52,"&lt;&gt;")</f>
-        <v>0.5</v>
-      </c>
-      <c r="D2" s="6">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E2" s="6">
         <f>SUMIF(Results!G2:G52,"&lt;&gt;#N/A")/COUNTIFS(Results!G2:G52,"&lt;&gt;#N/A",Results!G2:G52,"&lt;&gt;")</f>
-        <v>0.5</v>
-      </c>
-      <c r="E2" s="6">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F2" s="6">
         <f>SUMIF(Results!H2:H52,"&lt;&gt;#N/A")/COUNTIFS(Results!H2:H52,"&lt;&gt;#N/A",Results!H2:H52,"&lt;&gt;")</f>
         <v>0</v>
       </c>
-      <c r="F2" s="6" t="e">
+      <c r="G2" s="6" t="e">
         <f>SUMIF(Results!I2:I52,"&lt;&gt;#N/A")/COUNTIFS(Results!I2:I52,"&lt;&gt;#N/A",Results!I2:I52,"&lt;&gt;")</f>
         <v>#DIV/0!</v>
       </c>

</xml_diff>

<commit_message>
updated after episode 602 + additional summarizations
</commit_message>
<xml_diff>
--- a/SGU_Science_or_Fiction.xlsx
+++ b/SGU_Science_or_Fiction.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
   <si>
     <t>Episode</t>
   </si>
@@ -49,9 +49,6 @@
     <t>Bob</t>
   </si>
   <si>
-    <t>Kara</t>
-  </si>
-  <si>
     <t>Jay</t>
   </si>
   <si>
@@ -106,7 +103,43 @@
     <t>Climate models show that even if CO2 emissions were stopped entirely, global temperatures would continue to rise for at least a century</t>
   </si>
   <si>
-    <t>Overall % Wins</t>
+    <t>Cara</t>
+  </si>
+  <si>
+    <t>% Wins Overall</t>
+  </si>
+  <si>
+    <t>% Wins with Themes</t>
+  </si>
+  <si>
+    <t>% Wins without Themes</t>
+  </si>
+  <si>
+    <t>Longest Winning Streak</t>
+  </si>
+  <si>
+    <t>Longest Losing Streak</t>
+  </si>
+  <si>
+    <t>CorrectPanelist</t>
+  </si>
+  <si>
+    <t>% Correct Guesses with Theme</t>
+  </si>
+  <si>
+    <t>% Correct Guesses without Theme</t>
+  </si>
+  <si>
+    <t>Summary Across All Panelists</t>
+  </si>
+  <si>
+    <t>Consecutive Wins</t>
+  </si>
+  <si>
+    <t>Consecutive Losses</t>
+  </si>
+  <si>
+    <t>Panelists</t>
   </si>
 </sst>
 </file>
@@ -116,7 +149,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,13 +172,53 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -157,11 +230,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -177,8 +252,29 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="3" builtinId="27"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -461,7 +557,7 @@
   <dimension ref="A1:N53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,7 +570,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -486,7 +582,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>4</v>
@@ -498,19 +594,19 @@
         <v>6</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="N1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -518,16 +614,16 @@
         <v>600</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
       </c>
       <c r="F2" s="1" t="e">
         <f>NA()</f>
@@ -537,7 +633,7 @@
         <v>2</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I2" s="1">
         <v>1</v>
@@ -569,13 +665,13 @@
         <v>#N/A</v>
       </c>
       <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>20</v>
-      </c>
-      <c r="E3" t="s">
-        <v>21</v>
       </c>
       <c r="F3" t="e">
         <f>NA()</f>
@@ -585,7 +681,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I3" s="1">
         <v>1</v>
@@ -613,16 +709,16 @@
         <v>602</v>
       </c>
       <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>23</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>24</v>
-      </c>
-      <c r="E4" t="s">
-        <v>25</v>
       </c>
       <c r="F4" t="e">
         <f>NA()</f>
@@ -632,7 +728,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I4" s="1">
         <v>2</v>
@@ -1055,182 +1151,417 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:X5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:J4"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="11" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="str">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="M1" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="str">
         <f>Data!A1</f>
         <v>Episode</v>
       </c>
-      <c r="B1" s="2" t="str">
+      <c r="B2" s="2" t="str">
         <f>Data!B1</f>
         <v>Theme</v>
       </c>
-      <c r="C1" s="2" t="str">
+      <c r="C2" s="2" t="str">
         <f>Data!H1</f>
         <v>Host</v>
       </c>
-      <c r="D1" s="2" t="str">
+      <c r="D2" s="2" t="str">
         <f>Data!I1</f>
         <v>Bob</v>
       </c>
-      <c r="E1" s="2" t="str">
+      <c r="E2" s="2" t="str">
         <f>Data!J1</f>
-        <v>Kara</v>
-      </c>
-      <c r="F1" s="2" t="str">
+        <v>Cara</v>
+      </c>
+      <c r="F2" s="2" t="str">
         <f>Data!K1</f>
         <v>Jay</v>
       </c>
-      <c r="G1" s="2" t="str">
+      <c r="G2" s="2" t="str">
         <f>Data!L1</f>
         <v>Evan</v>
       </c>
-      <c r="H1" s="2" t="str">
+      <c r="H2" s="2" t="str">
         <f>Data!M1</f>
         <v>George</v>
       </c>
-      <c r="I1" s="2" t="str">
+      <c r="I2" s="2" t="str">
         <f>Data!N1</f>
         <v>Steve</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="J2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="10" t="str">
+        <f>D2</f>
+        <v>Bob</v>
+      </c>
+      <c r="N2" s="10" t="str">
+        <f t="shared" ref="N2:R2" si="0">E2</f>
+        <v>Cara</v>
+      </c>
+      <c r="O2" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>Jay</v>
+      </c>
+      <c r="P2" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>Evan</v>
+      </c>
+      <c r="Q2" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>George</v>
+      </c>
+      <c r="R2" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>Steve</v>
+      </c>
+      <c r="S2" s="13" t="str">
+        <f>M2</f>
+        <v>Bob</v>
+      </c>
+      <c r="T2" s="13" t="str">
+        <f>N2</f>
+        <v>Cara</v>
+      </c>
+      <c r="U2" s="13" t="str">
+        <f t="shared" ref="U2:X2" si="1">O2</f>
+        <v>Jay</v>
+      </c>
+      <c r="V2" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>Evan</v>
+      </c>
+      <c r="W2" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>George</v>
+      </c>
+      <c r="X2" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>Steve</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
         <f>Data!A2</f>
         <v>600</v>
       </c>
-      <c r="B2" s="4" t="str">
+      <c r="B3" s="4" t="str">
         <f>Data!B2</f>
         <v>Inventors</v>
       </c>
-      <c r="C2" s="5" t="str">
+      <c r="C3" s="5" t="str">
         <f>Data!H2</f>
         <v>Steve</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D3" s="1">
         <f>IF(Data!I2=Data!$G2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="E2" s="1" t="e">
+      <c r="E3" s="1" t="e">
         <f>IF(Data!J2=Data!$G2,1,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F3" s="1">
         <f>IF(Data!K2=Data!$G2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G3" s="1">
         <f>IF(Data!L2=Data!$G2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H3" s="1">
         <f>IF(Data!M2=Data!$G2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="I2" s="1" t="e">
+      <c r="I3" s="1" t="e">
         <f>IF(Data!N2=Data!$G2,1,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="J2" s="1">
-        <f>IF(SUMIF(D2:I2,"&lt;&gt;#N/A")=0, 1, 0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="J3" s="1">
+        <f>COUNTIF(D3:I3,"&lt;&gt;#N/A")</f>
+        <v>4</v>
+      </c>
+      <c r="K3" s="1">
+        <f>SUMIF(D3:I3,"&lt;&gt;#N/A")</f>
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
+        <f>IF(SUMIF(D3:I3,"&lt;&gt;#N/A")=0, 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="M3" s="8">
+        <v>0</v>
+      </c>
+      <c r="N3" s="8">
+        <v>0</v>
+      </c>
+      <c r="O3" s="8">
+        <v>0</v>
+      </c>
+      <c r="P3" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="8">
+        <v>0</v>
+      </c>
+      <c r="R3" s="8">
+        <v>0</v>
+      </c>
+      <c r="S3" s="11">
+        <v>1</v>
+      </c>
+      <c r="T3" s="11">
+        <v>0</v>
+      </c>
+      <c r="U3" s="11">
+        <v>1</v>
+      </c>
+      <c r="V3" s="11">
+        <v>1</v>
+      </c>
+      <c r="W3" s="11">
+        <v>1</v>
+      </c>
+      <c r="X3" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
         <f>Data!A3</f>
         <v>601</v>
       </c>
-      <c r="B3" s="4" t="e">
+      <c r="B4" s="4" t="e">
         <f>Data!B3</f>
         <v>#N/A</v>
       </c>
-      <c r="C3" s="5" t="str">
+      <c r="C4" s="5" t="str">
         <f>Data!H3</f>
         <v>Steve</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D4" s="1">
         <f>IF(Data!I3=Data!$G3,1,0)</f>
         <v>1</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E4" s="1">
         <f>IF(Data!J3=Data!$G3,1,0)</f>
         <v>0</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F4" s="1">
         <f>IF(Data!K3=Data!$G3,1,0)</f>
         <v>1</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G4" s="1">
         <f>IF(Data!L3=Data!$G3,1,0)</f>
         <v>1</v>
       </c>
-      <c r="H3" s="1" t="e">
+      <c r="H4" s="1" t="e">
         <f>IF(Data!M3=Data!$G3,1,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="I3" s="1" t="e">
+      <c r="I4" s="1" t="e">
         <f>IF(Data!N3=Data!$G3,1,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="J3" s="1">
-        <f>IF(SUMIF(D3:I3,"&lt;&gt;#N/A")=0, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="J4" s="1">
+        <f t="shared" ref="J4:J5" si="2">COUNTIF(D4:I4,"&lt;&gt;#N/A")</f>
+        <v>4</v>
+      </c>
+      <c r="K4" s="1">
+        <f t="shared" ref="K4:K5" si="3">SUMIF(D4:I4,"&lt;&gt;#N/A")</f>
+        <v>3</v>
+      </c>
+      <c r="L4" s="1">
+        <f>IF(SUMIF(D4:I4,"&lt;&gt;#N/A")=0, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M4" s="8">
+        <f t="shared" ref="M4:M5" si="4">IF(ISNA(D4),M3,IF(D4=1,M3+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="N4" s="8">
+        <f t="shared" ref="N4:N5" si="5">IF(ISNA(E4),N3,IF(E4=1,N3+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="O4" s="8">
+        <f t="shared" ref="O4:O5" si="6">IF(ISNA(F4),O3,IF(F4=1,O3+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="P4" s="8">
+        <f t="shared" ref="P4:P5" si="7">IF(ISNA(G4),P3,IF(G4=1,P3+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="Q4" s="8">
+        <f>IF(ISNA(H4),Q3,IF(H4=1,Q3+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="R4" s="8">
+        <f t="shared" ref="R4:R5" si="8">IF(ISNA(I4),R3,IF(I4=1,R3+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="S4" s="11">
+        <f>IF(ISNA(D4),S3,IF(D4=0,S3+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="T4" s="11">
+        <f>IF(ISNA(E4),T3,IF(E4=0,T3+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="U4" s="11">
+        <f t="shared" ref="U4:X5" si="9">IF(ISNA(F4),U3,IF(F4=0,U3+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="V4" s="11">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="W4" s="11">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="X4" s="11">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <f>Data!A4</f>
         <v>602</v>
       </c>
-      <c r="B4" s="4" t="str">
+      <c r="B5" s="4" t="str">
         <f>Data!B4</f>
         <v>Global warming</v>
       </c>
-      <c r="C4" s="5" t="str">
+      <c r="C5" s="5" t="str">
         <f>Data!H4</f>
         <v>Steve</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D5" s="1">
         <f>IF(Data!I4=Data!$G4,1,0)</f>
         <v>0</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E5" s="1">
         <f>IF(Data!J4=Data!$G4,1,0)</f>
         <v>1</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F5" s="1">
         <f>IF(Data!K4=Data!$G4,1,0)</f>
         <v>1</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G5" s="1">
         <f>IF(Data!L4=Data!$G4,1,0)</f>
         <v>1</v>
       </c>
-      <c r="H4" s="1" t="e">
+      <c r="H5" s="1" t="e">
         <f>IF(Data!M4=Data!$G4,1,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="I4" s="1" t="e">
+      <c r="I5" s="1" t="e">
         <f>IF(Data!N4=Data!$G4,1,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="J4" s="1">
-        <f>IF(SUMIF(D4:I4,"&lt;&gt;#N/A")=0, 1, 0)</f>
+      <c r="J5" s="1">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="K5" s="1">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="L5" s="1">
+        <f>IF(SUMIF(D5:I5,"&lt;&gt;#N/A")=0, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M5" s="8">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N5" s="8">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O5" s="8">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="P5" s="8">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="Q5" s="8">
+        <f t="shared" ref="Q5" si="10">IF(ISNA(H5),Q4,IF(H5=1,Q4+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="R5" s="8">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="S5" s="11">
+        <f>IF(ISNA(D5),S4,IF(D5=0,S4+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="T5" s="11">
+        <f>IF(ISNA(E5),T4,IF(E5=0,T4+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="U5" s="11">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="V5" s="11">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="W5" s="11">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="X5" s="11">
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="M1:R1"/>
+    <mergeCell ref="S1:X1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
@@ -1238,40 +1569,40 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="1" max="1" width="33.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="str">
-        <f>Results!D1</f>
+        <f>Results!D2</f>
         <v>Bob</v>
       </c>
       <c r="C1" s="2" t="str">
-        <f>Results!E1</f>
-        <v>Kara</v>
+        <f>Results!E2</f>
+        <v>Cara</v>
       </c>
       <c r="D1" s="2" t="str">
-        <f>Results!F1</f>
+        <f>Results!F2</f>
         <v>Jay</v>
       </c>
       <c r="E1" s="2" t="str">
-        <f>Results!G1</f>
+        <f>Results!G2</f>
         <v>Evan</v>
       </c>
       <c r="F1" s="2" t="str">
-        <f>Results!H1</f>
+        <f>Results!H2</f>
         <v>George</v>
       </c>
       <c r="G1" s="2" t="str">
-        <f>Results!I1</f>
+        <f>Results!I2</f>
         <v>Steve</v>
       </c>
     </row>
@@ -1280,28 +1611,167 @@
         <v>26</v>
       </c>
       <c r="B2" s="6">
-        <f>SUMIF(Results!D2:D52,"&lt;&gt;#N/A")/COUNTIFS(Results!D2:D52,"&lt;&gt;#N/A",Results!D2:D52,"&lt;&gt;")</f>
+        <f>SUMIF(Results!D3:D53,"&lt;&gt;#N/A")/COUNTIFS(Results!D3:D53,"&lt;&gt;#N/A",Results!D3:D53,"&lt;&gt;")</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="C2" s="6">
-        <f>SUMIF(Results!E2:E52,"&lt;&gt;#N/A")/COUNTIFS(Results!E2:E52,"&lt;&gt;#N/A",Results!E2:E52,"&lt;&gt;")</f>
+        <f>SUMIF(Results!E3:E53,"&lt;&gt;#N/A")/COUNTIFS(Results!E3:E53,"&lt;&gt;#N/A",Results!E3:E53,"&lt;&gt;")</f>
         <v>0.5</v>
       </c>
       <c r="D2" s="6">
-        <f>SUMIF(Results!F2:F52,"&lt;&gt;#N/A")/COUNTIFS(Results!F2:F52,"&lt;&gt;#N/A",Results!F2:F52,"&lt;&gt;")</f>
+        <f>SUMIF(Results!F3:F53,"&lt;&gt;#N/A")/COUNTIFS(Results!F3:F53,"&lt;&gt;#N/A",Results!F3:F53,"&lt;&gt;")</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="E2" s="6">
-        <f>SUMIF(Results!G2:G52,"&lt;&gt;#N/A")/COUNTIFS(Results!G2:G52,"&lt;&gt;#N/A",Results!G2:G52,"&lt;&gt;")</f>
+        <f>SUMIF(Results!G3:G53,"&lt;&gt;#N/A")/COUNTIFS(Results!G3:G53,"&lt;&gt;#N/A",Results!G3:G53,"&lt;&gt;")</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="F2" s="6">
-        <f>SUMIF(Results!H2:H52,"&lt;&gt;#N/A")/COUNTIFS(Results!H2:H52,"&lt;&gt;#N/A",Results!H2:H52,"&lt;&gt;")</f>
+        <f>SUMIF(Results!H3:H53,"&lt;&gt;#N/A")/COUNTIFS(Results!H3:H53,"&lt;&gt;#N/A",Results!H3:H53,"&lt;&gt;")</f>
         <v>0</v>
       </c>
       <c r="G2" s="6" t="e">
-        <f>SUMIF(Results!I2:I52,"&lt;&gt;#N/A")/COUNTIFS(Results!I2:I52,"&lt;&gt;#N/A",Results!I2:I52,"&lt;&gt;")</f>
+        <f>SUMIF(Results!I3:I53,"&lt;&gt;#N/A")/COUNTIFS(Results!I3:I53,"&lt;&gt;#N/A",Results!I3:I53,"&lt;&gt;")</f>
         <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="6">
+        <f>SUMIFS(Results!D3:D53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!D3:D53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!D3:D53, "&lt;&gt;#N/A", Results!D3:D53, "&lt;&gt;")</f>
+        <v>0</v>
+      </c>
+      <c r="C3" s="6">
+        <f>SUMIFS(Results!E3:E53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!E3:E53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!E3:E53, "&lt;&gt;#N/A", Results!E3:E53, "&lt;&gt;")</f>
+        <v>1</v>
+      </c>
+      <c r="D3" s="6">
+        <f>SUMIFS(Results!F3:F53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!F3:F53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!F3:F53, "&lt;&gt;#N/A", Results!F3:F53, "&lt;&gt;")</f>
+        <v>0.5</v>
+      </c>
+      <c r="E3" s="6">
+        <f>SUMIFS(Results!G3:G53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!G3:G53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!G3:G53, "&lt;&gt;#N/A", Results!G3:G53, "&lt;&gt;")</f>
+        <v>0.5</v>
+      </c>
+      <c r="F3" s="6">
+        <f>SUMIFS(Results!H3:H53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!H3:H53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!H3:H53, "&lt;&gt;#N/A", Results!H3:H53, "&lt;&gt;")</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="6" t="e">
+        <f>SUMIFS(Results!I3:I53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!I3:I53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!I3:I53, "&lt;&gt;#N/A", Results!I3:I53, "&lt;&gt;")</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="6">
+        <f>SUMIFS(Results!D3:D53,Results!$B$3:$B$53,"=#N/A",Results!D3:D53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!D3:D53, "&lt;&gt;#N/A", Results!D3:D53, "&lt;&gt;")</f>
+        <v>1</v>
+      </c>
+      <c r="C4" s="6">
+        <f>SUMIFS(Results!E3:E53,Results!$B$3:$B$53,"=#N/A",Results!E3:E53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!E3:E53, "&lt;&gt;#N/A", Results!E3:E53, "&lt;&gt;")</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="6">
+        <f>SUMIFS(Results!F3:F53,Results!$B$3:$B$53,"=#N/A",Results!F3:F53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!F3:F53, "&lt;&gt;#N/A", Results!F3:F53, "&lt;&gt;")</f>
+        <v>1</v>
+      </c>
+      <c r="E4" s="6">
+        <f>SUMIFS(Results!G3:G53,Results!$B$3:$B$53,"=#N/A",Results!G3:G53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!G3:G53, "&lt;&gt;#N/A", Results!G3:G53, "&lt;&gt;")</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="6" t="e">
+        <f>SUMIFS(Results!H3:H53,Results!$B$3:$B$53,"=#N/A",Results!H3:H53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!H3:H53, "&lt;&gt;#N/A", Results!H3:H53, "&lt;&gt;")</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G4" s="6" t="e">
+        <f>SUMIFS(Results!I3:I53,Results!$B$3:$B$53,"=#N/A",Results!I3:I53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!I3:I53, "&lt;&gt;#N/A", Results!I3:I53, "&lt;&gt;")</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="1">
+        <f>MAX(Results!M3:M52)</f>
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <f>MAX(Results!N3:N52)</f>
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <f>MAX(Results!O3:O52)</f>
+        <v>2</v>
+      </c>
+      <c r="E5" s="1">
+        <f>MAX(Results!P3:P52)</f>
+        <v>2</v>
+      </c>
+      <c r="F5" s="1">
+        <f>MAX(Results!Q3:Q52)</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <f>MAX(Results!R3:R52)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="1">
+        <f>MAX(Results!S3:S52)</f>
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <f>MAX(Results!T3:T52)</f>
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <f>MAX(Results!U3:U52)</f>
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <f>MAX(Results!V3:V52)</f>
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <f>MAX(Results!W3:W52)</f>
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <f>MAX(Results!X3:X52)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="7">
+        <f>SUMIF(Results!B3:B53,"&lt;&gt;#N/A",Results!K3:K53)/SUMIF(Results!B3:B53,"&lt;&gt;#N/A",Results!J3:J53)</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="7">
+        <f>SUMIF(Results!B3:B53,"=#N/A",Results!K3:K53)/SUMIF(Results!B3:B53,"=#N/A",Results!J3:J53)</f>
+        <v>0.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated after episode 603 + Lone Wolf summarization
</commit_message>
<xml_diff>
--- a/SGU_Science_or_Fiction.xlsx
+++ b/SGU_Science_or_Fiction.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>Episode</t>
   </si>
@@ -140,6 +140,27 @@
   </si>
   <si>
     <t>Panelists</t>
+  </si>
+  <si>
+    <t>Extinct Species</t>
+  </si>
+  <si>
+    <t>The Great Auk was a large flightless sea bird resembling a penguin but living in the North Atlantic. It was driven to extinction by over-hunting in 1844.</t>
+  </si>
+  <si>
+    <t>The Swift Fox was driven to extinction in the 1930s as part of a deliberate program of predator control in the United States.</t>
+  </si>
+  <si>
+    <t>The Golden Toad was a common species in Costa Rica, but its population steadily declined with the last sighting in 1989. This was the first species extinction blamed on global warming, but later evidence has cast doubt on that conclusion.</t>
+  </si>
+  <si>
+    <t>The Zanzibar Leopard once inhabited the Zanzibar archipelago in Tanzania, but was deliberated hunted to extinction because they were thought to be the servants of witches</t>
+  </si>
+  <si>
+    <t>Lone Wolf</t>
+  </si>
+  <si>
+    <t>Lone Wolf Wins</t>
   </si>
 </sst>
 </file>
@@ -259,13 +280,13 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
@@ -557,7 +578,7 @@
   <dimension ref="A1:N53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -752,12 +773,50 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
+      <c r="A5">
+        <v>603</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="1">
+        <v>2</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="1">
+        <v>4</v>
+      </c>
+      <c r="J5" s="1">
+        <v>2</v>
+      </c>
+      <c r="K5" s="1">
+        <v>2</v>
+      </c>
+      <c r="L5" s="1">
+        <v>2</v>
+      </c>
+      <c r="M5" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N5" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G6" s="1"/>
@@ -1151,36 +1210,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X5"/>
+  <dimension ref="A1:Y6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3:M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="11" max="11" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="M1" s="9" t="s">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="N1" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="12" t="s">
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12"/>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="13"/>
+      <c r="X1" s="13"/>
+      <c r="Y1" s="13"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="str">
         <f>Data!A1</f>
         <v>Episode</v>
@@ -1226,56 +1286,59 @@
       <c r="L2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="10" t="str">
+      <c r="M2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N2" s="9" t="str">
         <f>D2</f>
         <v>Bob</v>
       </c>
-      <c r="N2" s="10" t="str">
-        <f t="shared" ref="N2:R2" si="0">E2</f>
+      <c r="O2" s="9" t="str">
+        <f>E2</f>
         <v>Cara</v>
       </c>
-      <c r="O2" s="10" t="str">
-        <f t="shared" si="0"/>
+      <c r="P2" s="9" t="str">
+        <f>F2</f>
         <v>Jay</v>
       </c>
-      <c r="P2" s="10" t="str">
+      <c r="Q2" s="9" t="str">
+        <f>G2</f>
+        <v>Evan</v>
+      </c>
+      <c r="R2" s="9" t="str">
+        <f>H2</f>
+        <v>George</v>
+      </c>
+      <c r="S2" s="9" t="str">
+        <f>I2</f>
+        <v>Steve</v>
+      </c>
+      <c r="T2" s="11" t="str">
+        <f>N2</f>
+        <v>Bob</v>
+      </c>
+      <c r="U2" s="11" t="str">
+        <f>O2</f>
+        <v>Cara</v>
+      </c>
+      <c r="V2" s="11" t="str">
+        <f t="shared" ref="V2:Y2" si="0">P2</f>
+        <v>Jay</v>
+      </c>
+      <c r="W2" s="11" t="str">
         <f t="shared" si="0"/>
         <v>Evan</v>
       </c>
-      <c r="Q2" s="10" t="str">
+      <c r="X2" s="11" t="str">
         <f t="shared" si="0"/>
         <v>George</v>
       </c>
-      <c r="R2" s="10" t="str">
+      <c r="Y2" s="11" t="str">
         <f t="shared" si="0"/>
         <v>Steve</v>
       </c>
-      <c r="S2" s="13" t="str">
-        <f>M2</f>
-        <v>Bob</v>
-      </c>
-      <c r="T2" s="13" t="str">
-        <f>N2</f>
-        <v>Cara</v>
-      </c>
-      <c r="U2" s="13" t="str">
-        <f t="shared" ref="U2:X2" si="1">O2</f>
-        <v>Jay</v>
-      </c>
-      <c r="V2" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>Evan</v>
-      </c>
-      <c r="W2" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>George</v>
-      </c>
-      <c r="X2" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>Steve</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <f>Data!A2</f>
         <v>600</v>
@@ -1324,8 +1387,9 @@
         <f>IF(SUMIF(D3:I3,"&lt;&gt;#N/A")=0, 1, 0)</f>
         <v>1</v>
       </c>
-      <c r="M3" s="8">
-        <v>0</v>
+      <c r="M3" s="1" t="e">
+        <f t="shared" ref="M3:M6" si="1">IF(K3=1,INDEX($D$2:$I$2,1,MATCH(1,D3:I3,0)),NA())</f>
+        <v>#N/A</v>
       </c>
       <c r="N3" s="8">
         <v>0</v>
@@ -1342,26 +1406,29 @@
       <c r="R3" s="8">
         <v>0</v>
       </c>
-      <c r="S3" s="11">
-        <v>1</v>
-      </c>
-      <c r="T3" s="11">
-        <v>0</v>
-      </c>
-      <c r="U3" s="11">
-        <v>1</v>
-      </c>
-      <c r="V3" s="11">
-        <v>1</v>
-      </c>
-      <c r="W3" s="11">
-        <v>1</v>
-      </c>
-      <c r="X3" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S3" s="8">
+        <v>0</v>
+      </c>
+      <c r="T3" s="10">
+        <v>1</v>
+      </c>
+      <c r="U3" s="10">
+        <v>0</v>
+      </c>
+      <c r="V3" s="10">
+        <v>1</v>
+      </c>
+      <c r="W3" s="10">
+        <v>1</v>
+      </c>
+      <c r="X3" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <f>Data!A3</f>
         <v>601</v>
@@ -1410,56 +1477,60 @@
         <f>IF(SUMIF(D4:I4,"&lt;&gt;#N/A")=0, 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="M4" s="8">
-        <f t="shared" ref="M4:M5" si="4">IF(ISNA(D4),M3,IF(D4=1,M3+1,0))</f>
-        <v>1</v>
+      <c r="M4" s="1" t="e">
+        <f>IF(K4=1,INDEX($D$2:$I$2,1,MATCH(1,D4:I4,0)),NA())</f>
+        <v>#N/A</v>
       </c>
       <c r="N4" s="8">
-        <f t="shared" ref="N4:N5" si="5">IF(ISNA(E4),N3,IF(E4=1,N3+1,0))</f>
-        <v>0</v>
+        <f t="shared" ref="N4:N5" si="4">IF(ISNA(D4),N3,IF(D4=1,N3+1,0))</f>
+        <v>1</v>
       </c>
       <c r="O4" s="8">
-        <f t="shared" ref="O4:O5" si="6">IF(ISNA(F4),O3,IF(F4=1,O3+1,0))</f>
-        <v>1</v>
+        <f t="shared" ref="O4:O5" si="5">IF(ISNA(E4),O3,IF(E4=1,O3+1,0))</f>
+        <v>0</v>
       </c>
       <c r="P4" s="8">
-        <f t="shared" ref="P4:P5" si="7">IF(ISNA(G4),P3,IF(G4=1,P3+1,0))</f>
+        <f t="shared" ref="P4:P5" si="6">IF(ISNA(F4),P3,IF(F4=1,P3+1,0))</f>
         <v>1</v>
       </c>
       <c r="Q4" s="8">
-        <f>IF(ISNA(H4),Q3,IF(H4=1,Q3+1,0))</f>
-        <v>0</v>
+        <f t="shared" ref="Q4:Q5" si="7">IF(ISNA(G4),Q3,IF(G4=1,Q3+1,0))</f>
+        <v>1</v>
       </c>
       <c r="R4" s="8">
-        <f t="shared" ref="R4:R5" si="8">IF(ISNA(I4),R3,IF(I4=1,R3+1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="S4" s="11">
-        <f>IF(ISNA(D4),S3,IF(D4=0,S3+1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="T4" s="11">
-        <f>IF(ISNA(E4),T3,IF(E4=0,T3+1,0))</f>
-        <v>1</v>
-      </c>
-      <c r="U4" s="11">
-        <f t="shared" ref="U4:X5" si="9">IF(ISNA(F4),U3,IF(F4=0,U3+1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="V4" s="11">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="W4" s="11">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="X4" s="11">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+        <f>IF(ISNA(H4),R3,IF(H4=1,R3+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="S4" s="8">
+        <f t="shared" ref="S4:S5" si="8">IF(ISNA(I4),S3,IF(I4=1,S3+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="T4" s="10">
+        <f>IF(ISNA(D4),T3,IF(D4=0,T3+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="U4" s="10">
+        <f>IF(ISNA(E4),U3,IF(E4=0,U3+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="V4" s="10">
+        <f>IF(ISNA(F4),V3,IF(F4=0,V3+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="W4" s="10">
+        <f>IF(ISNA(G4),W3,IF(G4=0,W3+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="X4" s="10">
+        <f>IF(ISNA(H4),X3,IF(H4=0,X3+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="Y4" s="10">
+        <f>IF(ISNA(I4),Y3,IF(I4=0,Y3+1,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <f>Data!A4</f>
         <v>602</v>
@@ -1508,59 +1579,165 @@
         <f>IF(SUMIF(D5:I5,"&lt;&gt;#N/A")=0, 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="M5" s="8">
+      <c r="M5" s="1" t="e">
+        <f t="shared" ref="M5:M6" si="9">IF(K5=1,INDEX($D$2:$I$2,1,MATCH(1,D5:I5,0)),NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N5" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="N5" s="8">
+      <c r="O5" s="8">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="O5" s="8">
+      <c r="P5" s="8">
         <f t="shared" si="6"/>
         <v>2</v>
       </c>
-      <c r="P5" s="8">
+      <c r="Q5" s="8">
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
-      <c r="Q5" s="8">
-        <f t="shared" ref="Q5" si="10">IF(ISNA(H5),Q4,IF(H5=1,Q4+1,0))</f>
-        <v>0</v>
-      </c>
       <c r="R5" s="8">
+        <f t="shared" ref="R5" si="10">IF(ISNA(H5),R4,IF(H5=1,R4+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="S5" s="8">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S5" s="11">
-        <f>IF(ISNA(D5),S4,IF(D5=0,S4+1,0))</f>
-        <v>1</v>
-      </c>
-      <c r="T5" s="11">
-        <f>IF(ISNA(E5),T4,IF(E5=0,T4+1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="U5" s="11">
+      <c r="T5" s="10">
+        <f>IF(ISNA(D5),T4,IF(D5=0,T4+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="U5" s="10">
+        <f>IF(ISNA(E5),U4,IF(E5=0,U4+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="V5" s="10">
+        <f>IF(ISNA(F5),V4,IF(F5=0,V4+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="W5" s="10">
+        <f>IF(ISNA(G5),W4,IF(G5=0,W4+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="X5" s="10">
+        <f>IF(ISNA(H5),X4,IF(H5=0,X4+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="Y5" s="10">
+        <f>IF(ISNA(I5),Y4,IF(I5=0,Y4+1,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <f>Data!A5</f>
+        <v>603</v>
+      </c>
+      <c r="B6" s="4" t="str">
+        <f>Data!B5</f>
+        <v>Extinct Species</v>
+      </c>
+      <c r="C6" s="5" t="str">
+        <f>Data!H5</f>
+        <v>Steve</v>
+      </c>
+      <c r="D6" s="1">
+        <f>IF(Data!I5=Data!$G5,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <f>IF(Data!J5=Data!$G5,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <f>IF(Data!K5=Data!$G5,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <f>IF(Data!L5=Data!$G5,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H6" s="1" t="e">
+        <f>IF(Data!M5=Data!$G5,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I6" s="1" t="e">
+        <f>IF(Data!N5=Data!$G5,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" ref="J6" si="11">COUNTIF(D6:I6,"&lt;&gt;#N/A")</f>
+        <v>4</v>
+      </c>
+      <c r="K6" s="1">
+        <f t="shared" ref="K6" si="12">SUMIF(D6:I6,"&lt;&gt;#N/A")</f>
+        <v>3</v>
+      </c>
+      <c r="L6" s="1">
+        <f>IF(SUMIF(D6:I6,"&lt;&gt;#N/A")=0, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M6" s="1" t="e">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="V5" s="11">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="W5" s="11">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="X5" s="11">
-        <f t="shared" si="9"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N6" s="8">
+        <f t="shared" ref="N6" si="13">IF(ISNA(D6),N5,IF(D6=1,N5+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="O6" s="8">
+        <f t="shared" ref="O6" si="14">IF(ISNA(E6),O5,IF(E6=1,O5+1,0))</f>
+        <v>2</v>
+      </c>
+      <c r="P6" s="8">
+        <f t="shared" ref="P6" si="15">IF(ISNA(F6),P5,IF(F6=1,P5+1,0))</f>
+        <v>3</v>
+      </c>
+      <c r="Q6" s="8">
+        <f t="shared" ref="Q6" si="16">IF(ISNA(G6),Q5,IF(G6=1,Q5+1,0))</f>
+        <v>3</v>
+      </c>
+      <c r="R6" s="8">
+        <f t="shared" ref="R6" si="17">IF(ISNA(H6),R5,IF(H6=1,R5+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="S6" s="8">
+        <f t="shared" ref="S6" si="18">IF(ISNA(I6),S5,IF(I6=1,S5+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="T6" s="10">
+        <f>IF(ISNA(D6),T5,IF(D6=0,T5+1,0))</f>
+        <v>2</v>
+      </c>
+      <c r="U6" s="10">
+        <f>IF(ISNA(E6),U5,IF(E6=0,U5+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="V6" s="10">
+        <f t="shared" ref="V6" si="19">IF(ISNA(F6),V5,IF(F6=0,V5+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="W6" s="10">
+        <f t="shared" ref="W6" si="20">IF(ISNA(G6),W5,IF(G6=0,W5+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="X6" s="10">
+        <f t="shared" ref="X6" si="21">IF(ISNA(H6),X5,IF(H6=0,X5+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="Y6" s="10">
+        <f t="shared" ref="Y6" si="22">IF(ISNA(I6),Y5,IF(I6=0,Y5+1,0))</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="M1:R1"/>
-    <mergeCell ref="S1:X1"/>
+    <mergeCell ref="N1:S1"/>
+    <mergeCell ref="T1:Y1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -1572,7 +1749,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1612,19 +1789,19 @@
       </c>
       <c r="B2" s="6">
         <f>SUMIF(Results!D3:D53,"&lt;&gt;#N/A")/COUNTIFS(Results!D3:D53,"&lt;&gt;#N/A",Results!D3:D53,"&lt;&gt;")</f>
-        <v>0.33333333333333331</v>
+        <v>0.25</v>
       </c>
       <c r="C2" s="6">
         <f>SUMIF(Results!E3:E53,"&lt;&gt;#N/A")/COUNTIFS(Results!E3:E53,"&lt;&gt;#N/A",Results!E3:E53,"&lt;&gt;")</f>
-        <v>0.5</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="D2" s="6">
         <f>SUMIF(Results!F3:F53,"&lt;&gt;#N/A")/COUNTIFS(Results!F3:F53,"&lt;&gt;#N/A",Results!F3:F53,"&lt;&gt;")</f>
-        <v>0.66666666666666663</v>
+        <v>0.75</v>
       </c>
       <c r="E2" s="6">
         <f>SUMIF(Results!G3:G53,"&lt;&gt;#N/A")/COUNTIFS(Results!G3:G53,"&lt;&gt;#N/A",Results!G3:G53,"&lt;&gt;")</f>
-        <v>0.66666666666666663</v>
+        <v>0.75</v>
       </c>
       <c r="F2" s="6">
         <f>SUMIF(Results!H3:H53,"&lt;&gt;#N/A")/COUNTIFS(Results!H3:H53,"&lt;&gt;#N/A",Results!H3:H53,"&lt;&gt;")</f>
@@ -1649,11 +1826,11 @@
       </c>
       <c r="D3" s="6">
         <f>SUMIFS(Results!F3:F53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!F3:F53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!F3:F53, "&lt;&gt;#N/A", Results!F3:F53, "&lt;&gt;")</f>
-        <v>0.5</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="E3" s="6">
         <f>SUMIFS(Results!G3:G53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!G3:G53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!G3:G53, "&lt;&gt;#N/A", Results!G3:G53, "&lt;&gt;")</f>
-        <v>0.5</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F3" s="6">
         <f>SUMIFS(Results!H3:H53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!H3:H53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!H3:H53, "&lt;&gt;#N/A", Results!H3:H53, "&lt;&gt;")</f>
@@ -1698,27 +1875,27 @@
         <v>29</v>
       </c>
       <c r="B5" s="1">
-        <f>MAX(Results!M3:M52)</f>
+        <f>MAX(Results!N3:N53)</f>
         <v>1</v>
       </c>
       <c r="C5" s="1">
-        <f>MAX(Results!N3:N52)</f>
-        <v>1</v>
+        <f>MAX(Results!O3:O53)</f>
+        <v>2</v>
       </c>
       <c r="D5" s="1">
-        <f>MAX(Results!O3:O52)</f>
-        <v>2</v>
+        <f>MAX(Results!P3:P53)</f>
+        <v>3</v>
       </c>
       <c r="E5" s="1">
-        <f>MAX(Results!P3:P52)</f>
-        <v>2</v>
+        <f>MAX(Results!Q3:Q53)</f>
+        <v>3</v>
       </c>
       <c r="F5" s="1">
-        <f>MAX(Results!Q3:Q52)</f>
+        <f>MAX(Results!R3:R53)</f>
         <v>0</v>
       </c>
       <c r="G5" s="1">
-        <f>MAX(Results!R3:R52)</f>
+        <f>MAX(Results!S3:S53)</f>
         <v>0</v>
       </c>
     </row>
@@ -1727,27 +1904,56 @@
         <v>30</v>
       </c>
       <c r="B6" s="1">
-        <f>MAX(Results!S3:S52)</f>
-        <v>1</v>
+        <f>MAX(Results!T3:T53)</f>
+        <v>2</v>
       </c>
       <c r="C6" s="1">
-        <f>MAX(Results!T3:T52)</f>
+        <f>MAX(Results!U3:U53)</f>
         <v>1</v>
       </c>
       <c r="D6" s="1">
-        <f>MAX(Results!U3:U52)</f>
+        <f>MAX(Results!V3:V53)</f>
         <v>1</v>
       </c>
       <c r="E6" s="1">
-        <f>MAX(Results!V3:V52)</f>
+        <f>MAX(Results!W3:W53)</f>
         <v>1</v>
       </c>
       <c r="F6" s="1">
-        <f>MAX(Results!W3:W52)</f>
+        <f>MAX(Results!X3:X53)</f>
         <v>1</v>
       </c>
       <c r="G6" s="1">
-        <f>MAX(Results!X3:X52)</f>
+        <f>MAX(Results!Y3:Y53)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="1">
+        <f>COUNTIF(Results!M3:M53,Summary!B1)</f>
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <f>COUNTIF(Results!N3:N53,Summary!C1)</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <f>COUNTIF(Results!O3:O53,Summary!D1)</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <f>COUNTIF(Results!P3:P53,Summary!E1)</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <f>COUNTIF(Results!Q3:Q53,Summary!F1)</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <f>COUNTIF(Results!R3:R53,Summary!G1)</f>
         <v>0</v>
       </c>
     </row>
@@ -1762,7 +1968,7 @@
       </c>
       <c r="B11" s="7">
         <f>SUMIF(Results!B3:B53,"&lt;&gt;#N/A",Results!K3:K53)/SUMIF(Results!B3:B53,"&lt;&gt;#N/A",Results!J3:J53)</f>
-        <v>0.375</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated through Episode 605.  Added Who Answered First Metric'
</commit_message>
<xml_diff>
--- a/SGU_Science_or_Fiction.xlsx
+++ b/SGU_Science_or_Fiction.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
   <si>
     <t>Episode</t>
   </si>
@@ -161,6 +161,33 @@
   </si>
   <si>
     <t>Lone Wolf Wins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Horrible things animals do to each other </t>
+  </si>
+  <si>
+    <t>Manatees are highly territorial and protective of their food source, and are known to attack and kill competitors by laying on top of them in shallow water until they drown.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Crypt Keeper wasp lays it eggs in the nest of the gall wasp, where hatchlings infest their brains compelling them to dig out of the nest but in a hole that is too small so they get stuck, then the Crypt Keeper eats them from the inside until they finally burst forth through their head. </t>
+  </si>
+  <si>
+    <t>Sea otters have been observed raping baby harbor seals to death, and sometimes keeping and continuing to copulate with the corpse for up to a week.</t>
+  </si>
+  <si>
+    <t>Scientists report the first discovery of a white dwarf pulsar, the only one known, just 380 light years from Earth</t>
+  </si>
+  <si>
+    <t>Hebrew University archaeologists report that they have uncovered a 12th Dead Sea scroll cave with intact jars containing previously undiscovered scrolls.</t>
+  </si>
+  <si>
+    <t>A new study finds that, with a little provocation, two-thirds of subjects engaged in trolling behavior in online comments</t>
+  </si>
+  <si>
+    <t>First to Answer</t>
+  </si>
+  <si>
+    <t>Panel Performance When Answering First</t>
   </si>
 </sst>
 </file>
@@ -575,18 +602,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N53"/>
+  <dimension ref="A1:O53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -612,25 +640,28 @@
         <v>5</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>600</v>
       </c>
@@ -656,28 +687,31 @@
       <c r="H2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="1">
-        <v>1</v>
-      </c>
-      <c r="J2" s="1" t="e">
+      <c r="I2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="K2" s="1">
-        <v>1</v>
-      </c>
       <c r="L2" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M2" s="1">
         <v>3</v>
       </c>
-      <c r="N2" s="1" t="e">
+      <c r="N2" s="1">
+        <v>3</v>
+      </c>
+      <c r="O2" s="1" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>601</v>
       </c>
@@ -704,28 +738,31 @@
       <c r="H3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="1">
-        <v>1</v>
+      <c r="I3" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="J3" s="1">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1">
         <v>2</v>
       </c>
-      <c r="K3" s="1">
-        <v>1</v>
-      </c>
       <c r="L3" s="1">
         <v>1</v>
       </c>
-      <c r="M3" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="M3" s="1">
+        <v>1</v>
       </c>
       <c r="N3" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>602</v>
       </c>
@@ -751,28 +788,31 @@
       <c r="H4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="1">
         <v>2</v>
       </c>
-      <c r="J4" s="1">
-        <v>1</v>
-      </c>
       <c r="K4" s="1">
         <v>1</v>
       </c>
       <c r="L4" s="1">
         <v>1</v>
       </c>
-      <c r="M4" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="M4" s="1">
+        <v>1</v>
       </c>
       <c r="N4" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O4" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>603</v>
       </c>
@@ -797,11 +837,11 @@
       <c r="H5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="1">
         <v>4</v>
-      </c>
-      <c r="J5" s="1">
-        <v>2</v>
       </c>
       <c r="K5" s="1">
         <v>2</v>
@@ -809,398 +849,532 @@
       <c r="L5" s="1">
         <v>2</v>
       </c>
-      <c r="M5" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="M5" s="1">
+        <v>2</v>
       </c>
       <c r="N5" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O5" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>604</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" s="1">
+        <v>2</v>
+      </c>
+      <c r="K6" s="1">
+        <v>1</v>
+      </c>
+      <c r="L6" s="1">
+        <v>1</v>
+      </c>
+      <c r="M6" s="1">
+        <v>2</v>
+      </c>
+      <c r="N6" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O6" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>605</v>
+      </c>
+      <c r="B7" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G7" s="1">
+        <v>2</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" s="1">
+        <v>2</v>
+      </c>
+      <c r="K7" s="1">
+        <v>3</v>
+      </c>
+      <c r="L7" s="1">
+        <v>3</v>
+      </c>
+      <c r="M7" s="1">
+        <v>2</v>
+      </c>
+      <c r="N7" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O7" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M11" s="1"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M12" s="1"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M13" s="1"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M14" s="1"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M15" s="1"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
-    </row>
-    <row r="17" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="M16" s="1"/>
+    </row>
+    <row r="17" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
-    </row>
-    <row r="18" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="M17" s="1"/>
+    </row>
+    <row r="18" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
-    </row>
-    <row r="19" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="M18" s="1"/>
+    </row>
+    <row r="19" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
-    </row>
-    <row r="20" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="M19" s="1"/>
+    </row>
+    <row r="20" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
-    </row>
-    <row r="21" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="M20" s="1"/>
+    </row>
+    <row r="21" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
-    </row>
-    <row r="22" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="M21" s="1"/>
+    </row>
+    <row r="22" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
-    </row>
-    <row r="23" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="M22" s="1"/>
+    </row>
+    <row r="23" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
-    </row>
-    <row r="24" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="M23" s="1"/>
+    </row>
+    <row r="24" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
-    </row>
-    <row r="25" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="M24" s="1"/>
+    </row>
+    <row r="25" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
-    </row>
-    <row r="26" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="M25" s="1"/>
+    </row>
+    <row r="26" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
-    </row>
-    <row r="27" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="M26" s="1"/>
+    </row>
+    <row r="27" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
-    </row>
-    <row r="28" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="M27" s="1"/>
+    </row>
+    <row r="28" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
-    </row>
-    <row r="29" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="M28" s="1"/>
+    </row>
+    <row r="29" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
-    </row>
-    <row r="30" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="M29" s="1"/>
+    </row>
+    <row r="30" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
-    </row>
-    <row r="31" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="M30" s="1"/>
+    </row>
+    <row r="31" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
-    </row>
-    <row r="32" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="M31" s="1"/>
+    </row>
+    <row r="32" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
-    </row>
-    <row r="33" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="M32" s="1"/>
+    </row>
+    <row r="33" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
-    </row>
-    <row r="34" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="M33" s="1"/>
+    </row>
+    <row r="34" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
-    </row>
-    <row r="35" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="M34" s="1"/>
+    </row>
+    <row r="35" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
-    </row>
-    <row r="36" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="M35" s="1"/>
+    </row>
+    <row r="36" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
-    </row>
-    <row r="37" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="M36" s="1"/>
+    </row>
+    <row r="37" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
-    </row>
-    <row r="38" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="M37" s="1"/>
+    </row>
+    <row r="38" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
-    </row>
-    <row r="39" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="M38" s="1"/>
+    </row>
+    <row r="39" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
-    </row>
-    <row r="40" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="M39" s="1"/>
+    </row>
+    <row r="40" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
-    </row>
-    <row r="41" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="M40" s="1"/>
+    </row>
+    <row r="41" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
-    </row>
-    <row r="42" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="M41" s="1"/>
+    </row>
+    <row r="42" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
-    </row>
-    <row r="43" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="M42" s="1"/>
+    </row>
+    <row r="43" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
-    </row>
-    <row r="44" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="M43" s="1"/>
+    </row>
+    <row r="44" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
-    </row>
-    <row r="45" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="M44" s="1"/>
+    </row>
+    <row r="45" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
-    </row>
-    <row r="46" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="M45" s="1"/>
+    </row>
+    <row r="46" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
-    </row>
-    <row r="47" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="M46" s="1"/>
+    </row>
+    <row r="47" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
-    </row>
-    <row r="48" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="M47" s="1"/>
+    </row>
+    <row r="48" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
-    </row>
-    <row r="49" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="M48" s="1"/>
+    </row>
+    <row r="49" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
-    </row>
-    <row r="50" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="M49" s="1"/>
+    </row>
+    <row r="50" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
-    </row>
-    <row r="51" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="M50" s="1"/>
+    </row>
+    <row r="51" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
-    </row>
-    <row r="52" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="M51" s="1"/>
+    </row>
+    <row r="52" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
       <c r="L52" s="1"/>
-    </row>
-    <row r="53" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="M52" s="1"/>
+    </row>
+    <row r="53" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
+      <c r="M53" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1210,37 +1384,38 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y6"/>
+  <dimension ref="A1:Z8"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3:M6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="11" max="11" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="N1" s="12" t="s">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="O1" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="12"/>
       <c r="P1" s="12"/>
       <c r="Q1" s="12"/>
       <c r="R1" s="12"/>
       <c r="S1" s="12"/>
-      <c r="T1" s="13" t="s">
+      <c r="T1" s="12"/>
+      <c r="U1" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="U1" s="13"/>
       <c r="V1" s="13"/>
       <c r="W1" s="13"/>
       <c r="X1" s="13"/>
       <c r="Y1" s="13"/>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z1" s="13"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="str">
         <f>Data!A1</f>
         <v>Episode</v>
@@ -1255,90 +1430,94 @@
       </c>
       <c r="D2" s="2" t="str">
         <f>Data!I1</f>
-        <v>Bob</v>
+        <v>First to Answer</v>
       </c>
       <c r="E2" s="2" t="str">
         <f>Data!J1</f>
-        <v>Cara</v>
+        <v>Bob</v>
       </c>
       <c r="F2" s="2" t="str">
         <f>Data!K1</f>
-        <v>Jay</v>
+        <v>Cara</v>
       </c>
       <c r="G2" s="2" t="str">
         <f>Data!L1</f>
-        <v>Evan</v>
+        <v>Jay</v>
       </c>
       <c r="H2" s="2" t="str">
         <f>Data!M1</f>
-        <v>George</v>
+        <v>Evan</v>
       </c>
       <c r="I2" s="2" t="str">
         <f>Data!N1</f>
+        <v>George</v>
+      </c>
+      <c r="J2" s="2" t="str">
+        <f>Data!O1</f>
         <v>Steve</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="N2" s="9" t="str">
-        <f>D2</f>
+      <c r="O2" s="9" t="str">
+        <f t="shared" ref="O2:T2" si="0">E2</f>
         <v>Bob</v>
       </c>
-      <c r="O2" s="9" t="str">
-        <f>E2</f>
+      <c r="P2" s="9" t="str">
+        <f t="shared" si="0"/>
         <v>Cara</v>
       </c>
-      <c r="P2" s="9" t="str">
-        <f>F2</f>
+      <c r="Q2" s="9" t="str">
+        <f t="shared" si="0"/>
         <v>Jay</v>
       </c>
-      <c r="Q2" s="9" t="str">
-        <f>G2</f>
+      <c r="R2" s="9" t="str">
+        <f t="shared" si="0"/>
         <v>Evan</v>
       </c>
-      <c r="R2" s="9" t="str">
-        <f>H2</f>
+      <c r="S2" s="9" t="str">
+        <f t="shared" si="0"/>
         <v>George</v>
       </c>
-      <c r="S2" s="9" t="str">
-        <f>I2</f>
+      <c r="T2" s="9" t="str">
+        <f t="shared" si="0"/>
         <v>Steve</v>
-      </c>
-      <c r="T2" s="11" t="str">
-        <f>N2</f>
-        <v>Bob</v>
       </c>
       <c r="U2" s="11" t="str">
         <f>O2</f>
+        <v>Bob</v>
+      </c>
+      <c r="V2" s="11" t="str">
+        <f>P2</f>
         <v>Cara</v>
       </c>
-      <c r="V2" s="11" t="str">
-        <f t="shared" ref="V2:Y2" si="0">P2</f>
+      <c r="W2" s="11" t="str">
+        <f t="shared" ref="W2:Z2" si="1">Q2</f>
         <v>Jay</v>
       </c>
-      <c r="W2" s="11" t="str">
-        <f t="shared" si="0"/>
+      <c r="X2" s="11" t="str">
+        <f t="shared" si="1"/>
         <v>Evan</v>
       </c>
-      <c r="X2" s="11" t="str">
-        <f t="shared" si="0"/>
+      <c r="Y2" s="11" t="str">
+        <f t="shared" si="1"/>
         <v>George</v>
       </c>
-      <c r="Y2" s="11" t="str">
-        <f t="shared" si="0"/>
+      <c r="Z2" s="11" t="str">
+        <f t="shared" si="1"/>
         <v>Steve</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <f>Data!A2</f>
         <v>600</v>
@@ -1351,17 +1530,17 @@
         <f>Data!H2</f>
         <v>Steve</v>
       </c>
-      <c r="D3" s="1">
-        <f>IF(Data!I2=Data!$G2,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="E3" s="1" t="e">
+      <c r="D3" s="2" t="str">
+        <f>Data!I2</f>
+        <v>Jay</v>
+      </c>
+      <c r="E3" s="1">
         <f>IF(Data!J2=Data!$G2,1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1" t="e">
         <f>IF(Data!K2=Data!$G2,1,0)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="G3" s="1">
         <f>IF(Data!L2=Data!$G2,1,0)</f>
@@ -1371,28 +1550,29 @@
         <f>IF(Data!M2=Data!$G2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="I3" s="1" t="e">
+      <c r="I3" s="1">
         <f>IF(Data!N2=Data!$G2,1,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J3" s="1">
-        <f>COUNTIF(D3:I3,"&lt;&gt;#N/A")</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="1" t="e">
+        <f>IF(Data!O2=Data!$G2,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K3" s="1">
+        <f>COUNTIF(E3:J3,"&lt;&gt;#N/A")</f>
         <v>4</v>
       </c>
-      <c r="K3" s="1">
-        <f>SUMIF(D3:I3,"&lt;&gt;#N/A")</f>
-        <v>0</v>
-      </c>
       <c r="L3" s="1">
-        <f>IF(SUMIF(D3:I3,"&lt;&gt;#N/A")=0, 1, 0)</f>
-        <v>1</v>
-      </c>
-      <c r="M3" s="1" t="e">
-        <f t="shared" ref="M3:M6" si="1">IF(K3=1,INDEX($D$2:$I$2,1,MATCH(1,D3:I3,0)),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N3" s="8">
-        <v>0</v>
+        <f>SUMIF(E3:J3,"&lt;&gt;#N/A")</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="1">
+        <f t="shared" ref="M3:M8" si="2">IF(SUMIF(E3:J3,"&lt;&gt;#N/A")=0, 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="N3" s="1" t="e">
+        <f t="shared" ref="N3" si="3">IF(L3=1,INDEX($E$2:$J$2,1,MATCH(1,E3:J3,0)),NA())</f>
+        <v>#N/A</v>
       </c>
       <c r="O3" s="8">
         <v>0</v>
@@ -1409,14 +1589,14 @@
       <c r="S3" s="8">
         <v>0</v>
       </c>
-      <c r="T3" s="10">
-        <v>1</v>
+      <c r="T3" s="8">
+        <v>0</v>
       </c>
       <c r="U3" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V3" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W3" s="10">
         <v>1</v>
@@ -1425,10 +1605,13 @@
         <v>1</v>
       </c>
       <c r="Y3" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <f>Data!A3</f>
         <v>601</v>
@@ -1441,96 +1624,100 @@
         <f>Data!H3</f>
         <v>Steve</v>
       </c>
-      <c r="D4" s="1">
-        <f>IF(Data!I3=Data!$G3,1,0)</f>
-        <v>1</v>
+      <c r="D4" s="2" t="str">
+        <f>Data!I3</f>
+        <v>Cara</v>
       </c>
       <c r="E4" s="1">
         <f>IF(Data!J3=Data!$G3,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="1">
         <f>IF(Data!K3=Data!$G3,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" s="1">
         <f>IF(Data!L3=Data!$G3,1,0)</f>
         <v>1</v>
       </c>
-      <c r="H4" s="1" t="e">
+      <c r="H4" s="1">
         <f>IF(Data!M3=Data!$G3,1,0)</f>
-        <v>#N/A</v>
+        <v>1</v>
       </c>
       <c r="I4" s="1" t="e">
         <f>IF(Data!N3=Data!$G3,1,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="J4" s="1">
-        <f t="shared" ref="J4:J5" si="2">COUNTIF(D4:I4,"&lt;&gt;#N/A")</f>
+      <c r="J4" s="1" t="e">
+        <f>IF(Data!O3=Data!$G3,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K4" s="1">
+        <f t="shared" ref="K4:K5" si="4">COUNTIF(E4:J4,"&lt;&gt;#N/A")</f>
         <v>4</v>
       </c>
-      <c r="K4" s="1">
-        <f t="shared" ref="K4:K5" si="3">SUMIF(D4:I4,"&lt;&gt;#N/A")</f>
+      <c r="L4" s="1">
+        <f t="shared" ref="L4:L5" si="5">SUMIF(E4:J4,"&lt;&gt;#N/A")</f>
         <v>3</v>
       </c>
-      <c r="L4" s="1">
-        <f>IF(SUMIF(D4:I4,"&lt;&gt;#N/A")=0, 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="M4" s="1" t="e">
-        <f>IF(K4=1,INDEX($D$2:$I$2,1,MATCH(1,D4:I4,0)),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N4" s="8">
-        <f t="shared" ref="N4:N5" si="4">IF(ISNA(D4),N3,IF(D4=1,N3+1,0))</f>
-        <v>1</v>
+      <c r="M4" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N4" s="1" t="e">
+        <f>IF(L4=1,INDEX($E$2:$J$2,1,MATCH(1,E4:J4,0)),NA())</f>
+        <v>#N/A</v>
       </c>
       <c r="O4" s="8">
-        <f t="shared" ref="O4:O5" si="5">IF(ISNA(E4),O3,IF(E4=1,O3+1,0))</f>
-        <v>0</v>
+        <f t="shared" ref="O4:O5" si="6">IF(ISNA(E4),O3,IF(E4=1,O3+1,0))</f>
+        <v>1</v>
       </c>
       <c r="P4" s="8">
-        <f t="shared" ref="P4:P5" si="6">IF(ISNA(F4),P3,IF(F4=1,P3+1,0))</f>
-        <v>1</v>
+        <f t="shared" ref="P4:P5" si="7">IF(ISNA(F4),P3,IF(F4=1,P3+1,0))</f>
+        <v>0</v>
       </c>
       <c r="Q4" s="8">
-        <f t="shared" ref="Q4:Q5" si="7">IF(ISNA(G4),Q3,IF(G4=1,Q3+1,0))</f>
+        <f t="shared" ref="Q4:Q5" si="8">IF(ISNA(G4),Q3,IF(G4=1,Q3+1,0))</f>
         <v>1</v>
       </c>
       <c r="R4" s="8">
-        <f>IF(ISNA(H4),R3,IF(H4=1,R3+1,0))</f>
-        <v>0</v>
+        <f t="shared" ref="R4:R5" si="9">IF(ISNA(H4),R3,IF(H4=1,R3+1,0))</f>
+        <v>1</v>
       </c>
       <c r="S4" s="8">
-        <f t="shared" ref="S4:S5" si="8">IF(ISNA(I4),S3,IF(I4=1,S3+1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="T4" s="10">
-        <f>IF(ISNA(D4),T3,IF(D4=0,T3+1,0))</f>
+        <f>IF(ISNA(I4),S3,IF(I4=1,S3+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="T4" s="8">
+        <f t="shared" ref="T4:T5" si="10">IF(ISNA(J4),T3,IF(J4=1,T3+1,0))</f>
         <v>0</v>
       </c>
       <c r="U4" s="10">
-        <f>IF(ISNA(E4),U3,IF(E4=0,U3+1,0))</f>
-        <v>1</v>
+        <f t="shared" ref="U4:Z5" si="11">IF(ISNA(E4),U3,IF(E4=0,U3+1,0))</f>
+        <v>0</v>
       </c>
       <c r="V4" s="10">
-        <f>IF(ISNA(F4),V3,IF(F4=0,V3+1,0))</f>
-        <v>0</v>
+        <f t="shared" si="11"/>
+        <v>1</v>
       </c>
       <c r="W4" s="10">
-        <f>IF(ISNA(G4),W3,IF(G4=0,W3+1,0))</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="X4" s="10">
-        <f>IF(ISNA(H4),X3,IF(H4=0,X3+1,0))</f>
-        <v>1</v>
+        <f t="shared" si="11"/>
+        <v>0</v>
       </c>
       <c r="Y4" s="10">
-        <f>IF(ISNA(I4),Y3,IF(I4=0,Y3+1,0))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="Z4" s="10">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <f>Data!A4</f>
         <v>602</v>
@@ -1543,13 +1730,13 @@
         <f>Data!H4</f>
         <v>Steve</v>
       </c>
-      <c r="D5" s="1">
-        <f>IF(Data!I4=Data!$G4,1,0)</f>
-        <v>0</v>
+      <c r="D5" s="2" t="str">
+        <f>Data!I4</f>
+        <v>Evan</v>
       </c>
       <c r="E5" s="1">
         <f>IF(Data!J4=Data!$G4,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" s="1">
         <f>IF(Data!K4=Data!$G4,1,0)</f>
@@ -1559,80 +1746,84 @@
         <f>IF(Data!L4=Data!$G4,1,0)</f>
         <v>1</v>
       </c>
-      <c r="H5" s="1" t="e">
+      <c r="H5" s="1">
         <f>IF(Data!M4=Data!$G4,1,0)</f>
-        <v>#N/A</v>
+        <v>1</v>
       </c>
       <c r="I5" s="1" t="e">
         <f>IF(Data!N4=Data!$G4,1,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J5" s="1" t="e">
+        <f>IF(Data!O4=Data!$G4,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K5" s="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="L5" s="1">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="M5" s="1">
         <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="K5" s="1">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="L5" s="1">
-        <f>IF(SUMIF(D5:I5,"&lt;&gt;#N/A")=0, 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="M5" s="1" t="e">
-        <f t="shared" ref="M5:M6" si="9">IF(K5=1,INDEX($D$2:$I$2,1,MATCH(1,D5:I5,0)),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N5" s="8">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="N5" s="1" t="e">
+        <f t="shared" ref="N5:N6" si="12">IF(L5=1,INDEX($E$2:$J$2,1,MATCH(1,E5:J5,0)),NA())</f>
+        <v>#N/A</v>
       </c>
       <c r="O5" s="8">
-        <f t="shared" si="5"/>
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="P5" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="Q5" s="8">
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
-      <c r="Q5" s="8">
-        <f t="shared" si="7"/>
+      <c r="R5" s="8">
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
-      <c r="R5" s="8">
-        <f t="shared" ref="R5" si="10">IF(ISNA(H5),R4,IF(H5=1,R4+1,0))</f>
-        <v>0</v>
-      </c>
       <c r="S5" s="8">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="T5" s="10">
-        <f>IF(ISNA(D5),T4,IF(D5=0,T4+1,0))</f>
-        <v>1</v>
+        <f t="shared" ref="S5" si="13">IF(ISNA(I5),S4,IF(I5=1,S4+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="T5" s="8">
+        <f t="shared" si="10"/>
+        <v>0</v>
       </c>
       <c r="U5" s="10">
-        <f>IF(ISNA(E5),U4,IF(E5=0,U4+1,0))</f>
-        <v>0</v>
+        <f t="shared" si="11"/>
+        <v>1</v>
       </c>
       <c r="V5" s="10">
-        <f>IF(ISNA(F5),V4,IF(F5=0,V4+1,0))</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="W5" s="10">
-        <f>IF(ISNA(G5),W4,IF(G5=0,W4+1,0))</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="X5" s="10">
-        <f>IF(ISNA(H5),X4,IF(H5=0,X4+1,0))</f>
-        <v>1</v>
+        <f t="shared" si="11"/>
+        <v>0</v>
       </c>
       <c r="Y5" s="10">
-        <f>IF(ISNA(I5),Y4,IF(I5=0,Y4+1,0))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="Z5" s="10">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <f>Data!A5</f>
         <v>603</v>
@@ -1645,13 +1836,13 @@
         <f>Data!H5</f>
         <v>Steve</v>
       </c>
-      <c r="D6" s="1">
-        <f>IF(Data!I5=Data!$G5,1,0)</f>
-        <v>0</v>
+      <c r="D6" s="2" t="str">
+        <f>Data!I5</f>
+        <v>Bob</v>
       </c>
       <c r="E6" s="1">
         <f>IF(Data!J5=Data!$G5,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" s="1">
         <f>IF(Data!K5=Data!$G5,1,0)</f>
@@ -1661,83 +1852,299 @@
         <f>IF(Data!L5=Data!$G5,1,0)</f>
         <v>1</v>
       </c>
-      <c r="H6" s="1" t="e">
+      <c r="H6" s="1">
         <f>IF(Data!M5=Data!$G5,1,0)</f>
-        <v>#N/A</v>
+        <v>1</v>
       </c>
       <c r="I6" s="1" t="e">
         <f>IF(Data!N5=Data!$G5,1,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="J6" s="1">
-        <f t="shared" ref="J6" si="11">COUNTIF(D6:I6,"&lt;&gt;#N/A")</f>
+      <c r="J6" s="1" t="e">
+        <f>IF(Data!O5=Data!$G5,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K6" s="1">
+        <f t="shared" ref="K6" si="14">COUNTIF(E6:J6,"&lt;&gt;#N/A")</f>
         <v>4</v>
       </c>
-      <c r="K6" s="1">
-        <f t="shared" ref="K6" si="12">SUMIF(D6:I6,"&lt;&gt;#N/A")</f>
+      <c r="L6" s="1">
+        <f t="shared" ref="L6" si="15">SUMIF(E6:J6,"&lt;&gt;#N/A")</f>
         <v>3</v>
       </c>
-      <c r="L6" s="1">
-        <f>IF(SUMIF(D6:I6,"&lt;&gt;#N/A")=0, 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="M6" s="1" t="e">
-        <f t="shared" si="9"/>
-        <v>#N/A</v>
-      </c>
-      <c r="N6" s="8">
-        <f t="shared" ref="N6" si="13">IF(ISNA(D6),N5,IF(D6=1,N5+1,0))</f>
-        <v>0</v>
+      <c r="M6" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N6" s="1" t="e">
+        <f t="shared" si="12"/>
+        <v>#N/A</v>
       </c>
       <c r="O6" s="8">
-        <f t="shared" ref="O6" si="14">IF(ISNA(E6),O5,IF(E6=1,O5+1,0))</f>
+        <f t="shared" ref="O6" si="16">IF(ISNA(E6),O5,IF(E6=1,O5+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="P6" s="8">
+        <f t="shared" ref="P6" si="17">IF(ISNA(F6),P5,IF(F6=1,P5+1,0))</f>
         <v>2</v>
       </c>
-      <c r="P6" s="8">
-        <f t="shared" ref="P6" si="15">IF(ISNA(F6),P5,IF(F6=1,P5+1,0))</f>
+      <c r="Q6" s="8">
+        <f t="shared" ref="Q6" si="18">IF(ISNA(G6),Q5,IF(G6=1,Q5+1,0))</f>
         <v>3</v>
       </c>
-      <c r="Q6" s="8">
-        <f t="shared" ref="Q6" si="16">IF(ISNA(G6),Q5,IF(G6=1,Q5+1,0))</f>
+      <c r="R6" s="8">
+        <f t="shared" ref="R6" si="19">IF(ISNA(H6),R5,IF(H6=1,R5+1,0))</f>
         <v>3</v>
       </c>
-      <c r="R6" s="8">
-        <f t="shared" ref="R6" si="17">IF(ISNA(H6),R5,IF(H6=1,R5+1,0))</f>
-        <v>0</v>
-      </c>
       <c r="S6" s="8">
-        <f t="shared" ref="S6" si="18">IF(ISNA(I6),S5,IF(I6=1,S5+1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="T6" s="10">
-        <f>IF(ISNA(D6),T5,IF(D6=0,T5+1,0))</f>
+        <f t="shared" ref="S6" si="20">IF(ISNA(I6),S5,IF(I6=1,S5+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="T6" s="8">
+        <f t="shared" ref="T6" si="21">IF(ISNA(J6),T5,IF(J6=1,T5+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="U6" s="10">
+        <f t="shared" ref="U6:V8" si="22">IF(ISNA(E6),U5,IF(E6=0,U5+1,0))</f>
         <v>2</v>
       </c>
-      <c r="U6" s="10">
-        <f>IF(ISNA(E6),U5,IF(E6=0,U5+1,0))</f>
-        <v>0</v>
-      </c>
       <c r="V6" s="10">
-        <f t="shared" ref="V6" si="19">IF(ISNA(F6),V5,IF(F6=0,V5+1,0))</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="W6" s="10">
-        <f t="shared" ref="W6" si="20">IF(ISNA(G6),W5,IF(G6=0,W5+1,0))</f>
+        <f t="shared" ref="W6" si="23">IF(ISNA(G6),W5,IF(G6=0,W5+1,0))</f>
         <v>0</v>
       </c>
       <c r="X6" s="10">
-        <f t="shared" ref="X6" si="21">IF(ISNA(H6),X5,IF(H6=0,X5+1,0))</f>
-        <v>1</v>
+        <f t="shared" ref="X6" si="24">IF(ISNA(H6),X5,IF(H6=0,X5+1,0))</f>
+        <v>0</v>
       </c>
       <c r="Y6" s="10">
-        <f t="shared" ref="Y6" si="22">IF(ISNA(I6),Y5,IF(I6=0,Y5+1,0))</f>
+        <f t="shared" ref="Y6" si="25">IF(ISNA(I6),Y5,IF(I6=0,Y5+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="Z6" s="10">
+        <f t="shared" ref="Z6" si="26">IF(ISNA(J6),Z5,IF(J6=0,Z5+1,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <f>Data!A6</f>
+        <v>604</v>
+      </c>
+      <c r="B7" s="4" t="str">
+        <f>Data!B6</f>
+        <v xml:space="preserve">Horrible things animals do to each other </v>
+      </c>
+      <c r="C7" s="5" t="str">
+        <f>Data!H6</f>
+        <v>Steve</v>
+      </c>
+      <c r="D7" s="2" t="str">
+        <f>Data!I6</f>
+        <v>Jay</v>
+      </c>
+      <c r="E7" s="1">
+        <f>IF(Data!J6=Data!$G6,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <f>IF(Data!K6=Data!$G6,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <f>IF(Data!L6=Data!$G6,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H7" s="1">
+        <f>IF(Data!M6=Data!$G6,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="1" t="e">
+        <f>IF(Data!N6=Data!$G6,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J7" s="1" t="e">
+        <f>IF(Data!O6=Data!$G6,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K7" s="1">
+        <f t="shared" ref="K7" si="27">COUNTIF(E7:J7,"&lt;&gt;#N/A")</f>
+        <v>4</v>
+      </c>
+      <c r="L7" s="1">
+        <f t="shared" ref="L7" si="28">SUMIF(E7:J7,"&lt;&gt;#N/A")</f>
+        <v>2</v>
+      </c>
+      <c r="M7" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N7" s="1" t="e">
+        <f t="shared" ref="N7" si="29">IF(L7=1,INDEX($E$2:$J$2,1,MATCH(1,E7:J7,0)),NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O7" s="8">
+        <f t="shared" ref="O7" si="30">IF(ISNA(E7),O6,IF(E7=1,O6+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="P7" s="8">
+        <f t="shared" ref="P7" si="31">IF(ISNA(F7),P6,IF(F7=1,P6+1,0))</f>
+        <v>3</v>
+      </c>
+      <c r="Q7" s="8">
+        <f t="shared" ref="Q7" si="32">IF(ISNA(G7),Q6,IF(G7=1,Q6+1,0))</f>
+        <v>4</v>
+      </c>
+      <c r="R7" s="8">
+        <f t="shared" ref="R7" si="33">IF(ISNA(H7),R6,IF(H7=1,R6+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="S7" s="8">
+        <f t="shared" ref="S7" si="34">IF(ISNA(I7),S6,IF(I7=1,S6+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="T7" s="8">
+        <f t="shared" ref="T7" si="35">IF(ISNA(J7),T6,IF(J7=1,T6+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="U7" s="10">
+        <f t="shared" si="22"/>
+        <v>3</v>
+      </c>
+      <c r="V7" s="10">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="W7" s="10">
+        <f t="shared" ref="W7" si="36">IF(ISNA(G7),W6,IF(G7=0,W6+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="X7" s="10">
+        <f t="shared" ref="X7" si="37">IF(ISNA(H7),X6,IF(H7=0,X6+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="Y7" s="10">
+        <f t="shared" ref="Y7" si="38">IF(ISNA(I7),Y6,IF(I7=0,Y6+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="Z7" s="10">
+        <f t="shared" ref="Z7" si="39">IF(ISNA(J7),Z6,IF(J7=0,Z6+1,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <f>Data!A7</f>
+        <v>605</v>
+      </c>
+      <c r="B8" s="4" t="e">
+        <f>Data!B7</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C8" s="5" t="str">
+        <f>Data!H7</f>
+        <v>Steve</v>
+      </c>
+      <c r="D8" s="2" t="str">
+        <f>Data!I7</f>
+        <v>Cara</v>
+      </c>
+      <c r="E8" s="1">
+        <f>IF(Data!J7=Data!$G7,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <f>IF(Data!K7=Data!$G7,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <f>IF(Data!L7=Data!$G7,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <f>IF(Data!M7=Data!$G7,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="I8" s="1" t="e">
+        <f>IF(Data!N7=Data!$G7,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J8" s="1" t="e">
+        <f>IF(Data!O7=Data!$G7,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K8" s="1">
+        <f t="shared" ref="K8" si="40">COUNTIF(E8:J8,"&lt;&gt;#N/A")</f>
+        <v>4</v>
+      </c>
+      <c r="L8" s="1">
+        <f t="shared" ref="L8" si="41">SUMIF(E8:J8,"&lt;&gt;#N/A")</f>
+        <v>2</v>
+      </c>
+      <c r="M8" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N8" s="1" t="e">
+        <f t="shared" ref="N8" si="42">IF(L8=1,INDEX($E$2:$J$2,1,MATCH(1,E8:J8,0)),NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O8" s="8">
+        <f t="shared" ref="O8" si="43">IF(ISNA(E8),O7,IF(E8=1,O7+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="P8" s="8">
+        <f t="shared" ref="P8" si="44">IF(ISNA(F8),P7,IF(F8=1,P7+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="8">
+        <f t="shared" ref="Q8" si="45">IF(ISNA(G8),Q7,IF(G8=1,Q7+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="R8" s="8">
+        <f t="shared" ref="R8" si="46">IF(ISNA(H8),R7,IF(H8=1,R7+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="S8" s="8">
+        <f t="shared" ref="S8" si="47">IF(ISNA(I8),S7,IF(I8=1,S7+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="T8" s="8">
+        <f t="shared" ref="T8" si="48">IF(ISNA(J8),T7,IF(J8=1,T7+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="U8" s="10">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="V8" s="10">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="W8" s="10">
+        <f t="shared" ref="W8" si="49">IF(ISNA(G8),W7,IF(G8=0,W7+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="X8" s="10">
+        <f t="shared" ref="X8" si="50">IF(ISNA(H8),X7,IF(H8=0,X7+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="Y8" s="10">
+        <f t="shared" ref="Y8" si="51">IF(ISNA(I8),Y7,IF(I8=0,Y7+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="Z8" s="10">
+        <f t="shared" ref="Z8" si="52">IF(ISNA(J8),Z7,IF(J8=0,Z7+1,0))</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="N1:S1"/>
-    <mergeCell ref="T1:Y1"/>
+    <mergeCell ref="O1:T1"/>
+    <mergeCell ref="U1:Z1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -1746,40 +2153,40 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.5703125" customWidth="1"/>
+    <col min="1" max="1" width="38.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="str">
-        <f>Results!D2</f>
+        <f>Results!E2</f>
         <v>Bob</v>
       </c>
       <c r="C1" s="2" t="str">
-        <f>Results!E2</f>
+        <f>Results!F2</f>
         <v>Cara</v>
       </c>
       <c r="D1" s="2" t="str">
-        <f>Results!F2</f>
+        <f>Results!G2</f>
         <v>Jay</v>
       </c>
       <c r="E1" s="2" t="str">
-        <f>Results!G2</f>
+        <f>Results!H2</f>
         <v>Evan</v>
       </c>
       <c r="F1" s="2" t="str">
-        <f>Results!H2</f>
+        <f>Results!I2</f>
         <v>George</v>
       </c>
       <c r="G1" s="2" t="str">
-        <f>Results!I2</f>
+        <f>Results!J2</f>
         <v>Steve</v>
       </c>
     </row>
@@ -1788,27 +2195,27 @@
         <v>26</v>
       </c>
       <c r="B2" s="6">
-        <f>SUMIF(Results!D3:D53,"&lt;&gt;#N/A")/COUNTIFS(Results!D3:D53,"&lt;&gt;#N/A",Results!D3:D53,"&lt;&gt;")</f>
-        <v>0.25</v>
+        <f>SUMIF(Results!E3:E53,"&lt;&gt;#N/A")/COUNTIFS(Results!E3:E53,"&lt;&gt;#N/A",Results!E3:E53,"&lt;&gt;")</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="C2" s="6">
-        <f>SUMIF(Results!E3:E53,"&lt;&gt;#N/A")/COUNTIFS(Results!E3:E53,"&lt;&gt;#N/A",Results!E3:E53,"&lt;&gt;")</f>
+        <f>SUMIF(Results!F3:F53,"&lt;&gt;#N/A")/COUNTIFS(Results!F3:F53,"&lt;&gt;#N/A",Results!F3:F53,"&lt;&gt;")</f>
+        <v>0.6</v>
+      </c>
+      <c r="D2" s="6">
+        <f>SUMIF(Results!G3:G53,"&lt;&gt;#N/A")/COUNTIFS(Results!G3:G53,"&lt;&gt;#N/A",Results!G3:G53,"&lt;&gt;")</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="D2" s="6">
-        <f>SUMIF(Results!F3:F53,"&lt;&gt;#N/A")/COUNTIFS(Results!F3:F53,"&lt;&gt;#N/A",Results!F3:F53,"&lt;&gt;")</f>
-        <v>0.75</v>
-      </c>
       <c r="E2" s="6">
-        <f>SUMIF(Results!G3:G53,"&lt;&gt;#N/A")/COUNTIFS(Results!G3:G53,"&lt;&gt;#N/A",Results!G3:G53,"&lt;&gt;")</f>
-        <v>0.75</v>
+        <f>SUMIF(Results!H3:H53,"&lt;&gt;#N/A")/COUNTIFS(Results!H3:H53,"&lt;&gt;#N/A",Results!H3:H53,"&lt;&gt;")</f>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F2" s="6">
-        <f>SUMIF(Results!H3:H53,"&lt;&gt;#N/A")/COUNTIFS(Results!H3:H53,"&lt;&gt;#N/A",Results!H3:H53,"&lt;&gt;")</f>
+        <f>SUMIF(Results!I3:I53,"&lt;&gt;#N/A")/COUNTIFS(Results!I3:I53,"&lt;&gt;#N/A",Results!I3:I53,"&lt;&gt;")</f>
         <v>0</v>
       </c>
       <c r="G2" s="6" t="e">
-        <f>SUMIF(Results!I3:I53,"&lt;&gt;#N/A")/COUNTIFS(Results!I3:I53,"&lt;&gt;#N/A",Results!I3:I53,"&lt;&gt;")</f>
+        <f>SUMIF(Results!J3:J53,"&lt;&gt;#N/A")/COUNTIFS(Results!J3:J53,"&lt;&gt;#N/A",Results!J3:J53,"&lt;&gt;")</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1817,27 +2224,27 @@
         <v>27</v>
       </c>
       <c r="B3" s="6">
-        <f>SUMIFS(Results!D3:D53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!D3:D53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!D3:D53, "&lt;&gt;#N/A", Results!D3:D53, "&lt;&gt;")</f>
+        <f>SUMIFS(Results!E3:E53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!E3:E53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!E3:E53, "&lt;&gt;#N/A", Results!E3:E53, "&lt;&gt;")</f>
         <v>0</v>
       </c>
       <c r="C3" s="6">
-        <f>SUMIFS(Results!E3:E53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!E3:E53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!E3:E53, "&lt;&gt;#N/A", Results!E3:E53, "&lt;&gt;")</f>
+        <f>SUMIFS(Results!F3:F53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!F3:F53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!F3:F53, "&lt;&gt;#N/A", Results!F3:F53, "&lt;&gt;")</f>
         <v>1</v>
       </c>
       <c r="D3" s="6">
-        <f>SUMIFS(Results!F3:F53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!F3:F53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!F3:F53, "&lt;&gt;#N/A", Results!F3:F53, "&lt;&gt;")</f>
-        <v>0.66666666666666663</v>
+        <f>SUMIFS(Results!G3:G53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!G3:G53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!G3:G53, "&lt;&gt;#N/A", Results!G3:G53, "&lt;&gt;")</f>
+        <v>0.75</v>
       </c>
       <c r="E3" s="6">
-        <f>SUMIFS(Results!G3:G53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!G3:G53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!G3:G53, "&lt;&gt;#N/A", Results!G3:G53, "&lt;&gt;")</f>
-        <v>0.66666666666666663</v>
+        <f>SUMIFS(Results!H3:H53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!H3:H53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!H3:H53, "&lt;&gt;#N/A", Results!H3:H53, "&lt;&gt;")</f>
+        <v>0.5</v>
       </c>
       <c r="F3" s="6">
-        <f>SUMIFS(Results!H3:H53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!H3:H53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!H3:H53, "&lt;&gt;#N/A", Results!H3:H53, "&lt;&gt;")</f>
+        <f>SUMIFS(Results!I3:I53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!I3:I53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!I3:I53, "&lt;&gt;#N/A", Results!I3:I53, "&lt;&gt;")</f>
         <v>0</v>
       </c>
       <c r="G3" s="6" t="e">
-        <f>SUMIFS(Results!I3:I53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!I3:I53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!I3:I53, "&lt;&gt;#N/A", Results!I3:I53, "&lt;&gt;")</f>
+        <f>SUMIFS(Results!J3:J53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!J3:J53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!J3:J53, "&lt;&gt;#N/A", Results!J3:J53, "&lt;&gt;")</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1846,27 +2253,27 @@
         <v>28</v>
       </c>
       <c r="B4" s="6">
-        <f>SUMIFS(Results!D3:D53,Results!$B$3:$B$53,"=#N/A",Results!D3:D53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!D3:D53, "&lt;&gt;#N/A", Results!D3:D53, "&lt;&gt;")</f>
+        <f>SUMIFS(Results!E3:E53,Results!$B$3:$B$53,"=#N/A",Results!E3:E53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!E3:E53, "&lt;&gt;#N/A", Results!E3:E53, "&lt;&gt;")</f>
         <v>1</v>
       </c>
       <c r="C4" s="6">
-        <f>SUMIFS(Results!E3:E53,Results!$B$3:$B$53,"=#N/A",Results!E3:E53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!E3:E53, "&lt;&gt;#N/A", Results!E3:E53, "&lt;&gt;")</f>
+        <f>SUMIFS(Results!F3:F53,Results!$B$3:$B$53,"=#N/A",Results!F3:F53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!F3:F53, "&lt;&gt;#N/A", Results!F3:F53, "&lt;&gt;")</f>
         <v>0</v>
       </c>
       <c r="D4" s="6">
-        <f>SUMIFS(Results!F3:F53,Results!$B$3:$B$53,"=#N/A",Results!F3:F53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!F3:F53, "&lt;&gt;#N/A", Results!F3:F53, "&lt;&gt;")</f>
-        <v>1</v>
+        <f>SUMIFS(Results!G3:G53,Results!$B$3:$B$53,"=#N/A",Results!G3:G53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!G3:G53, "&lt;&gt;#N/A", Results!G3:G53, "&lt;&gt;")</f>
+        <v>0.5</v>
       </c>
       <c r="E4" s="6">
-        <f>SUMIFS(Results!G3:G53,Results!$B$3:$B$53,"=#N/A",Results!G3:G53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!G3:G53, "&lt;&gt;#N/A", Results!G3:G53, "&lt;&gt;")</f>
+        <f>SUMIFS(Results!H3:H53,Results!$B$3:$B$53,"=#N/A",Results!H3:H53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!H3:H53, "&lt;&gt;#N/A", Results!H3:H53, "&lt;&gt;")</f>
         <v>1</v>
       </c>
       <c r="F4" s="6" t="e">
-        <f>SUMIFS(Results!H3:H53,Results!$B$3:$B$53,"=#N/A",Results!H3:H53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!H3:H53, "&lt;&gt;#N/A", Results!H3:H53, "&lt;&gt;")</f>
+        <f>SUMIFS(Results!I3:I53,Results!$B$3:$B$53,"=#N/A",Results!I3:I53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!I3:I53, "&lt;&gt;#N/A", Results!I3:I53, "&lt;&gt;")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G4" s="6" t="e">
-        <f>SUMIFS(Results!I3:I53,Results!$B$3:$B$53,"=#N/A",Results!I3:I53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!I3:I53, "&lt;&gt;#N/A", Results!I3:I53, "&lt;&gt;")</f>
+        <f>SUMIFS(Results!J3:J53,Results!$B$3:$B$53,"=#N/A",Results!J3:J53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!J3:J53, "&lt;&gt;#N/A", Results!J3:J53, "&lt;&gt;")</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1875,27 +2282,27 @@
         <v>29</v>
       </c>
       <c r="B5" s="1">
-        <f>MAX(Results!N3:N53)</f>
+        <f>MAX(Results!O3:O53)</f>
         <v>1</v>
       </c>
       <c r="C5" s="1">
-        <f>MAX(Results!O3:O53)</f>
-        <v>2</v>
-      </c>
-      <c r="D5" s="1">
         <f>MAX(Results!P3:P53)</f>
         <v>3</v>
       </c>
+      <c r="D5" s="1">
+        <f>MAX(Results!Q3:Q53)</f>
+        <v>4</v>
+      </c>
       <c r="E5" s="1">
-        <f>MAX(Results!Q3:Q53)</f>
+        <f>MAX(Results!R3:R53)</f>
         <v>3</v>
       </c>
       <c r="F5" s="1">
-        <f>MAX(Results!R3:R53)</f>
+        <f>MAX(Results!S3:S53)</f>
         <v>0</v>
       </c>
       <c r="G5" s="1">
-        <f>MAX(Results!S3:S53)</f>
+        <f>MAX(Results!T3:T53)</f>
         <v>0</v>
       </c>
     </row>
@@ -1904,27 +2311,27 @@
         <v>30</v>
       </c>
       <c r="B6" s="1">
-        <f>MAX(Results!T3:T53)</f>
-        <v>2</v>
+        <f>MAX(Results!U3:U53)</f>
+        <v>3</v>
       </c>
       <c r="C6" s="1">
-        <f>MAX(Results!U3:U53)</f>
+        <f>MAX(Results!V3:V53)</f>
         <v>1</v>
       </c>
       <c r="D6" s="1">
-        <f>MAX(Results!V3:V53)</f>
+        <f>MAX(Results!W3:W53)</f>
         <v>1</v>
       </c>
       <c r="E6" s="1">
-        <f>MAX(Results!W3:W53)</f>
+        <f>MAX(Results!X3:X53)</f>
         <v>1</v>
       </c>
       <c r="F6" s="1">
-        <f>MAX(Results!X3:X53)</f>
+        <f>MAX(Results!Y3:Y53)</f>
         <v>1</v>
       </c>
       <c r="G6" s="1">
-        <f>MAX(Results!Y3:Y53)</f>
+        <f>MAX(Results!Z3:Z53)</f>
         <v>0</v>
       </c>
     </row>
@@ -1933,28 +2340,57 @@
         <v>44</v>
       </c>
       <c r="B7" s="1">
-        <f>COUNTIF(Results!M3:M53,Summary!B1)</f>
+        <f>COUNTIF(Results!N3:N53,Summary!B1)</f>
         <v>0</v>
       </c>
       <c r="C7" s="1">
-        <f>COUNTIF(Results!N3:N53,Summary!C1)</f>
+        <f>COUNTIF(Results!O3:O53,Summary!C1)</f>
         <v>0</v>
       </c>
       <c r="D7" s="1">
-        <f>COUNTIF(Results!O3:O53,Summary!D1)</f>
+        <f>COUNTIF(Results!P3:P53,Summary!D1)</f>
         <v>0</v>
       </c>
       <c r="E7" s="1">
-        <f>COUNTIF(Results!P3:P53,Summary!E1)</f>
+        <f>COUNTIF(Results!Q3:Q53,Summary!E1)</f>
         <v>0</v>
       </c>
       <c r="F7" s="1">
-        <f>COUNTIF(Results!Q3:Q53,Summary!F1)</f>
+        <f>COUNTIF(Results!R3:R53,Summary!F1)</f>
         <v>0</v>
       </c>
       <c r="G7" s="1">
-        <f>COUNTIF(Results!R3:R53,Summary!G1)</f>
-        <v>0</v>
+        <f>COUNTIF(Results!S3:S53,Summary!G1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="7">
+        <f>SUMIF(Results!$D$3:$D$53,B1,Results!$L$3:$L$53)/SUMIF(Results!$D$3:$D$53,B1,Results!$K$3:$K$53)</f>
+        <v>0.75</v>
+      </c>
+      <c r="C8" s="7">
+        <f>SUMIF(Results!$D$3:$D$53,C1,Results!$L$3:$L$53)/SUMIF(Results!$D$3:$D$53,C1,Results!$K$3:$K$53)</f>
+        <v>0.625</v>
+      </c>
+      <c r="D8" s="7">
+        <f>SUMIF(Results!$D$3:$D$53,D1,Results!$L$3:$L$53)/SUMIF(Results!$D$3:$D$53,D1,Results!$K$3:$K$53)</f>
+        <v>0.25</v>
+      </c>
+      <c r="E8" s="7">
+        <f>SUMIF(Results!$D$3:$D$53,E1,Results!$L$3:$L$53)/SUMIF(Results!$D$3:$D$53,E1,Results!$K$3:$K$53)</f>
+        <v>0.75</v>
+      </c>
+      <c r="F8" s="7" t="e">
+        <f>SUMIF(Results!$D$3:$D$53,F1,Results!$L$3:$L$53)/SUMIF(Results!$D$3:$D$53,F1,Results!$K$3:$K$53)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G8" s="7" t="e">
+        <f>SUMIF(Results!$D$3:$D$53,G1,Results!$L$3:$L$53)/SUMIF(Results!$D$3:$D$53,G1,Results!$K$3:$K$53)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1967,7 +2403,7 @@
         <v>32</v>
       </c>
       <c r="B11" s="7">
-        <f>SUMIF(Results!B3:B53,"&lt;&gt;#N/A",Results!K3:K53)/SUMIF(Results!B3:B53,"&lt;&gt;#N/A",Results!J3:J53)</f>
+        <f>SUMIF(Results!B3:B53,"&lt;&gt;#N/A",Results!L3:L53)/SUMIF(Results!B3:B53,"&lt;&gt;#N/A",Results!K3:K53)</f>
         <v>0.5</v>
       </c>
     </row>
@@ -1976,9 +2412,12 @@
         <v>33</v>
       </c>
       <c r="B12" s="7">
-        <f>SUMIF(Results!B3:B53,"=#N/A",Results!K3:K53)/SUMIF(Results!B3:B53,"=#N/A",Results!J3:J53)</f>
-        <v>0.75</v>
-      </c>
+        <f>SUMIF(Results!B3:B53,"=#N/A",Results!L3:L53)/SUMIF(Results!B3:B53,"=#N/A",Results!K3:K53)</f>
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated through Episode 606. Renamed a few columns to remove spaces'
</commit_message>
<xml_diff>
--- a/SGU_Science_or_Fiction.xlsx
+++ b/SGU_Science_or_Fiction.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="62">
   <si>
     <t>Episode</t>
   </si>
@@ -40,9 +40,6 @@
     <t>Item 3</t>
   </si>
   <si>
-    <t>Fiction Item</t>
-  </si>
-  <si>
     <t>Host</t>
   </si>
   <si>
@@ -124,15 +121,6 @@
     <t>CorrectPanelist</t>
   </si>
   <si>
-    <t>% Correct Guesses with Theme</t>
-  </si>
-  <si>
-    <t>% Correct Guesses without Theme</t>
-  </si>
-  <si>
-    <t>Summary Across All Panelists</t>
-  </si>
-  <si>
     <t>Consecutive Wins</t>
   </si>
   <si>
@@ -157,12 +145,6 @@
     <t>The Zanzibar Leopard once inhabited the Zanzibar archipelago in Tanzania, but was deliberated hunted to extinction because they were thought to be the servants of witches</t>
   </si>
   <si>
-    <t>Lone Wolf</t>
-  </si>
-  <si>
-    <t>Lone Wolf Wins</t>
-  </si>
-  <si>
     <t xml:space="preserve">Horrible things animals do to each other </t>
   </si>
   <si>
@@ -184,10 +166,52 @@
     <t>A new study finds that, with a little provocation, two-thirds of subjects engaged in trolling behavior in online comments</t>
   </si>
   <si>
-    <t>First to Answer</t>
-  </si>
-  <si>
     <t>Panel Performance When Answering First</t>
+  </si>
+  <si>
+    <t>FictionItem</t>
+  </si>
+  <si>
+    <t>FirstToAnswer</t>
+  </si>
+  <si>
+    <t>The Brain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A new study supports the hypothesis that comprehending a word that relates to motor function involves the relevant part of the motor cortex, and not just language cortex. </t>
+  </si>
+  <si>
+    <t>Using MRI scans, researchers have been able to predict which high-risk infants will go on to develop autism with 90% accuracy as young as 3 months of age.</t>
+  </si>
+  <si>
+    <t>Engineers have developed brain electrodes that are 1000 times more flexible than previous electrodes, allowing for a stable connection that does not form scar tissue.</t>
+  </si>
+  <si>
+    <t>SoloWin</t>
+  </si>
+  <si>
+    <t>Solo Wins</t>
+  </si>
+  <si>
+    <t>ALL</t>
+  </si>
+  <si>
+    <t>Correct Guesses Overall</t>
+  </si>
+  <si>
+    <t>Total Guesses Overall</t>
+  </si>
+  <si>
+    <t>Correct Guesses with Themes</t>
+  </si>
+  <si>
+    <t>Total Guesses with Themes</t>
+  </si>
+  <si>
+    <t>Correct Guesses without Themes</t>
+  </si>
+  <si>
+    <t>Total Guesses without Themes</t>
   </si>
 </sst>
 </file>
@@ -337,6 +361,1444 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>XXX Has</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> the Highest Percentage of Wins Overall</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>% Wins Overall</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="0%" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Summary!$B$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Bob</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Cara</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Jay</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Evan</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>George</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Steve</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>ALL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$B$2:$H$2</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.2857142857142857</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5714285714285714</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7142857142857143</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="202779344"/>
+        <c:axId val="250002264"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Summary!$A$3</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>% Wins with Themes</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent2"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Summary!$B$1:$H$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>Bob</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Cara</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Jay</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Evan</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>George</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Steve</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>ALL</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Summary!$B$3:$H$3</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.0%</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.75</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.6</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.6</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.45</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Summary!$A$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>% Wins without Themes</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent3"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Summary!$B$1:$H$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>Bob</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Cara</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Jay</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Evan</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>George</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Steve</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>ALL</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Summary!$B$4:$H$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.0%</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.5</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.625</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
+      </c:barChart>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total Guesses Overall</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inBase"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$B$10:$H$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>28</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="480661040"/>
+        <c:axId val="480661432"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="202779344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="250002264"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="250002264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="202779344"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="480661432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="none"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="480661040"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="480661040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="480661432"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>157370</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>106846</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>438978</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>183046</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -605,7 +2067,7 @@
   <dimension ref="A1:O53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,7 +2081,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -631,34 +2093,34 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="O1" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -666,16 +2128,16 @@
         <v>600</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
       </c>
       <c r="F2" s="1" t="e">
         <f>NA()</f>
@@ -685,10 +2147,10 @@
         <v>2</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J2" s="1">
         <v>1</v>
@@ -720,13 +2182,13 @@
         <v>#N/A</v>
       </c>
       <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
       </c>
       <c r="F3" t="e">
         <f>NA()</f>
@@ -736,10 +2198,10 @@
         <v>1</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J3" s="1">
         <v>1</v>
@@ -767,16 +2229,16 @@
         <v>602</v>
       </c>
       <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>22</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
       </c>
       <c r="F4" t="e">
         <f>NA()</f>
@@ -786,10 +2248,10 @@
         <v>1</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J4" s="1">
         <v>2</v>
@@ -817,28 +2279,28 @@
         <v>603</v>
       </c>
       <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" t="s">
         <v>38</v>
-      </c>
-      <c r="C5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F5" t="s">
-        <v>42</v>
       </c>
       <c r="G5" s="1">
         <v>2</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J5" s="1">
         <v>4</v>
@@ -866,16 +2328,16 @@
         <v>604</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F6" t="e">
         <f>NA()</f>
@@ -885,10 +2347,10 @@
         <v>1</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J6" s="1">
         <v>2</v>
@@ -920,13 +2382,13 @@
         <v>#N/A</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E7" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F7" t="e">
         <f>NA()</f>
@@ -936,10 +2398,10 @@
         <v>2</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J7" s="1">
         <v>2</v>
@@ -963,13 +2425,54 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
+      <c r="A8">
+        <v>606</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G8" s="1">
+        <v>2</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1</v>
+      </c>
+      <c r="K8" s="1">
+        <v>3</v>
+      </c>
+      <c r="L8" s="1">
+        <v>1</v>
+      </c>
+      <c r="M8" s="1">
+        <v>2</v>
+      </c>
+      <c r="N8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O8" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G9" s="1"/>
@@ -1384,10 +2887,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z8"/>
+  <dimension ref="A1:Z9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1399,7 +2902,7 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="O1" s="12" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="P1" s="12"/>
       <c r="Q1" s="12"/>
@@ -1407,7 +2910,7 @@
       <c r="S1" s="12"/>
       <c r="T1" s="12"/>
       <c r="U1" s="13" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="V1" s="13"/>
       <c r="W1" s="13"/>
@@ -1430,7 +2933,7 @@
       </c>
       <c r="D2" s="2" t="str">
         <f>Data!I1</f>
-        <v>First to Answer</v>
+        <v>FirstToAnswer</v>
       </c>
       <c r="E2" s="2" t="str">
         <f>Data!J1</f>
@@ -1457,16 +2960,16 @@
         <v>Steve</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="O2" s="9" t="str">
         <f t="shared" ref="O2:T2" si="0">E2</f>
@@ -2138,6 +3641,112 @@
       </c>
       <c r="Z8" s="10">
         <f t="shared" ref="Z8" si="52">IF(ISNA(J8),Z7,IF(J8=0,Z7+1,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <f>Data!A8</f>
+        <v>606</v>
+      </c>
+      <c r="B9" s="4" t="str">
+        <f>Data!B8</f>
+        <v>The Brain</v>
+      </c>
+      <c r="C9" s="5" t="str">
+        <f>Data!H8</f>
+        <v>Steve</v>
+      </c>
+      <c r="D9" s="2" t="str">
+        <f>Data!I8</f>
+        <v>Bob</v>
+      </c>
+      <c r="E9" s="1">
+        <f>IF(Data!J8=Data!$G8,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <f>IF(Data!K8=Data!$G8,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <f>IF(Data!L8=Data!$G8,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <f>IF(Data!M8=Data!$G8,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="I9" s="1" t="e">
+        <f>IF(Data!N8=Data!$G8,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J9" s="1" t="e">
+        <f>IF(Data!O8=Data!$G8,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K9" s="1">
+        <f t="shared" ref="K9" si="53">COUNTIF(E9:J9,"&lt;&gt;#N/A")</f>
+        <v>4</v>
+      </c>
+      <c r="L9" s="1">
+        <f t="shared" ref="L9" si="54">SUMIF(E9:J9,"&lt;&gt;#N/A")</f>
+        <v>1</v>
+      </c>
+      <c r="M9" s="1">
+        <f t="shared" ref="M9" si="55">IF(SUMIF(E9:J9,"&lt;&gt;#N/A")=0, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="N9" s="1" t="str">
+        <f t="shared" ref="N9" si="56">IF(L9=1,INDEX($E$2:$J$2,1,MATCH(1,E9:J9,0)),NA())</f>
+        <v>Evan</v>
+      </c>
+      <c r="O9" s="8">
+        <f t="shared" ref="O9" si="57">IF(ISNA(E9),O8,IF(E9=1,O8+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="P9" s="8">
+        <f t="shared" ref="P9" si="58">IF(ISNA(F9),P8,IF(F9=1,P8+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="8">
+        <f t="shared" ref="Q9" si="59">IF(ISNA(G9),Q8,IF(G9=1,Q8+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="R9" s="8">
+        <f t="shared" ref="R9" si="60">IF(ISNA(H9),R8,IF(H9=1,R8+1,0))</f>
+        <v>2</v>
+      </c>
+      <c r="S9" s="8">
+        <f t="shared" ref="S9" si="61">IF(ISNA(I9),S8,IF(I9=1,S8+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="T9" s="8">
+        <f t="shared" ref="T9" si="62">IF(ISNA(J9),T8,IF(J9=1,T8+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="U9" s="10">
+        <f t="shared" ref="U9" si="63">IF(ISNA(E9),U8,IF(E9=0,U8+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="V9" s="10">
+        <f t="shared" ref="V9" si="64">IF(ISNA(F9),V8,IF(F9=0,V8+1,0))</f>
+        <v>2</v>
+      </c>
+      <c r="W9" s="10">
+        <f t="shared" ref="W9" si="65">IF(ISNA(G9),W8,IF(G9=0,W8+1,0))</f>
+        <v>2</v>
+      </c>
+      <c r="X9" s="10">
+        <f t="shared" ref="X9" si="66">IF(ISNA(H9),X8,IF(H9=0,X8+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="Y9" s="10">
+        <f t="shared" ref="Y9" si="67">IF(ISNA(I9),Y8,IF(I9=0,Y8+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="Z9" s="10">
+        <f t="shared" ref="Z9" si="68">IF(ISNA(J9),Z8,IF(J9=0,Z8+1,0))</f>
         <v>0</v>
       </c>
     </row>
@@ -2153,10 +3762,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2164,7 +3773,7 @@
     <col min="1" max="1" width="38.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="str">
         <f>Results!E2</f>
         <v>Bob</v>
@@ -2189,26 +3798,29 @@
         <f>Results!J2</f>
         <v>Steve</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="6">
         <f>SUMIF(Results!E3:E53,"&lt;&gt;#N/A")/COUNTIFS(Results!E3:E53,"&lt;&gt;#N/A",Results!E3:E53,"&lt;&gt;")</f>
-        <v>0.33333333333333331</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="C2" s="6">
         <f>SUMIF(Results!F3:F53,"&lt;&gt;#N/A")/COUNTIFS(Results!F3:F53,"&lt;&gt;#N/A",Results!F3:F53,"&lt;&gt;")</f>
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="D2" s="6">
         <f>SUMIF(Results!G3:G53,"&lt;&gt;#N/A")/COUNTIFS(Results!G3:G53,"&lt;&gt;#N/A",Results!G3:G53,"&lt;&gt;")</f>
-        <v>0.66666666666666663</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="E2" s="6">
         <f>SUMIF(Results!H3:H53,"&lt;&gt;#N/A")/COUNTIFS(Results!H3:H53,"&lt;&gt;#N/A",Results!H3:H53,"&lt;&gt;")</f>
-        <v>0.66666666666666663</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="F2" s="6">
         <f>SUMIF(Results!I3:I53,"&lt;&gt;#N/A")/COUNTIFS(Results!I3:I53,"&lt;&gt;#N/A",Results!I3:I53,"&lt;&gt;")</f>
@@ -2218,10 +3830,14 @@
         <f>SUMIF(Results!J3:J53,"&lt;&gt;#N/A")/COUNTIFS(Results!J3:J53,"&lt;&gt;#N/A",Results!J3:J53,"&lt;&gt;")</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="6">
+        <f>SUM(Results!L3:L53)/SUM(Results!K3:K53)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="6">
         <f>SUMIFS(Results!E3:E53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!E3:E53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!E3:E53, "&lt;&gt;#N/A", Results!E3:E53, "&lt;&gt;")</f>
@@ -2229,15 +3845,15 @@
       </c>
       <c r="C3" s="6">
         <f>SUMIFS(Results!F3:F53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!F3:F53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!F3:F53, "&lt;&gt;#N/A", Results!F3:F53, "&lt;&gt;")</f>
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="D3" s="6">
         <f>SUMIFS(Results!G3:G53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!G3:G53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!G3:G53, "&lt;&gt;#N/A", Results!G3:G53, "&lt;&gt;")</f>
-        <v>0.75</v>
+        <v>0.6</v>
       </c>
       <c r="E3" s="6">
         <f>SUMIFS(Results!H3:H53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!H3:H53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!H3:H53, "&lt;&gt;#N/A", Results!H3:H53, "&lt;&gt;")</f>
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="F3" s="6">
         <f>SUMIFS(Results!I3:I53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!I3:I53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!I3:I53, "&lt;&gt;#N/A", Results!I3:I53, "&lt;&gt;")</f>
@@ -2247,10 +3863,14 @@
         <f>SUMIFS(Results!J3:J53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!J3:J53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!J3:J53, "&lt;&gt;#N/A", Results!J3:J53, "&lt;&gt;")</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="6">
+        <f>SUMIF(Results!B3:B53,"&lt;&gt;#N/A",Results!L3:L53)/SUMIF(Results!B3:B53,"&lt;&gt;#N/A",Results!K3:K53)</f>
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="6">
         <f>SUMIFS(Results!E3:E53,Results!$B$3:$B$53,"=#N/A",Results!E3:E53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!E3:E53, "&lt;&gt;#N/A", Results!E3:E53, "&lt;&gt;")</f>
@@ -2276,10 +3896,14 @@
         <f>SUMIFS(Results!J3:J53,Results!$B$3:$B$53,"=#N/A",Results!J3:J53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!J3:J53, "&lt;&gt;#N/A", Results!J3:J53, "&lt;&gt;")</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="6">
+        <f>SUMIF(Results!B3:B53,"=#N/A",Results!L3:L53)/SUMIF(Results!B3:B53,"=#N/A",Results!K3:K53)</f>
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="1">
         <f>MAX(Results!O3:O53)</f>
@@ -2305,10 +3929,14 @@
         <f>MAX(Results!T3:T53)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="1">
+        <f>MAX(B5:G5)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="1">
         <f>MAX(Results!U3:U53)</f>
@@ -2316,11 +3944,11 @@
       </c>
       <c r="C6" s="1">
         <f>MAX(Results!V3:V53)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" s="1">
         <f>MAX(Results!W3:W53)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" s="1">
         <f>MAX(Results!X3:X53)</f>
@@ -2334,43 +3962,51 @@
         <f>MAX(Results!Z3:Z53)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="1">
+        <f>MAX(B6:G6)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B7" s="1">
-        <f>COUNTIF(Results!N3:N53,Summary!B1)</f>
+        <f>COUNTIF(Results!$N$3:$N$53,Summary!B1)</f>
         <v>0</v>
       </c>
       <c r="C7" s="1">
-        <f>COUNTIF(Results!O3:O53,Summary!C1)</f>
+        <f>COUNTIF(Results!$N$3:$N$53,Summary!C1)</f>
         <v>0</v>
       </c>
       <c r="D7" s="1">
-        <f>COUNTIF(Results!P3:P53,Summary!D1)</f>
+        <f>COUNTIF(Results!$N$3:$N$53,Summary!D1)</f>
         <v>0</v>
       </c>
       <c r="E7" s="1">
-        <f>COUNTIF(Results!Q3:Q53,Summary!E1)</f>
-        <v>0</v>
+        <f>COUNTIF(Results!$N$3:$N$53,Summary!E1)</f>
+        <v>1</v>
       </c>
       <c r="F7" s="1">
-        <f>COUNTIF(Results!R3:R53,Summary!F1)</f>
+        <f>COUNTIF(Results!$N$3:$N$53,Summary!F1)</f>
         <v>0</v>
       </c>
       <c r="G7" s="1">
-        <f>COUNTIF(Results!S3:S53,Summary!G1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <f>COUNTIF(Results!$N$3:$N$53,Summary!G1)</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <f>MAX(B7:G7)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B8" s="7">
         <f>SUMIF(Results!$D$3:$D$53,B1,Results!$L$3:$L$53)/SUMIF(Results!$D$3:$D$53,B1,Results!$K$3:$K$53)</f>
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="C8" s="7">
         <f>SUMIF(Results!$D$3:$D$53,C1,Results!$L$3:$L$53)/SUMIF(Results!$D$3:$D$53,C1,Results!$K$3:$K$53)</f>
@@ -2392,35 +4028,212 @@
         <f>SUMIF(Results!$D$3:$D$53,G1,Results!$L$3:$L$53)/SUMIF(Results!$D$3:$D$53,G1,Results!$K$3:$K$53)</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="7">
-        <f>SUMIF(Results!B3:B53,"&lt;&gt;#N/A",Results!L3:L53)/SUMIF(Results!B3:B53,"&lt;&gt;#N/A",Results!K3:K53)</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="7">
-        <f>SUMIF(Results!B3:B53,"=#N/A",Results!L3:L53)/SUMIF(Results!B3:B53,"=#N/A",Results!K3:K53)</f>
-        <v>0.625</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="7"/>
+      <c r="H8" s="1" t="e">
+        <f>MAX(B8:G8)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="1">
+        <f>SUMIF(Results!E3:E53,"&lt;&gt;#N/A")</f>
+        <v>2</v>
+      </c>
+      <c r="C9" s="1">
+        <f>SUMIF(Results!F3:F53,"&lt;&gt;#N/A")</f>
+        <v>3</v>
+      </c>
+      <c r="D9" s="1">
+        <f>SUMIF(Results!G3:G53,"&lt;&gt;#N/A")</f>
+        <v>4</v>
+      </c>
+      <c r="E9" s="1">
+        <f>SUMIF(Results!H3:H53,"&lt;&gt;#N/A")</f>
+        <v>5</v>
+      </c>
+      <c r="F9" s="1">
+        <f>SUMIF(Results!I3:I53,"&lt;&gt;#N/A")</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <f>SUMIF(Results!J3:J53,"&lt;&gt;#N/A")</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <f>SUM(B9:G9)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="1">
+        <f>COUNTIFS(Results!E3:E53,"&lt;&gt;#N/A",Results!E3:E53,"&lt;&gt;")</f>
+        <v>7</v>
+      </c>
+      <c r="C10" s="1">
+        <f>COUNTIFS(Results!F3:F53,"&lt;&gt;#N/A",Results!F3:F53,"&lt;&gt;")</f>
+        <v>6</v>
+      </c>
+      <c r="D10" s="1">
+        <f>COUNTIFS(Results!G3:G53,"&lt;&gt;#N/A",Results!G3:G53,"&lt;&gt;")</f>
+        <v>7</v>
+      </c>
+      <c r="E10" s="1">
+        <f>COUNTIFS(Results!H3:H53,"&lt;&gt;#N/A",Results!H3:H53,"&lt;&gt;")</f>
+        <v>7</v>
+      </c>
+      <c r="F10" s="1">
+        <f>COUNTIFS(Results!I3:I53,"&lt;&gt;#N/A",Results!I3:I53,"&lt;&gt;")</f>
+        <v>1</v>
+      </c>
+      <c r="G10" s="1">
+        <f>COUNTIFS(Results!J3:J53,"&lt;&gt;#N/A",Results!J3:J53,"&lt;&gt;")</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" ref="H10:H14" si="0">SUM(B10:G10)</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="1">
+        <f>SUMIFS(Results!E3:E53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!E3:E53, "&lt;&gt;#N/A")</f>
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <f>SUMIFS(Results!F3:F53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!F3:F53, "&lt;&gt;#N/A")</f>
+        <v>3</v>
+      </c>
+      <c r="D11" s="1">
+        <f>SUMIFS(Results!G3:G53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!G3:G53, "&lt;&gt;#N/A")</f>
+        <v>3</v>
+      </c>
+      <c r="E11" s="1">
+        <f>SUMIFS(Results!H3:H53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!H3:H53, "&lt;&gt;#N/A")</f>
+        <v>3</v>
+      </c>
+      <c r="F11" s="1">
+        <f>SUMIFS(Results!I3:I53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!I3:I53, "&lt;&gt;#N/A")</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <f>SUMIFS(Results!J3:J53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!J3:J53, "&lt;&gt;#N/A")</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="1">
+        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!E3:E53, "&lt;&gt;#N/A", Results!E3:E53, "&lt;&gt;")</f>
+        <v>5</v>
+      </c>
+      <c r="C12" s="1">
+        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!F3:F53, "&lt;&gt;#N/A", Results!F3:F53, "&lt;&gt;")</f>
+        <v>4</v>
+      </c>
+      <c r="D12" s="1">
+        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!G3:G53, "&lt;&gt;#N/A", Results!G3:G53, "&lt;&gt;")</f>
+        <v>5</v>
+      </c>
+      <c r="E12" s="1">
+        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!H3:H53, "&lt;&gt;#N/A", Results!H3:H53, "&lt;&gt;")</f>
+        <v>5</v>
+      </c>
+      <c r="F12" s="1">
+        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!I3:I53, "&lt;&gt;#N/A", Results!I3:I53, "&lt;&gt;")</f>
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
+        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!J3:J53, "&lt;&gt;#N/A", Results!J3:J53, "&lt;&gt;")</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="1">
+        <f>SUMIFS(Results!E3:E53,Results!$B$3:$B$53,"=#N/A",Results!E3:E53, "&lt;&gt;#N/A")</f>
+        <v>2</v>
+      </c>
+      <c r="C13" s="1">
+        <f>SUMIFS(Results!F3:F53,Results!$B$3:$B$53,"=#N/A",Results!F3:F53, "&lt;&gt;#N/A")</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <f>SUMIFS(Results!G3:G53,Results!$B$3:$B$53,"=#N/A",Results!G3:G53, "&lt;&gt;#N/A")</f>
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
+        <f>SUMIFS(Results!H3:H53,Results!$B$3:$B$53,"=#N/A",Results!H3:H53, "&lt;&gt;#N/A")</f>
+        <v>2</v>
+      </c>
+      <c r="F13" s="1">
+        <f>SUMIFS(Results!I3:I53,Results!$B$3:$B$53,"=#N/A",Results!I3:I53, "&lt;&gt;#N/A")</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
+        <f>SUMIFS(Results!J3:J53,Results!$B$3:$B$53,"=#N/A",Results!J3:J53, "&lt;&gt;#N/A")</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="1">
+        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!E3:E53, "&lt;&gt;#N/A", Results!E3:E53, "&lt;&gt;")</f>
+        <v>2</v>
+      </c>
+      <c r="C14" s="1">
+        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!F3:F53, "&lt;&gt;#N/A", Results!F3:F53, "&lt;&gt;")</f>
+        <v>2</v>
+      </c>
+      <c r="D14" s="1">
+        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!G3:G53, "&lt;&gt;#N/A", Results!G3:G53, "&lt;&gt;")</f>
+        <v>2</v>
+      </c>
+      <c r="E14" s="1">
+        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!H3:H53, "&lt;&gt;#N/A", Results!H3:H53, "&lt;&gt;")</f>
+        <v>2</v>
+      </c>
+      <c r="F14" s="1">
+        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!I3:I53, "&lt;&gt;#N/A", Results!I3:I53, "&lt;&gt;")</f>
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!J3:J53, "&lt;&gt;#N/A", Results!J3:J53, "&lt;&gt;")</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated through episode 607
</commit_message>
<xml_diff>
--- a/SGU_Science_or_Fiction.xlsx
+++ b/SGU_Science_or_Fiction.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Results" sheetId="2" r:id="rId2"/>
     <sheet name="Summary" sheetId="3" r:id="rId3"/>
+    <sheet name="Visuals" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="65">
   <si>
     <t>Episode</t>
   </si>
@@ -212,6 +213,15 @@
   </si>
   <si>
     <t>Total Guesses without Themes</t>
+  </si>
+  <si>
+    <t>Researchers demonstrate how they can steal data from a computer, even one that is currently air-gapped, by simply imaging the blinking light on the hard drive</t>
+  </si>
+  <si>
+    <t>Physicists at the LHC have found for the first time an asymmetry between normal baryonic matter and its anti-matter counterpart</t>
+  </si>
+  <si>
+    <t>A new study finds that cat ownership as a child increases the risk of developing schizophrenia by age 20 by up to 30%</t>
   </si>
 </sst>
 </file>
@@ -470,6 +480,46 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.0185067526415994E-16"/>
+                  <c:y val="-0.1388888888888889"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-0.1388888888888889"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:numFmt formatCode="0%" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
@@ -564,16 +614,16 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.2857142857142857</c:v>
+                  <c:v>0.375</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.5</c:v>
+                  <c:v>0.5714285714285714</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.5714285714285714</c:v>
+                  <c:v>0.625</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.7142857142857143</c:v>
+                  <c:v>0.625</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -582,7 +632,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.5</c:v>
+                  <c:v>0.53125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -598,8 +648,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="202779344"/>
-        <c:axId val="250002264"/>
+        <c:axId val="425637632"/>
+        <c:axId val="425638024"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -712,7 +762,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Summary!$A$4</c15:sqref>
@@ -739,7 +789,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Summary!$B$1:$H$1</c15:sqref>
@@ -774,7 +824,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Summary!$B$4:$H$4</c15:sqref>
@@ -788,13 +838,13 @@
                         <c:v>1</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0</c:v>
+                        <c:v>0.33333333333333331</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.5</c:v>
+                        <c:v>0.66666666666666663</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>1</c:v>
+                        <c:v>0.66666666666666663</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>0</c:v>
@@ -803,7 +853,7 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>0.625</c:v>
+                        <c:v>0.66666666666666663</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -827,6 +877,1291 @@
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>Total Guesses Overall</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="2.1369203849518809E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inBase"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$B$10:$H$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="425638808"/>
+        <c:axId val="425638416"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="425637632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="425638024"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="425638024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="425637632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="425638416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="none"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="425638808"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="425638808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="425638416"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>XXX Has</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> the Highest Percentage of Wins</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>Segments With a Theme</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>% Wins with Themes</c:v>
+                </c:pt>
+              </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-6.5166676073929619E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-5.7500008300526199E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:numFmt formatCode="0%" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Summary!$B$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Bob</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Cara</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Jay</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Evan</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>George</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Steve</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>ALL</c:v>
+                </c:pt>
+              </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$B$3:$H$3</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.45</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="425639984"/>
+        <c:axId val="425640376"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Summary!$A$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>% Wins Overall</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:dLbl>
+                    <c:idx val="4"/>
+                    <c:layout>
+                      <c:manualLayout>
+                        <c:x val="-1.0185067526415994E-16"/>
+                        <c:y val="-0.1388888888888889"/>
+                      </c:manualLayout>
+                    </c:layout>
+                    <c:showLegendKey val="0"/>
+                    <c:showVal val="1"/>
+                    <c:showCatName val="0"/>
+                    <c:showSerName val="0"/>
+                    <c:showPercent val="0"/>
+                    <c:showBubbleSize val="0"/>
+                    <c:extLst>
+                      <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                    </c:extLst>
+                  </c:dLbl>
+                  <c:dLbl>
+                    <c:idx val="5"/>
+                    <c:layout>
+                      <c:manualLayout>
+                        <c:x val="0"/>
+                        <c:y val="-0.1388888888888889"/>
+                      </c:manualLayout>
+                    </c:layout>
+                    <c:showLegendKey val="0"/>
+                    <c:showVal val="1"/>
+                    <c:showCatName val="0"/>
+                    <c:showSerName val="0"/>
+                    <c:showPercent val="0"/>
+                    <c:showBubbleSize val="0"/>
+                    <c:extLst>
+                      <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                    </c:extLst>
+                  </c:dLbl>
+                  <c:numFmt formatCode="0%" sourceLinked="0"/>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1">
+                              <a:lumMod val="75000"/>
+                              <a:lumOff val="25000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:round/>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Summary!$B$1:$H$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>Bob</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Cara</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Jay</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Evan</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>George</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Steve</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>ALL</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Summary!$B$2:$H$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.0%</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>0.375</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.5714285714285714</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.625</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.625</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.53125</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Summary!$A$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>% Wins without Themes</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent3"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Summary!$B$1:$H$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>Bob</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Cara</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Jay</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Evan</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>George</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Steve</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>ALL</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Summary!$B$4:$H$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.0%</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.33333333333333331</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.66666666666666663</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.66666666666666663</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.66666666666666663</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Summary!$A$10</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Total Guesses Overall</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:dLbl>
+                    <c:idx val="4"/>
+                    <c:layout>
+                      <c:manualLayout>
+                        <c:x val="0"/>
+                        <c:y val="2.1369203849518809E-2"/>
+                      </c:manualLayout>
+                    </c:layout>
+                    <c:dLblPos val="outEnd"/>
+                    <c:showLegendKey val="0"/>
+                    <c:showVal val="1"/>
+                    <c:showCatName val="0"/>
+                    <c:showSerName val="0"/>
+                    <c:showPercent val="0"/>
+                    <c:showBubbleSize val="0"/>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                    </c:extLst>
+                  </c:dLbl>
+                  <c:dLbl>
+                    <c:idx val="5"/>
+                    <c:layout>
+                      <c:manualLayout>
+                        <c:x val="0"/>
+                        <c:y val="0"/>
+                      </c:manualLayout>
+                    </c:layout>
+                    <c:dLblPos val="outEnd"/>
+                    <c:showLegendKey val="0"/>
+                    <c:showVal val="1"/>
+                    <c:showCatName val="0"/>
+                    <c:showSerName val="0"/>
+                    <c:showPercent val="0"/>
+                    <c:showBubbleSize val="0"/>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                    </c:extLst>
+                  </c:dLbl>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1">
+                              <a:lumMod val="75000"/>
+                              <a:lumOff val="25000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="inBase"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:round/>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Summary!$B$10:$H$10</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>32</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="5"/>
+                <c:order val="5"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Summary!$A$14</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Total Guesses without Themes</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent6"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Summary!$B$14:$H$14</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>12</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
+      </c:barChart>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total Guesses with Themes</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -900,21 +2235,21 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Summary!$B$10:$H$10</c:f>
+              <c:f>Summary!$B$12:$H$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
@@ -923,7 +2258,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -939,11 +2274,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="480661040"/>
-        <c:axId val="480661432"/>
+        <c:axId val="425940848"/>
+        <c:axId val="425640768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="202779344"/>
+        <c:axId val="425639984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -986,7 +2321,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="250002264"/>
+        <c:crossAx val="425640376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -994,7 +2329,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="250002264"/>
+        <c:axId val="425640376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1045,12 +2380,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202779344"/>
+        <c:crossAx val="425639984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="480661432"/>
+        <c:axId val="425640768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1087,12 +2422,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="480661040"/>
+        <c:crossAx val="425940848"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="480661040"/>
+        <c:axId val="425940848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1101,7 +2436,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="480661432"/>
+        <c:crossAx val="425640768"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -1156,6 +2492,1407 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>XXX Has</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> the Highest Percentage of Wins</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>Segments Without a Theme</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>% Wins without Themes</c:v>
+                </c:pt>
+              </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="8.9925739401415813E-17"/>
+                  <c:y val="-6.1333342187227947E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-6.9000009960631353E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:numFmt formatCode="0%" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Summary!$B$1:$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Bob</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Cara</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Jay</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Evan</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>George</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Steve</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>ALL</c:v>
+                </c:pt>
+              </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$B$4:$H$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.66666666666666663</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.66666666666666663</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.66666666666666663</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="425942024"/>
+        <c:axId val="425942416"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Summary!$A$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>% Wins Overall</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:dLbl>
+                    <c:idx val="4"/>
+                    <c:layout>
+                      <c:manualLayout>
+                        <c:x val="-1.0185067526415994E-16"/>
+                        <c:y val="-0.1388888888888889"/>
+                      </c:manualLayout>
+                    </c:layout>
+                    <c:showLegendKey val="0"/>
+                    <c:showVal val="1"/>
+                    <c:showCatName val="0"/>
+                    <c:showSerName val="0"/>
+                    <c:showPercent val="0"/>
+                    <c:showBubbleSize val="0"/>
+                    <c:extLst>
+                      <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                    </c:extLst>
+                  </c:dLbl>
+                  <c:dLbl>
+                    <c:idx val="5"/>
+                    <c:layout>
+                      <c:manualLayout>
+                        <c:x val="0"/>
+                        <c:y val="-0.1388888888888889"/>
+                      </c:manualLayout>
+                    </c:layout>
+                    <c:showLegendKey val="0"/>
+                    <c:showVal val="1"/>
+                    <c:showCatName val="0"/>
+                    <c:showSerName val="0"/>
+                    <c:showPercent val="0"/>
+                    <c:showBubbleSize val="0"/>
+                    <c:extLst>
+                      <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                    </c:extLst>
+                  </c:dLbl>
+                  <c:numFmt formatCode="0%" sourceLinked="0"/>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1">
+                              <a:lumMod val="75000"/>
+                              <a:lumOff val="25000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:round/>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Summary!$B$1:$H$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>Bob</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Cara</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Jay</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Evan</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>George</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Steve</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>ALL</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Summary!$B$2:$H$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.0%</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>0.375</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.5714285714285714</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.625</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.625</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.53125</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Summary!$A$3</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>% Wins with Themes</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent2"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:dLbl>
+                    <c:idx val="4"/>
+                    <c:layout>
+                      <c:manualLayout>
+                        <c:x val="0"/>
+                        <c:y val="-6.5166676073929619E-2"/>
+                      </c:manualLayout>
+                    </c:layout>
+                    <c:showLegendKey val="0"/>
+                    <c:showVal val="1"/>
+                    <c:showCatName val="0"/>
+                    <c:showSerName val="0"/>
+                    <c:showPercent val="0"/>
+                    <c:showBubbleSize val="0"/>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                    </c:extLst>
+                  </c:dLbl>
+                  <c:dLbl>
+                    <c:idx val="5"/>
+                    <c:layout>
+                      <c:manualLayout>
+                        <c:x val="0"/>
+                        <c:y val="-5.7500008300526199E-2"/>
+                      </c:manualLayout>
+                    </c:layout>
+                    <c:showLegendKey val="0"/>
+                    <c:showVal val="1"/>
+                    <c:showCatName val="0"/>
+                    <c:showSerName val="0"/>
+                    <c:showPercent val="0"/>
+                    <c:showBubbleSize val="0"/>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                    </c:extLst>
+                  </c:dLbl>
+                  <c:numFmt formatCode="0%" sourceLinked="0"/>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1">
+                              <a:lumMod val="75000"/>
+                              <a:lumOff val="25000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:round/>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Summary!$B$1:$H$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>Bob</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Cara</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Jay</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Evan</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>George</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Steve</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>ALL</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Summary!$B$3:$H$3</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.0%</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.75</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.6</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.6</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.45</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Summary!$A$10</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Total Guesses Overall</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:dLbl>
+                    <c:idx val="4"/>
+                    <c:layout>
+                      <c:manualLayout>
+                        <c:x val="0"/>
+                        <c:y val="2.1369203849518809E-2"/>
+                      </c:manualLayout>
+                    </c:layout>
+                    <c:dLblPos val="outEnd"/>
+                    <c:showLegendKey val="0"/>
+                    <c:showVal val="1"/>
+                    <c:showCatName val="0"/>
+                    <c:showSerName val="0"/>
+                    <c:showPercent val="0"/>
+                    <c:showBubbleSize val="0"/>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                    </c:extLst>
+                  </c:dLbl>
+                  <c:dLbl>
+                    <c:idx val="5"/>
+                    <c:layout>
+                      <c:manualLayout>
+                        <c:x val="0"/>
+                        <c:y val="0"/>
+                      </c:manualLayout>
+                    </c:layout>
+                    <c:dLblPos val="outEnd"/>
+                    <c:showLegendKey val="0"/>
+                    <c:showVal val="1"/>
+                    <c:showCatName val="0"/>
+                    <c:showSerName val="0"/>
+                    <c:showPercent val="0"/>
+                    <c:showBubbleSize val="0"/>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                    </c:extLst>
+                  </c:dLbl>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1">
+                              <a:lumMod val="75000"/>
+                              <a:lumOff val="25000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="inBase"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:round/>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Summary!$B$10:$H$10</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>32</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="4"/>
+                <c:order val="4"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Summary!$A$12</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Total Guesses with Themes</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1">
+                              <a:lumMod val="75000"/>
+                              <a:lumOff val="25000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="inBase"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:round/>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Summary!$B$12:$H$12</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>20</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
+      </c:barChart>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total Guesses without Themes</c:v>
+                </c:pt>
+              </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inBase"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$B$14:$H$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="425943200"/>
+        <c:axId val="425942808"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="425942024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="425942416"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="425942416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="425942024"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="425942808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="none"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="425943200"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="425943200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="425942808"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -1263,6 +4000,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -1766,25 +4583,1033 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>157370</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>106846</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>438978</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>183046</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>274982</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>74543</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1793,6 +5618,70 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>273326</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>548308</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>74543</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>554934</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>217004</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>74543</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2067,7 +5956,7 @@
   <dimension ref="A1:O53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2475,13 +6364,55 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
+      <c r="A9">
+        <v>607</v>
+      </c>
+      <c r="B9" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G9" s="1">
+        <v>3</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J9" s="1">
+        <v>3</v>
+      </c>
+      <c r="K9" s="1">
+        <v>3</v>
+      </c>
+      <c r="L9" s="1">
+        <v>3</v>
+      </c>
+      <c r="M9" s="1">
+        <v>2</v>
+      </c>
+      <c r="N9" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O9" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G10" s="1"/>
@@ -2887,10 +6818,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z9"/>
+  <dimension ref="A1:Z10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+      <selection activeCell="A10" sqref="A10:Z10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3747,6 +7678,112 @@
       </c>
       <c r="Z9" s="10">
         <f t="shared" ref="Z9" si="68">IF(ISNA(J9),Z8,IF(J9=0,Z8+1,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <f>Data!A9</f>
+        <v>607</v>
+      </c>
+      <c r="B10" s="4" t="e">
+        <f>Data!B9</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C10" s="5" t="str">
+        <f>Data!H9</f>
+        <v>Steve</v>
+      </c>
+      <c r="D10" s="2" t="str">
+        <f>Data!I9</f>
+        <v>Evan</v>
+      </c>
+      <c r="E10" s="1">
+        <f>IF(Data!J9=Data!$G9,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <f>IF(Data!K9=Data!$G9,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G10" s="1">
+        <f>IF(Data!L9=Data!$G9,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H10" s="1">
+        <f>IF(Data!M9=Data!$G9,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="1" t="e">
+        <f>IF(Data!N9=Data!$G9,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J10" s="1" t="e">
+        <f>IF(Data!O9=Data!$G9,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K10" s="1">
+        <f t="shared" ref="K10" si="69">COUNTIF(E10:J10,"&lt;&gt;#N/A")</f>
+        <v>4</v>
+      </c>
+      <c r="L10" s="1">
+        <f t="shared" ref="L10" si="70">SUMIF(E10:J10,"&lt;&gt;#N/A")</f>
+        <v>3</v>
+      </c>
+      <c r="M10" s="1">
+        <f t="shared" ref="M10" si="71">IF(SUMIF(E10:J10,"&lt;&gt;#N/A")=0, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="N10" s="1" t="e">
+        <f t="shared" ref="N10" si="72">IF(L10=1,INDEX($E$2:$J$2,1,MATCH(1,E10:J10,0)),NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O10" s="8">
+        <f t="shared" ref="O10" si="73">IF(ISNA(E10),O9,IF(E10=1,O9+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="P10" s="8">
+        <f t="shared" ref="P10" si="74">IF(ISNA(F10),P9,IF(F10=1,P9+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="Q10" s="8">
+        <f t="shared" ref="Q10" si="75">IF(ISNA(G10),Q9,IF(G10=1,Q9+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="R10" s="8">
+        <f t="shared" ref="R10" si="76">IF(ISNA(H10),R9,IF(H10=1,R9+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="S10" s="8">
+        <f t="shared" ref="S10" si="77">IF(ISNA(I10),S9,IF(I10=1,S9+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="T10" s="8">
+        <f t="shared" ref="T10" si="78">IF(ISNA(J10),T9,IF(J10=1,T9+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="U10" s="10">
+        <f t="shared" ref="U10" si="79">IF(ISNA(E10),U9,IF(E10=0,U9+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="V10" s="10">
+        <f t="shared" ref="V10" si="80">IF(ISNA(F10),V9,IF(F10=0,V9+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="W10" s="10">
+        <f t="shared" ref="W10" si="81">IF(ISNA(G10),W9,IF(G10=0,W9+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="X10" s="10">
+        <f t="shared" ref="X10" si="82">IF(ISNA(H10),X9,IF(H10=0,X9+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="Y10" s="10">
+        <f t="shared" ref="Y10" si="83">IF(ISNA(I10),Y9,IF(I10=0,Y9+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="Z10" s="10">
+        <f t="shared" ref="Z10" si="84">IF(ISNA(J10),Z9,IF(J10=0,Z9+1,0))</f>
         <v>0</v>
       </c>
     </row>
@@ -3764,8 +7801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3808,19 +7845,19 @@
       </c>
       <c r="B2" s="6">
         <f>SUMIF(Results!E3:E53,"&lt;&gt;#N/A")/COUNTIFS(Results!E3:E53,"&lt;&gt;#N/A",Results!E3:E53,"&lt;&gt;")</f>
-        <v>0.2857142857142857</v>
+        <v>0.375</v>
       </c>
       <c r="C2" s="6">
         <f>SUMIF(Results!F3:F53,"&lt;&gt;#N/A")/COUNTIFS(Results!F3:F53,"&lt;&gt;#N/A",Results!F3:F53,"&lt;&gt;")</f>
-        <v>0.5</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="D2" s="6">
         <f>SUMIF(Results!G3:G53,"&lt;&gt;#N/A")/COUNTIFS(Results!G3:G53,"&lt;&gt;#N/A",Results!G3:G53,"&lt;&gt;")</f>
-        <v>0.5714285714285714</v>
+        <v>0.625</v>
       </c>
       <c r="E2" s="6">
         <f>SUMIF(Results!H3:H53,"&lt;&gt;#N/A")/COUNTIFS(Results!H3:H53,"&lt;&gt;#N/A",Results!H3:H53,"&lt;&gt;")</f>
-        <v>0.7142857142857143</v>
+        <v>0.625</v>
       </c>
       <c r="F2" s="6">
         <f>SUMIF(Results!I3:I53,"&lt;&gt;#N/A")/COUNTIFS(Results!I3:I53,"&lt;&gt;#N/A",Results!I3:I53,"&lt;&gt;")</f>
@@ -3832,7 +7869,7 @@
       </c>
       <c r="H2" s="6">
         <f>SUM(Results!L3:L53)/SUM(Results!K3:K53)</f>
-        <v>0.5</v>
+        <v>0.53125</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -3878,15 +7915,15 @@
       </c>
       <c r="C4" s="6">
         <f>SUMIFS(Results!F3:F53,Results!$B$3:$B$53,"=#N/A",Results!F3:F53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!F3:F53, "&lt;&gt;#N/A", Results!F3:F53, "&lt;&gt;")</f>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D4" s="6">
         <f>SUMIFS(Results!G3:G53,Results!$B$3:$B$53,"=#N/A",Results!G3:G53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!G3:G53, "&lt;&gt;#N/A", Results!G3:G53, "&lt;&gt;")</f>
-        <v>0.5</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="E4" s="6">
         <f>SUMIFS(Results!H3:H53,Results!$B$3:$B$53,"=#N/A",Results!H3:H53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!H3:H53, "&lt;&gt;#N/A", Results!H3:H53, "&lt;&gt;")</f>
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F4" s="6" t="e">
         <f>SUMIFS(Results!I3:I53,Results!$B$3:$B$53,"=#N/A",Results!I3:I53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!I3:I53, "&lt;&gt;#N/A", Results!I3:I53, "&lt;&gt;")</f>
@@ -3898,7 +7935,7 @@
       </c>
       <c r="H4" s="6">
         <f>SUMIF(Results!B3:B53,"=#N/A",Results!L3:L53)/SUMIF(Results!B3:B53,"=#N/A",Results!K3:K53)</f>
-        <v>0.625</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -4039,15 +8076,15 @@
       </c>
       <c r="B9" s="1">
         <f>SUMIF(Results!E3:E53,"&lt;&gt;#N/A")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C9" s="1">
         <f>SUMIF(Results!F3:F53,"&lt;&gt;#N/A")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D9" s="1">
         <f>SUMIF(Results!G3:G53,"&lt;&gt;#N/A")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E9" s="1">
         <f>SUMIF(Results!H3:H53,"&lt;&gt;#N/A")</f>
@@ -4063,7 +8100,7 @@
       </c>
       <c r="H9" s="1">
         <f>SUM(B9:G9)</f>
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -4072,19 +8109,19 @@
       </c>
       <c r="B10" s="1">
         <f>COUNTIFS(Results!E3:E53,"&lt;&gt;#N/A",Results!E3:E53,"&lt;&gt;")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C10" s="1">
         <f>COUNTIFS(Results!F3:F53,"&lt;&gt;#N/A",Results!F3:F53,"&lt;&gt;")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D10" s="1">
         <f>COUNTIFS(Results!G3:G53,"&lt;&gt;#N/A",Results!G3:G53,"&lt;&gt;")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E10" s="1">
         <f>COUNTIFS(Results!H3:H53,"&lt;&gt;#N/A",Results!H3:H53,"&lt;&gt;")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F10" s="1">
         <f>COUNTIFS(Results!I3:I53,"&lt;&gt;#N/A",Results!I3:I53,"&lt;&gt;")</f>
@@ -4096,7 +8133,7 @@
       </c>
       <c r="H10" s="1">
         <f t="shared" ref="H10:H14" si="0">SUM(B10:G10)</f>
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -4171,15 +8208,15 @@
       </c>
       <c r="B13" s="1">
         <f>SUMIFS(Results!E3:E53,Results!$B$3:$B$53,"=#N/A",Results!E3:E53, "&lt;&gt;#N/A")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C13" s="1">
         <f>SUMIFS(Results!F3:F53,Results!$B$3:$B$53,"=#N/A",Results!F3:F53, "&lt;&gt;#N/A")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="1">
         <f>SUMIFS(Results!G3:G53,Results!$B$3:$B$53,"=#N/A",Results!G3:G53, "&lt;&gt;#N/A")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13" s="1">
         <f>SUMIFS(Results!H3:H53,Results!$B$3:$B$53,"=#N/A",Results!H3:H53, "&lt;&gt;#N/A")</f>
@@ -4195,7 +8232,7 @@
       </c>
       <c r="H13" s="1">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -4204,19 +8241,19 @@
       </c>
       <c r="B14" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!E3:E53, "&lt;&gt;#N/A", Results!E3:E53, "&lt;&gt;")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C14" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!F3:F53, "&lt;&gt;#N/A", Results!F3:F53, "&lt;&gt;")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D14" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!G3:G53, "&lt;&gt;#N/A", Results!G3:G53, "&lt;&gt;")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E14" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!H3:H53, "&lt;&gt;#N/A", Results!H3:H53, "&lt;&gt;")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F14" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!I3:I53, "&lt;&gt;#N/A", Results!I3:I53, "&lt;&gt;")</f>
@@ -4228,12 +8265,26 @@
       </c>
       <c r="H14" s="1">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated through episode 610; added field for panelist sweep
</commit_message>
<xml_diff>
--- a/SGU_Science_or_Fiction.xlsx
+++ b/SGU_Science_or_Fiction.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="76">
   <si>
     <t>Episode</t>
   </si>
@@ -75,9 +75,6 @@
   </si>
   <si>
     <t>Item 4</t>
-  </si>
-  <si>
-    <t>Sweep</t>
   </si>
   <si>
     <t>A new study finds that exercising only on the weekends, compared to being inactive, has no measurable benefit in terms of heart health and mortality. http://jamanetwork.com/journals/jamainternalmedicine/fullarticle/2596007</t>
@@ -222,6 +219,42 @@
   </si>
   <si>
     <t>A new study finds that cat ownership as a child increases the risk of developing schizophrenia by age 20 by up to 30%</t>
+  </si>
+  <si>
+    <t>Paleontologists have found the world’s oldest fossils, at least 3.7 billion years old, in Quebec, Canada</t>
+  </si>
+  <si>
+    <t>The 94 year old inventor of the lithium-ion battery announced a new battery breakthrough, that has 3 times the energy density, more recharge cycles, greater stability, faster recharge, out of cheaper and environmentally friendly materials.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A new study finds that American homeowners actually lost over $1 billion last year by refinancing incorrectly. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Researchers have uncovered evidence that Neanderthal Man was self-medicating with aspirin 50,000 years ago. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Researchers report that they were able to grow potatoes in simulated Martian soil and atmosphere. </t>
+  </si>
+  <si>
+    <t>A major review of climate change research finds that there is significant publication bias favoring positive studies.</t>
+  </si>
+  <si>
+    <t>Scientists report that, for the first time, they were able to change adult skin cells into neural stem cells without making any genetic changes</t>
+  </si>
+  <si>
+    <t>A newly published estimate concludes that worldwide spiders consume between 400-800 million tons of insects and other invertebrates each year.</t>
+  </si>
+  <si>
+    <t>HostSweep</t>
+  </si>
+  <si>
+    <t>PanelSweep</t>
+  </si>
+  <si>
+    <t>Host Sweeps</t>
+  </si>
+  <si>
+    <t>Panelist Sweeps</t>
   </si>
 </sst>
 </file>
@@ -614,16 +647,16 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.375</c:v>
+                  <c:v>0.45454545454545453</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.5714285714285714</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.625</c:v>
+                  <c:v>0.72727272727272729</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.625</c:v>
+                  <c:v>0.63636363636363635</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -632,7 +665,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.53125</c:v>
+                  <c:v>0.61363636363636365</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -648,8 +681,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="425637632"/>
-        <c:axId val="425638024"/>
+        <c:axId val="165056888"/>
+        <c:axId val="392918112"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -835,13 +868,13 @@
                       <c:formatCode>0.0%</c:formatCode>
                       <c:ptCount val="7"/>
                       <c:pt idx="0">
-                        <c:v>1</c:v>
+                        <c:v>0.83333333333333337</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.33333333333333331</c:v>
+                        <c:v>0.66666666666666663</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.66666666666666663</c:v>
+                        <c:v>0.83333333333333337</c:v>
                       </c:pt>
                       <c:pt idx="3">
                         <c:v>0.66666666666666663</c:v>
@@ -853,7 +886,7 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>0.66666666666666663</c:v>
+                        <c:v>0.75</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -997,16 +1030,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
@@ -1015,7 +1048,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>32</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1031,11 +1064,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="425638808"/>
-        <c:axId val="425638416"/>
+        <c:axId val="392916936"/>
+        <c:axId val="392914584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="425637632"/>
+        <c:axId val="165056888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1078,7 +1111,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="425638024"/>
+        <c:crossAx val="392918112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1086,7 +1119,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="425638024"/>
+        <c:axId val="392918112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1137,12 +1170,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="425637632"/>
+        <c:crossAx val="165056888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="425638416"/>
+        <c:axId val="392914584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1179,12 +1212,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="425638808"/>
+        <c:crossAx val="392916936"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="425638808"/>
+        <c:axId val="392916936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1193,7 +1226,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="425638416"/>
+        <c:crossAx val="392914584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1368,7 +1401,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t>Segments With a Theme</a:t>
+              <a:t>For Segments With a Theme</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -1607,8 +1640,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="425639984"/>
-        <c:axId val="425640376"/>
+        <c:axId val="210393400"/>
+        <c:axId val="399057864"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -1784,16 +1817,16 @@
                       <c:formatCode>0.0%</c:formatCode>
                       <c:ptCount val="7"/>
                       <c:pt idx="0">
-                        <c:v>0.375</c:v>
+                        <c:v>0.45454545454545453</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.5714285714285714</c:v>
+                        <c:v>0.7</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.625</c:v>
+                        <c:v>0.72727272727272729</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0.625</c:v>
+                        <c:v>0.63636363636363635</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>0</c:v>
@@ -1802,7 +1835,7 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>0.53125</c:v>
+                        <c:v>0.61363636363636365</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1888,13 +1921,13 @@
                       <c:formatCode>0.0%</c:formatCode>
                       <c:ptCount val="7"/>
                       <c:pt idx="0">
-                        <c:v>1</c:v>
+                        <c:v>0.83333333333333337</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.33333333333333331</c:v>
+                        <c:v>0.66666666666666663</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.66666666666666663</c:v>
+                        <c:v>0.83333333333333337</c:v>
                       </c:pt>
                       <c:pt idx="3">
                         <c:v>0.66666666666666663</c:v>
@@ -1906,7 +1939,7 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>0.66666666666666663</c:v>
+                        <c:v>0.75</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2051,16 +2084,16 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="7"/>
                       <c:pt idx="0">
-                        <c:v>8</c:v>
+                        <c:v>11</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>7</c:v>
+                        <c:v>10</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>8</c:v>
+                        <c:v>11</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>8</c:v>
+                        <c:v>11</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>1</c:v>
@@ -2069,7 +2102,7 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>32</c:v>
+                        <c:v>44</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2120,16 +2153,16 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="7"/>
                       <c:pt idx="0">
-                        <c:v>3</c:v>
+                        <c:v>6</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>3</c:v>
+                        <c:v>6</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>3</c:v>
+                        <c:v>6</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>3</c:v>
+                        <c:v>6</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>0</c:v>
@@ -2138,7 +2171,7 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>12</c:v>
+                        <c:v>24</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2274,11 +2307,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="425940848"/>
-        <c:axId val="425640768"/>
+        <c:axId val="399058648"/>
+        <c:axId val="399058256"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="425639984"/>
+        <c:axId val="210393400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2321,7 +2354,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="425640376"/>
+        <c:crossAx val="399057864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2329,7 +2362,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="425640376"/>
+        <c:axId val="399057864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2380,12 +2413,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="425639984"/>
+        <c:crossAx val="210393400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="425640768"/>
+        <c:axId val="399058256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2422,12 +2455,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="425940848"/>
+        <c:crossAx val="399058648"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="425940848"/>
+        <c:axId val="399058648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2436,7 +2469,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="425640768"/>
+        <c:crossAx val="399058256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2611,7 +2644,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t>Segments Without a Theme</a:t>
+              <a:t>For Segments Without a Theme</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -2815,13 +2848,13 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0.83333333333333337</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.33333333333333331</c:v>
+                  <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.66666666666666663</c:v>
+                  <c:v>0.83333333333333337</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.66666666666666663</c:v>
@@ -2833,7 +2866,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.66666666666666663</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -2850,8 +2883,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="425942024"/>
-        <c:axId val="425942416"/>
+        <c:axId val="399059824"/>
+        <c:axId val="399060216"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -3027,16 +3060,16 @@
                       <c:formatCode>0.0%</c:formatCode>
                       <c:ptCount val="7"/>
                       <c:pt idx="0">
-                        <c:v>0.375</c:v>
+                        <c:v>0.45454545454545453</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.5714285714285714</c:v>
+                        <c:v>0.7</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.625</c:v>
+                        <c:v>0.72727272727272729</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0.625</c:v>
+                        <c:v>0.63636363636363635</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>0</c:v>
@@ -3045,7 +3078,7 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>0.53125</c:v>
+                        <c:v>0.61363636363636365</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3388,16 +3421,16 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="7"/>
                       <c:pt idx="0">
-                        <c:v>8</c:v>
+                        <c:v>11</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>7</c:v>
+                        <c:v>10</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>8</c:v>
+                        <c:v>11</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>8</c:v>
+                        <c:v>11</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>1</c:v>
@@ -3406,7 +3439,7 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>32</c:v>
+                        <c:v>44</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3634,16 +3667,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -3652,7 +3685,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -3669,11 +3702,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="425943200"/>
-        <c:axId val="425942808"/>
+        <c:axId val="399061000"/>
+        <c:axId val="399060608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="425942024"/>
+        <c:axId val="399059824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3716,7 +3749,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="425942416"/>
+        <c:crossAx val="399060216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3724,7 +3757,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="425942416"/>
+        <c:axId val="399060216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3775,12 +3808,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="425942024"/>
+        <c:crossAx val="399059824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="425942808"/>
+        <c:axId val="399060608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3819,12 +3852,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="425943200"/>
+        <c:crossAx val="399061000"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="425943200"/>
+        <c:axId val="399061000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3833,7 +3866,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="425942808"/>
+        <c:crossAx val="399060608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5956,7 +5989,7 @@
   <dimension ref="A1:O53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5985,19 +6018,19 @@
         <v>15</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>6</v>
@@ -6071,13 +6104,13 @@
         <v>#N/A</v>
       </c>
       <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
       </c>
       <c r="F3" t="e">
         <f>NA()</f>
@@ -6090,7 +6123,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J3" s="1">
         <v>1</v>
@@ -6118,16 +6151,16 @@
         <v>602</v>
       </c>
       <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
         <v>20</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>21</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
       </c>
       <c r="F4" t="e">
         <f>NA()</f>
@@ -6168,19 +6201,19 @@
         <v>603</v>
       </c>
       <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
         <v>34</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>35</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>36</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>37</v>
-      </c>
-      <c r="F5" t="s">
-        <v>38</v>
       </c>
       <c r="G5" s="1">
         <v>2</v>
@@ -6217,16 +6250,16 @@
         <v>604</v>
       </c>
       <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
         <v>39</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>40</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>41</v>
-      </c>
-      <c r="E6" t="s">
-        <v>42</v>
       </c>
       <c r="F6" t="e">
         <f>NA()</f>
@@ -6271,13 +6304,13 @@
         <v>#N/A</v>
       </c>
       <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
         <v>43</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>44</v>
-      </c>
-      <c r="E7" t="s">
-        <v>45</v>
       </c>
       <c r="F7" t="e">
         <f>NA()</f>
@@ -6290,7 +6323,7 @@
         <v>12</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J7" s="1">
         <v>2</v>
@@ -6318,16 +6351,16 @@
         <v>606</v>
       </c>
       <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" t="s">
         <v>49</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>50</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>51</v>
-      </c>
-      <c r="E8" t="s">
-        <v>52</v>
       </c>
       <c r="F8" t="e">
         <f>NA()</f>
@@ -6372,13 +6405,13 @@
         <v>#N/A</v>
       </c>
       <c r="C9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" t="s">
         <v>62</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>63</v>
-      </c>
-      <c r="E9" t="s">
-        <v>64</v>
       </c>
       <c r="F9" t="e">
         <f>NA()</f>
@@ -6415,31 +6448,157 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
+      <c r="A10">
+        <v>608</v>
+      </c>
+      <c r="B10" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G10" s="1">
+        <v>3</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J10" s="1">
+        <v>2</v>
+      </c>
+      <c r="K10" s="1">
+        <v>3</v>
+      </c>
+      <c r="L10" s="1">
+        <v>3</v>
+      </c>
+      <c r="M10" s="1">
+        <v>3</v>
+      </c>
+      <c r="N10" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O10" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
+      <c r="A11">
+        <v>609</v>
+      </c>
+      <c r="B11" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G11" s="1">
+        <v>2</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" s="1">
+        <v>2</v>
+      </c>
+      <c r="K11" s="1">
+        <v>2</v>
+      </c>
+      <c r="L11" s="1">
+        <v>2</v>
+      </c>
+      <c r="M11" s="1">
+        <v>3</v>
+      </c>
+      <c r="N11" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O11" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
+      <c r="A12">
+        <v>610</v>
+      </c>
+      <c r="B12" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" t="s">
+        <v>71</v>
+      </c>
+      <c r="F12" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" s="1">
+        <v>1</v>
+      </c>
+      <c r="K12" s="1">
+        <v>1</v>
+      </c>
+      <c r="L12" s="1">
+        <v>1</v>
+      </c>
+      <c r="M12" s="1">
+        <v>1</v>
+      </c>
+      <c r="N12" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O12" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G13" s="1"/>
@@ -6818,38 +6977,40 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z10"/>
+  <dimension ref="A1:AA13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:Z10"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:AA13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" customWidth="1"/>
+    <col min="15" max="15" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="O1" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="P1" s="12"/>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="P1" s="12" t="s">
+        <v>30</v>
+      </c>
       <c r="Q1" s="12"/>
       <c r="R1" s="12"/>
       <c r="S1" s="12"/>
       <c r="T1" s="12"/>
-      <c r="U1" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="V1" s="13"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="13" t="s">
+        <v>31</v>
+      </c>
       <c r="W1" s="13"/>
       <c r="X1" s="13"/>
       <c r="Y1" s="13"/>
       <c r="Z1" s="13"/>
+      <c r="AA1" s="13"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="str">
         <f>Data!A1</f>
         <v>Episode</v>
@@ -6891,67 +7052,70 @@
         <v>Steve</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="O2" s="9" t="str">
-        <f t="shared" ref="O2:T2" si="0">E2</f>
+        <v>73</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="P2" s="9" t="str">
+        <f>E2</f>
         <v>Bob</v>
       </c>
-      <c r="P2" s="9" t="str">
-        <f t="shared" si="0"/>
+      <c r="Q2" s="9" t="str">
+        <f>F2</f>
         <v>Cara</v>
       </c>
-      <c r="Q2" s="9" t="str">
-        <f t="shared" si="0"/>
+      <c r="R2" s="9" t="str">
+        <f>G2</f>
         <v>Jay</v>
       </c>
-      <c r="R2" s="9" t="str">
+      <c r="S2" s="9" t="str">
+        <f>H2</f>
+        <v>Evan</v>
+      </c>
+      <c r="T2" s="9" t="str">
+        <f>I2</f>
+        <v>George</v>
+      </c>
+      <c r="U2" s="9" t="str">
+        <f>J2</f>
+        <v>Steve</v>
+      </c>
+      <c r="V2" s="11" t="str">
+        <f>P2</f>
+        <v>Bob</v>
+      </c>
+      <c r="W2" s="11" t="str">
+        <f>Q2</f>
+        <v>Cara</v>
+      </c>
+      <c r="X2" s="11" t="str">
+        <f t="shared" ref="X2:AA2" si="0">R2</f>
+        <v>Jay</v>
+      </c>
+      <c r="Y2" s="11" t="str">
         <f t="shared" si="0"/>
         <v>Evan</v>
       </c>
-      <c r="S2" s="9" t="str">
+      <c r="Z2" s="11" t="str">
         <f t="shared" si="0"/>
         <v>George</v>
       </c>
-      <c r="T2" s="9" t="str">
+      <c r="AA2" s="11" t="str">
         <f t="shared" si="0"/>
         <v>Steve</v>
       </c>
-      <c r="U2" s="11" t="str">
-        <f>O2</f>
-        <v>Bob</v>
-      </c>
-      <c r="V2" s="11" t="str">
-        <f>P2</f>
-        <v>Cara</v>
-      </c>
-      <c r="W2" s="11" t="str">
-        <f t="shared" ref="W2:Z2" si="1">Q2</f>
-        <v>Jay</v>
-      </c>
-      <c r="X2" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>Evan</v>
-      </c>
-      <c r="Y2" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>George</v>
-      </c>
-      <c r="Z2" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>Steve</v>
-      </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <f>Data!A2</f>
         <v>600</v>
@@ -7001,16 +7165,17 @@
         <v>0</v>
       </c>
       <c r="M3" s="1">
-        <f t="shared" ref="M3:M8" si="2">IF(SUMIF(E3:J3,"&lt;&gt;#N/A")=0, 1, 0)</f>
-        <v>1</v>
-      </c>
-      <c r="N3" s="1" t="e">
-        <f t="shared" ref="N3" si="3">IF(L3=1,INDEX($E$2:$J$2,1,MATCH(1,E3:J3,0)),NA())</f>
+        <f t="shared" ref="M3:M8" si="1">IF(SUMIF(E3:J3,"&lt;&gt;#N/A")=0, 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="N3" s="1">
+        <f>IF(K3=L3,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O3" s="1" t="e">
+        <f t="shared" ref="O3" si="2">IF(L3=1,INDEX($E$2:$J$2,1,MATCH(1,E3:J3,0)),NA())</f>
         <v>#N/A</v>
       </c>
-      <c r="O3" s="8">
-        <v>0</v>
-      </c>
       <c r="P3" s="8">
         <v>0</v>
       </c>
@@ -7026,14 +7191,14 @@
       <c r="T3" s="8">
         <v>0</v>
       </c>
-      <c r="U3" s="10">
-        <v>1</v>
+      <c r="U3" s="8">
+        <v>0</v>
       </c>
       <c r="V3" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W3" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X3" s="10">
         <v>1</v>
@@ -7042,10 +7207,13 @@
         <v>1</v>
       </c>
       <c r="Z3" s="10">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <f>Data!A3</f>
         <v>601</v>
@@ -7087,71 +7255,75 @@
         <v>#N/A</v>
       </c>
       <c r="K4" s="1">
-        <f t="shared" ref="K4:K5" si="4">COUNTIF(E4:J4,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="K4:K5" si="3">COUNTIF(E4:J4,"&lt;&gt;#N/A")</f>
         <v>4</v>
       </c>
       <c r="L4" s="1">
-        <f t="shared" ref="L4:L5" si="5">SUMIF(E4:J4,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="L4:L5" si="4">SUMIF(E4:J4,"&lt;&gt;#N/A")</f>
         <v>3</v>
       </c>
       <c r="M4" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N4" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N4" s="1">
+        <f t="shared" ref="N4:N13" si="5">IF(K4=L4,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O4" s="1" t="e">
         <f>IF(L4=1,INDEX($E$2:$J$2,1,MATCH(1,E4:J4,0)),NA())</f>
         <v>#N/A</v>
       </c>
-      <c r="O4" s="8">
-        <f t="shared" ref="O4:O5" si="6">IF(ISNA(E4),O3,IF(E4=1,O3+1,0))</f>
-        <v>1</v>
-      </c>
       <c r="P4" s="8">
-        <f t="shared" ref="P4:P5" si="7">IF(ISNA(F4),P3,IF(F4=1,P3+1,0))</f>
-        <v>0</v>
+        <f t="shared" ref="P4:P5" si="6">IF(ISNA(E4),P3,IF(E4=1,P3+1,0))</f>
+        <v>1</v>
       </c>
       <c r="Q4" s="8">
-        <f t="shared" ref="Q4:Q5" si="8">IF(ISNA(G4),Q3,IF(G4=1,Q3+1,0))</f>
-        <v>1</v>
+        <f t="shared" ref="Q4:Q5" si="7">IF(ISNA(F4),Q3,IF(F4=1,Q3+1,0))</f>
+        <v>0</v>
       </c>
       <c r="R4" s="8">
-        <f t="shared" ref="R4:R5" si="9">IF(ISNA(H4),R3,IF(H4=1,R3+1,0))</f>
+        <f t="shared" ref="R4:R5" si="8">IF(ISNA(G4),R3,IF(G4=1,R3+1,0))</f>
         <v>1</v>
       </c>
       <c r="S4" s="8">
-        <f>IF(ISNA(I4),S3,IF(I4=1,S3+1,0))</f>
-        <v>0</v>
+        <f t="shared" ref="S4:S5" si="9">IF(ISNA(H4),S3,IF(H4=1,S3+1,0))</f>
+        <v>1</v>
       </c>
       <c r="T4" s="8">
-        <f t="shared" ref="T4:T5" si="10">IF(ISNA(J4),T3,IF(J4=1,T3+1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="U4" s="10">
-        <f t="shared" ref="U4:Z5" si="11">IF(ISNA(E4),U3,IF(E4=0,U3+1,0))</f>
+        <f>IF(ISNA(I4),T3,IF(I4=1,T3+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="U4" s="8">
+        <f t="shared" ref="U4:U5" si="10">IF(ISNA(J4),U3,IF(J4=1,U3+1,0))</f>
         <v>0</v>
       </c>
       <c r="V4" s="10">
-        <f t="shared" si="11"/>
-        <v>1</v>
+        <f>IF(ISNA(E4),V3,IF(E4=0,V3+1,0))</f>
+        <v>0</v>
       </c>
       <c r="W4" s="10">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f>IF(ISNA(F4),W3,IF(F4=0,W3+1,0))</f>
+        <v>1</v>
       </c>
       <c r="X4" s="10">
-        <f t="shared" si="11"/>
+        <f>IF(ISNA(G4),X3,IF(G4=0,X3+1,0))</f>
         <v>0</v>
       </c>
       <c r="Y4" s="10">
-        <f t="shared" si="11"/>
-        <v>1</v>
+        <f>IF(ISNA(H4),Y3,IF(H4=0,Y3+1,0))</f>
+        <v>0</v>
       </c>
       <c r="Z4" s="10">
-        <f t="shared" si="11"/>
+        <f>IF(ISNA(I4),Z3,IF(I4=0,Z3+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AA4" s="10">
+        <f>IF(ISNA(J4),AA3,IF(J4=0,AA3+1,0))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <f>Data!A4</f>
         <v>602</v>
@@ -7193,71 +7365,75 @@
         <v>#N/A</v>
       </c>
       <c r="K5" s="1">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="L5" s="1">
         <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="L5" s="1">
+        <v>3</v>
+      </c>
+      <c r="M5" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N5" s="1">
         <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-      <c r="M5" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N5" s="1" t="e">
-        <f t="shared" ref="N5:N6" si="12">IF(L5=1,INDEX($E$2:$J$2,1,MATCH(1,E5:J5,0)),NA())</f>
+        <v>0</v>
+      </c>
+      <c r="O5" s="1" t="e">
+        <f t="shared" ref="O5:O6" si="11">IF(L5=1,INDEX($E$2:$J$2,1,MATCH(1,E5:J5,0)),NA())</f>
         <v>#N/A</v>
       </c>
-      <c r="O5" s="8">
+      <c r="P5" s="8">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P5" s="8">
+      <c r="Q5" s="8">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="Q5" s="8">
+      <c r="R5" s="8">
         <f t="shared" si="8"/>
         <v>2</v>
       </c>
-      <c r="R5" s="8">
+      <c r="S5" s="8">
         <f t="shared" si="9"/>
         <v>2</v>
       </c>
-      <c r="S5" s="8">
-        <f t="shared" ref="S5" si="13">IF(ISNA(I5),S4,IF(I5=1,S4+1,0))</f>
-        <v>0</v>
-      </c>
       <c r="T5" s="8">
+        <f t="shared" ref="T5" si="12">IF(ISNA(I5),T4,IF(I5=1,T4+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="U5" s="8">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="U5" s="10">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
       <c r="V5" s="10">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f>IF(ISNA(E5),V4,IF(E5=0,V4+1,0))</f>
+        <v>1</v>
       </c>
       <c r="W5" s="10">
-        <f t="shared" si="11"/>
+        <f>IF(ISNA(F5),W4,IF(F5=0,W4+1,0))</f>
         <v>0</v>
       </c>
       <c r="X5" s="10">
-        <f t="shared" si="11"/>
+        <f>IF(ISNA(G5),X4,IF(G5=0,X4+1,0))</f>
         <v>0</v>
       </c>
       <c r="Y5" s="10">
-        <f t="shared" si="11"/>
-        <v>1</v>
+        <f>IF(ISNA(H5),Y4,IF(H5=0,Y4+1,0))</f>
+        <v>0</v>
       </c>
       <c r="Z5" s="10">
-        <f t="shared" si="11"/>
+        <f>IF(ISNA(I5),Z4,IF(I5=0,Z4+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AA5" s="10">
+        <f>IF(ISNA(J5),AA4,IF(J5=0,AA4+1,0))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <f>Data!A5</f>
         <v>603</v>
@@ -7299,71 +7475,75 @@
         <v>#N/A</v>
       </c>
       <c r="K6" s="1">
-        <f t="shared" ref="K6" si="14">COUNTIF(E6:J6,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="K6" si="13">COUNTIF(E6:J6,"&lt;&gt;#N/A")</f>
         <v>4</v>
       </c>
       <c r="L6" s="1">
-        <f t="shared" ref="L6" si="15">SUMIF(E6:J6,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="L6" si="14">SUMIF(E6:J6,"&lt;&gt;#N/A")</f>
         <v>3</v>
       </c>
       <c r="M6" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N6" s="1" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N6" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O6" s="1" t="e">
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
-      <c r="O6" s="8">
-        <f t="shared" ref="O6" si="16">IF(ISNA(E6),O5,IF(E6=1,O5+1,0))</f>
-        <v>0</v>
-      </c>
       <c r="P6" s="8">
-        <f t="shared" ref="P6" si="17">IF(ISNA(F6),P5,IF(F6=1,P5+1,0))</f>
+        <f t="shared" ref="P6" si="15">IF(ISNA(E6),P5,IF(E6=1,P5+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="8">
+        <f t="shared" ref="Q6" si="16">IF(ISNA(F6),Q5,IF(F6=1,Q5+1,0))</f>
         <v>2</v>
       </c>
-      <c r="Q6" s="8">
-        <f t="shared" ref="Q6" si="18">IF(ISNA(G6),Q5,IF(G6=1,Q5+1,0))</f>
+      <c r="R6" s="8">
+        <f t="shared" ref="R6" si="17">IF(ISNA(G6),R5,IF(G6=1,R5+1,0))</f>
         <v>3</v>
       </c>
-      <c r="R6" s="8">
-        <f t="shared" ref="R6" si="19">IF(ISNA(H6),R5,IF(H6=1,R5+1,0))</f>
+      <c r="S6" s="8">
+        <f t="shared" ref="S6" si="18">IF(ISNA(H6),S5,IF(H6=1,S5+1,0))</f>
         <v>3</v>
       </c>
-      <c r="S6" s="8">
-        <f t="shared" ref="S6" si="20">IF(ISNA(I6),S5,IF(I6=1,S5+1,0))</f>
-        <v>0</v>
-      </c>
       <c r="T6" s="8">
-        <f t="shared" ref="T6" si="21">IF(ISNA(J6),T5,IF(J6=1,T5+1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="U6" s="10">
-        <f t="shared" ref="U6:V8" si="22">IF(ISNA(E6),U5,IF(E6=0,U5+1,0))</f>
+        <f t="shared" ref="T6" si="19">IF(ISNA(I6),T5,IF(I6=1,T5+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="U6" s="8">
+        <f t="shared" ref="U6" si="20">IF(ISNA(J6),U5,IF(J6=1,U5+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="V6" s="10">
+        <f>IF(ISNA(E6),V5,IF(E6=0,V5+1,0))</f>
         <v>2</v>
       </c>
-      <c r="V6" s="10">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
       <c r="W6" s="10">
-        <f t="shared" ref="W6" si="23">IF(ISNA(G6),W5,IF(G6=0,W5+1,0))</f>
+        <f>IF(ISNA(F6),W5,IF(F6=0,W5+1,0))</f>
         <v>0</v>
       </c>
       <c r="X6" s="10">
-        <f t="shared" ref="X6" si="24">IF(ISNA(H6),X5,IF(H6=0,X5+1,0))</f>
+        <f t="shared" ref="X6" si="21">IF(ISNA(G6),X5,IF(G6=0,X5+1,0))</f>
         <v>0</v>
       </c>
       <c r="Y6" s="10">
-        <f t="shared" ref="Y6" si="25">IF(ISNA(I6),Y5,IF(I6=0,Y5+1,0))</f>
-        <v>1</v>
+        <f t="shared" ref="Y6" si="22">IF(ISNA(H6),Y5,IF(H6=0,Y5+1,0))</f>
+        <v>0</v>
       </c>
       <c r="Z6" s="10">
-        <f t="shared" ref="Z6" si="26">IF(ISNA(J6),Z5,IF(J6=0,Z5+1,0))</f>
+        <f t="shared" ref="Z6" si="23">IF(ISNA(I6),Z5,IF(I6=0,Z5+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AA6" s="10">
+        <f t="shared" ref="AA6" si="24">IF(ISNA(J6),AA5,IF(J6=0,AA5+1,0))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <f>Data!A6</f>
         <v>604</v>
@@ -7405,71 +7585,75 @@
         <v>#N/A</v>
       </c>
       <c r="K7" s="1">
-        <f t="shared" ref="K7" si="27">COUNTIF(E7:J7,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="K7" si="25">COUNTIF(E7:J7,"&lt;&gt;#N/A")</f>
         <v>4</v>
       </c>
       <c r="L7" s="1">
-        <f t="shared" ref="L7" si="28">SUMIF(E7:J7,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="L7" si="26">SUMIF(E7:J7,"&lt;&gt;#N/A")</f>
         <v>2</v>
       </c>
       <c r="M7" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N7" s="1" t="e">
-        <f t="shared" ref="N7" si="29">IF(L7=1,INDEX($E$2:$J$2,1,MATCH(1,E7:J7,0)),NA())</f>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N7" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O7" s="1" t="e">
+        <f t="shared" ref="O7" si="27">IF(L7=1,INDEX($E$2:$J$2,1,MATCH(1,E7:J7,0)),NA())</f>
         <v>#N/A</v>
       </c>
-      <c r="O7" s="8">
-        <f t="shared" ref="O7" si="30">IF(ISNA(E7),O6,IF(E7=1,O6+1,0))</f>
-        <v>0</v>
-      </c>
       <c r="P7" s="8">
-        <f t="shared" ref="P7" si="31">IF(ISNA(F7),P6,IF(F7=1,P6+1,0))</f>
+        <f t="shared" ref="P7" si="28">IF(ISNA(E7),P6,IF(E7=1,P6+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="8">
+        <f t="shared" ref="Q7" si="29">IF(ISNA(F7),Q6,IF(F7=1,Q6+1,0))</f>
         <v>3</v>
       </c>
-      <c r="Q7" s="8">
-        <f t="shared" ref="Q7" si="32">IF(ISNA(G7),Q6,IF(G7=1,Q6+1,0))</f>
+      <c r="R7" s="8">
+        <f t="shared" ref="R7" si="30">IF(ISNA(G7),R6,IF(G7=1,R6+1,0))</f>
         <v>4</v>
       </c>
-      <c r="R7" s="8">
-        <f t="shared" ref="R7" si="33">IF(ISNA(H7),R6,IF(H7=1,R6+1,0))</f>
-        <v>0</v>
-      </c>
       <c r="S7" s="8">
-        <f t="shared" ref="S7" si="34">IF(ISNA(I7),S6,IF(I7=1,S6+1,0))</f>
+        <f t="shared" ref="S7" si="31">IF(ISNA(H7),S6,IF(H7=1,S6+1,0))</f>
         <v>0</v>
       </c>
       <c r="T7" s="8">
-        <f t="shared" ref="T7" si="35">IF(ISNA(J7),T6,IF(J7=1,T6+1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="U7" s="10">
-        <f t="shared" si="22"/>
+        <f t="shared" ref="T7" si="32">IF(ISNA(I7),T6,IF(I7=1,T6+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="U7" s="8">
+        <f t="shared" ref="U7" si="33">IF(ISNA(J7),U6,IF(J7=1,U6+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="V7" s="10">
+        <f>IF(ISNA(E7),V6,IF(E7=0,V6+1,0))</f>
         <v>3</v>
       </c>
-      <c r="V7" s="10">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
       <c r="W7" s="10">
-        <f t="shared" ref="W7" si="36">IF(ISNA(G7),W6,IF(G7=0,W6+1,0))</f>
+        <f>IF(ISNA(F7),W6,IF(F7=0,W6+1,0))</f>
         <v>0</v>
       </c>
       <c r="X7" s="10">
-        <f t="shared" ref="X7" si="37">IF(ISNA(H7),X6,IF(H7=0,X6+1,0))</f>
-        <v>1</v>
+        <f t="shared" ref="X7" si="34">IF(ISNA(G7),X6,IF(G7=0,X6+1,0))</f>
+        <v>0</v>
       </c>
       <c r="Y7" s="10">
-        <f t="shared" ref="Y7" si="38">IF(ISNA(I7),Y6,IF(I7=0,Y6+1,0))</f>
+        <f t="shared" ref="Y7" si="35">IF(ISNA(H7),Y6,IF(H7=0,Y6+1,0))</f>
         <v>1</v>
       </c>
       <c r="Z7" s="10">
-        <f t="shared" ref="Z7" si="39">IF(ISNA(J7),Z6,IF(J7=0,Z6+1,0))</f>
+        <f t="shared" ref="Z7" si="36">IF(ISNA(I7),Z6,IF(I7=0,Z6+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AA7" s="10">
+        <f t="shared" ref="AA7" si="37">IF(ISNA(J7),AA6,IF(J7=0,AA6+1,0))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <f>Data!A7</f>
         <v>605</v>
@@ -7511,71 +7695,75 @@
         <v>#N/A</v>
       </c>
       <c r="K8" s="1">
-        <f t="shared" ref="K8" si="40">COUNTIF(E8:J8,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="K8" si="38">COUNTIF(E8:J8,"&lt;&gt;#N/A")</f>
         <v>4</v>
       </c>
       <c r="L8" s="1">
-        <f t="shared" ref="L8" si="41">SUMIF(E8:J8,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="L8" si="39">SUMIF(E8:J8,"&lt;&gt;#N/A")</f>
         <v>2</v>
       </c>
       <c r="M8" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N8" s="1" t="e">
-        <f t="shared" ref="N8" si="42">IF(L8=1,INDEX($E$2:$J$2,1,MATCH(1,E8:J8,0)),NA())</f>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N8" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O8" s="1" t="e">
+        <f t="shared" ref="O8" si="40">IF(L8=1,INDEX($E$2:$J$2,1,MATCH(1,E8:J8,0)),NA())</f>
         <v>#N/A</v>
       </c>
-      <c r="O8" s="8">
-        <f t="shared" ref="O8" si="43">IF(ISNA(E8),O7,IF(E8=1,O7+1,0))</f>
-        <v>1</v>
-      </c>
       <c r="P8" s="8">
-        <f t="shared" ref="P8" si="44">IF(ISNA(F8),P7,IF(F8=1,P7+1,0))</f>
-        <v>0</v>
+        <f t="shared" ref="P8" si="41">IF(ISNA(E8),P7,IF(E8=1,P7+1,0))</f>
+        <v>1</v>
       </c>
       <c r="Q8" s="8">
-        <f t="shared" ref="Q8" si="45">IF(ISNA(G8),Q7,IF(G8=1,Q7+1,0))</f>
+        <f t="shared" ref="Q8" si="42">IF(ISNA(F8),Q7,IF(F8=1,Q7+1,0))</f>
         <v>0</v>
       </c>
       <c r="R8" s="8">
-        <f t="shared" ref="R8" si="46">IF(ISNA(H8),R7,IF(H8=1,R7+1,0))</f>
-        <v>1</v>
+        <f t="shared" ref="R8" si="43">IF(ISNA(G8),R7,IF(G8=1,R7+1,0))</f>
+        <v>0</v>
       </c>
       <c r="S8" s="8">
-        <f t="shared" ref="S8" si="47">IF(ISNA(I8),S7,IF(I8=1,S7+1,0))</f>
-        <v>0</v>
+        <f t="shared" ref="S8" si="44">IF(ISNA(H8),S7,IF(H8=1,S7+1,0))</f>
+        <v>1</v>
       </c>
       <c r="T8" s="8">
-        <f t="shared" ref="T8" si="48">IF(ISNA(J8),T7,IF(J8=1,T7+1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="U8" s="10">
-        <f t="shared" si="22"/>
+        <f t="shared" ref="T8" si="45">IF(ISNA(I8),T7,IF(I8=1,T7+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="U8" s="8">
+        <f t="shared" ref="U8" si="46">IF(ISNA(J8),U7,IF(J8=1,U7+1,0))</f>
         <v>0</v>
       </c>
       <c r="V8" s="10">
-        <f t="shared" si="22"/>
-        <v>1</v>
+        <f>IF(ISNA(E8),V7,IF(E8=0,V7+1,0))</f>
+        <v>0</v>
       </c>
       <c r="W8" s="10">
-        <f t="shared" ref="W8" si="49">IF(ISNA(G8),W7,IF(G8=0,W7+1,0))</f>
+        <f>IF(ISNA(F8),W7,IF(F8=0,W7+1,0))</f>
         <v>1</v>
       </c>
       <c r="X8" s="10">
-        <f t="shared" ref="X8" si="50">IF(ISNA(H8),X7,IF(H8=0,X7+1,0))</f>
-        <v>0</v>
+        <f t="shared" ref="X8" si="47">IF(ISNA(G8),X7,IF(G8=0,X7+1,0))</f>
+        <v>1</v>
       </c>
       <c r="Y8" s="10">
-        <f t="shared" ref="Y8" si="51">IF(ISNA(I8),Y7,IF(I8=0,Y7+1,0))</f>
-        <v>1</v>
+        <f t="shared" ref="Y8" si="48">IF(ISNA(H8),Y7,IF(H8=0,Y7+1,0))</f>
+        <v>0</v>
       </c>
       <c r="Z8" s="10">
-        <f t="shared" ref="Z8" si="52">IF(ISNA(J8),Z7,IF(J8=0,Z7+1,0))</f>
+        <f t="shared" ref="Z8" si="49">IF(ISNA(I8),Z7,IF(I8=0,Z7+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AA8" s="10">
+        <f t="shared" ref="AA8" si="50">IF(ISNA(J8),AA7,IF(J8=0,AA7+1,0))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <f>Data!A8</f>
         <v>606</v>
@@ -7617,71 +7805,75 @@
         <v>#N/A</v>
       </c>
       <c r="K9" s="1">
-        <f t="shared" ref="K9" si="53">COUNTIF(E9:J9,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="K9" si="51">COUNTIF(E9:J9,"&lt;&gt;#N/A")</f>
         <v>4</v>
       </c>
       <c r="L9" s="1">
-        <f t="shared" ref="L9" si="54">SUMIF(E9:J9,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="L9" si="52">SUMIF(E9:J9,"&lt;&gt;#N/A")</f>
         <v>1</v>
       </c>
       <c r="M9" s="1">
-        <f t="shared" ref="M9" si="55">IF(SUMIF(E9:J9,"&lt;&gt;#N/A")=0, 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="N9" s="1" t="str">
-        <f t="shared" ref="N9" si="56">IF(L9=1,INDEX($E$2:$J$2,1,MATCH(1,E9:J9,0)),NA())</f>
+        <f t="shared" ref="M9" si="53">IF(SUMIF(E9:J9,"&lt;&gt;#N/A")=0, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="N9" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O9" s="1" t="str">
+        <f t="shared" ref="O9" si="54">IF(L9=1,INDEX($E$2:$J$2,1,MATCH(1,E9:J9,0)),NA())</f>
         <v>Evan</v>
       </c>
-      <c r="O9" s="8">
-        <f t="shared" ref="O9" si="57">IF(ISNA(E9),O8,IF(E9=1,O8+1,0))</f>
-        <v>0</v>
-      </c>
       <c r="P9" s="8">
-        <f t="shared" ref="P9" si="58">IF(ISNA(F9),P8,IF(F9=1,P8+1,0))</f>
+        <f t="shared" ref="P9" si="55">IF(ISNA(E9),P8,IF(E9=1,P8+1,0))</f>
         <v>0</v>
       </c>
       <c r="Q9" s="8">
-        <f t="shared" ref="Q9" si="59">IF(ISNA(G9),Q8,IF(G9=1,Q8+1,0))</f>
+        <f t="shared" ref="Q9" si="56">IF(ISNA(F9),Q8,IF(F9=1,Q8+1,0))</f>
         <v>0</v>
       </c>
       <c r="R9" s="8">
-        <f t="shared" ref="R9" si="60">IF(ISNA(H9),R8,IF(H9=1,R8+1,0))</f>
+        <f t="shared" ref="R9" si="57">IF(ISNA(G9),R8,IF(G9=1,R8+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="S9" s="8">
+        <f t="shared" ref="S9" si="58">IF(ISNA(H9),S8,IF(H9=1,S8+1,0))</f>
         <v>2</v>
       </c>
-      <c r="S9" s="8">
-        <f t="shared" ref="S9" si="61">IF(ISNA(I9),S8,IF(I9=1,S8+1,0))</f>
-        <v>0</v>
-      </c>
       <c r="T9" s="8">
-        <f t="shared" ref="T9" si="62">IF(ISNA(J9),T8,IF(J9=1,T8+1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="U9" s="10">
-        <f t="shared" ref="U9" si="63">IF(ISNA(E9),U8,IF(E9=0,U8+1,0))</f>
-        <v>1</v>
+        <f t="shared" ref="T9" si="59">IF(ISNA(I9),T8,IF(I9=1,T8+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="U9" s="8">
+        <f t="shared" ref="U9" si="60">IF(ISNA(J9),U8,IF(J9=1,U8+1,0))</f>
+        <v>0</v>
       </c>
       <c r="V9" s="10">
-        <f t="shared" ref="V9" si="64">IF(ISNA(F9),V8,IF(F9=0,V8+1,0))</f>
+        <f t="shared" ref="V9" si="61">IF(ISNA(E9),V8,IF(E9=0,V8+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="W9" s="10">
+        <f t="shared" ref="W9" si="62">IF(ISNA(F9),W8,IF(F9=0,W8+1,0))</f>
         <v>2</v>
       </c>
-      <c r="W9" s="10">
-        <f t="shared" ref="W9" si="65">IF(ISNA(G9),W8,IF(G9=0,W8+1,0))</f>
+      <c r="X9" s="10">
+        <f t="shared" ref="X9" si="63">IF(ISNA(G9),X8,IF(G9=0,X8+1,0))</f>
         <v>2</v>
       </c>
-      <c r="X9" s="10">
-        <f t="shared" ref="X9" si="66">IF(ISNA(H9),X8,IF(H9=0,X8+1,0))</f>
-        <v>0</v>
-      </c>
       <c r="Y9" s="10">
-        <f t="shared" ref="Y9" si="67">IF(ISNA(I9),Y8,IF(I9=0,Y8+1,0))</f>
-        <v>1</v>
+        <f t="shared" ref="Y9" si="64">IF(ISNA(H9),Y8,IF(H9=0,Y8+1,0))</f>
+        <v>0</v>
       </c>
       <c r="Z9" s="10">
-        <f t="shared" ref="Z9" si="68">IF(ISNA(J9),Z8,IF(J9=0,Z8+1,0))</f>
+        <f t="shared" ref="Z9" si="65">IF(ISNA(I9),Z8,IF(I9=0,Z8+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AA9" s="10">
+        <f t="shared" ref="AA9" si="66">IF(ISNA(J9),AA8,IF(J9=0,AA8+1,0))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <f>Data!A9</f>
         <v>607</v>
@@ -7723,74 +7915,408 @@
         <v>#N/A</v>
       </c>
       <c r="K10" s="1">
-        <f t="shared" ref="K10" si="69">COUNTIF(E10:J10,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="K10" si="67">COUNTIF(E10:J10,"&lt;&gt;#N/A")</f>
         <v>4</v>
       </c>
       <c r="L10" s="1">
-        <f t="shared" ref="L10" si="70">SUMIF(E10:J10,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="L10" si="68">SUMIF(E10:J10,"&lt;&gt;#N/A")</f>
         <v>3</v>
       </c>
       <c r="M10" s="1">
-        <f t="shared" ref="M10" si="71">IF(SUMIF(E10:J10,"&lt;&gt;#N/A")=0, 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="N10" s="1" t="e">
-        <f t="shared" ref="N10" si="72">IF(L10=1,INDEX($E$2:$J$2,1,MATCH(1,E10:J10,0)),NA())</f>
+        <f t="shared" ref="M10" si="69">IF(SUMIF(E10:J10,"&lt;&gt;#N/A")=0, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="N10" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O10" s="1" t="e">
+        <f t="shared" ref="O10" si="70">IF(L10=1,INDEX($E$2:$J$2,1,MATCH(1,E10:J10,0)),NA())</f>
         <v>#N/A</v>
       </c>
-      <c r="O10" s="8">
-        <f t="shared" ref="O10" si="73">IF(ISNA(E10),O9,IF(E10=1,O9+1,0))</f>
-        <v>1</v>
-      </c>
       <c r="P10" s="8">
-        <f t="shared" ref="P10" si="74">IF(ISNA(F10),P9,IF(F10=1,P9+1,0))</f>
+        <f t="shared" ref="P10" si="71">IF(ISNA(E10),P9,IF(E10=1,P9+1,0))</f>
         <v>1</v>
       </c>
       <c r="Q10" s="8">
-        <f t="shared" ref="Q10" si="75">IF(ISNA(G10),Q9,IF(G10=1,Q9+1,0))</f>
+        <f t="shared" ref="Q10" si="72">IF(ISNA(F10),Q9,IF(F10=1,Q9+1,0))</f>
         <v>1</v>
       </c>
       <c r="R10" s="8">
-        <f t="shared" ref="R10" si="76">IF(ISNA(H10),R9,IF(H10=1,R9+1,0))</f>
-        <v>0</v>
+        <f t="shared" ref="R10" si="73">IF(ISNA(G10),R9,IF(G10=1,R9+1,0))</f>
+        <v>1</v>
       </c>
       <c r="S10" s="8">
-        <f t="shared" ref="S10" si="77">IF(ISNA(I10),S9,IF(I10=1,S9+1,0))</f>
+        <f t="shared" ref="S10" si="74">IF(ISNA(H10),S9,IF(H10=1,S9+1,0))</f>
         <v>0</v>
       </c>
       <c r="T10" s="8">
-        <f t="shared" ref="T10" si="78">IF(ISNA(J10),T9,IF(J10=1,T9+1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="U10" s="10">
-        <f t="shared" ref="U10" si="79">IF(ISNA(E10),U9,IF(E10=0,U9+1,0))</f>
+        <f t="shared" ref="T10" si="75">IF(ISNA(I10),T9,IF(I10=1,T9+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="U10" s="8">
+        <f t="shared" ref="U10" si="76">IF(ISNA(J10),U9,IF(J10=1,U9+1,0))</f>
         <v>0</v>
       </c>
       <c r="V10" s="10">
-        <f t="shared" ref="V10" si="80">IF(ISNA(F10),V9,IF(F10=0,V9+1,0))</f>
+        <f t="shared" ref="V10" si="77">IF(ISNA(E10),V9,IF(E10=0,V9+1,0))</f>
         <v>0</v>
       </c>
       <c r="W10" s="10">
-        <f t="shared" ref="W10" si="81">IF(ISNA(G10),W9,IF(G10=0,W9+1,0))</f>
+        <f t="shared" ref="W10" si="78">IF(ISNA(F10),W9,IF(F10=0,W9+1,0))</f>
         <v>0</v>
       </c>
       <c r="X10" s="10">
-        <f t="shared" ref="X10" si="82">IF(ISNA(H10),X9,IF(H10=0,X9+1,0))</f>
-        <v>1</v>
+        <f t="shared" ref="X10" si="79">IF(ISNA(G10),X9,IF(G10=0,X9+1,0))</f>
+        <v>0</v>
       </c>
       <c r="Y10" s="10">
-        <f t="shared" ref="Y10" si="83">IF(ISNA(I10),Y9,IF(I10=0,Y9+1,0))</f>
+        <f t="shared" ref="Y10" si="80">IF(ISNA(H10),Y9,IF(H10=0,Y9+1,0))</f>
         <v>1</v>
       </c>
       <c r="Z10" s="10">
-        <f t="shared" ref="Z10" si="84">IF(ISNA(J10),Z9,IF(J10=0,Z9+1,0))</f>
+        <f t="shared" ref="Z10" si="81">IF(ISNA(I10),Z9,IF(I10=0,Z9+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AA10" s="10">
+        <f t="shared" ref="AA10" si="82">IF(ISNA(J10),AA9,IF(J10=0,AA9+1,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <f>Data!A10</f>
+        <v>608</v>
+      </c>
+      <c r="B11" s="4" t="e">
+        <f>Data!B10</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C11" s="5" t="str">
+        <f>Data!H10</f>
+        <v>Steve</v>
+      </c>
+      <c r="D11" s="2" t="str">
+        <f>Data!I10</f>
+        <v>Bob</v>
+      </c>
+      <c r="E11" s="1">
+        <f>IF(Data!J10=Data!$G10,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <f>IF(Data!K10=Data!$G10,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G11" s="1">
+        <f>IF(Data!L10=Data!$G10,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H11" s="1">
+        <f>IF(Data!M10=Data!$G10,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="I11" s="1" t="e">
+        <f>IF(Data!N10=Data!$G10,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J11" s="1" t="e">
+        <f>IF(Data!O10=Data!$G10,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K11" s="1">
+        <f t="shared" ref="K11" si="83">COUNTIF(E11:J11,"&lt;&gt;#N/A")</f>
+        <v>4</v>
+      </c>
+      <c r="L11" s="1">
+        <f t="shared" ref="L11" si="84">SUMIF(E11:J11,"&lt;&gt;#N/A")</f>
+        <v>3</v>
+      </c>
+      <c r="M11" s="1">
+        <f t="shared" ref="M11" si="85">IF(SUMIF(E11:J11,"&lt;&gt;#N/A")=0, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="N11" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O11" s="1" t="e">
+        <f t="shared" ref="O11" si="86">IF(L11=1,INDEX($E$2:$J$2,1,MATCH(1,E11:J11,0)),NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P11" s="8">
+        <f t="shared" ref="P11" si="87">IF(ISNA(E11),P10,IF(E11=1,P10+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="Q11" s="8">
+        <f t="shared" ref="Q11" si="88">IF(ISNA(F11),Q10,IF(F11=1,Q10+1,0))</f>
+        <v>2</v>
+      </c>
+      <c r="R11" s="8">
+        <f t="shared" ref="R11" si="89">IF(ISNA(G11),R10,IF(G11=1,R10+1,0))</f>
+        <v>2</v>
+      </c>
+      <c r="S11" s="8">
+        <f t="shared" ref="S11" si="90">IF(ISNA(H11),S10,IF(H11=1,S10+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="T11" s="8">
+        <f t="shared" ref="T11" si="91">IF(ISNA(I11),T10,IF(I11=1,T10+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="U11" s="8">
+        <f t="shared" ref="U11" si="92">IF(ISNA(J11),U10,IF(J11=1,U10+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="V11" s="10">
+        <f t="shared" ref="V11" si="93">IF(ISNA(E11),V10,IF(E11=0,V10+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="W11" s="10">
+        <f t="shared" ref="W11" si="94">IF(ISNA(F11),W10,IF(F11=0,W10+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="X11" s="10">
+        <f t="shared" ref="X11" si="95">IF(ISNA(G11),X10,IF(G11=0,X10+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="Y11" s="10">
+        <f t="shared" ref="Y11" si="96">IF(ISNA(H11),Y10,IF(H11=0,Y10+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="Z11" s="10">
+        <f t="shared" ref="Z11" si="97">IF(ISNA(I11),Z10,IF(I11=0,Z10+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AA11" s="10">
+        <f t="shared" ref="AA11" si="98">IF(ISNA(J11),AA10,IF(J11=0,AA10+1,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <f>Data!A11</f>
+        <v>609</v>
+      </c>
+      <c r="B12" s="4" t="e">
+        <f>Data!B11</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C12" s="5" t="str">
+        <f>Data!H11</f>
+        <v>Steve</v>
+      </c>
+      <c r="D12" s="2" t="str">
+        <f>Data!I11</f>
+        <v>Evan</v>
+      </c>
+      <c r="E12" s="1">
+        <f>IF(Data!J11=Data!$G11,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <f>IF(Data!K11=Data!$G11,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
+        <f>IF(Data!L11=Data!$G11,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H12" s="1">
+        <f>IF(Data!M11=Data!$G11,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="1" t="e">
+        <f>IF(Data!N11=Data!$G11,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J12" s="1" t="e">
+        <f>IF(Data!O11=Data!$G11,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K12" s="1">
+        <f t="shared" ref="K12" si="99">COUNTIF(E12:J12,"&lt;&gt;#N/A")</f>
+        <v>4</v>
+      </c>
+      <c r="L12" s="1">
+        <f t="shared" ref="L12" si="100">SUMIF(E12:J12,"&lt;&gt;#N/A")</f>
+        <v>3</v>
+      </c>
+      <c r="M12" s="1">
+        <f t="shared" ref="M12" si="101">IF(SUMIF(E12:J12,"&lt;&gt;#N/A")=0, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="N12" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O12" s="1" t="e">
+        <f t="shared" ref="O12" si="102">IF(L12=1,INDEX($E$2:$J$2,1,MATCH(1,E12:J12,0)),NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P12" s="8">
+        <f t="shared" ref="P12" si="103">IF(ISNA(E12),P11,IF(E12=1,P11+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="Q12" s="8">
+        <f t="shared" ref="Q12" si="104">IF(ISNA(F12),Q11,IF(F12=1,Q11+1,0))</f>
+        <v>3</v>
+      </c>
+      <c r="R12" s="8">
+        <f t="shared" ref="R12" si="105">IF(ISNA(G12),R11,IF(G12=1,R11+1,0))</f>
+        <v>3</v>
+      </c>
+      <c r="S12" s="8">
+        <f t="shared" ref="S12" si="106">IF(ISNA(H12),S11,IF(H12=1,S11+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="T12" s="8">
+        <f t="shared" ref="T12" si="107">IF(ISNA(I12),T11,IF(I12=1,T11+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="U12" s="8">
+        <f t="shared" ref="U12" si="108">IF(ISNA(J12),U11,IF(J12=1,U11+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="V12" s="10">
+        <f t="shared" ref="V12" si="109">IF(ISNA(E12),V11,IF(E12=0,V11+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="W12" s="10">
+        <f t="shared" ref="W12" si="110">IF(ISNA(F12),W11,IF(F12=0,W11+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="X12" s="10">
+        <f t="shared" ref="X12" si="111">IF(ISNA(G12),X11,IF(G12=0,X11+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="Y12" s="10">
+        <f t="shared" ref="Y12" si="112">IF(ISNA(H12),Y11,IF(H12=0,Y11+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="Z12" s="10">
+        <f t="shared" ref="Z12" si="113">IF(ISNA(I12),Z11,IF(I12=0,Z11+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AA12" s="10">
+        <f t="shared" ref="AA12" si="114">IF(ISNA(J12),AA11,IF(J12=0,AA11+1,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <f>Data!A12</f>
+        <v>610</v>
+      </c>
+      <c r="B13" s="4" t="e">
+        <f>Data!B12</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C13" s="5" t="str">
+        <f>Data!H12</f>
+        <v>Steve</v>
+      </c>
+      <c r="D13" s="2" t="str">
+        <f>Data!I12</f>
+        <v>Cara</v>
+      </c>
+      <c r="E13" s="1">
+        <f>IF(Data!J12=Data!$G12,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F13" s="1">
+        <f>IF(Data!K12=Data!$G12,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G13" s="1">
+        <f>IF(Data!L12=Data!$G12,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H13" s="1">
+        <f>IF(Data!M12=Data!$G12,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="I13" s="1" t="e">
+        <f>IF(Data!N12=Data!$G12,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J13" s="1" t="e">
+        <f>IF(Data!O12=Data!$G12,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K13" s="1">
+        <f t="shared" ref="K13" si="115">COUNTIF(E13:J13,"&lt;&gt;#N/A")</f>
+        <v>4</v>
+      </c>
+      <c r="L13" s="1">
+        <f t="shared" ref="L13" si="116">SUMIF(E13:J13,"&lt;&gt;#N/A")</f>
+        <v>4</v>
+      </c>
+      <c r="M13" s="1">
+        <f t="shared" ref="M13" si="117">IF(SUMIF(E13:J13,"&lt;&gt;#N/A")=0, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="N13" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O13" s="1" t="e">
+        <f t="shared" ref="O13" si="118">IF(L13=1,INDEX($E$2:$J$2,1,MATCH(1,E13:J13,0)),NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P13" s="8">
+        <f t="shared" ref="P13" si="119">IF(ISNA(E13),P12,IF(E13=1,P12+1,0))</f>
+        <v>2</v>
+      </c>
+      <c r="Q13" s="8">
+        <f t="shared" ref="Q13" si="120">IF(ISNA(F13),Q12,IF(F13=1,Q12+1,0))</f>
+        <v>4</v>
+      </c>
+      <c r="R13" s="8">
+        <f t="shared" ref="R13" si="121">IF(ISNA(G13),R12,IF(G13=1,R12+1,0))</f>
+        <v>4</v>
+      </c>
+      <c r="S13" s="8">
+        <f t="shared" ref="S13" si="122">IF(ISNA(H13),S12,IF(H13=1,S12+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="T13" s="8">
+        <f t="shared" ref="T13" si="123">IF(ISNA(I13),T12,IF(I13=1,T12+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="U13" s="8">
+        <f t="shared" ref="U13" si="124">IF(ISNA(J13),U12,IF(J13=1,U12+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="V13" s="10">
+        <f t="shared" ref="V13" si="125">IF(ISNA(E13),V12,IF(E13=0,V12+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="W13" s="10">
+        <f t="shared" ref="W13" si="126">IF(ISNA(F13),W12,IF(F13=0,W12+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="X13" s="10">
+        <f t="shared" ref="X13" si="127">IF(ISNA(G13),X12,IF(G13=0,X12+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="Y13" s="10">
+        <f t="shared" ref="Y13" si="128">IF(ISNA(H13),Y12,IF(H13=0,Y12+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="Z13" s="10">
+        <f t="shared" ref="Z13" si="129">IF(ISNA(I13),Z12,IF(I13=0,Z12+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AA13" s="10">
+        <f t="shared" ref="AA13" si="130">IF(ISNA(J13),AA12,IF(J13=0,AA12+1,0))</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="O1:T1"/>
-    <mergeCell ref="U1:Z1"/>
+    <mergeCell ref="P1:U1"/>
+    <mergeCell ref="V1:AA1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -7799,10 +8325,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7836,28 +8362,28 @@
         <v>Steve</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="6">
         <f>SUMIF(Results!E3:E53,"&lt;&gt;#N/A")/COUNTIFS(Results!E3:E53,"&lt;&gt;#N/A",Results!E3:E53,"&lt;&gt;")</f>
-        <v>0.375</v>
+        <v>0.45454545454545453</v>
       </c>
       <c r="C2" s="6">
         <f>SUMIF(Results!F3:F53,"&lt;&gt;#N/A")/COUNTIFS(Results!F3:F53,"&lt;&gt;#N/A",Results!F3:F53,"&lt;&gt;")</f>
-        <v>0.5714285714285714</v>
+        <v>0.7</v>
       </c>
       <c r="D2" s="6">
         <f>SUMIF(Results!G3:G53,"&lt;&gt;#N/A")/COUNTIFS(Results!G3:G53,"&lt;&gt;#N/A",Results!G3:G53,"&lt;&gt;")</f>
-        <v>0.625</v>
+        <v>0.72727272727272729</v>
       </c>
       <c r="E2" s="6">
         <f>SUMIF(Results!H3:H53,"&lt;&gt;#N/A")/COUNTIFS(Results!H3:H53,"&lt;&gt;#N/A",Results!H3:H53,"&lt;&gt;")</f>
-        <v>0.625</v>
+        <v>0.63636363636363635</v>
       </c>
       <c r="F2" s="6">
         <f>SUMIF(Results!I3:I53,"&lt;&gt;#N/A")/COUNTIFS(Results!I3:I53,"&lt;&gt;#N/A",Results!I3:I53,"&lt;&gt;")</f>
@@ -7869,12 +8395,12 @@
       </c>
       <c r="H2" s="6">
         <f>SUM(Results!L3:L53)/SUM(Results!K3:K53)</f>
-        <v>0.53125</v>
+        <v>0.61363636363636365</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="6">
         <f>SUMIFS(Results!E3:E53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!E3:E53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!E3:E53, "&lt;&gt;#N/A", Results!E3:E53, "&lt;&gt;")</f>
@@ -7907,19 +8433,19 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" s="6">
         <f>SUMIFS(Results!E3:E53,Results!$B$3:$B$53,"=#N/A",Results!E3:E53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!E3:E53, "&lt;&gt;#N/A", Results!E3:E53, "&lt;&gt;")</f>
-        <v>1</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="C4" s="6">
         <f>SUMIFS(Results!F3:F53,Results!$B$3:$B$53,"=#N/A",Results!F3:F53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!F3:F53, "&lt;&gt;#N/A", Results!F3:F53, "&lt;&gt;")</f>
-        <v>0.33333333333333331</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="D4" s="6">
         <f>SUMIFS(Results!G3:G53,Results!$B$3:$B$53,"=#N/A",Results!G3:G53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!G3:G53, "&lt;&gt;#N/A", Results!G3:G53, "&lt;&gt;")</f>
-        <v>0.66666666666666663</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="E4" s="6">
         <f>SUMIFS(Results!H3:H53,Results!$B$3:$B$53,"=#N/A",Results!H3:H53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!H3:H53, "&lt;&gt;#N/A", Results!H3:H53, "&lt;&gt;")</f>
@@ -7935,35 +8461,35 @@
       </c>
       <c r="H4" s="6">
         <f>SUMIF(Results!B3:B53,"=#N/A",Results!L3:L53)/SUMIF(Results!B3:B53,"=#N/A",Results!K3:K53)</f>
-        <v>0.66666666666666663</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" s="1">
-        <f>MAX(Results!O3:O53)</f>
-        <v>1</v>
+        <f>MAX(Results!P3:P53)</f>
+        <v>2</v>
       </c>
       <c r="C5" s="1">
-        <f>MAX(Results!P3:P53)</f>
-        <v>3</v>
-      </c>
-      <c r="D5" s="1">
         <f>MAX(Results!Q3:Q53)</f>
         <v>4</v>
       </c>
+      <c r="D5" s="1">
+        <f>MAX(Results!R3:R53)</f>
+        <v>4</v>
+      </c>
       <c r="E5" s="1">
-        <f>MAX(Results!R3:R53)</f>
+        <f>MAX(Results!S3:S53)</f>
         <v>3</v>
       </c>
       <c r="F5" s="1">
-        <f>MAX(Results!S3:S53)</f>
+        <f>MAX(Results!T3:T53)</f>
         <v>0</v>
       </c>
       <c r="G5" s="1">
-        <f>MAX(Results!T3:T53)</f>
+        <f>MAX(Results!U3:U53)</f>
         <v>0</v>
       </c>
       <c r="H5" s="1">
@@ -7973,30 +8499,30 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1">
-        <f>MAX(Results!U3:U53)</f>
+        <f>MAX(Results!V3:V53)</f>
         <v>3</v>
       </c>
       <c r="C6" s="1">
-        <f>MAX(Results!V3:V53)</f>
-        <v>2</v>
-      </c>
-      <c r="D6" s="1">
         <f>MAX(Results!W3:W53)</f>
         <v>2</v>
       </c>
+      <c r="D6" s="1">
+        <f>MAX(Results!X3:X53)</f>
+        <v>2</v>
+      </c>
       <c r="E6" s="1">
-        <f>MAX(Results!X3:X53)</f>
+        <f>MAX(Results!Y3:Y53)</f>
         <v>1</v>
       </c>
       <c r="F6" s="1">
-        <f>MAX(Results!Y3:Y53)</f>
+        <f>MAX(Results!Z3:Z53)</f>
         <v>1</v>
       </c>
       <c r="G6" s="1">
-        <f>MAX(Results!Z3:Z53)</f>
+        <f>MAX(Results!AA3:AA53)</f>
         <v>0</v>
       </c>
       <c r="H6" s="1">
@@ -8006,30 +8532,30 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7" s="1">
-        <f>COUNTIF(Results!$N$3:$N$53,Summary!B1)</f>
+        <f>COUNTIF(Results!$O$3:$O$53,Summary!B1)</f>
         <v>0</v>
       </c>
       <c r="C7" s="1">
-        <f>COUNTIF(Results!$N$3:$N$53,Summary!C1)</f>
+        <f>COUNTIF(Results!$O$3:$O$53,Summary!C1)</f>
         <v>0</v>
       </c>
       <c r="D7" s="1">
-        <f>COUNTIF(Results!$N$3:$N$53,Summary!D1)</f>
+        <f>COUNTIF(Results!$O$3:$O$53,Summary!D1)</f>
         <v>0</v>
       </c>
       <c r="E7" s="1">
-        <f>COUNTIF(Results!$N$3:$N$53,Summary!E1)</f>
+        <f>COUNTIF(Results!$O$3:$O$53,Summary!E1)</f>
         <v>1</v>
       </c>
       <c r="F7" s="1">
-        <f>COUNTIF(Results!$N$3:$N$53,Summary!F1)</f>
+        <f>COUNTIF(Results!$O$3:$O$53,Summary!F1)</f>
         <v>0</v>
       </c>
       <c r="G7" s="1">
-        <f>COUNTIF(Results!$N$3:$N$53,Summary!G1)</f>
+        <f>COUNTIF(Results!$O$3:$O$53,Summary!G1)</f>
         <v>0</v>
       </c>
       <c r="H7" s="1">
@@ -8039,15 +8565,15 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" s="7">
         <f>SUMIF(Results!$D$3:$D$53,B1,Results!$L$3:$L$53)/SUMIF(Results!$D$3:$D$53,B1,Results!$K$3:$K$53)</f>
-        <v>0.5</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="C8" s="7">
         <f>SUMIF(Results!$D$3:$D$53,C1,Results!$L$3:$L$53)/SUMIF(Results!$D$3:$D$53,C1,Results!$K$3:$K$53)</f>
-        <v>0.625</v>
+        <v>0.75</v>
       </c>
       <c r="D8" s="7">
         <f>SUMIF(Results!$D$3:$D$53,D1,Results!$L$3:$L$53)/SUMIF(Results!$D$3:$D$53,D1,Results!$K$3:$K$53)</f>
@@ -8072,23 +8598,23 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B9" s="1">
         <f>SUMIF(Results!E3:E53,"&lt;&gt;#N/A")</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C9" s="1">
         <f>SUMIF(Results!F3:F53,"&lt;&gt;#N/A")</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D9" s="1">
         <f>SUMIF(Results!G3:G53,"&lt;&gt;#N/A")</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E9" s="1">
         <f>SUMIF(Results!H3:H53,"&lt;&gt;#N/A")</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F9" s="1">
         <f>SUMIF(Results!I3:I53,"&lt;&gt;#N/A")</f>
@@ -8100,28 +8626,28 @@
       </c>
       <c r="H9" s="1">
         <f>SUM(B9:G9)</f>
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B10" s="1">
         <f>COUNTIFS(Results!E3:E53,"&lt;&gt;#N/A",Results!E3:E53,"&lt;&gt;")</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C10" s="1">
         <f>COUNTIFS(Results!F3:F53,"&lt;&gt;#N/A",Results!F3:F53,"&lt;&gt;")</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D10" s="1">
         <f>COUNTIFS(Results!G3:G53,"&lt;&gt;#N/A",Results!G3:G53,"&lt;&gt;")</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E10" s="1">
         <f>COUNTIFS(Results!H3:H53,"&lt;&gt;#N/A",Results!H3:H53,"&lt;&gt;")</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F10" s="1">
         <f>COUNTIFS(Results!I3:I53,"&lt;&gt;#N/A",Results!I3:I53,"&lt;&gt;")</f>
@@ -8133,12 +8659,12 @@
       </c>
       <c r="H10" s="1">
         <f t="shared" ref="H10:H14" si="0">SUM(B10:G10)</f>
-        <v>32</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B11" s="1">
         <f>SUMIFS(Results!E3:E53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!E3:E53, "&lt;&gt;#N/A")</f>
@@ -8171,7 +8697,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B12" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!E3:E53, "&lt;&gt;#N/A", Results!E3:E53, "&lt;&gt;")</f>
@@ -8204,23 +8730,23 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B13" s="1">
         <f>SUMIFS(Results!E3:E53,Results!$B$3:$B$53,"=#N/A",Results!E3:E53, "&lt;&gt;#N/A")</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C13" s="1">
         <f>SUMIFS(Results!F3:F53,Results!$B$3:$B$53,"=#N/A",Results!F3:F53, "&lt;&gt;#N/A")</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D13" s="1">
         <f>SUMIFS(Results!G3:G53,Results!$B$3:$B$53,"=#N/A",Results!G3:G53, "&lt;&gt;#N/A")</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E13" s="1">
         <f>SUMIFS(Results!H3:H53,Results!$B$3:$B$53,"=#N/A",Results!H3:H53, "&lt;&gt;#N/A")</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F13" s="1">
         <f>SUMIFS(Results!I3:I53,Results!$B$3:$B$53,"=#N/A",Results!I3:I53, "&lt;&gt;#N/A")</f>
@@ -8232,28 +8758,28 @@
       </c>
       <c r="H13" s="1">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B14" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!E3:E53, "&lt;&gt;#N/A", Results!E3:E53, "&lt;&gt;")</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C14" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!F3:F53, "&lt;&gt;#N/A", Results!F3:F53, "&lt;&gt;")</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D14" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!G3:G53, "&lt;&gt;#N/A", Results!G3:G53, "&lt;&gt;")</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E14" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!H3:H53, "&lt;&gt;#N/A", Results!H3:H53, "&lt;&gt;")</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F14" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!I3:I53, "&lt;&gt;#N/A", Results!I3:I53, "&lt;&gt;")</f>
@@ -8265,7 +8791,73 @@
       </c>
       <c r="H14" s="1">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="1">
+        <f>SUMIF(Results!$C$3:$C$53,Summary!B1,Results!$M$3:$M$53)</f>
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
+        <f>SUMIF(Results!$C$3:$C$53,Summary!C1,Results!$M$3:$M$53)</f>
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <f>SUMIF(Results!$C$3:$C$53,Summary!D1,Results!$M$3:$M$53)</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <f>SUMIF(Results!$C$3:$C$53,Summary!E1,Results!$M$3:$M$53)</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <f>SUMIF(Results!$C$3:$C$53,Summary!F1,Results!$M$3:$M$53)</f>
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
+        <f>SUMIF(Results!$C$3:$C$53,Summary!G1,Results!$M$3:$M$53)</f>
+        <v>1</v>
+      </c>
+      <c r="H15" s="1">
+        <f>SUM(B15:G15)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="1">
+        <f>SUMIF(Results!E3:E53,"&lt;&gt;#N/A",Results!$N$3:$N$53)</f>
+        <v>1</v>
+      </c>
+      <c r="C16" s="1">
+        <f>SUMIF(Results!F3:F53,"&lt;&gt;#N/A",Results!$N$3:$N$53)</f>
+        <v>1</v>
+      </c>
+      <c r="D16" s="1">
+        <f>SUMIF(Results!G3:G53,"&lt;&gt;#N/A",Results!$N$3:$N$53)</f>
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
+        <f>SUMIF(Results!H3:H53,"&lt;&gt;#N/A",Results!$N$3:$N$53)</f>
+        <v>1</v>
+      </c>
+      <c r="F16" s="1">
+        <f>SUMIF(Results!I3:I53,"&lt;&gt;#N/A",Results!$N$3:$N$53)</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <f>SUMIF(Results!J3:J53,"&lt;&gt;#N/A",Results!$N$3:$N$53)</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="1">
+        <f>SUM(Results!N3:N53)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -8279,7 +8871,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+      <selection activeCell="V22" sqref="V22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated through episode 613
</commit_message>
<xml_diff>
--- a/SGU_Science_or_Fiction.xlsx
+++ b/SGU_Science_or_Fiction.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6135"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6135" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="88">
   <si>
     <t>Episode</t>
   </si>
@@ -255,6 +255,42 @@
   </si>
   <si>
     <t>Panelist Sweeps</t>
+  </si>
+  <si>
+    <t>Jewie or Fiction</t>
+  </si>
+  <si>
+    <t>Joshie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bakers are required to remove a piece of the dough prior to baking, the piece, called a challah, is then burned and wasted. </t>
+  </si>
+  <si>
+    <t>A Passover Goy purchases all the bread products in the home of an orthodox Jew so that they do not own any bread in their house for Passover.</t>
+  </si>
+  <si>
+    <t>Women during their 'unclean' menstrual period must wash their clothes in a separate machine so as not to contaminate the clothes of others in the house.</t>
+  </si>
+  <si>
+    <t>Dinosaurs</t>
+  </si>
+  <si>
+    <t>Two dinosaurs, a velociraptor and a protoceratops, were preserved in a literal action pose, in the act of combat as they clawed and bit each other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Most dinosaurs did not chew their food, but hadrosaurs did, with their (approximately) 1000 teeth. </t>
+  </si>
+  <si>
+    <t>Sauropods, the largest dinosaurs, had an enlargement at the base of their spinal cords that acted as a relay center or second brain.</t>
+  </si>
+  <si>
+    <t>A new review of research concludes that adults need significantly less sleep as they age.</t>
+  </si>
+  <si>
+    <t>In a series of studies, Japanese researchers demonstrate that children as young as six months old are attracted to the heroic acts of others.</t>
+  </si>
+  <si>
+    <t>A new DNA analysis finds that indigenous people living in the Pacific Northwest display genetic continuity with local populations for at least 10,000 years.</t>
   </si>
 </sst>
 </file>
@@ -647,16 +683,16 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.45454545454545453</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.7</c:v>
+                  <c:v>0.69230769230769229</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.72727272727272729</c:v>
+                  <c:v>0.6428571428571429</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.63636363636363635</c:v>
+                  <c:v>0.6428571428571429</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -665,7 +701,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.61363636363636365</c:v>
+                  <c:v>0.59649122807017541</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -681,8 +717,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="165056888"/>
-        <c:axId val="392918112"/>
+        <c:axId val="327145408"/>
+        <c:axId val="327149888"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -764,16 +800,16 @@
                       <c:formatCode>0.0%</c:formatCode>
                       <c:ptCount val="7"/>
                       <c:pt idx="0">
-                        <c:v>0</c:v>
+                        <c:v>0.14285714285714285</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.75</c:v>
+                        <c:v>0.66666666666666663</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.6</c:v>
+                        <c:v>0.42857142857142855</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0.6</c:v>
+                        <c:v>0.5714285714285714</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>0</c:v>
@@ -782,7 +818,7 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>0.45</c:v>
+                        <c:v>0.41379310344827586</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -868,16 +904,16 @@
                       <c:formatCode>0.0%</c:formatCode>
                       <c:ptCount val="7"/>
                       <c:pt idx="0">
-                        <c:v>0.83333333333333337</c:v>
+                        <c:v>0.8571428571428571</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.66666666666666663</c:v>
+                        <c:v>0.7142857142857143</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.83333333333333337</c:v>
+                        <c:v>0.8571428571428571</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0.66666666666666663</c:v>
+                        <c:v>0.7142857142857143</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>0</c:v>
@@ -886,7 +922,7 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>0.75</c:v>
+                        <c:v>0.7857142857142857</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1030,25 +1066,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>11</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1064,11 +1100,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="392916936"/>
-        <c:axId val="392914584"/>
+        <c:axId val="327154752"/>
+        <c:axId val="327150272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="165056888"/>
+        <c:axId val="327145408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1111,7 +1147,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="392918112"/>
+        <c:crossAx val="327149888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1119,7 +1155,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="392918112"/>
+        <c:axId val="327149888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1170,12 +1206,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="165056888"/>
+        <c:crossAx val="327145408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="392914584"/>
+        <c:axId val="327150272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1212,12 +1248,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="392916936"/>
+        <c:crossAx val="327154752"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="392916936"/>
+        <c:axId val="327154752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1226,7 +1262,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="392914584"/>
+        <c:crossAx val="327150272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1605,16 +1641,16 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.14285714285714285</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.75</c:v>
+                  <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.6</c:v>
+                  <c:v>0.42857142857142855</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.6</c:v>
+                  <c:v>0.5714285714285714</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1623,7 +1659,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.45</c:v>
+                  <c:v>0.41379310344827586</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -1640,8 +1676,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="210393400"/>
-        <c:axId val="399057864"/>
+        <c:axId val="327772344"/>
+        <c:axId val="327776824"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -1817,16 +1853,16 @@
                       <c:formatCode>0.0%</c:formatCode>
                       <c:ptCount val="7"/>
                       <c:pt idx="0">
-                        <c:v>0.45454545454545453</c:v>
+                        <c:v>0.5</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.7</c:v>
+                        <c:v>0.69230769230769229</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.72727272727272729</c:v>
+                        <c:v>0.6428571428571429</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0.63636363636363635</c:v>
+                        <c:v>0.6428571428571429</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>0</c:v>
@@ -1835,7 +1871,7 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>0.61363636363636365</c:v>
+                        <c:v>0.59649122807017541</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1921,16 +1957,16 @@
                       <c:formatCode>0.0%</c:formatCode>
                       <c:ptCount val="7"/>
                       <c:pt idx="0">
-                        <c:v>0.83333333333333337</c:v>
+                        <c:v>0.8571428571428571</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.66666666666666663</c:v>
+                        <c:v>0.7142857142857143</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.83333333333333337</c:v>
+                        <c:v>0.8571428571428571</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0.66666666666666663</c:v>
+                        <c:v>0.7142857142857143</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>0</c:v>
@@ -1939,7 +1975,7 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>0.75</c:v>
+                        <c:v>0.7857142857142857</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2084,25 +2120,25 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="7"/>
                       <c:pt idx="0">
-                        <c:v>11</c:v>
+                        <c:v>14</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>10</c:v>
+                        <c:v>13</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>11</c:v>
+                        <c:v>14</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>11</c:v>
+                        <c:v>14</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>1</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>0</c:v>
+                        <c:v>1</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>44</c:v>
+                        <c:v>57</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2153,16 +2189,16 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="7"/>
                       <c:pt idx="0">
-                        <c:v>6</c:v>
+                        <c:v>7</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>6</c:v>
+                        <c:v>7</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>6</c:v>
+                        <c:v>7</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>6</c:v>
+                        <c:v>7</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>0</c:v>
@@ -2171,7 +2207,7 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>24</c:v>
+                        <c:v>28</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2273,25 +2309,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2307,11 +2343,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="399058648"/>
-        <c:axId val="399058256"/>
+        <c:axId val="327777592"/>
+        <c:axId val="327777208"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="210393400"/>
+        <c:axId val="327772344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2354,7 +2390,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="399057864"/>
+        <c:crossAx val="327776824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2362,7 +2398,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="399057864"/>
+        <c:axId val="327776824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2413,12 +2449,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210393400"/>
+        <c:crossAx val="327772344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="399058256"/>
+        <c:axId val="327777208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2455,12 +2491,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="399058648"/>
+        <c:crossAx val="327777592"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="399058648"/>
+        <c:axId val="327777592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2469,7 +2505,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="399058256"/>
+        <c:crossAx val="327777208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2848,16 +2884,16 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.83333333333333337</c:v>
+                  <c:v>0.8571428571428571</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.66666666666666663</c:v>
+                  <c:v>0.7142857142857143</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.83333333333333337</c:v>
+                  <c:v>0.8571428571428571</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.66666666666666663</c:v>
+                  <c:v>0.7142857142857143</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2866,7 +2902,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.75</c:v>
+                  <c:v>0.7857142857142857</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -2883,8 +2919,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="399059824"/>
-        <c:axId val="399060216"/>
+        <c:axId val="328044312"/>
+        <c:axId val="106416152"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -3060,16 +3096,16 @@
                       <c:formatCode>0.0%</c:formatCode>
                       <c:ptCount val="7"/>
                       <c:pt idx="0">
-                        <c:v>0.45454545454545453</c:v>
+                        <c:v>0.5</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.7</c:v>
+                        <c:v>0.69230769230769229</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.72727272727272729</c:v>
+                        <c:v>0.6428571428571429</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0.63636363636363635</c:v>
+                        <c:v>0.6428571428571429</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>0</c:v>
@@ -3078,7 +3114,7 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>0.61363636363636365</c:v>
+                        <c:v>0.59649122807017541</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3258,16 +3294,16 @@
                       <c:formatCode>0.0%</c:formatCode>
                       <c:ptCount val="7"/>
                       <c:pt idx="0">
-                        <c:v>0</c:v>
+                        <c:v>0.14285714285714285</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.75</c:v>
+                        <c:v>0.66666666666666663</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.6</c:v>
+                        <c:v>0.42857142857142855</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0.6</c:v>
+                        <c:v>0.5714285714285714</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>0</c:v>
@@ -3276,7 +3312,7 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>0.45</c:v>
+                        <c:v>0.41379310344827586</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3421,25 +3457,25 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="7"/>
                       <c:pt idx="0">
-                        <c:v>11</c:v>
+                        <c:v>14</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>10</c:v>
+                        <c:v>13</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>11</c:v>
+                        <c:v>14</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>11</c:v>
+                        <c:v>14</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>1</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>0</c:v>
+                        <c:v>1</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>44</c:v>
+                        <c:v>57</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3546,25 +3582,25 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="7"/>
                       <c:pt idx="0">
-                        <c:v>5</c:v>
+                        <c:v>7</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>4</c:v>
+                        <c:v>6</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>5</c:v>
+                        <c:v>7</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>5</c:v>
+                        <c:v>7</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>1</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>0</c:v>
+                        <c:v>1</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>20</c:v>
+                        <c:v>29</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3667,16 +3703,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -3685,7 +3721,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>24</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -3702,11 +3738,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="399061000"/>
-        <c:axId val="399060608"/>
+        <c:axId val="106416936"/>
+        <c:axId val="106416544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="399059824"/>
+        <c:axId val="328044312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3749,7 +3785,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="399060216"/>
+        <c:crossAx val="106416152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3757,7 +3793,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="399060216"/>
+        <c:axId val="106416152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3808,12 +3844,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="399059824"/>
+        <c:crossAx val="328044312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="399060608"/>
+        <c:axId val="106416544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3852,12 +3888,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="399061000"/>
+        <c:crossAx val="106416936"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="399061000"/>
+        <c:axId val="106416936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3866,7 +3902,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="399060608"/>
+        <c:crossAx val="106416544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5988,8 +6024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6601,31 +6637,154 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
+      <c r="A13">
+        <v>611</v>
+      </c>
+      <c r="B13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" t="s">
+        <v>80</v>
+      </c>
+      <c r="F13" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G13" s="1">
+        <v>3</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J13" s="1">
+        <v>3</v>
+      </c>
+      <c r="K13" s="1">
+        <v>1</v>
+      </c>
+      <c r="L13" s="1">
+        <v>1</v>
+      </c>
+      <c r="M13" s="1">
+        <v>1</v>
+      </c>
+      <c r="N13" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O13" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
+      <c r="A14">
+        <v>612</v>
+      </c>
+      <c r="B14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" t="s">
+        <v>83</v>
+      </c>
+      <c r="E14" t="s">
+        <v>84</v>
+      </c>
+      <c r="F14" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G14" s="1">
+        <v>3</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J14" s="1">
+        <v>2</v>
+      </c>
+      <c r="K14" s="1">
+        <v>3</v>
+      </c>
+      <c r="L14" s="1">
+        <v>1</v>
+      </c>
+      <c r="M14" s="1">
+        <v>3</v>
+      </c>
+      <c r="N14" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O14" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
+      <c r="A15">
+        <v>613</v>
+      </c>
+      <c r="B15" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F15" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G15" s="1">
+        <v>1</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J15" s="1">
+        <v>1</v>
+      </c>
+      <c r="K15" s="1">
+        <v>1</v>
+      </c>
+      <c r="L15" s="1">
+        <v>1</v>
+      </c>
+      <c r="M15" s="1">
+        <v>1</v>
+      </c>
+      <c r="N15" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O15" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G16" s="1"/>
@@ -6977,10 +7136,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA13"/>
+  <dimension ref="A1:AA16"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:AA13"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:AA16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7067,27 +7226,27 @@
         <v>52</v>
       </c>
       <c r="P2" s="9" t="str">
-        <f>E2</f>
+        <f t="shared" ref="P2:U2" si="0">E2</f>
         <v>Bob</v>
       </c>
       <c r="Q2" s="9" t="str">
-        <f>F2</f>
+        <f t="shared" si="0"/>
         <v>Cara</v>
       </c>
       <c r="R2" s="9" t="str">
-        <f>G2</f>
+        <f t="shared" si="0"/>
         <v>Jay</v>
       </c>
       <c r="S2" s="9" t="str">
-        <f>H2</f>
+        <f t="shared" si="0"/>
         <v>Evan</v>
       </c>
       <c r="T2" s="9" t="str">
-        <f>I2</f>
+        <f t="shared" si="0"/>
         <v>George</v>
       </c>
       <c r="U2" s="9" t="str">
-        <f>J2</f>
+        <f t="shared" si="0"/>
         <v>Steve</v>
       </c>
       <c r="V2" s="11" t="str">
@@ -7099,19 +7258,19 @@
         <v>Cara</v>
       </c>
       <c r="X2" s="11" t="str">
-        <f t="shared" ref="X2:AA2" si="0">R2</f>
+        <f t="shared" ref="X2:AA2" si="1">R2</f>
         <v>Jay</v>
       </c>
       <c r="Y2" s="11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Evan</v>
       </c>
       <c r="Z2" s="11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>George</v>
       </c>
       <c r="AA2" s="11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Steve</v>
       </c>
     </row>
@@ -7165,7 +7324,7 @@
         <v>0</v>
       </c>
       <c r="M3" s="1">
-        <f t="shared" ref="M3:M8" si="1">IF(SUMIF(E3:J3,"&lt;&gt;#N/A")=0, 1, 0)</f>
+        <f t="shared" ref="M3:M8" si="2">IF(SUMIF(E3:J3,"&lt;&gt;#N/A")=0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="N3" s="1">
@@ -7173,7 +7332,7 @@
         <v>0</v>
       </c>
       <c r="O3" s="1" t="e">
-        <f t="shared" ref="O3" si="2">IF(L3=1,INDEX($E$2:$J$2,1,MATCH(1,E3:J3,0)),NA())</f>
+        <f t="shared" ref="O3" si="3">IF(L3=1,INDEX($E$2:$J$2,1,MATCH(1,E3:J3,0)),NA())</f>
         <v>#N/A</v>
       </c>
       <c r="P3" s="8">
@@ -7255,19 +7414,19 @@
         <v>#N/A</v>
       </c>
       <c r="K4" s="1">
-        <f t="shared" ref="K4:K5" si="3">COUNTIF(E4:J4,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="K4:K5" si="4">COUNTIF(E4:J4,"&lt;&gt;#N/A")</f>
         <v>4</v>
       </c>
       <c r="L4" s="1">
-        <f t="shared" ref="L4:L5" si="4">SUMIF(E4:J4,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="L4:L5" si="5">SUMIF(E4:J4,"&lt;&gt;#N/A")</f>
         <v>3</v>
       </c>
       <c r="M4" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N4" s="1">
-        <f t="shared" ref="N4:N13" si="5">IF(K4=L4,1,0)</f>
+        <f t="shared" ref="N4:N13" si="6">IF(K4=L4,1,0)</f>
         <v>0</v>
       </c>
       <c r="O4" s="1" t="e">
@@ -7275,19 +7434,19 @@
         <v>#N/A</v>
       </c>
       <c r="P4" s="8">
-        <f t="shared" ref="P4:P5" si="6">IF(ISNA(E4),P3,IF(E4=1,P3+1,0))</f>
+        <f t="shared" ref="P4:P5" si="7">IF(ISNA(E4),P3,IF(E4=1,P3+1,0))</f>
         <v>1</v>
       </c>
       <c r="Q4" s="8">
-        <f t="shared" ref="Q4:Q5" si="7">IF(ISNA(F4),Q3,IF(F4=1,Q3+1,0))</f>
+        <f t="shared" ref="Q4:Q5" si="8">IF(ISNA(F4),Q3,IF(F4=1,Q3+1,0))</f>
         <v>0</v>
       </c>
       <c r="R4" s="8">
-        <f t="shared" ref="R4:R5" si="8">IF(ISNA(G4),R3,IF(G4=1,R3+1,0))</f>
+        <f t="shared" ref="R4:R5" si="9">IF(ISNA(G4),R3,IF(G4=1,R3+1,0))</f>
         <v>1</v>
       </c>
       <c r="S4" s="8">
-        <f t="shared" ref="S4:S5" si="9">IF(ISNA(H4),S3,IF(H4=1,S3+1,0))</f>
+        <f t="shared" ref="S4:S5" si="10">IF(ISNA(H4),S3,IF(H4=1,S3+1,0))</f>
         <v>1</v>
       </c>
       <c r="T4" s="8">
@@ -7295,31 +7454,31 @@
         <v>0</v>
       </c>
       <c r="U4" s="8">
-        <f t="shared" ref="U4:U5" si="10">IF(ISNA(J4),U3,IF(J4=1,U3+1,0))</f>
+        <f t="shared" ref="U4:U5" si="11">IF(ISNA(J4),U3,IF(J4=1,U3+1,0))</f>
         <v>0</v>
       </c>
       <c r="V4" s="10">
-        <f>IF(ISNA(E4),V3,IF(E4=0,V3+1,0))</f>
+        <f t="shared" ref="V4:AA5" si="12">IF(ISNA(E4),V3,IF(E4=0,V3+1,0))</f>
         <v>0</v>
       </c>
       <c r="W4" s="10">
-        <f>IF(ISNA(F4),W3,IF(F4=0,W3+1,0))</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="X4" s="10">
-        <f>IF(ISNA(G4),X3,IF(G4=0,X3+1,0))</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Y4" s="10">
-        <f>IF(ISNA(H4),Y3,IF(H4=0,Y3+1,0))</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Z4" s="10">
-        <f>IF(ISNA(I4),Z3,IF(I4=0,Z3+1,0))</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="AA4" s="10">
-        <f>IF(ISNA(J4),AA3,IF(J4=0,AA3+1,0))</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -7365,71 +7524,71 @@
         <v>#N/A</v>
       </c>
       <c r="K5" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="L5" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="M5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N5" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O5" s="1" t="e">
-        <f t="shared" ref="O5:O6" si="11">IF(L5=1,INDEX($E$2:$J$2,1,MATCH(1,E5:J5,0)),NA())</f>
+        <f t="shared" ref="O5:O6" si="13">IF(L5=1,INDEX($E$2:$J$2,1,MATCH(1,E5:J5,0)),NA())</f>
         <v>#N/A</v>
       </c>
       <c r="P5" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q5" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="R5" s="8">
-        <f t="shared" si="8"/>
-        <v>2</v>
-      </c>
-      <c r="S5" s="8">
         <f t="shared" si="9"/>
         <v>2</v>
       </c>
+      <c r="S5" s="8">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
       <c r="T5" s="8">
-        <f t="shared" ref="T5" si="12">IF(ISNA(I5),T4,IF(I5=1,T4+1,0))</f>
+        <f t="shared" ref="T5" si="14">IF(ISNA(I5),T4,IF(I5=1,T4+1,0))</f>
         <v>0</v>
       </c>
       <c r="U5" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="V5" s="10">
-        <f>IF(ISNA(E5),V4,IF(E5=0,V4+1,0))</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="W5" s="10">
-        <f>IF(ISNA(F5),W4,IF(F5=0,W4+1,0))</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="X5" s="10">
-        <f>IF(ISNA(G5),X4,IF(G5=0,X4+1,0))</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Y5" s="10">
-        <f>IF(ISNA(H5),Y4,IF(H5=0,Y4+1,0))</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Z5" s="10">
-        <f>IF(ISNA(I5),Z4,IF(I5=0,Z4+1,0))</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="AA5" s="10">
-        <f>IF(ISNA(J5),AA4,IF(J5=0,AA4+1,0))</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -7475,71 +7634,71 @@
         <v>#N/A</v>
       </c>
       <c r="K6" s="1">
-        <f t="shared" ref="K6" si="13">COUNTIF(E6:J6,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="K6" si="15">COUNTIF(E6:J6,"&lt;&gt;#N/A")</f>
         <v>4</v>
       </c>
       <c r="L6" s="1">
-        <f t="shared" ref="L6" si="14">SUMIF(E6:J6,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="L6" si="16">SUMIF(E6:J6,"&lt;&gt;#N/A")</f>
         <v>3</v>
       </c>
       <c r="M6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N6" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O6" s="1" t="e">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>#N/A</v>
       </c>
       <c r="P6" s="8">
-        <f t="shared" ref="P6" si="15">IF(ISNA(E6),P5,IF(E6=1,P5+1,0))</f>
+        <f t="shared" ref="P6" si="17">IF(ISNA(E6),P5,IF(E6=1,P5+1,0))</f>
         <v>0</v>
       </c>
       <c r="Q6" s="8">
-        <f t="shared" ref="Q6" si="16">IF(ISNA(F6),Q5,IF(F6=1,Q5+1,0))</f>
+        <f t="shared" ref="Q6" si="18">IF(ISNA(F6),Q5,IF(F6=1,Q5+1,0))</f>
         <v>2</v>
       </c>
       <c r="R6" s="8">
-        <f t="shared" ref="R6" si="17">IF(ISNA(G6),R5,IF(G6=1,R5+1,0))</f>
+        <f t="shared" ref="R6" si="19">IF(ISNA(G6),R5,IF(G6=1,R5+1,0))</f>
         <v>3</v>
       </c>
       <c r="S6" s="8">
-        <f t="shared" ref="S6" si="18">IF(ISNA(H6),S5,IF(H6=1,S5+1,0))</f>
+        <f t="shared" ref="S6" si="20">IF(ISNA(H6),S5,IF(H6=1,S5+1,0))</f>
         <v>3</v>
       </c>
       <c r="T6" s="8">
-        <f t="shared" ref="T6" si="19">IF(ISNA(I6),T5,IF(I6=1,T5+1,0))</f>
+        <f t="shared" ref="T6" si="21">IF(ISNA(I6),T5,IF(I6=1,T5+1,0))</f>
         <v>0</v>
       </c>
       <c r="U6" s="8">
-        <f t="shared" ref="U6" si="20">IF(ISNA(J6),U5,IF(J6=1,U5+1,0))</f>
+        <f t="shared" ref="U6" si="22">IF(ISNA(J6),U5,IF(J6=1,U5+1,0))</f>
         <v>0</v>
       </c>
       <c r="V6" s="10">
-        <f>IF(ISNA(E6),V5,IF(E6=0,V5+1,0))</f>
+        <f t="shared" ref="V6:W8" si="23">IF(ISNA(E6),V5,IF(E6=0,V5+1,0))</f>
         <v>2</v>
       </c>
       <c r="W6" s="10">
-        <f>IF(ISNA(F6),W5,IF(F6=0,W5+1,0))</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="X6" s="10">
-        <f t="shared" ref="X6" si="21">IF(ISNA(G6),X5,IF(G6=0,X5+1,0))</f>
+        <f t="shared" ref="X6" si="24">IF(ISNA(G6),X5,IF(G6=0,X5+1,0))</f>
         <v>0</v>
       </c>
       <c r="Y6" s="10">
-        <f t="shared" ref="Y6" si="22">IF(ISNA(H6),Y5,IF(H6=0,Y5+1,0))</f>
+        <f t="shared" ref="Y6" si="25">IF(ISNA(H6),Y5,IF(H6=0,Y5+1,0))</f>
         <v>0</v>
       </c>
       <c r="Z6" s="10">
-        <f t="shared" ref="Z6" si="23">IF(ISNA(I6),Z5,IF(I6=0,Z5+1,0))</f>
+        <f t="shared" ref="Z6" si="26">IF(ISNA(I6),Z5,IF(I6=0,Z5+1,0))</f>
         <v>1</v>
       </c>
       <c r="AA6" s="10">
-        <f t="shared" ref="AA6" si="24">IF(ISNA(J6),AA5,IF(J6=0,AA5+1,0))</f>
+        <f t="shared" ref="AA6" si="27">IF(ISNA(J6),AA5,IF(J6=0,AA5+1,0))</f>
         <v>0</v>
       </c>
     </row>
@@ -7585,71 +7744,71 @@
         <v>#N/A</v>
       </c>
       <c r="K7" s="1">
-        <f t="shared" ref="K7" si="25">COUNTIF(E7:J7,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="K7" si="28">COUNTIF(E7:J7,"&lt;&gt;#N/A")</f>
         <v>4</v>
       </c>
       <c r="L7" s="1">
-        <f t="shared" ref="L7" si="26">SUMIF(E7:J7,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="L7" si="29">SUMIF(E7:J7,"&lt;&gt;#N/A")</f>
         <v>2</v>
       </c>
       <c r="M7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N7" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O7" s="1" t="e">
-        <f t="shared" ref="O7" si="27">IF(L7=1,INDEX($E$2:$J$2,1,MATCH(1,E7:J7,0)),NA())</f>
+        <f t="shared" ref="O7" si="30">IF(L7=1,INDEX($E$2:$J$2,1,MATCH(1,E7:J7,0)),NA())</f>
         <v>#N/A</v>
       </c>
       <c r="P7" s="8">
-        <f t="shared" ref="P7" si="28">IF(ISNA(E7),P6,IF(E7=1,P6+1,0))</f>
+        <f t="shared" ref="P7" si="31">IF(ISNA(E7),P6,IF(E7=1,P6+1,0))</f>
         <v>0</v>
       </c>
       <c r="Q7" s="8">
-        <f t="shared" ref="Q7" si="29">IF(ISNA(F7),Q6,IF(F7=1,Q6+1,0))</f>
+        <f t="shared" ref="Q7" si="32">IF(ISNA(F7),Q6,IF(F7=1,Q6+1,0))</f>
         <v>3</v>
       </c>
       <c r="R7" s="8">
-        <f t="shared" ref="R7" si="30">IF(ISNA(G7),R6,IF(G7=1,R6+1,0))</f>
+        <f t="shared" ref="R7" si="33">IF(ISNA(G7),R6,IF(G7=1,R6+1,0))</f>
         <v>4</v>
       </c>
       <c r="S7" s="8">
-        <f t="shared" ref="S7" si="31">IF(ISNA(H7),S6,IF(H7=1,S6+1,0))</f>
+        <f t="shared" ref="S7" si="34">IF(ISNA(H7),S6,IF(H7=1,S6+1,0))</f>
         <v>0</v>
       </c>
       <c r="T7" s="8">
-        <f t="shared" ref="T7" si="32">IF(ISNA(I7),T6,IF(I7=1,T6+1,0))</f>
+        <f t="shared" ref="T7" si="35">IF(ISNA(I7),T6,IF(I7=1,T6+1,0))</f>
         <v>0</v>
       </c>
       <c r="U7" s="8">
-        <f t="shared" ref="U7" si="33">IF(ISNA(J7),U6,IF(J7=1,U6+1,0))</f>
+        <f t="shared" ref="U7" si="36">IF(ISNA(J7),U6,IF(J7=1,U6+1,0))</f>
         <v>0</v>
       </c>
       <c r="V7" s="10">
-        <f>IF(ISNA(E7),V6,IF(E7=0,V6+1,0))</f>
+        <f t="shared" si="23"/>
         <v>3</v>
       </c>
       <c r="W7" s="10">
-        <f>IF(ISNA(F7),W6,IF(F7=0,W6+1,0))</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="X7" s="10">
-        <f t="shared" ref="X7" si="34">IF(ISNA(G7),X6,IF(G7=0,X6+1,0))</f>
+        <f t="shared" ref="X7" si="37">IF(ISNA(G7),X6,IF(G7=0,X6+1,0))</f>
         <v>0</v>
       </c>
       <c r="Y7" s="10">
-        <f t="shared" ref="Y7" si="35">IF(ISNA(H7),Y6,IF(H7=0,Y6+1,0))</f>
+        <f t="shared" ref="Y7" si="38">IF(ISNA(H7),Y6,IF(H7=0,Y6+1,0))</f>
         <v>1</v>
       </c>
       <c r="Z7" s="10">
-        <f t="shared" ref="Z7" si="36">IF(ISNA(I7),Z6,IF(I7=0,Z6+1,0))</f>
+        <f t="shared" ref="Z7" si="39">IF(ISNA(I7),Z6,IF(I7=0,Z6+1,0))</f>
         <v>1</v>
       </c>
       <c r="AA7" s="10">
-        <f t="shared" ref="AA7" si="37">IF(ISNA(J7),AA6,IF(J7=0,AA6+1,0))</f>
+        <f t="shared" ref="AA7" si="40">IF(ISNA(J7),AA6,IF(J7=0,AA6+1,0))</f>
         <v>0</v>
       </c>
     </row>
@@ -7695,71 +7854,71 @@
         <v>#N/A</v>
       </c>
       <c r="K8" s="1">
-        <f t="shared" ref="K8" si="38">COUNTIF(E8:J8,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="K8" si="41">COUNTIF(E8:J8,"&lt;&gt;#N/A")</f>
         <v>4</v>
       </c>
       <c r="L8" s="1">
-        <f t="shared" ref="L8" si="39">SUMIF(E8:J8,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="L8" si="42">SUMIF(E8:J8,"&lt;&gt;#N/A")</f>
         <v>2</v>
       </c>
       <c r="M8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N8" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O8" s="1" t="e">
-        <f t="shared" ref="O8" si="40">IF(L8=1,INDEX($E$2:$J$2,1,MATCH(1,E8:J8,0)),NA())</f>
+        <f t="shared" ref="O8" si="43">IF(L8=1,INDEX($E$2:$J$2,1,MATCH(1,E8:J8,0)),NA())</f>
         <v>#N/A</v>
       </c>
       <c r="P8" s="8">
-        <f t="shared" ref="P8" si="41">IF(ISNA(E8),P7,IF(E8=1,P7+1,0))</f>
+        <f t="shared" ref="P8" si="44">IF(ISNA(E8),P7,IF(E8=1,P7+1,0))</f>
         <v>1</v>
       </c>
       <c r="Q8" s="8">
-        <f t="shared" ref="Q8" si="42">IF(ISNA(F8),Q7,IF(F8=1,Q7+1,0))</f>
+        <f t="shared" ref="Q8" si="45">IF(ISNA(F8),Q7,IF(F8=1,Q7+1,0))</f>
         <v>0</v>
       </c>
       <c r="R8" s="8">
-        <f t="shared" ref="R8" si="43">IF(ISNA(G8),R7,IF(G8=1,R7+1,0))</f>
+        <f t="shared" ref="R8" si="46">IF(ISNA(G8),R7,IF(G8=1,R7+1,0))</f>
         <v>0</v>
       </c>
       <c r="S8" s="8">
-        <f t="shared" ref="S8" si="44">IF(ISNA(H8),S7,IF(H8=1,S7+1,0))</f>
+        <f t="shared" ref="S8" si="47">IF(ISNA(H8),S7,IF(H8=1,S7+1,0))</f>
         <v>1</v>
       </c>
       <c r="T8" s="8">
-        <f t="shared" ref="T8" si="45">IF(ISNA(I8),T7,IF(I8=1,T7+1,0))</f>
+        <f t="shared" ref="T8" si="48">IF(ISNA(I8),T7,IF(I8=1,T7+1,0))</f>
         <v>0</v>
       </c>
       <c r="U8" s="8">
-        <f t="shared" ref="U8" si="46">IF(ISNA(J8),U7,IF(J8=1,U7+1,0))</f>
+        <f t="shared" ref="U8" si="49">IF(ISNA(J8),U7,IF(J8=1,U7+1,0))</f>
         <v>0</v>
       </c>
       <c r="V8" s="10">
-        <f>IF(ISNA(E8),V7,IF(E8=0,V7+1,0))</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="W8" s="10">
-        <f>IF(ISNA(F8),W7,IF(F8=0,W7+1,0))</f>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="X8" s="10">
-        <f t="shared" ref="X8" si="47">IF(ISNA(G8),X7,IF(G8=0,X7+1,0))</f>
+        <f t="shared" ref="X8" si="50">IF(ISNA(G8),X7,IF(G8=0,X7+1,0))</f>
         <v>1</v>
       </c>
       <c r="Y8" s="10">
-        <f t="shared" ref="Y8" si="48">IF(ISNA(H8),Y7,IF(H8=0,Y7+1,0))</f>
+        <f t="shared" ref="Y8" si="51">IF(ISNA(H8),Y7,IF(H8=0,Y7+1,0))</f>
         <v>0</v>
       </c>
       <c r="Z8" s="10">
-        <f t="shared" ref="Z8" si="49">IF(ISNA(I8),Z7,IF(I8=0,Z7+1,0))</f>
+        <f t="shared" ref="Z8" si="52">IF(ISNA(I8),Z7,IF(I8=0,Z7+1,0))</f>
         <v>1</v>
       </c>
       <c r="AA8" s="10">
-        <f t="shared" ref="AA8" si="50">IF(ISNA(J8),AA7,IF(J8=0,AA7+1,0))</f>
+        <f t="shared" ref="AA8" si="53">IF(ISNA(J8),AA7,IF(J8=0,AA7+1,0))</f>
         <v>0</v>
       </c>
     </row>
@@ -7805,71 +7964,71 @@
         <v>#N/A</v>
       </c>
       <c r="K9" s="1">
-        <f t="shared" ref="K9" si="51">COUNTIF(E9:J9,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="K9" si="54">COUNTIF(E9:J9,"&lt;&gt;#N/A")</f>
         <v>4</v>
       </c>
       <c r="L9" s="1">
-        <f t="shared" ref="L9" si="52">SUMIF(E9:J9,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="L9" si="55">SUMIF(E9:J9,"&lt;&gt;#N/A")</f>
         <v>1</v>
       </c>
       <c r="M9" s="1">
-        <f t="shared" ref="M9" si="53">IF(SUMIF(E9:J9,"&lt;&gt;#N/A")=0, 1, 0)</f>
+        <f t="shared" ref="M9" si="56">IF(SUMIF(E9:J9,"&lt;&gt;#N/A")=0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="N9" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O9" s="1" t="str">
-        <f t="shared" ref="O9" si="54">IF(L9=1,INDEX($E$2:$J$2,1,MATCH(1,E9:J9,0)),NA())</f>
+        <f t="shared" ref="O9" si="57">IF(L9=1,INDEX($E$2:$J$2,1,MATCH(1,E9:J9,0)),NA())</f>
         <v>Evan</v>
       </c>
       <c r="P9" s="8">
-        <f t="shared" ref="P9" si="55">IF(ISNA(E9),P8,IF(E9=1,P8+1,0))</f>
+        <f t="shared" ref="P9" si="58">IF(ISNA(E9),P8,IF(E9=1,P8+1,0))</f>
         <v>0</v>
       </c>
       <c r="Q9" s="8">
-        <f t="shared" ref="Q9" si="56">IF(ISNA(F9),Q8,IF(F9=1,Q8+1,0))</f>
+        <f t="shared" ref="Q9" si="59">IF(ISNA(F9),Q8,IF(F9=1,Q8+1,0))</f>
         <v>0</v>
       </c>
       <c r="R9" s="8">
-        <f t="shared" ref="R9" si="57">IF(ISNA(G9),R8,IF(G9=1,R8+1,0))</f>
+        <f t="shared" ref="R9" si="60">IF(ISNA(G9),R8,IF(G9=1,R8+1,0))</f>
         <v>0</v>
       </c>
       <c r="S9" s="8">
-        <f t="shared" ref="S9" si="58">IF(ISNA(H9),S8,IF(H9=1,S8+1,0))</f>
+        <f t="shared" ref="S9" si="61">IF(ISNA(H9),S8,IF(H9=1,S8+1,0))</f>
         <v>2</v>
       </c>
       <c r="T9" s="8">
-        <f t="shared" ref="T9" si="59">IF(ISNA(I9),T8,IF(I9=1,T8+1,0))</f>
+        <f t="shared" ref="T9" si="62">IF(ISNA(I9),T8,IF(I9=1,T8+1,0))</f>
         <v>0</v>
       </c>
       <c r="U9" s="8">
-        <f t="shared" ref="U9" si="60">IF(ISNA(J9),U8,IF(J9=1,U8+1,0))</f>
+        <f t="shared" ref="U9" si="63">IF(ISNA(J9),U8,IF(J9=1,U8+1,0))</f>
         <v>0</v>
       </c>
       <c r="V9" s="10">
-        <f t="shared" ref="V9" si="61">IF(ISNA(E9),V8,IF(E9=0,V8+1,0))</f>
+        <f t="shared" ref="V9" si="64">IF(ISNA(E9),V8,IF(E9=0,V8+1,0))</f>
         <v>1</v>
       </c>
       <c r="W9" s="10">
-        <f t="shared" ref="W9" si="62">IF(ISNA(F9),W8,IF(F9=0,W8+1,0))</f>
+        <f t="shared" ref="W9" si="65">IF(ISNA(F9),W8,IF(F9=0,W8+1,0))</f>
         <v>2</v>
       </c>
       <c r="X9" s="10">
-        <f t="shared" ref="X9" si="63">IF(ISNA(G9),X8,IF(G9=0,X8+1,0))</f>
+        <f t="shared" ref="X9" si="66">IF(ISNA(G9),X8,IF(G9=0,X8+1,0))</f>
         <v>2</v>
       </c>
       <c r="Y9" s="10">
-        <f t="shared" ref="Y9" si="64">IF(ISNA(H9),Y8,IF(H9=0,Y8+1,0))</f>
+        <f t="shared" ref="Y9" si="67">IF(ISNA(H9),Y8,IF(H9=0,Y8+1,0))</f>
         <v>0</v>
       </c>
       <c r="Z9" s="10">
-        <f t="shared" ref="Z9" si="65">IF(ISNA(I9),Z8,IF(I9=0,Z8+1,0))</f>
+        <f t="shared" ref="Z9" si="68">IF(ISNA(I9),Z8,IF(I9=0,Z8+1,0))</f>
         <v>1</v>
       </c>
       <c r="AA9" s="10">
-        <f t="shared" ref="AA9" si="66">IF(ISNA(J9),AA8,IF(J9=0,AA8+1,0))</f>
+        <f t="shared" ref="AA9" si="69">IF(ISNA(J9),AA8,IF(J9=0,AA8+1,0))</f>
         <v>0</v>
       </c>
     </row>
@@ -7915,71 +8074,71 @@
         <v>#N/A</v>
       </c>
       <c r="K10" s="1">
-        <f t="shared" ref="K10" si="67">COUNTIF(E10:J10,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="K10" si="70">COUNTIF(E10:J10,"&lt;&gt;#N/A")</f>
         <v>4</v>
       </c>
       <c r="L10" s="1">
-        <f t="shared" ref="L10" si="68">SUMIF(E10:J10,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="L10" si="71">SUMIF(E10:J10,"&lt;&gt;#N/A")</f>
         <v>3</v>
       </c>
       <c r="M10" s="1">
-        <f t="shared" ref="M10" si="69">IF(SUMIF(E10:J10,"&lt;&gt;#N/A")=0, 1, 0)</f>
+        <f t="shared" ref="M10" si="72">IF(SUMIF(E10:J10,"&lt;&gt;#N/A")=0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="N10" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O10" s="1" t="e">
-        <f t="shared" ref="O10" si="70">IF(L10=1,INDEX($E$2:$J$2,1,MATCH(1,E10:J10,0)),NA())</f>
+        <f t="shared" ref="O10" si="73">IF(L10=1,INDEX($E$2:$J$2,1,MATCH(1,E10:J10,0)),NA())</f>
         <v>#N/A</v>
       </c>
       <c r="P10" s="8">
-        <f t="shared" ref="P10" si="71">IF(ISNA(E10),P9,IF(E10=1,P9+1,0))</f>
+        <f t="shared" ref="P10" si="74">IF(ISNA(E10),P9,IF(E10=1,P9+1,0))</f>
         <v>1</v>
       </c>
       <c r="Q10" s="8">
-        <f t="shared" ref="Q10" si="72">IF(ISNA(F10),Q9,IF(F10=1,Q9+1,0))</f>
+        <f t="shared" ref="Q10" si="75">IF(ISNA(F10),Q9,IF(F10=1,Q9+1,0))</f>
         <v>1</v>
       </c>
       <c r="R10" s="8">
-        <f t="shared" ref="R10" si="73">IF(ISNA(G10),R9,IF(G10=1,R9+1,0))</f>
+        <f t="shared" ref="R10" si="76">IF(ISNA(G10),R9,IF(G10=1,R9+1,0))</f>
         <v>1</v>
       </c>
       <c r="S10" s="8">
-        <f t="shared" ref="S10" si="74">IF(ISNA(H10),S9,IF(H10=1,S9+1,0))</f>
+        <f t="shared" ref="S10" si="77">IF(ISNA(H10),S9,IF(H10=1,S9+1,0))</f>
         <v>0</v>
       </c>
       <c r="T10" s="8">
-        <f t="shared" ref="T10" si="75">IF(ISNA(I10),T9,IF(I10=1,T9+1,0))</f>
+        <f t="shared" ref="T10" si="78">IF(ISNA(I10),T9,IF(I10=1,T9+1,0))</f>
         <v>0</v>
       </c>
       <c r="U10" s="8">
-        <f t="shared" ref="U10" si="76">IF(ISNA(J10),U9,IF(J10=1,U9+1,0))</f>
+        <f t="shared" ref="U10" si="79">IF(ISNA(J10),U9,IF(J10=1,U9+1,0))</f>
         <v>0</v>
       </c>
       <c r="V10" s="10">
-        <f t="shared" ref="V10" si="77">IF(ISNA(E10),V9,IF(E10=0,V9+1,0))</f>
+        <f t="shared" ref="V10" si="80">IF(ISNA(E10),V9,IF(E10=0,V9+1,0))</f>
         <v>0</v>
       </c>
       <c r="W10" s="10">
-        <f t="shared" ref="W10" si="78">IF(ISNA(F10),W9,IF(F10=0,W9+1,0))</f>
+        <f t="shared" ref="W10" si="81">IF(ISNA(F10),W9,IF(F10=0,W9+1,0))</f>
         <v>0</v>
       </c>
       <c r="X10" s="10">
-        <f t="shared" ref="X10" si="79">IF(ISNA(G10),X9,IF(G10=0,X9+1,0))</f>
+        <f t="shared" ref="X10" si="82">IF(ISNA(G10),X9,IF(G10=0,X9+1,0))</f>
         <v>0</v>
       </c>
       <c r="Y10" s="10">
-        <f t="shared" ref="Y10" si="80">IF(ISNA(H10),Y9,IF(H10=0,Y9+1,0))</f>
+        <f t="shared" ref="Y10" si="83">IF(ISNA(H10),Y9,IF(H10=0,Y9+1,0))</f>
         <v>1</v>
       </c>
       <c r="Z10" s="10">
-        <f t="shared" ref="Z10" si="81">IF(ISNA(I10),Z9,IF(I10=0,Z9+1,0))</f>
+        <f t="shared" ref="Z10" si="84">IF(ISNA(I10),Z9,IF(I10=0,Z9+1,0))</f>
         <v>1</v>
       </c>
       <c r="AA10" s="10">
-        <f t="shared" ref="AA10" si="82">IF(ISNA(J10),AA9,IF(J10=0,AA9+1,0))</f>
+        <f t="shared" ref="AA10" si="85">IF(ISNA(J10),AA9,IF(J10=0,AA9+1,0))</f>
         <v>0</v>
       </c>
     </row>
@@ -8025,71 +8184,71 @@
         <v>#N/A</v>
       </c>
       <c r="K11" s="1">
-        <f t="shared" ref="K11" si="83">COUNTIF(E11:J11,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="K11" si="86">COUNTIF(E11:J11,"&lt;&gt;#N/A")</f>
         <v>4</v>
       </c>
       <c r="L11" s="1">
-        <f t="shared" ref="L11" si="84">SUMIF(E11:J11,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="L11" si="87">SUMIF(E11:J11,"&lt;&gt;#N/A")</f>
         <v>3</v>
       </c>
       <c r="M11" s="1">
-        <f t="shared" ref="M11" si="85">IF(SUMIF(E11:J11,"&lt;&gt;#N/A")=0, 1, 0)</f>
+        <f t="shared" ref="M11" si="88">IF(SUMIF(E11:J11,"&lt;&gt;#N/A")=0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="N11" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O11" s="1" t="e">
-        <f t="shared" ref="O11" si="86">IF(L11=1,INDEX($E$2:$J$2,1,MATCH(1,E11:J11,0)),NA())</f>
+        <f t="shared" ref="O11" si="89">IF(L11=1,INDEX($E$2:$J$2,1,MATCH(1,E11:J11,0)),NA())</f>
         <v>#N/A</v>
       </c>
       <c r="P11" s="8">
-        <f t="shared" ref="P11" si="87">IF(ISNA(E11),P10,IF(E11=1,P10+1,0))</f>
+        <f t="shared" ref="P11" si="90">IF(ISNA(E11),P10,IF(E11=1,P10+1,0))</f>
         <v>0</v>
       </c>
       <c r="Q11" s="8">
-        <f t="shared" ref="Q11" si="88">IF(ISNA(F11),Q10,IF(F11=1,Q10+1,0))</f>
+        <f t="shared" ref="Q11" si="91">IF(ISNA(F11),Q10,IF(F11=1,Q10+1,0))</f>
         <v>2</v>
       </c>
       <c r="R11" s="8">
-        <f t="shared" ref="R11" si="89">IF(ISNA(G11),R10,IF(G11=1,R10+1,0))</f>
+        <f t="shared" ref="R11" si="92">IF(ISNA(G11),R10,IF(G11=1,R10+1,0))</f>
         <v>2</v>
       </c>
       <c r="S11" s="8">
-        <f t="shared" ref="S11" si="90">IF(ISNA(H11),S10,IF(H11=1,S10+1,0))</f>
+        <f t="shared" ref="S11" si="93">IF(ISNA(H11),S10,IF(H11=1,S10+1,0))</f>
         <v>1</v>
       </c>
       <c r="T11" s="8">
-        <f t="shared" ref="T11" si="91">IF(ISNA(I11),T10,IF(I11=1,T10+1,0))</f>
+        <f t="shared" ref="T11" si="94">IF(ISNA(I11),T10,IF(I11=1,T10+1,0))</f>
         <v>0</v>
       </c>
       <c r="U11" s="8">
-        <f t="shared" ref="U11" si="92">IF(ISNA(J11),U10,IF(J11=1,U10+1,0))</f>
+        <f t="shared" ref="U11" si="95">IF(ISNA(J11),U10,IF(J11=1,U10+1,0))</f>
         <v>0</v>
       </c>
       <c r="V11" s="10">
-        <f t="shared" ref="V11" si="93">IF(ISNA(E11),V10,IF(E11=0,V10+1,0))</f>
+        <f t="shared" ref="V11" si="96">IF(ISNA(E11),V10,IF(E11=0,V10+1,0))</f>
         <v>1</v>
       </c>
       <c r="W11" s="10">
-        <f t="shared" ref="W11" si="94">IF(ISNA(F11),W10,IF(F11=0,W10+1,0))</f>
+        <f t="shared" ref="W11" si="97">IF(ISNA(F11),W10,IF(F11=0,W10+1,0))</f>
         <v>0</v>
       </c>
       <c r="X11" s="10">
-        <f t="shared" ref="X11" si="95">IF(ISNA(G11),X10,IF(G11=0,X10+1,0))</f>
+        <f t="shared" ref="X11" si="98">IF(ISNA(G11),X10,IF(G11=0,X10+1,0))</f>
         <v>0</v>
       </c>
       <c r="Y11" s="10">
-        <f t="shared" ref="Y11" si="96">IF(ISNA(H11),Y10,IF(H11=0,Y10+1,0))</f>
+        <f t="shared" ref="Y11" si="99">IF(ISNA(H11),Y10,IF(H11=0,Y10+1,0))</f>
         <v>0</v>
       </c>
       <c r="Z11" s="10">
-        <f t="shared" ref="Z11" si="97">IF(ISNA(I11),Z10,IF(I11=0,Z10+1,0))</f>
+        <f t="shared" ref="Z11" si="100">IF(ISNA(I11),Z10,IF(I11=0,Z10+1,0))</f>
         <v>1</v>
       </c>
       <c r="AA11" s="10">
-        <f t="shared" ref="AA11" si="98">IF(ISNA(J11),AA10,IF(J11=0,AA10+1,0))</f>
+        <f t="shared" ref="AA11" si="101">IF(ISNA(J11),AA10,IF(J11=0,AA10+1,0))</f>
         <v>0</v>
       </c>
     </row>
@@ -8135,71 +8294,71 @@
         <v>#N/A</v>
       </c>
       <c r="K12" s="1">
-        <f t="shared" ref="K12" si="99">COUNTIF(E12:J12,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="K12" si="102">COUNTIF(E12:J12,"&lt;&gt;#N/A")</f>
         <v>4</v>
       </c>
       <c r="L12" s="1">
-        <f t="shared" ref="L12" si="100">SUMIF(E12:J12,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="L12" si="103">SUMIF(E12:J12,"&lt;&gt;#N/A")</f>
         <v>3</v>
       </c>
       <c r="M12" s="1">
-        <f t="shared" ref="M12" si="101">IF(SUMIF(E12:J12,"&lt;&gt;#N/A")=0, 1, 0)</f>
+        <f t="shared" ref="M12" si="104">IF(SUMIF(E12:J12,"&lt;&gt;#N/A")=0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="N12" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O12" s="1" t="e">
-        <f t="shared" ref="O12" si="102">IF(L12=1,INDEX($E$2:$J$2,1,MATCH(1,E12:J12,0)),NA())</f>
+        <f t="shared" ref="O12" si="105">IF(L12=1,INDEX($E$2:$J$2,1,MATCH(1,E12:J12,0)),NA())</f>
         <v>#N/A</v>
       </c>
       <c r="P12" s="8">
-        <f t="shared" ref="P12" si="103">IF(ISNA(E12),P11,IF(E12=1,P11+1,0))</f>
+        <f t="shared" ref="P12" si="106">IF(ISNA(E12),P11,IF(E12=1,P11+1,0))</f>
         <v>1</v>
       </c>
       <c r="Q12" s="8">
-        <f t="shared" ref="Q12" si="104">IF(ISNA(F12),Q11,IF(F12=1,Q11+1,0))</f>
+        <f t="shared" ref="Q12" si="107">IF(ISNA(F12),Q11,IF(F12=1,Q11+1,0))</f>
         <v>3</v>
       </c>
       <c r="R12" s="8">
-        <f t="shared" ref="R12" si="105">IF(ISNA(G12),R11,IF(G12=1,R11+1,0))</f>
+        <f t="shared" ref="R12" si="108">IF(ISNA(G12),R11,IF(G12=1,R11+1,0))</f>
         <v>3</v>
       </c>
       <c r="S12" s="8">
-        <f t="shared" ref="S12" si="106">IF(ISNA(H12),S11,IF(H12=1,S11+1,0))</f>
+        <f t="shared" ref="S12" si="109">IF(ISNA(H12),S11,IF(H12=1,S11+1,0))</f>
         <v>0</v>
       </c>
       <c r="T12" s="8">
-        <f t="shared" ref="T12" si="107">IF(ISNA(I12),T11,IF(I12=1,T11+1,0))</f>
+        <f t="shared" ref="T12" si="110">IF(ISNA(I12),T11,IF(I12=1,T11+1,0))</f>
         <v>0</v>
       </c>
       <c r="U12" s="8">
-        <f t="shared" ref="U12" si="108">IF(ISNA(J12),U11,IF(J12=1,U11+1,0))</f>
+        <f t="shared" ref="U12" si="111">IF(ISNA(J12),U11,IF(J12=1,U11+1,0))</f>
         <v>0</v>
       </c>
       <c r="V12" s="10">
-        <f t="shared" ref="V12" si="109">IF(ISNA(E12),V11,IF(E12=0,V11+1,0))</f>
+        <f t="shared" ref="V12" si="112">IF(ISNA(E12),V11,IF(E12=0,V11+1,0))</f>
         <v>0</v>
       </c>
       <c r="W12" s="10">
-        <f t="shared" ref="W12" si="110">IF(ISNA(F12),W11,IF(F12=0,W11+1,0))</f>
+        <f t="shared" ref="W12" si="113">IF(ISNA(F12),W11,IF(F12=0,W11+1,0))</f>
         <v>0</v>
       </c>
       <c r="X12" s="10">
-        <f t="shared" ref="X12" si="111">IF(ISNA(G12),X11,IF(G12=0,X11+1,0))</f>
+        <f t="shared" ref="X12" si="114">IF(ISNA(G12),X11,IF(G12=0,X11+1,0))</f>
         <v>0</v>
       </c>
       <c r="Y12" s="10">
-        <f t="shared" ref="Y12" si="112">IF(ISNA(H12),Y11,IF(H12=0,Y11+1,0))</f>
+        <f t="shared" ref="Y12" si="115">IF(ISNA(H12),Y11,IF(H12=0,Y11+1,0))</f>
         <v>1</v>
       </c>
       <c r="Z12" s="10">
-        <f t="shared" ref="Z12" si="113">IF(ISNA(I12),Z11,IF(I12=0,Z11+1,0))</f>
+        <f t="shared" ref="Z12" si="116">IF(ISNA(I12),Z11,IF(I12=0,Z11+1,0))</f>
         <v>1</v>
       </c>
       <c r="AA12" s="10">
-        <f t="shared" ref="AA12" si="114">IF(ISNA(J12),AA11,IF(J12=0,AA11+1,0))</f>
+        <f t="shared" ref="AA12" si="117">IF(ISNA(J12),AA11,IF(J12=0,AA11+1,0))</f>
         <v>0</v>
       </c>
     </row>
@@ -8245,72 +8404,402 @@
         <v>#N/A</v>
       </c>
       <c r="K13" s="1">
-        <f t="shared" ref="K13" si="115">COUNTIF(E13:J13,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="K13" si="118">COUNTIF(E13:J13,"&lt;&gt;#N/A")</f>
         <v>4</v>
       </c>
       <c r="L13" s="1">
-        <f t="shared" ref="L13" si="116">SUMIF(E13:J13,"&lt;&gt;#N/A")</f>
+        <f t="shared" ref="L13" si="119">SUMIF(E13:J13,"&lt;&gt;#N/A")</f>
         <v>4</v>
       </c>
       <c r="M13" s="1">
-        <f t="shared" ref="M13" si="117">IF(SUMIF(E13:J13,"&lt;&gt;#N/A")=0, 1, 0)</f>
+        <f t="shared" ref="M13" si="120">IF(SUMIF(E13:J13,"&lt;&gt;#N/A")=0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="N13" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="O13" s="1" t="e">
-        <f t="shared" ref="O13" si="118">IF(L13=1,INDEX($E$2:$J$2,1,MATCH(1,E13:J13,0)),NA())</f>
+        <f t="shared" ref="O13" si="121">IF(L13=1,INDEX($E$2:$J$2,1,MATCH(1,E13:J13,0)),NA())</f>
         <v>#N/A</v>
       </c>
       <c r="P13" s="8">
-        <f t="shared" ref="P13" si="119">IF(ISNA(E13),P12,IF(E13=1,P12+1,0))</f>
+        <f t="shared" ref="P13" si="122">IF(ISNA(E13),P12,IF(E13=1,P12+1,0))</f>
         <v>2</v>
       </c>
       <c r="Q13" s="8">
-        <f t="shared" ref="Q13" si="120">IF(ISNA(F13),Q12,IF(F13=1,Q12+1,0))</f>
+        <f t="shared" ref="Q13" si="123">IF(ISNA(F13),Q12,IF(F13=1,Q12+1,0))</f>
         <v>4</v>
       </c>
       <c r="R13" s="8">
-        <f t="shared" ref="R13" si="121">IF(ISNA(G13),R12,IF(G13=1,R12+1,0))</f>
+        <f t="shared" ref="R13" si="124">IF(ISNA(G13),R12,IF(G13=1,R12+1,0))</f>
         <v>4</v>
       </c>
       <c r="S13" s="8">
-        <f t="shared" ref="S13" si="122">IF(ISNA(H13),S12,IF(H13=1,S12+1,0))</f>
+        <f t="shared" ref="S13" si="125">IF(ISNA(H13),S12,IF(H13=1,S12+1,0))</f>
         <v>1</v>
       </c>
       <c r="T13" s="8">
-        <f t="shared" ref="T13" si="123">IF(ISNA(I13),T12,IF(I13=1,T12+1,0))</f>
+        <f t="shared" ref="T13" si="126">IF(ISNA(I13),T12,IF(I13=1,T12+1,0))</f>
         <v>0</v>
       </c>
       <c r="U13" s="8">
-        <f t="shared" ref="U13" si="124">IF(ISNA(J13),U12,IF(J13=1,U12+1,0))</f>
+        <f t="shared" ref="U13" si="127">IF(ISNA(J13),U12,IF(J13=1,U12+1,0))</f>
         <v>0</v>
       </c>
       <c r="V13" s="10">
-        <f t="shared" ref="V13" si="125">IF(ISNA(E13),V12,IF(E13=0,V12+1,0))</f>
+        <f t="shared" ref="V13" si="128">IF(ISNA(E13),V12,IF(E13=0,V12+1,0))</f>
         <v>0</v>
       </c>
       <c r="W13" s="10">
-        <f t="shared" ref="W13" si="126">IF(ISNA(F13),W12,IF(F13=0,W12+1,0))</f>
+        <f t="shared" ref="W13" si="129">IF(ISNA(F13),W12,IF(F13=0,W12+1,0))</f>
         <v>0</v>
       </c>
       <c r="X13" s="10">
-        <f t="shared" ref="X13" si="127">IF(ISNA(G13),X12,IF(G13=0,X12+1,0))</f>
+        <f t="shared" ref="X13" si="130">IF(ISNA(G13),X12,IF(G13=0,X12+1,0))</f>
         <v>0</v>
       </c>
       <c r="Y13" s="10">
-        <f t="shared" ref="Y13" si="128">IF(ISNA(H13),Y12,IF(H13=0,Y12+1,0))</f>
+        <f t="shared" ref="Y13" si="131">IF(ISNA(H13),Y12,IF(H13=0,Y12+1,0))</f>
         <v>0</v>
       </c>
       <c r="Z13" s="10">
-        <f t="shared" ref="Z13" si="129">IF(ISNA(I13),Z12,IF(I13=0,Z12+1,0))</f>
+        <f t="shared" ref="Z13" si="132">IF(ISNA(I13),Z12,IF(I13=0,Z12+1,0))</f>
         <v>1</v>
       </c>
       <c r="AA13" s="10">
-        <f t="shared" ref="AA13" si="130">IF(ISNA(J13),AA12,IF(J13=0,AA12+1,0))</f>
-        <v>0</v>
+        <f t="shared" ref="AA13" si="133">IF(ISNA(J13),AA12,IF(J13=0,AA12+1,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <f>Data!A13</f>
+        <v>611</v>
+      </c>
+      <c r="B14" s="4" t="str">
+        <f>Data!B13</f>
+        <v>Jewie or Fiction</v>
+      </c>
+      <c r="C14" s="5" t="str">
+        <f>Data!H13</f>
+        <v>Joshie</v>
+      </c>
+      <c r="D14" s="2" t="str">
+        <f>Data!I13</f>
+        <v>Cara</v>
+      </c>
+      <c r="E14" s="1">
+        <f>IF(Data!J13=Data!$G13,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F14" s="1">
+        <f>IF(Data!K13=Data!$G13,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <f>IF(Data!L13=Data!$G13,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <f>IF(Data!M13=Data!$G13,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="1" t="e">
+        <f>IF(Data!N13=Data!$G13,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J14" s="1">
+        <f>IF(Data!O13=Data!$G13,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="K14" s="1">
+        <f t="shared" ref="K14" si="134">COUNTIF(E14:J14,"&lt;&gt;#N/A")</f>
+        <v>5</v>
+      </c>
+      <c r="L14" s="1">
+        <f t="shared" ref="L14" si="135">SUMIF(E14:J14,"&lt;&gt;#N/A")</f>
+        <v>1</v>
+      </c>
+      <c r="M14" s="1">
+        <f t="shared" ref="M14" si="136">IF(SUMIF(E14:J14,"&lt;&gt;#N/A")=0, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="N14" s="1">
+        <f t="shared" ref="N14" si="137">IF(K14=L14,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O14" s="1" t="str">
+        <f t="shared" ref="O14" si="138">IF(L14=1,INDEX($E$2:$J$2,1,MATCH(1,E14:J14,0)),NA())</f>
+        <v>Bob</v>
+      </c>
+      <c r="P14" s="8">
+        <f t="shared" ref="P14" si="139">IF(ISNA(E14),P13,IF(E14=1,P13+1,0))</f>
+        <v>3</v>
+      </c>
+      <c r="Q14" s="8">
+        <f t="shared" ref="Q14" si="140">IF(ISNA(F14),Q13,IF(F14=1,Q13+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="R14" s="8">
+        <f t="shared" ref="R14" si="141">IF(ISNA(G14),R13,IF(G14=1,R13+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="S14" s="8">
+        <f t="shared" ref="S14" si="142">IF(ISNA(H14),S13,IF(H14=1,S13+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="T14" s="8">
+        <f t="shared" ref="T14" si="143">IF(ISNA(I14),T13,IF(I14=1,T13+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="U14" s="8">
+        <f t="shared" ref="U14" si="144">IF(ISNA(J14),U13,IF(J14=1,U13+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="V14" s="10">
+        <f t="shared" ref="V14" si="145">IF(ISNA(E14),V13,IF(E14=0,V13+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="W14" s="10">
+        <f t="shared" ref="W14" si="146">IF(ISNA(F14),W13,IF(F14=0,W13+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="X14" s="10">
+        <f t="shared" ref="X14" si="147">IF(ISNA(G14),X13,IF(G14=0,X13+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="Y14" s="10">
+        <f t="shared" ref="Y14" si="148">IF(ISNA(H14),Y13,IF(H14=0,Y13+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="Z14" s="10">
+        <f t="shared" ref="Z14" si="149">IF(ISNA(I14),Z13,IF(I14=0,Z13+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AA14" s="10">
+        <f t="shared" ref="AA14" si="150">IF(ISNA(J14),AA13,IF(J14=0,AA13+1,0))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <f>Data!A14</f>
+        <v>612</v>
+      </c>
+      <c r="B15" s="4" t="str">
+        <f>Data!B14</f>
+        <v>Dinosaurs</v>
+      </c>
+      <c r="C15" s="5" t="str">
+        <f>Data!H14</f>
+        <v>Steve</v>
+      </c>
+      <c r="D15" s="2" t="str">
+        <f>Data!I14</f>
+        <v>Jay</v>
+      </c>
+      <c r="E15" s="1">
+        <f>IF(Data!J14=Data!$G14,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <f>IF(Data!K14=Data!$G14,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G15" s="1">
+        <f>IF(Data!L14=Data!$G14,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
+        <f>IF(Data!M14=Data!$G14,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="I15" s="1" t="e">
+        <f>IF(Data!N14=Data!$G14,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J15" s="1" t="e">
+        <f>IF(Data!O14=Data!$G14,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K15" s="1">
+        <f t="shared" ref="K15" si="151">COUNTIF(E15:J15,"&lt;&gt;#N/A")</f>
+        <v>4</v>
+      </c>
+      <c r="L15" s="1">
+        <f t="shared" ref="L15" si="152">SUMIF(E15:J15,"&lt;&gt;#N/A")</f>
+        <v>2</v>
+      </c>
+      <c r="M15" s="1">
+        <f t="shared" ref="M15" si="153">IF(SUMIF(E15:J15,"&lt;&gt;#N/A")=0, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="N15" s="1">
+        <f t="shared" ref="N15" si="154">IF(K15=L15,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O15" s="1" t="e">
+        <f t="shared" ref="O15" si="155">IF(L15=1,INDEX($E$2:$J$2,1,MATCH(1,E15:J15,0)),NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P15" s="8">
+        <f t="shared" ref="P15" si="156">IF(ISNA(E15),P14,IF(E15=1,P14+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="8">
+        <f t="shared" ref="Q15" si="157">IF(ISNA(F15),Q14,IF(F15=1,Q14+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="R15" s="8">
+        <f t="shared" ref="R15" si="158">IF(ISNA(G15),R14,IF(G15=1,R14+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="S15" s="8">
+        <f t="shared" ref="S15" si="159">IF(ISNA(H15),S14,IF(H15=1,S14+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="T15" s="8">
+        <f t="shared" ref="T15" si="160">IF(ISNA(I15),T14,IF(I15=1,T14+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="U15" s="8">
+        <f t="shared" ref="U15" si="161">IF(ISNA(J15),U14,IF(J15=1,U14+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="V15" s="10">
+        <f t="shared" ref="V15" si="162">IF(ISNA(E15),V14,IF(E15=0,V14+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="W15" s="10">
+        <f t="shared" ref="W15" si="163">IF(ISNA(F15),W14,IF(F15=0,W14+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="X15" s="10">
+        <f t="shared" ref="X15" si="164">IF(ISNA(G15),X14,IF(G15=0,X14+1,0))</f>
+        <v>2</v>
+      </c>
+      <c r="Y15" s="10">
+        <f t="shared" ref="Y15" si="165">IF(ISNA(H15),Y14,IF(H15=0,Y14+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="Z15" s="10">
+        <f t="shared" ref="Z15" si="166">IF(ISNA(I15),Z14,IF(I15=0,Z14+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AA15" s="10">
+        <f t="shared" ref="AA15" si="167">IF(ISNA(J15),AA14,IF(J15=0,AA14+1,0))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <f>Data!A15</f>
+        <v>613</v>
+      </c>
+      <c r="B16" s="4" t="e">
+        <f>Data!B15</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C16" s="5" t="str">
+        <f>Data!H15</f>
+        <v>Steve</v>
+      </c>
+      <c r="D16" s="2" t="str">
+        <f>Data!I15</f>
+        <v>Bob</v>
+      </c>
+      <c r="E16" s="1">
+        <f>IF(Data!J15=Data!$G15,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F16" s="1">
+        <f>IF(Data!K15=Data!$G15,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <f>IF(Data!L15=Data!$G15,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H16" s="1">
+        <f>IF(Data!M15=Data!$G15,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="I16" s="1" t="e">
+        <f>IF(Data!N15=Data!$G15,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J16" s="1" t="e">
+        <f>IF(Data!O15=Data!$G15,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K16" s="1">
+        <f t="shared" ref="K16" si="168">COUNTIF(E16:J16,"&lt;&gt;#N/A")</f>
+        <v>4</v>
+      </c>
+      <c r="L16" s="1">
+        <f t="shared" ref="L16" si="169">SUMIF(E16:J16,"&lt;&gt;#N/A")</f>
+        <v>4</v>
+      </c>
+      <c r="M16" s="1">
+        <f t="shared" ref="M16" si="170">IF(SUMIF(E16:J16,"&lt;&gt;#N/A")=0, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="N16" s="1">
+        <f t="shared" ref="N16" si="171">IF(K16=L16,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O16" s="1" t="e">
+        <f t="shared" ref="O16" si="172">IF(L16=1,INDEX($E$2:$J$2,1,MATCH(1,E16:J16,0)),NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P16" s="8">
+        <f t="shared" ref="P16" si="173">IF(ISNA(E16),P15,IF(E16=1,P15+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="Q16" s="8">
+        <f t="shared" ref="Q16" si="174">IF(ISNA(F16),Q15,IF(F16=1,Q15+1,0))</f>
+        <v>2</v>
+      </c>
+      <c r="R16" s="8">
+        <f t="shared" ref="R16" si="175">IF(ISNA(G16),R15,IF(G16=1,R15+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="S16" s="8">
+        <f t="shared" ref="S16" si="176">IF(ISNA(H16),S15,IF(H16=1,S15+1,0))</f>
+        <v>2</v>
+      </c>
+      <c r="T16" s="8">
+        <f t="shared" ref="T16" si="177">IF(ISNA(I16),T15,IF(I16=1,T15+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="U16" s="8">
+        <f t="shared" ref="U16" si="178">IF(ISNA(J16),U15,IF(J16=1,U15+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="V16" s="10">
+        <f t="shared" ref="V16" si="179">IF(ISNA(E16),V15,IF(E16=0,V15+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="W16" s="10">
+        <f t="shared" ref="W16" si="180">IF(ISNA(F16),W15,IF(F16=0,W15+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="X16" s="10">
+        <f t="shared" ref="X16" si="181">IF(ISNA(G16),X15,IF(G16=0,X15+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="Y16" s="10">
+        <f t="shared" ref="Y16" si="182">IF(ISNA(H16),Y15,IF(H16=0,Y15+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="Z16" s="10">
+        <f t="shared" ref="Z16" si="183">IF(ISNA(I16),Z15,IF(I16=0,Z15+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AA16" s="10">
+        <f t="shared" ref="AA16" si="184">IF(ISNA(J16),AA15,IF(J16=0,AA15+1,0))</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -8328,7 +8817,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8371,31 +8860,31 @@
       </c>
       <c r="B2" s="6">
         <f>SUMIF(Results!E3:E53,"&lt;&gt;#N/A")/COUNTIFS(Results!E3:E53,"&lt;&gt;#N/A",Results!E3:E53,"&lt;&gt;")</f>
-        <v>0.45454545454545453</v>
+        <v>0.5</v>
       </c>
       <c r="C2" s="6">
         <f>SUMIF(Results!F3:F53,"&lt;&gt;#N/A")/COUNTIFS(Results!F3:F53,"&lt;&gt;#N/A",Results!F3:F53,"&lt;&gt;")</f>
-        <v>0.7</v>
+        <v>0.69230769230769229</v>
       </c>
       <c r="D2" s="6">
         <f>SUMIF(Results!G3:G53,"&lt;&gt;#N/A")/COUNTIFS(Results!G3:G53,"&lt;&gt;#N/A",Results!G3:G53,"&lt;&gt;")</f>
-        <v>0.72727272727272729</v>
+        <v>0.6428571428571429</v>
       </c>
       <c r="E2" s="6">
         <f>SUMIF(Results!H3:H53,"&lt;&gt;#N/A")/COUNTIFS(Results!H3:H53,"&lt;&gt;#N/A",Results!H3:H53,"&lt;&gt;")</f>
-        <v>0.63636363636363635</v>
+        <v>0.6428571428571429</v>
       </c>
       <c r="F2" s="6">
         <f>SUMIF(Results!I3:I53,"&lt;&gt;#N/A")/COUNTIFS(Results!I3:I53,"&lt;&gt;#N/A",Results!I3:I53,"&lt;&gt;")</f>
         <v>0</v>
       </c>
-      <c r="G2" s="6" t="e">
+      <c r="G2" s="6">
         <f>SUMIF(Results!J3:J53,"&lt;&gt;#N/A")/COUNTIFS(Results!J3:J53,"&lt;&gt;#N/A",Results!J3:J53,"&lt;&gt;")</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="H2" s="6">
         <f>SUM(Results!L3:L53)/SUM(Results!K3:K53)</f>
-        <v>0.61363636363636365</v>
+        <v>0.59649122807017541</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -8404,31 +8893,31 @@
       </c>
       <c r="B3" s="6">
         <f>SUMIFS(Results!E3:E53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!E3:E53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!E3:E53, "&lt;&gt;#N/A", Results!E3:E53, "&lt;&gt;")</f>
-        <v>0</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="C3" s="6">
         <f>SUMIFS(Results!F3:F53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!F3:F53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!F3:F53, "&lt;&gt;#N/A", Results!F3:F53, "&lt;&gt;")</f>
-        <v>0.75</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="D3" s="6">
         <f>SUMIFS(Results!G3:G53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!G3:G53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!G3:G53, "&lt;&gt;#N/A", Results!G3:G53, "&lt;&gt;")</f>
-        <v>0.6</v>
+        <v>0.42857142857142855</v>
       </c>
       <c r="E3" s="6">
         <f>SUMIFS(Results!H3:H53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!H3:H53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!H3:H53, "&lt;&gt;#N/A", Results!H3:H53, "&lt;&gt;")</f>
-        <v>0.6</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="F3" s="6">
         <f>SUMIFS(Results!I3:I53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!I3:I53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!I3:I53, "&lt;&gt;#N/A", Results!I3:I53, "&lt;&gt;")</f>
         <v>0</v>
       </c>
-      <c r="G3" s="6" t="e">
+      <c r="G3" s="6">
         <f>SUMIFS(Results!J3:J53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!J3:J53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!J3:J53, "&lt;&gt;#N/A", Results!J3:J53, "&lt;&gt;")</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="H3" s="6">
         <f>SUMIF(Results!B3:B53,"&lt;&gt;#N/A",Results!L3:L53)/SUMIF(Results!B3:B53,"&lt;&gt;#N/A",Results!K3:K53)</f>
-        <v>0.45</v>
+        <v>0.41379310344827586</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -8437,19 +8926,19 @@
       </c>
       <c r="B4" s="6">
         <f>SUMIFS(Results!E3:E53,Results!$B$3:$B$53,"=#N/A",Results!E3:E53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!E3:E53, "&lt;&gt;#N/A", Results!E3:E53, "&lt;&gt;")</f>
-        <v>0.83333333333333337</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="C4" s="6">
         <f>SUMIFS(Results!F3:F53,Results!$B$3:$B$53,"=#N/A",Results!F3:F53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!F3:F53, "&lt;&gt;#N/A", Results!F3:F53, "&lt;&gt;")</f>
-        <v>0.66666666666666663</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="D4" s="6">
         <f>SUMIFS(Results!G3:G53,Results!$B$3:$B$53,"=#N/A",Results!G3:G53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!G3:G53, "&lt;&gt;#N/A", Results!G3:G53, "&lt;&gt;")</f>
-        <v>0.83333333333333337</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="E4" s="6">
         <f>SUMIFS(Results!H3:H53,Results!$B$3:$B$53,"=#N/A",Results!H3:H53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!H3:H53, "&lt;&gt;#N/A", Results!H3:H53, "&lt;&gt;")</f>
-        <v>0.66666666666666663</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="F4" s="6" t="e">
         <f>SUMIFS(Results!I3:I53,Results!$B$3:$B$53,"=#N/A",Results!I3:I53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!I3:I53, "&lt;&gt;#N/A", Results!I3:I53, "&lt;&gt;")</f>
@@ -8461,7 +8950,7 @@
       </c>
       <c r="H4" s="6">
         <f>SUMIF(Results!B3:B53,"=#N/A",Results!L3:L53)/SUMIF(Results!B3:B53,"=#N/A",Results!K3:K53)</f>
-        <v>0.75</v>
+        <v>0.7857142857142857</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -8470,7 +8959,7 @@
       </c>
       <c r="B5" s="1">
         <f>MAX(Results!P3:P53)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1">
         <f>MAX(Results!Q3:Q53)</f>
@@ -8523,7 +9012,7 @@
       </c>
       <c r="G6" s="1">
         <f>MAX(Results!AA3:AA53)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="1">
         <f>MAX(B6:G6)</f>
@@ -8536,7 +9025,7 @@
       </c>
       <c r="B7" s="1">
         <f>COUNTIF(Results!$O$3:$O$53,Summary!B1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1">
         <f>COUNTIF(Results!$O$3:$O$53,Summary!C1)</f>
@@ -8569,15 +9058,15 @@
       </c>
       <c r="B8" s="7">
         <f>SUMIF(Results!$D$3:$D$53,B1,Results!$L$3:$L$53)/SUMIF(Results!$D$3:$D$53,B1,Results!$K$3:$K$53)</f>
-        <v>0.58333333333333337</v>
+        <v>0.6875</v>
       </c>
       <c r="C8" s="7">
         <f>SUMIF(Results!$D$3:$D$53,C1,Results!$L$3:$L$53)/SUMIF(Results!$D$3:$D$53,C1,Results!$K$3:$K$53)</f>
-        <v>0.75</v>
+        <v>0.58823529411764708</v>
       </c>
       <c r="D8" s="7">
         <f>SUMIF(Results!$D$3:$D$53,D1,Results!$L$3:$L$53)/SUMIF(Results!$D$3:$D$53,D1,Results!$K$3:$K$53)</f>
-        <v>0.25</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E8" s="7">
         <f>SUMIF(Results!$D$3:$D$53,E1,Results!$L$3:$L$53)/SUMIF(Results!$D$3:$D$53,E1,Results!$K$3:$K$53)</f>
@@ -8602,19 +9091,19 @@
       </c>
       <c r="B9" s="1">
         <f>SUMIF(Results!E3:E53,"&lt;&gt;#N/A")</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C9" s="1">
         <f>SUMIF(Results!F3:F53,"&lt;&gt;#N/A")</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D9" s="1">
         <f>SUMIF(Results!G3:G53,"&lt;&gt;#N/A")</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E9" s="1">
         <f>SUMIF(Results!H3:H53,"&lt;&gt;#N/A")</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F9" s="1">
         <f>SUMIF(Results!I3:I53,"&lt;&gt;#N/A")</f>
@@ -8626,7 +9115,7 @@
       </c>
       <c r="H9" s="1">
         <f>SUM(B9:G9)</f>
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -8635,19 +9124,19 @@
       </c>
       <c r="B10" s="1">
         <f>COUNTIFS(Results!E3:E53,"&lt;&gt;#N/A",Results!E3:E53,"&lt;&gt;")</f>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C10" s="1">
         <f>COUNTIFS(Results!F3:F53,"&lt;&gt;#N/A",Results!F3:F53,"&lt;&gt;")</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D10" s="1">
         <f>COUNTIFS(Results!G3:G53,"&lt;&gt;#N/A",Results!G3:G53,"&lt;&gt;")</f>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E10" s="1">
         <f>COUNTIFS(Results!H3:H53,"&lt;&gt;#N/A",Results!H3:H53,"&lt;&gt;")</f>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F10" s="1">
         <f>COUNTIFS(Results!I3:I53,"&lt;&gt;#N/A",Results!I3:I53,"&lt;&gt;")</f>
@@ -8655,11 +9144,11 @@
       </c>
       <c r="G10" s="1">
         <f>COUNTIFS(Results!J3:J53,"&lt;&gt;#N/A",Results!J3:J53,"&lt;&gt;")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="1">
         <f t="shared" ref="H10:H14" si="0">SUM(B10:G10)</f>
-        <v>44</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -8668,11 +9157,11 @@
       </c>
       <c r="B11" s="1">
         <f>SUMIFS(Results!E3:E53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!E3:E53, "&lt;&gt;#N/A")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="1">
         <f>SUMIFS(Results!F3:F53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!F3:F53, "&lt;&gt;#N/A")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D11" s="1">
         <f>SUMIFS(Results!G3:G53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!G3:G53, "&lt;&gt;#N/A")</f>
@@ -8680,7 +9169,7 @@
       </c>
       <c r="E11" s="1">
         <f>SUMIFS(Results!H3:H53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!H3:H53, "&lt;&gt;#N/A")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F11" s="1">
         <f>SUMIFS(Results!I3:I53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!I3:I53, "&lt;&gt;#N/A")</f>
@@ -8692,7 +9181,7 @@
       </c>
       <c r="H11" s="1">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -8701,19 +9190,19 @@
       </c>
       <c r="B12" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!E3:E53, "&lt;&gt;#N/A", Results!E3:E53, "&lt;&gt;")</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C12" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!F3:F53, "&lt;&gt;#N/A", Results!F3:F53, "&lt;&gt;")</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D12" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!G3:G53, "&lt;&gt;#N/A", Results!G3:G53, "&lt;&gt;")</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E12" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!H3:H53, "&lt;&gt;#N/A", Results!H3:H53, "&lt;&gt;")</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F12" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!I3:I53, "&lt;&gt;#N/A", Results!I3:I53, "&lt;&gt;")</f>
@@ -8721,11 +9210,11 @@
       </c>
       <c r="G12" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!J3:J53, "&lt;&gt;#N/A", Results!J3:J53, "&lt;&gt;")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -8734,19 +9223,19 @@
       </c>
       <c r="B13" s="1">
         <f>SUMIFS(Results!E3:E53,Results!$B$3:$B$53,"=#N/A",Results!E3:E53, "&lt;&gt;#N/A")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C13" s="1">
         <f>SUMIFS(Results!F3:F53,Results!$B$3:$B$53,"=#N/A",Results!F3:F53, "&lt;&gt;#N/A")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D13" s="1">
         <f>SUMIFS(Results!G3:G53,Results!$B$3:$B$53,"=#N/A",Results!G3:G53, "&lt;&gt;#N/A")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E13" s="1">
         <f>SUMIFS(Results!H3:H53,Results!$B$3:$B$53,"=#N/A",Results!H3:H53, "&lt;&gt;#N/A")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F13" s="1">
         <f>SUMIFS(Results!I3:I53,Results!$B$3:$B$53,"=#N/A",Results!I3:I53, "&lt;&gt;#N/A")</f>
@@ -8758,7 +9247,7 @@
       </c>
       <c r="H13" s="1">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -8767,19 +9256,19 @@
       </c>
       <c r="B14" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!E3:E53, "&lt;&gt;#N/A", Results!E3:E53, "&lt;&gt;")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C14" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!F3:F53, "&lt;&gt;#N/A", Results!F3:F53, "&lt;&gt;")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D14" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!G3:G53, "&lt;&gt;#N/A", Results!G3:G53, "&lt;&gt;")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E14" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!H3:H53, "&lt;&gt;#N/A", Results!H3:H53, "&lt;&gt;")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F14" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!I3:I53, "&lt;&gt;#N/A", Results!I3:I53, "&lt;&gt;")</f>
@@ -8791,7 +9280,7 @@
       </c>
       <c r="H14" s="1">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -8833,19 +9322,19 @@
       </c>
       <c r="B16" s="1">
         <f>SUMIF(Results!E3:E53,"&lt;&gt;#N/A",Results!$N$3:$N$53)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C16" s="1">
         <f>SUMIF(Results!F3:F53,"&lt;&gt;#N/A",Results!$N$3:$N$53)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" s="1">
         <f>SUMIF(Results!G3:G53,"&lt;&gt;#N/A",Results!$N$3:$N$53)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E16" s="1">
         <f>SUMIF(Results!H3:H53,"&lt;&gt;#N/A",Results!$N$3:$N$53)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F16" s="1">
         <f>SUMIF(Results!I3:I53,"&lt;&gt;#N/A",Results!$N$3:$N$53)</f>
@@ -8857,7 +9346,7 @@
       </c>
       <c r="H16" s="1">
         <f>SUM(Results!N3:N53)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -8870,7 +9359,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="V22" sqref="V22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated through episode 618
</commit_message>
<xml_diff>
--- a/SGU_Science_or_Fiction.xlsx
+++ b/SGU_Science_or_Fiction.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6135" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6135"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="107">
   <si>
     <t>Episode</t>
   </si>
@@ -291,6 +291,63 @@
   </si>
   <si>
     <t>A new DNA analysis finds that indigenous people living in the Pacific Northwest display genetic continuity with local populations for at least 10,000 years.</t>
+  </si>
+  <si>
+    <t>What's Bigger</t>
+  </si>
+  <si>
+    <t>Blue whales are heavier than the ten largest known dinosaur species combined</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jupiter has more mass and volume than all other objects in the solar system, except for the sun, combined. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The military budget of the US is greater than the military budgets of the next 7 largest combined. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Amazon river has more discharge then the next 7 largest rivers combined. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">In a new study researchers find that neurons are able to form a network in the absence of synaptic activity. </t>
+  </si>
+  <si>
+    <t>Scientists have shown that homing pigeons are able to pass on knowledge to subsequent generations, the first non-primate species to demonstrate this ability.</t>
+  </si>
+  <si>
+    <t>Scientists find that even starting with a single female cockroach, they are able to reproduce asexually and indefinitely maintain a large population.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Socrates left behind no writings. We know of him only from the accounts of others. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">he ancient Greeks greatly revered large penis size, which they believed was a source of strength and courage. </t>
+  </si>
+  <si>
+    <t>There were proctologists in ancient Egypt who were called, neru phuyt, which literally translates to 'shepherd of the anus'</t>
+  </si>
+  <si>
+    <t>Weird Stuff About the Ancient World</t>
+  </si>
+  <si>
+    <t>Homo naledi</t>
+  </si>
+  <si>
+    <t>So far specimens have been found from at least 18 individuals, and researchers expect the cave contain many more specimens.</t>
+  </si>
+  <si>
+    <t>Evidence suggests that the naledi bones were likely brought to the cave by predators. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Although the naledi specimens share primitive traits with Australopithecines millions of years old, the remains have been dated to between 335 and 236 thousand years ago. </t>
+  </si>
+  <si>
+    <t>New research finds that being bilingual increases one’s ability to estimate the subjective passage of time</t>
+  </si>
+  <si>
+    <t>In a recent large study, social smokers had as much of an increase in cardiovascular risk factors as daily smokers.</t>
+  </si>
+  <si>
+    <t>Scientists report in a recent study that honey bee hives are healthier in the presence of traditional agriculture compared to non-agricultural areas.</t>
   </si>
 </sst>
 </file>
@@ -487,7 +544,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -564,9 +620,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -584,9 +638,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:numFmt formatCode="0%" sourceLinked="0"/>
@@ -628,7 +680,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -683,16 +734,16 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.5</c:v>
+                  <c:v>0.57894736842105265</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.69230769230769229</c:v>
+                  <c:v>0.61111111111111116</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.6428571428571429</c:v>
+                  <c:v>0.63157894736842102</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.6428571428571429</c:v>
+                  <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -701,7 +752,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.59649122807017541</c:v>
+                  <c:v>0.60526315789473684</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -717,8 +768,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="327145408"/>
-        <c:axId val="327149888"/>
+        <c:axId val="245594112"/>
+        <c:axId val="245594504"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -800,16 +851,16 @@
                       <c:formatCode>0.0%</c:formatCode>
                       <c:ptCount val="7"/>
                       <c:pt idx="0">
-                        <c:v>0.14285714285714285</c:v>
+                        <c:v>0.4</c:v>
                       </c:pt>
                       <c:pt idx="1">
                         <c:v>0.66666666666666663</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.42857142857142855</c:v>
+                        <c:v>0.5</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0.5714285714285714</c:v>
+                        <c:v>0.66666666666666663</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>0</c:v>
@@ -818,7 +869,7 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>0.41379310344827586</c:v>
+                        <c:v>0.52500000000000002</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -904,16 +955,16 @@
                       <c:formatCode>0.0%</c:formatCode>
                       <c:ptCount val="7"/>
                       <c:pt idx="0">
-                        <c:v>0.8571428571428571</c:v>
+                        <c:v>0.77777777777777779</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.7142857142857143</c:v>
+                        <c:v>0.55555555555555558</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.8571428571428571</c:v>
+                        <c:v>0.77777777777777779</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0.7142857142857143</c:v>
+                        <c:v>0.66666666666666663</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>0</c:v>
@@ -922,7 +973,7 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>0.7857142857142857</c:v>
+                        <c:v>0.69444444444444442</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -975,9 +1026,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -996,9 +1045,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -1040,7 +1087,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1066,16 +1112,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>14</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
@@ -1084,7 +1130,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>57</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1100,11 +1146,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="327154752"/>
-        <c:axId val="327150272"/>
+        <c:axId val="245299512"/>
+        <c:axId val="245594896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="327145408"/>
+        <c:axId val="245594112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1147,7 +1193,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="327149888"/>
+        <c:crossAx val="245594504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1155,7 +1201,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="327149888"/>
+        <c:axId val="245594504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1206,12 +1252,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="327145408"/>
+        <c:crossAx val="245594112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="327150272"/>
+        <c:axId val="245594896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1248,12 +1294,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="327154752"/>
+        <c:crossAx val="245299512"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="327154752"/>
+        <c:axId val="245299512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1262,7 +1308,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="327150272"/>
+        <c:crossAx val="245594896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1322,7 +1368,6 @@
         <c:idx val="1"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1443,7 +1488,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1521,9 +1565,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1541,9 +1583,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:numFmt formatCode="0%" sourceLinked="0"/>
@@ -1585,7 +1625,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1641,16 +1680,16 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.14285714285714285</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.42857142857142855</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5714285714285714</c:v>
+                  <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1659,7 +1698,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.41379310344827586</c:v>
+                  <c:v>0.52500000000000002</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -1676,8 +1715,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="327772344"/>
-        <c:axId val="327776824"/>
+        <c:axId val="245300688"/>
+        <c:axId val="245301080"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -1853,16 +1892,16 @@
                       <c:formatCode>0.0%</c:formatCode>
                       <c:ptCount val="7"/>
                       <c:pt idx="0">
-                        <c:v>0.5</c:v>
+                        <c:v>0.57894736842105265</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.69230769230769229</c:v>
+                        <c:v>0.61111111111111116</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.6428571428571429</c:v>
+                        <c:v>0.63157894736842102</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0.6428571428571429</c:v>
+                        <c:v>0.66666666666666663</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>0</c:v>
@@ -1871,7 +1910,7 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>0.59649122807017541</c:v>
+                        <c:v>0.60526315789473684</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1957,16 +1996,16 @@
                       <c:formatCode>0.0%</c:formatCode>
                       <c:ptCount val="7"/>
                       <c:pt idx="0">
-                        <c:v>0.8571428571428571</c:v>
+                        <c:v>0.77777777777777779</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.7142857142857143</c:v>
+                        <c:v>0.55555555555555558</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.8571428571428571</c:v>
+                        <c:v>0.77777777777777779</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0.7142857142857143</c:v>
+                        <c:v>0.66666666666666663</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>0</c:v>
@@ -1975,7 +2014,7 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>0.7857142857142857</c:v>
+                        <c:v>0.69444444444444442</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2120,16 +2159,16 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="7"/>
                       <c:pt idx="0">
-                        <c:v>14</c:v>
+                        <c:v>19</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>13</c:v>
+                        <c:v>18</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>14</c:v>
+                        <c:v>19</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>14</c:v>
+                        <c:v>18</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>1</c:v>
@@ -2138,7 +2177,7 @@
                         <c:v>1</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>57</c:v>
+                        <c:v>76</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2189,16 +2228,16 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="7"/>
                       <c:pt idx="0">
-                        <c:v>7</c:v>
+                        <c:v>9</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>7</c:v>
+                        <c:v>9</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>7</c:v>
+                        <c:v>9</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>7</c:v>
+                        <c:v>9</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>0</c:v>
@@ -2207,7 +2246,7 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>28</c:v>
+                        <c:v>36</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2283,7 +2322,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2309,16 +2347,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
@@ -2327,7 +2365,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>29</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2343,11 +2381,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="327777592"/>
-        <c:axId val="327777208"/>
+        <c:axId val="244187472"/>
+        <c:axId val="244187080"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="327772344"/>
+        <c:axId val="245300688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2390,7 +2428,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="327776824"/>
+        <c:crossAx val="245301080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2398,7 +2436,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="327776824"/>
+        <c:axId val="245301080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2449,12 +2487,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="327772344"/>
+        <c:crossAx val="245300688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="327777208"/>
+        <c:axId val="244187080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2491,12 +2529,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="327777592"/>
+        <c:crossAx val="244187472"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="327777592"/>
+        <c:axId val="244187472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2505,7 +2543,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="327777208"/>
+        <c:crossAx val="244187080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2565,7 +2603,6 @@
         <c:idx val="1"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2686,7 +2723,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2764,9 +2800,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -2784,9 +2818,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:numFmt formatCode="0%" sourceLinked="0"/>
@@ -2828,7 +2860,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2884,16 +2915,16 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.8571428571428571</c:v>
+                  <c:v>0.77777777777777779</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.7142857142857143</c:v>
+                  <c:v>0.55555555555555558</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.8571428571428571</c:v>
+                  <c:v>0.77777777777777779</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.7142857142857143</c:v>
+                  <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2902,7 +2933,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.7857142857142857</c:v>
+                  <c:v>0.69444444444444442</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -2919,8 +2950,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="328044312"/>
-        <c:axId val="106416152"/>
+        <c:axId val="244188648"/>
+        <c:axId val="246291448"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -3096,16 +3127,16 @@
                       <c:formatCode>0.0%</c:formatCode>
                       <c:ptCount val="7"/>
                       <c:pt idx="0">
-                        <c:v>0.5</c:v>
+                        <c:v>0.57894736842105265</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.69230769230769229</c:v>
+                        <c:v>0.61111111111111116</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.6428571428571429</c:v>
+                        <c:v>0.63157894736842102</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0.6428571428571429</c:v>
+                        <c:v>0.66666666666666663</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>0</c:v>
@@ -3114,7 +3145,7 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>0.59649122807017541</c:v>
+                        <c:v>0.60526315789473684</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3294,16 +3325,16 @@
                       <c:formatCode>0.0%</c:formatCode>
                       <c:ptCount val="7"/>
                       <c:pt idx="0">
-                        <c:v>0.14285714285714285</c:v>
+                        <c:v>0.4</c:v>
                       </c:pt>
                       <c:pt idx="1">
                         <c:v>0.66666666666666663</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.42857142857142855</c:v>
+                        <c:v>0.5</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0.5714285714285714</c:v>
+                        <c:v>0.66666666666666663</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>0</c:v>
@@ -3312,7 +3343,7 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>0.41379310344827586</c:v>
+                        <c:v>0.52500000000000002</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3457,16 +3488,16 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="7"/>
                       <c:pt idx="0">
-                        <c:v>14</c:v>
+                        <c:v>19</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>13</c:v>
+                        <c:v>18</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>14</c:v>
+                        <c:v>19</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>14</c:v>
+                        <c:v>18</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>1</c:v>
@@ -3475,7 +3506,7 @@
                         <c:v>1</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>57</c:v>
+                        <c:v>76</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3582,16 +3613,16 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="7"/>
                       <c:pt idx="0">
-                        <c:v>7</c:v>
+                        <c:v>10</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>6</c:v>
+                        <c:v>9</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>7</c:v>
+                        <c:v>10</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>7</c:v>
+                        <c:v>9</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>1</c:v>
@@ -3600,7 +3631,7 @@
                         <c:v>1</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>29</c:v>
+                        <c:v>40</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3677,7 +3708,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3703,16 +3733,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -3721,7 +3751,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -3738,11 +3768,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="106416936"/>
-        <c:axId val="106416544"/>
+        <c:axId val="246292232"/>
+        <c:axId val="246291840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="328044312"/>
+        <c:axId val="244188648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3785,7 +3815,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="106416152"/>
+        <c:crossAx val="246291448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3793,7 +3823,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106416152"/>
+        <c:axId val="246291448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3844,12 +3874,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="328044312"/>
+        <c:crossAx val="244188648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="106416544"/>
+        <c:axId val="246291840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3888,12 +3918,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="106416936"/>
+        <c:crossAx val="246292232"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="106416936"/>
+        <c:axId val="246292232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3902,7 +3932,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106416544"/>
+        <c:crossAx val="246291840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3962,7 +3992,6 @@
         <c:idx val="1"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6024,8 +6053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6787,51 +6816,258 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
+      <c r="A16">
+        <v>614</v>
+      </c>
+      <c r="B16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" t="s">
+        <v>91</v>
+      </c>
+      <c r="F16" t="s">
+        <v>92</v>
+      </c>
+      <c r="G16" s="1">
+        <v>1</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J16" s="1">
+        <v>1</v>
+      </c>
+      <c r="K16" s="1">
+        <v>2</v>
+      </c>
+      <c r="L16" s="1">
+        <v>1</v>
+      </c>
+      <c r="M16" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N16" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O16" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
     </row>
-    <row r="17" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>615</v>
+      </c>
+      <c r="B17" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C17" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E17" t="s">
+        <v>95</v>
+      </c>
+      <c r="F17" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G17" s="1">
+        <v>3</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J17" s="1">
+        <v>3</v>
+      </c>
+      <c r="K17" s="1">
+        <v>1</v>
+      </c>
+      <c r="L17" s="1">
+        <v>1</v>
+      </c>
+      <c r="M17" s="1">
+        <v>1</v>
+      </c>
+      <c r="N17" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O17" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
     </row>
-    <row r="18" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>616</v>
+      </c>
+      <c r="B18" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D18" t="s">
+        <v>97</v>
+      </c>
+      <c r="E18" t="s">
+        <v>98</v>
+      </c>
+      <c r="F18" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G18" s="1">
+        <v>2</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J18" s="1">
+        <v>2</v>
+      </c>
+      <c r="K18" s="1">
+        <v>2</v>
+      </c>
+      <c r="L18" s="1">
+        <v>2</v>
+      </c>
+      <c r="M18" s="1">
+        <v>2</v>
+      </c>
+      <c r="N18" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O18" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
     </row>
-    <row r="19" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>617</v>
+      </c>
+      <c r="B19" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D19" t="s">
+        <v>105</v>
+      </c>
+      <c r="E19" t="s">
+        <v>106</v>
+      </c>
+      <c r="F19" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G19" s="1">
+        <v>1</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J19" s="1">
+        <v>3</v>
+      </c>
+      <c r="K19" s="1">
+        <v>3</v>
+      </c>
+      <c r="L19" s="1">
+        <v>1</v>
+      </c>
+      <c r="M19" s="1">
+        <v>1</v>
+      </c>
+      <c r="N19" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O19" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
     </row>
-    <row r="20" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>618</v>
+      </c>
+      <c r="B20" t="s">
+        <v>100</v>
+      </c>
+      <c r="C20" t="s">
+        <v>101</v>
+      </c>
+      <c r="D20" t="s">
+        <v>102</v>
+      </c>
+      <c r="E20" t="s">
+        <v>103</v>
+      </c>
+      <c r="F20" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G20" s="1">
+        <v>2</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J20" s="1">
+        <v>2</v>
+      </c>
+      <c r="K20" s="1">
+        <v>2</v>
+      </c>
+      <c r="L20" s="1">
+        <v>1</v>
+      </c>
+      <c r="M20" s="1">
+        <v>2</v>
+      </c>
+      <c r="N20" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O20" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
     </row>
-    <row r="21" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -6840,7 +7076,7 @@
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
     </row>
-    <row r="22" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -6849,7 +7085,7 @@
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
     </row>
-    <row r="23" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
@@ -6858,7 +7094,7 @@
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
     </row>
-    <row r="24" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
@@ -6867,7 +7103,7 @@
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
     </row>
-    <row r="25" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -6876,7 +7112,7 @@
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
     </row>
-    <row r="26" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
@@ -6885,7 +7121,7 @@
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
     </row>
-    <row r="27" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
@@ -6894,7 +7130,7 @@
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
     </row>
-    <row r="28" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
@@ -6903,7 +7139,7 @@
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
     </row>
-    <row r="29" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
@@ -6912,7 +7148,7 @@
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
     </row>
-    <row r="30" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
@@ -6921,7 +7157,7 @@
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
     </row>
-    <row r="31" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
@@ -6930,7 +7166,7 @@
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
     </row>
-    <row r="32" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
@@ -7136,10 +7372,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA16"/>
+  <dimension ref="A1:AA21"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:AA16"/>
+      <selection activeCell="A21" sqref="A21:AA21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8799,6 +9035,556 @@
       </c>
       <c r="AA16" s="10">
         <f t="shared" ref="AA16" si="184">IF(ISNA(J16),AA15,IF(J16=0,AA15+1,0))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <f>Data!A16</f>
+        <v>614</v>
+      </c>
+      <c r="B17" s="4" t="str">
+        <f>Data!B16</f>
+        <v>What's Bigger</v>
+      </c>
+      <c r="C17" s="5" t="str">
+        <f>Data!H16</f>
+        <v>Steve</v>
+      </c>
+      <c r="D17" s="2" t="str">
+        <f>Data!I16</f>
+        <v>Cara</v>
+      </c>
+      <c r="E17" s="1">
+        <f>IF(Data!J16=Data!$G16,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F17" s="1">
+        <f>IF(Data!K16=Data!$G16,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <f>IF(Data!L16=Data!$G16,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H17" s="1" t="e">
+        <f>IF(Data!M16=Data!$G16,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I17" s="1" t="e">
+        <f>IF(Data!N16=Data!$G16,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J17" s="1" t="e">
+        <f>IF(Data!O16=Data!$G16,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K17" s="1">
+        <f t="shared" ref="K17" si="185">COUNTIF(E17:J17,"&lt;&gt;#N/A")</f>
+        <v>3</v>
+      </c>
+      <c r="L17" s="1">
+        <f t="shared" ref="L17" si="186">SUMIF(E17:J17,"&lt;&gt;#N/A")</f>
+        <v>2</v>
+      </c>
+      <c r="M17" s="1">
+        <f t="shared" ref="M17" si="187">IF(SUMIF(E17:J17,"&lt;&gt;#N/A")=0, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="N17" s="1">
+        <f t="shared" ref="N17" si="188">IF(K17=L17,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O17" s="1" t="e">
+        <f t="shared" ref="O17" si="189">IF(L17=1,INDEX($E$2:$J$2,1,MATCH(1,E17:J17,0)),NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P17" s="8">
+        <f t="shared" ref="P17" si="190">IF(ISNA(E17),P16,IF(E17=1,P16+1,0))</f>
+        <v>2</v>
+      </c>
+      <c r="Q17" s="8">
+        <f t="shared" ref="Q17" si="191">IF(ISNA(F17),Q16,IF(F17=1,Q16+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="R17" s="8">
+        <f t="shared" ref="R17" si="192">IF(ISNA(G17),R16,IF(G17=1,R16+1,0))</f>
+        <v>2</v>
+      </c>
+      <c r="S17" s="8">
+        <f t="shared" ref="S17" si="193">IF(ISNA(H17),S16,IF(H17=1,S16+1,0))</f>
+        <v>2</v>
+      </c>
+      <c r="T17" s="8">
+        <f t="shared" ref="T17" si="194">IF(ISNA(I17),T16,IF(I17=1,T16+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="U17" s="8">
+        <f t="shared" ref="U17" si="195">IF(ISNA(J17),U16,IF(J17=1,U16+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="V17" s="10">
+        <f t="shared" ref="V17" si="196">IF(ISNA(E17),V16,IF(E17=0,V16+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="W17" s="10">
+        <f t="shared" ref="W17" si="197">IF(ISNA(F17),W16,IF(F17=0,W16+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="X17" s="10">
+        <f t="shared" ref="X17" si="198">IF(ISNA(G17),X16,IF(G17=0,X16+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="Y17" s="10">
+        <f t="shared" ref="Y17" si="199">IF(ISNA(H17),Y16,IF(H17=0,Y16+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="Z17" s="10">
+        <f t="shared" ref="Z17" si="200">IF(ISNA(I17),Z16,IF(I17=0,Z16+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AA17" s="10">
+        <f t="shared" ref="AA17" si="201">IF(ISNA(J17),AA16,IF(J17=0,AA16+1,0))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <f>Data!A17</f>
+        <v>615</v>
+      </c>
+      <c r="B18" s="4" t="e">
+        <f>Data!B17</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C18" s="5" t="str">
+        <f>Data!H17</f>
+        <v>Steve</v>
+      </c>
+      <c r="D18" s="2" t="str">
+        <f>Data!I17</f>
+        <v>Jay</v>
+      </c>
+      <c r="E18" s="1">
+        <f>IF(Data!J17=Data!$G17,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F18" s="1">
+        <f>IF(Data!K17=Data!$G17,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
+        <f>IF(Data!L17=Data!$G17,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="1">
+        <f>IF(Data!M17=Data!$G17,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="1" t="e">
+        <f>IF(Data!N17=Data!$G17,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J18" s="1" t="e">
+        <f>IF(Data!O17=Data!$G17,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K18" s="1">
+        <f t="shared" ref="K18" si="202">COUNTIF(E18:J18,"&lt;&gt;#N/A")</f>
+        <v>4</v>
+      </c>
+      <c r="L18" s="1">
+        <f t="shared" ref="L18" si="203">SUMIF(E18:J18,"&lt;&gt;#N/A")</f>
+        <v>1</v>
+      </c>
+      <c r="M18" s="1">
+        <f t="shared" ref="M18" si="204">IF(SUMIF(E18:J18,"&lt;&gt;#N/A")=0, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="N18" s="1">
+        <f t="shared" ref="N18" si="205">IF(K18=L18,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O18" s="1" t="str">
+        <f t="shared" ref="O18" si="206">IF(L18=1,INDEX($E$2:$J$2,1,MATCH(1,E18:J18,0)),NA())</f>
+        <v>Bob</v>
+      </c>
+      <c r="P18" s="8">
+        <f t="shared" ref="P18" si="207">IF(ISNA(E18),P17,IF(E18=1,P17+1,0))</f>
+        <v>3</v>
+      </c>
+      <c r="Q18" s="8">
+        <f t="shared" ref="Q18" si="208">IF(ISNA(F18),Q17,IF(F18=1,Q17+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="R18" s="8">
+        <f t="shared" ref="R18" si="209">IF(ISNA(G18),R17,IF(G18=1,R17+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="S18" s="8">
+        <f t="shared" ref="S18" si="210">IF(ISNA(H18),S17,IF(H18=1,S17+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="T18" s="8">
+        <f t="shared" ref="T18" si="211">IF(ISNA(I18),T17,IF(I18=1,T17+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="U18" s="8">
+        <f t="shared" ref="U18" si="212">IF(ISNA(J18),U17,IF(J18=1,U17+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="V18" s="10">
+        <f t="shared" ref="V18" si="213">IF(ISNA(E18),V17,IF(E18=0,V17+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="W18" s="10">
+        <f t="shared" ref="W18" si="214">IF(ISNA(F18),W17,IF(F18=0,W17+1,0))</f>
+        <v>2</v>
+      </c>
+      <c r="X18" s="10">
+        <f t="shared" ref="X18" si="215">IF(ISNA(G18),X17,IF(G18=0,X17+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="Y18" s="10">
+        <f t="shared" ref="Y18" si="216">IF(ISNA(H18),Y17,IF(H18=0,Y17+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="Z18" s="10">
+        <f t="shared" ref="Z18" si="217">IF(ISNA(I18),Z17,IF(I18=0,Z17+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AA18" s="10">
+        <f t="shared" ref="AA18" si="218">IF(ISNA(J18),AA17,IF(J18=0,AA17+1,0))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <f>Data!A18</f>
+        <v>616</v>
+      </c>
+      <c r="B19" s="4" t="str">
+        <f>Data!B18</f>
+        <v>Weird Stuff About the Ancient World</v>
+      </c>
+      <c r="C19" s="5" t="str">
+        <f>Data!H18</f>
+        <v>Steve</v>
+      </c>
+      <c r="D19" s="2" t="str">
+        <f>Data!I18</f>
+        <v>Jay</v>
+      </c>
+      <c r="E19" s="1">
+        <f>IF(Data!J18=Data!$G18,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F19" s="1">
+        <f>IF(Data!K18=Data!$G18,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G19" s="1">
+        <f>IF(Data!L18=Data!$G18,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H19" s="1">
+        <f>IF(Data!M18=Data!$G18,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="I19" s="1" t="e">
+        <f>IF(Data!N18=Data!$G18,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J19" s="1" t="e">
+        <f>IF(Data!O18=Data!$G18,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K19" s="1">
+        <f t="shared" ref="K19" si="219">COUNTIF(E19:J19,"&lt;&gt;#N/A")</f>
+        <v>4</v>
+      </c>
+      <c r="L19" s="1">
+        <f t="shared" ref="L19" si="220">SUMIF(E19:J19,"&lt;&gt;#N/A")</f>
+        <v>4</v>
+      </c>
+      <c r="M19" s="1">
+        <f t="shared" ref="M19" si="221">IF(SUMIF(E19:J19,"&lt;&gt;#N/A")=0, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="N19" s="1">
+        <f t="shared" ref="N19" si="222">IF(K19=L19,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O19" s="1" t="e">
+        <f t="shared" ref="O19" si="223">IF(L19=1,INDEX($E$2:$J$2,1,MATCH(1,E19:J19,0)),NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P19" s="8">
+        <f t="shared" ref="P19" si="224">IF(ISNA(E19),P18,IF(E19=1,P18+1,0))</f>
+        <v>4</v>
+      </c>
+      <c r="Q19" s="8">
+        <f t="shared" ref="Q19" si="225">IF(ISNA(F19),Q18,IF(F19=1,Q18+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="R19" s="8">
+        <f t="shared" ref="R19" si="226">IF(ISNA(G19),R18,IF(G19=1,R18+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="S19" s="8">
+        <f t="shared" ref="S19" si="227">IF(ISNA(H19),S18,IF(H19=1,S18+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="T19" s="8">
+        <f t="shared" ref="T19" si="228">IF(ISNA(I19),T18,IF(I19=1,T18+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="U19" s="8">
+        <f t="shared" ref="U19" si="229">IF(ISNA(J19),U18,IF(J19=1,U18+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="V19" s="10">
+        <f t="shared" ref="V19" si="230">IF(ISNA(E19),V18,IF(E19=0,V18+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="W19" s="10">
+        <f t="shared" ref="W19" si="231">IF(ISNA(F19),W18,IF(F19=0,W18+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="X19" s="10">
+        <f t="shared" ref="X19" si="232">IF(ISNA(G19),X18,IF(G19=0,X18+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="Y19" s="10">
+        <f t="shared" ref="Y19" si="233">IF(ISNA(H19),Y18,IF(H19=0,Y18+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="Z19" s="10">
+        <f t="shared" ref="Z19" si="234">IF(ISNA(I19),Z18,IF(I19=0,Z18+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AA19" s="10">
+        <f t="shared" ref="AA19" si="235">IF(ISNA(J19),AA18,IF(J19=0,AA18+1,0))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <f>Data!A19</f>
+        <v>617</v>
+      </c>
+      <c r="B20" s="4" t="e">
+        <f>Data!B19</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C20" s="5" t="str">
+        <f>Data!H19</f>
+        <v>Steve</v>
+      </c>
+      <c r="D20" s="2" t="str">
+        <f>Data!I19</f>
+        <v>Cara</v>
+      </c>
+      <c r="E20" s="1">
+        <f>IF(Data!J19=Data!$G19,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="1">
+        <f>IF(Data!K19=Data!$G19,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G20" s="1">
+        <f>IF(Data!L19=Data!$G19,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H20" s="1">
+        <f>IF(Data!M19=Data!$G19,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="I20" s="1" t="e">
+        <f>IF(Data!N19=Data!$G19,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J20" s="1" t="e">
+        <f>IF(Data!O19=Data!$G19,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K20" s="1">
+        <f t="shared" ref="K20" si="236">COUNTIF(E20:J20,"&lt;&gt;#N/A")</f>
+        <v>4</v>
+      </c>
+      <c r="L20" s="1">
+        <f t="shared" ref="L20" si="237">SUMIF(E20:J20,"&lt;&gt;#N/A")</f>
+        <v>2</v>
+      </c>
+      <c r="M20" s="1">
+        <f t="shared" ref="M20" si="238">IF(SUMIF(E20:J20,"&lt;&gt;#N/A")=0, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="N20" s="1">
+        <f t="shared" ref="N20" si="239">IF(K20=L20,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O20" s="1" t="e">
+        <f t="shared" ref="O20" si="240">IF(L20=1,INDEX($E$2:$J$2,1,MATCH(1,E20:J20,0)),NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P20" s="8">
+        <f t="shared" ref="P20" si="241">IF(ISNA(E20),P19,IF(E20=1,P19+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="Q20" s="8">
+        <f t="shared" ref="Q20" si="242">IF(ISNA(F20),Q19,IF(F20=1,Q19+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="R20" s="8">
+        <f t="shared" ref="R20" si="243">IF(ISNA(G20),R19,IF(G20=1,R19+1,0))</f>
+        <v>2</v>
+      </c>
+      <c r="S20" s="8">
+        <f t="shared" ref="S20" si="244">IF(ISNA(H20),S19,IF(H20=1,S19+1,0))</f>
+        <v>2</v>
+      </c>
+      <c r="T20" s="8">
+        <f t="shared" ref="T20" si="245">IF(ISNA(I20),T19,IF(I20=1,T19+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="U20" s="8">
+        <f t="shared" ref="U20" si="246">IF(ISNA(J20),U19,IF(J20=1,U19+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="V20" s="10">
+        <f t="shared" ref="V20" si="247">IF(ISNA(E20),V19,IF(E20=0,V19+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="W20" s="10">
+        <f t="shared" ref="W20" si="248">IF(ISNA(F20),W19,IF(F20=0,W19+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="X20" s="10">
+        <f t="shared" ref="X20" si="249">IF(ISNA(G20),X19,IF(G20=0,X19+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="Y20" s="10">
+        <f t="shared" ref="Y20" si="250">IF(ISNA(H20),Y19,IF(H20=0,Y19+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="Z20" s="10">
+        <f t="shared" ref="Z20" si="251">IF(ISNA(I20),Z19,IF(I20=0,Z19+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AA20" s="10">
+        <f t="shared" ref="AA20" si="252">IF(ISNA(J20),AA19,IF(J20=0,AA19+1,0))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <f>Data!A20</f>
+        <v>618</v>
+      </c>
+      <c r="B21" s="4" t="str">
+        <f>Data!B20</f>
+        <v>Homo naledi</v>
+      </c>
+      <c r="C21" s="5" t="str">
+        <f>Data!H20</f>
+        <v>Steve</v>
+      </c>
+      <c r="D21" s="2" t="str">
+        <f>Data!I20</f>
+        <v>Jay</v>
+      </c>
+      <c r="E21" s="1">
+        <f>IF(Data!J20=Data!$G20,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F21" s="1">
+        <f>IF(Data!K20=Data!$G20,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G21" s="1">
+        <f>IF(Data!L20=Data!$G20,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="1">
+        <f>IF(Data!M20=Data!$G20,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="I21" s="1" t="e">
+        <f>IF(Data!N20=Data!$G20,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J21" s="1" t="e">
+        <f>IF(Data!O20=Data!$G20,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K21" s="1">
+        <f t="shared" ref="K21" si="253">COUNTIF(E21:J21,"&lt;&gt;#N/A")</f>
+        <v>4</v>
+      </c>
+      <c r="L21" s="1">
+        <f t="shared" ref="L21" si="254">SUMIF(E21:J21,"&lt;&gt;#N/A")</f>
+        <v>3</v>
+      </c>
+      <c r="M21" s="1">
+        <f t="shared" ref="M21" si="255">IF(SUMIF(E21:J21,"&lt;&gt;#N/A")=0, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="N21" s="1">
+        <f t="shared" ref="N21" si="256">IF(K21=L21,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O21" s="1" t="e">
+        <f t="shared" ref="O21" si="257">IF(L21=1,INDEX($E$2:$J$2,1,MATCH(1,E21:J21,0)),NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P21" s="8">
+        <f t="shared" ref="P21" si="258">IF(ISNA(E21),P20,IF(E21=1,P20+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="Q21" s="8">
+        <f t="shared" ref="Q21" si="259">IF(ISNA(F21),Q20,IF(F21=1,Q20+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="R21" s="8">
+        <f t="shared" ref="R21" si="260">IF(ISNA(G21),R20,IF(G21=1,R20+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="S21" s="8">
+        <f t="shared" ref="S21" si="261">IF(ISNA(H21),S20,IF(H21=1,S20+1,0))</f>
+        <v>3</v>
+      </c>
+      <c r="T21" s="8">
+        <f t="shared" ref="T21" si="262">IF(ISNA(I21),T20,IF(I21=1,T20+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="U21" s="8">
+        <f t="shared" ref="U21" si="263">IF(ISNA(J21),U20,IF(J21=1,U20+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="V21" s="10">
+        <f t="shared" ref="V21" si="264">IF(ISNA(E21),V20,IF(E21=0,V20+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="W21" s="10">
+        <f t="shared" ref="W21" si="265">IF(ISNA(F21),W20,IF(F21=0,W20+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="X21" s="10">
+        <f t="shared" ref="X21" si="266">IF(ISNA(G21),X20,IF(G21=0,X20+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="Y21" s="10">
+        <f t="shared" ref="Y21" si="267">IF(ISNA(H21),Y20,IF(H21=0,Y20+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="Z21" s="10">
+        <f t="shared" ref="Z21" si="268">IF(ISNA(I21),Z20,IF(I21=0,Z20+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AA21" s="10">
+        <f t="shared" ref="AA21" si="269">IF(ISNA(J21),AA20,IF(J21=0,AA20+1,0))</f>
         <v>1</v>
       </c>
     </row>
@@ -8860,19 +9646,19 @@
       </c>
       <c r="B2" s="6">
         <f>SUMIF(Results!E3:E53,"&lt;&gt;#N/A")/COUNTIFS(Results!E3:E53,"&lt;&gt;#N/A",Results!E3:E53,"&lt;&gt;")</f>
-        <v>0.5</v>
+        <v>0.57894736842105265</v>
       </c>
       <c r="C2" s="6">
         <f>SUMIF(Results!F3:F53,"&lt;&gt;#N/A")/COUNTIFS(Results!F3:F53,"&lt;&gt;#N/A",Results!F3:F53,"&lt;&gt;")</f>
-        <v>0.69230769230769229</v>
+        <v>0.61111111111111116</v>
       </c>
       <c r="D2" s="6">
         <f>SUMIF(Results!G3:G53,"&lt;&gt;#N/A")/COUNTIFS(Results!G3:G53,"&lt;&gt;#N/A",Results!G3:G53,"&lt;&gt;")</f>
-        <v>0.6428571428571429</v>
+        <v>0.63157894736842102</v>
       </c>
       <c r="E2" s="6">
         <f>SUMIF(Results!H3:H53,"&lt;&gt;#N/A")/COUNTIFS(Results!H3:H53,"&lt;&gt;#N/A",Results!H3:H53,"&lt;&gt;")</f>
-        <v>0.6428571428571429</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F2" s="6">
         <f>SUMIF(Results!I3:I53,"&lt;&gt;#N/A")/COUNTIFS(Results!I3:I53,"&lt;&gt;#N/A",Results!I3:I53,"&lt;&gt;")</f>
@@ -8884,7 +9670,7 @@
       </c>
       <c r="H2" s="6">
         <f>SUM(Results!L3:L53)/SUM(Results!K3:K53)</f>
-        <v>0.59649122807017541</v>
+        <v>0.60526315789473684</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -8893,7 +9679,7 @@
       </c>
       <c r="B3" s="6">
         <f>SUMIFS(Results!E3:E53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!E3:E53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!E3:E53, "&lt;&gt;#N/A", Results!E3:E53, "&lt;&gt;")</f>
-        <v>0.14285714285714285</v>
+        <v>0.4</v>
       </c>
       <c r="C3" s="6">
         <f>SUMIFS(Results!F3:F53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!F3:F53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!F3:F53, "&lt;&gt;#N/A", Results!F3:F53, "&lt;&gt;")</f>
@@ -8901,11 +9687,11 @@
       </c>
       <c r="D3" s="6">
         <f>SUMIFS(Results!G3:G53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!G3:G53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!G3:G53, "&lt;&gt;#N/A", Results!G3:G53, "&lt;&gt;")</f>
-        <v>0.42857142857142855</v>
+        <v>0.5</v>
       </c>
       <c r="E3" s="6">
         <f>SUMIFS(Results!H3:H53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!H3:H53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!H3:H53, "&lt;&gt;#N/A", Results!H3:H53, "&lt;&gt;")</f>
-        <v>0.5714285714285714</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F3" s="6">
         <f>SUMIFS(Results!I3:I53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!I3:I53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!I3:I53, "&lt;&gt;#N/A", Results!I3:I53, "&lt;&gt;")</f>
@@ -8917,7 +9703,7 @@
       </c>
       <c r="H3" s="6">
         <f>SUMIF(Results!B3:B53,"&lt;&gt;#N/A",Results!L3:L53)/SUMIF(Results!B3:B53,"&lt;&gt;#N/A",Results!K3:K53)</f>
-        <v>0.41379310344827586</v>
+        <v>0.52500000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -8926,19 +9712,19 @@
       </c>
       <c r="B4" s="6">
         <f>SUMIFS(Results!E3:E53,Results!$B$3:$B$53,"=#N/A",Results!E3:E53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!E3:E53, "&lt;&gt;#N/A", Results!E3:E53, "&lt;&gt;")</f>
-        <v>0.8571428571428571</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="C4" s="6">
         <f>SUMIFS(Results!F3:F53,Results!$B$3:$B$53,"=#N/A",Results!F3:F53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!F3:F53, "&lt;&gt;#N/A", Results!F3:F53, "&lt;&gt;")</f>
-        <v>0.7142857142857143</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="D4" s="6">
         <f>SUMIFS(Results!G3:G53,Results!$B$3:$B$53,"=#N/A",Results!G3:G53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!G3:G53, "&lt;&gt;#N/A", Results!G3:G53, "&lt;&gt;")</f>
-        <v>0.8571428571428571</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="E4" s="6">
         <f>SUMIFS(Results!H3:H53,Results!$B$3:$B$53,"=#N/A",Results!H3:H53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!H3:H53, "&lt;&gt;#N/A", Results!H3:H53, "&lt;&gt;")</f>
-        <v>0.7142857142857143</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F4" s="6" t="e">
         <f>SUMIFS(Results!I3:I53,Results!$B$3:$B$53,"=#N/A",Results!I3:I53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!I3:I53, "&lt;&gt;#N/A", Results!I3:I53, "&lt;&gt;")</f>
@@ -8950,7 +9736,7 @@
       </c>
       <c r="H4" s="6">
         <f>SUMIF(Results!B3:B53,"=#N/A",Results!L3:L53)/SUMIF(Results!B3:B53,"=#N/A",Results!K3:K53)</f>
-        <v>0.7857142857142857</v>
+        <v>0.69444444444444442</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -8959,7 +9745,7 @@
       </c>
       <c r="B5" s="1">
         <f>MAX(Results!P3:P53)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1">
         <f>MAX(Results!Q3:Q53)</f>
@@ -9025,7 +9811,7 @@
       </c>
       <c r="B7" s="1">
         <f>COUNTIF(Results!$O$3:$O$53,Summary!B1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1">
         <f>COUNTIF(Results!$O$3:$O$53,Summary!C1)</f>
@@ -9049,7 +9835,7 @@
       </c>
       <c r="H7" s="1">
         <f>MAX(B7:G7)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -9062,11 +9848,11 @@
       </c>
       <c r="C8" s="7">
         <f>SUMIF(Results!$D$3:$D$53,C1,Results!$L$3:$L$53)/SUMIF(Results!$D$3:$D$53,C1,Results!$K$3:$K$53)</f>
-        <v>0.58823529411764708</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="D8" s="7">
         <f>SUMIF(Results!$D$3:$D$53,D1,Results!$L$3:$L$53)/SUMIF(Results!$D$3:$D$53,D1,Results!$K$3:$K$53)</f>
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="E8" s="7">
         <f>SUMIF(Results!$D$3:$D$53,E1,Results!$L$3:$L$53)/SUMIF(Results!$D$3:$D$53,E1,Results!$K$3:$K$53)</f>
@@ -9091,19 +9877,19 @@
       </c>
       <c r="B9" s="1">
         <f>SUMIF(Results!E3:E53,"&lt;&gt;#N/A")</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C9" s="1">
         <f>SUMIF(Results!F3:F53,"&lt;&gt;#N/A")</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D9" s="1">
         <f>SUMIF(Results!G3:G53,"&lt;&gt;#N/A")</f>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E9" s="1">
         <f>SUMIF(Results!H3:H53,"&lt;&gt;#N/A")</f>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F9" s="1">
         <f>SUMIF(Results!I3:I53,"&lt;&gt;#N/A")</f>
@@ -9115,7 +9901,7 @@
       </c>
       <c r="H9" s="1">
         <f>SUM(B9:G9)</f>
-        <v>34</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -9124,19 +9910,19 @@
       </c>
       <c r="B10" s="1">
         <f>COUNTIFS(Results!E3:E53,"&lt;&gt;#N/A",Results!E3:E53,"&lt;&gt;")</f>
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C10" s="1">
         <f>COUNTIFS(Results!F3:F53,"&lt;&gt;#N/A",Results!F3:F53,"&lt;&gt;")</f>
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D10" s="1">
         <f>COUNTIFS(Results!G3:G53,"&lt;&gt;#N/A",Results!G3:G53,"&lt;&gt;")</f>
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E10" s="1">
         <f>COUNTIFS(Results!H3:H53,"&lt;&gt;#N/A",Results!H3:H53,"&lt;&gt;")</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F10" s="1">
         <f>COUNTIFS(Results!I3:I53,"&lt;&gt;#N/A",Results!I3:I53,"&lt;&gt;")</f>
@@ -9148,7 +9934,7 @@
       </c>
       <c r="H10" s="1">
         <f t="shared" ref="H10:H14" si="0">SUM(B10:G10)</f>
-        <v>57</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -9157,19 +9943,19 @@
       </c>
       <c r="B11" s="1">
         <f>SUMIFS(Results!E3:E53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!E3:E53, "&lt;&gt;#N/A")</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C11" s="1">
         <f>SUMIFS(Results!F3:F53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!F3:F53, "&lt;&gt;#N/A")</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D11" s="1">
         <f>SUMIFS(Results!G3:G53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!G3:G53, "&lt;&gt;#N/A")</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E11" s="1">
         <f>SUMIFS(Results!H3:H53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!H3:H53, "&lt;&gt;#N/A")</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F11" s="1">
         <f>SUMIFS(Results!I3:I53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!I3:I53, "&lt;&gt;#N/A")</f>
@@ -9181,7 +9967,7 @@
       </c>
       <c r="H11" s="1">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -9190,19 +9976,19 @@
       </c>
       <c r="B12" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!E3:E53, "&lt;&gt;#N/A", Results!E3:E53, "&lt;&gt;")</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C12" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!F3:F53, "&lt;&gt;#N/A", Results!F3:F53, "&lt;&gt;")</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D12" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!G3:G53, "&lt;&gt;#N/A", Results!G3:G53, "&lt;&gt;")</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E12" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!H3:H53, "&lt;&gt;#N/A", Results!H3:H53, "&lt;&gt;")</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F12" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!I3:I53, "&lt;&gt;#N/A", Results!I3:I53, "&lt;&gt;")</f>
@@ -9214,7 +10000,7 @@
       </c>
       <c r="H12" s="1">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -9223,7 +10009,7 @@
       </c>
       <c r="B13" s="1">
         <f>SUMIFS(Results!E3:E53,Results!$B$3:$B$53,"=#N/A",Results!E3:E53, "&lt;&gt;#N/A")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C13" s="1">
         <f>SUMIFS(Results!F3:F53,Results!$B$3:$B$53,"=#N/A",Results!F3:F53, "&lt;&gt;#N/A")</f>
@@ -9231,11 +10017,11 @@
       </c>
       <c r="D13" s="1">
         <f>SUMIFS(Results!G3:G53,Results!$B$3:$B$53,"=#N/A",Results!G3:G53, "&lt;&gt;#N/A")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E13" s="1">
         <f>SUMIFS(Results!H3:H53,Results!$B$3:$B$53,"=#N/A",Results!H3:H53, "&lt;&gt;#N/A")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F13" s="1">
         <f>SUMIFS(Results!I3:I53,Results!$B$3:$B$53,"=#N/A",Results!I3:I53, "&lt;&gt;#N/A")</f>
@@ -9247,7 +10033,7 @@
       </c>
       <c r="H13" s="1">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -9256,19 +10042,19 @@
       </c>
       <c r="B14" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!E3:E53, "&lt;&gt;#N/A", Results!E3:E53, "&lt;&gt;")</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C14" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!F3:F53, "&lt;&gt;#N/A", Results!F3:F53, "&lt;&gt;")</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D14" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!G3:G53, "&lt;&gt;#N/A", Results!G3:G53, "&lt;&gt;")</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E14" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!H3:H53, "&lt;&gt;#N/A", Results!H3:H53, "&lt;&gt;")</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F14" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!I3:I53, "&lt;&gt;#N/A", Results!I3:I53, "&lt;&gt;")</f>
@@ -9280,7 +10066,7 @@
       </c>
       <c r="H14" s="1">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -9322,19 +10108,19 @@
       </c>
       <c r="B16" s="1">
         <f>SUMIF(Results!E3:E53,"&lt;&gt;#N/A",Results!$N$3:$N$53)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C16" s="1">
         <f>SUMIF(Results!F3:F53,"&lt;&gt;#N/A",Results!$N$3:$N$53)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D16" s="1">
         <f>SUMIF(Results!G3:G53,"&lt;&gt;#N/A",Results!$N$3:$N$53)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E16" s="1">
         <f>SUMIF(Results!H3:H53,"&lt;&gt;#N/A",Results!$N$3:$N$53)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F16" s="1">
         <f>SUMIF(Results!I3:I53,"&lt;&gt;#N/A",Results!$N$3:$N$53)</f>
@@ -9346,7 +10132,7 @@
       </c>
       <c r="H16" s="1">
         <f>SUM(Results!N3:N53)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -9359,7 +10145,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="V22" sqref="V22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated through episode 622. Added number of times first to Summary tab
</commit_message>
<xml_diff>
--- a/SGU_Science_or_Fiction.xlsx
+++ b/SGU_Science_or_Fiction.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="123">
   <si>
     <t>Episode</t>
   </si>
@@ -348,6 +348,54 @@
   </si>
   <si>
     <t>Scientists report in a recent study that honey bee hives are healthier in the presence of traditional agriculture compared to non-agricultural areas.</t>
+  </si>
+  <si>
+    <t>Because of their rebellious nature, goats were difficult to domesticate, which likely did not occur until about 3,000 years ago</t>
+  </si>
+  <si>
+    <t>pread the trees.</t>
+  </si>
+  <si>
+    <t>Scientists have found that goats have regional accents, and will change their accent when they move to a new region</t>
+  </si>
+  <si>
+    <t>Goats milk is naturally homogenized, contains less fat and is consumed by more people around the world than cow’s milk</t>
+  </si>
+  <si>
+    <t>Goats</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NASA data finds that terrestrial radio communications push the Van Allen Belts and other high energy radiation away from the Earth, and may be useful as a shield against harmful space weather. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A new study supports the hypothesis that metabolism arose prior to RNA in the origins of life on Earth. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">New evidence suggests that the first mass extinction at the end of the Ordovician was caused by climate change triggered by a massive coronal mass ejection. </t>
+  </si>
+  <si>
+    <t>Trees</t>
+  </si>
+  <si>
+    <t>Scientists have sequenced the genome of mice that have been treated with CRISPR-Cas9 and found over 1,500 unintended mutations.</t>
+  </si>
+  <si>
+    <t>Astronomers have discovered that some large stars may collapse directly into a black hole without ever going supernova, and estimate this happens 10-30% of the time</t>
+  </si>
+  <si>
+    <t>In a new study scientists found that washing your hands with water at 100 degrees F (37 C) killed more than three times as many bacteria as washing in 60 degree (15 C) water.</t>
+  </si>
+  <si>
+    <t>lmost all trees use the less efficient C3 cycle.</t>
+  </si>
+  <si>
+    <t>A 206 acre stand of aspen trees in Utah is actually a single organism weighing 6 million kilograms and estimated to be 80,000 years old.</t>
+  </si>
+  <si>
+    <t>The Dragon’s Blood tree has deep red sap that has been used for centuries as a medicinal and a varnish, and contains a powerful hallucinogen similar in chemistry and effect to LSD.</t>
+  </si>
+  <si>
+    <t>Number of Times Answering First</t>
   </si>
 </sst>
 </file>
@@ -734,16 +782,16 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.57894736842105265</c:v>
+                  <c:v>0.56521739130434778</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.61111111111111116</c:v>
+                  <c:v>0.68181818181818177</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.63157894736842102</c:v>
+                  <c:v>0.65217391304347827</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.66666666666666663</c:v>
+                  <c:v>0.63636363636363635</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -752,7 +800,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.60526315789473684</c:v>
+                  <c:v>0.61956521739130432</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -768,8 +816,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="245594112"/>
-        <c:axId val="245594504"/>
+        <c:axId val="233011688"/>
+        <c:axId val="232552664"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -851,16 +899,16 @@
                       <c:formatCode>0.0%</c:formatCode>
                       <c:ptCount val="7"/>
                       <c:pt idx="0">
-                        <c:v>0.4</c:v>
+                        <c:v>0.41666666666666669</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.66666666666666663</c:v>
+                        <c:v>0.72727272727272729</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.5</c:v>
+                        <c:v>0.58333333333333337</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0.66666666666666663</c:v>
+                        <c:v>0.63636363636363635</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>0</c:v>
@@ -869,7 +917,7 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>0.52500000000000002</c:v>
+                        <c:v>0.5625</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -955,16 +1003,16 @@
                       <c:formatCode>0.0%</c:formatCode>
                       <c:ptCount val="7"/>
                       <c:pt idx="0">
-                        <c:v>0.77777777777777779</c:v>
+                        <c:v>0.72727272727272729</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.55555555555555558</c:v>
+                        <c:v>0.63636363636363635</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.77777777777777779</c:v>
+                        <c:v>0.72727272727272729</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0.66666666666666663</c:v>
+                        <c:v>0.63636363636363635</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>0</c:v>
@@ -973,7 +1021,7 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>0.69444444444444442</c:v>
+                        <c:v>0.68181818181818177</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -992,7 +1040,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Summary!$A$10</c:f>
+              <c:f>Summary!$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1107,21 +1155,21 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Summary!$B$10:$H$10</c:f>
+              <c:f>Summary!$B$11:$H$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>19</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
@@ -1130,7 +1178,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>76</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1146,11 +1194,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="245299512"/>
-        <c:axId val="245594896"/>
+        <c:axId val="136331088"/>
+        <c:axId val="232553056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="245594112"/>
+        <c:axId val="233011688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1193,7 +1241,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245594504"/>
+        <c:crossAx val="232552664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1201,7 +1249,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="245594504"/>
+        <c:axId val="232552664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1252,12 +1300,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245594112"/>
+        <c:crossAx val="233011688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="245594896"/>
+        <c:axId val="232553056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1294,12 +1342,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245299512"/>
+        <c:crossAx val="136331088"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="245299512"/>
+        <c:axId val="136331088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1308,7 +1356,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="245594896"/>
+        <c:crossAx val="232553056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1680,16 +1728,16 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.4</c:v>
+                  <c:v>0.41666666666666669</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.66666666666666663</c:v>
+                  <c:v>0.72727272727272729</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.5</c:v>
+                  <c:v>0.58333333333333337</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.66666666666666663</c:v>
+                  <c:v>0.63636363636363635</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1698,7 +1746,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.52500000000000002</c:v>
+                  <c:v>0.5625</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -1715,8 +1763,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="245300688"/>
-        <c:axId val="245301080"/>
+        <c:axId val="235154632"/>
+        <c:axId val="235155024"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -1892,16 +1940,16 @@
                       <c:formatCode>0.0%</c:formatCode>
                       <c:ptCount val="7"/>
                       <c:pt idx="0">
-                        <c:v>0.57894736842105265</c:v>
+                        <c:v>0.56521739130434778</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.61111111111111116</c:v>
+                        <c:v>0.68181818181818177</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.63157894736842102</c:v>
+                        <c:v>0.65217391304347827</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0.66666666666666663</c:v>
+                        <c:v>0.63636363636363635</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>0</c:v>
@@ -1910,7 +1958,7 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>0.60526315789473684</c:v>
+                        <c:v>0.61956521739130432</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1996,16 +2044,16 @@
                       <c:formatCode>0.0%</c:formatCode>
                       <c:ptCount val="7"/>
                       <c:pt idx="0">
-                        <c:v>0.77777777777777779</c:v>
+                        <c:v>0.72727272727272729</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.55555555555555558</c:v>
+                        <c:v>0.63636363636363635</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.77777777777777779</c:v>
+                        <c:v>0.72727272727272729</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0.66666666666666663</c:v>
+                        <c:v>0.63636363636363635</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>0</c:v>
@@ -2014,7 +2062,7 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>0.69444444444444442</c:v>
+                        <c:v>0.68181818181818177</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2030,7 +2078,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Summary!$A$10</c15:sqref>
+                          <c15:sqref>Summary!$A$11</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -2151,7 +2199,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Summary!$B$10:$H$10</c15:sqref>
+                          <c15:sqref>Summary!$B$11:$H$11</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -2159,16 +2207,16 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="7"/>
                       <c:pt idx="0">
-                        <c:v>19</c:v>
+                        <c:v>23</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>18</c:v>
+                        <c:v>22</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>19</c:v>
+                        <c:v>23</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>18</c:v>
+                        <c:v>22</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>1</c:v>
@@ -2177,7 +2225,7 @@
                         <c:v>1</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>76</c:v>
+                        <c:v>92</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2193,7 +2241,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Summary!$A$14</c15:sqref>
+                          <c15:sqref>Summary!$A$15</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -2220,7 +2268,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Summary!$B$14:$H$14</c15:sqref>
+                          <c15:sqref>Summary!$B$15:$H$15</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -2228,16 +2276,16 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="7"/>
                       <c:pt idx="0">
-                        <c:v>9</c:v>
+                        <c:v>11</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>9</c:v>
+                        <c:v>11</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>9</c:v>
+                        <c:v>11</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>9</c:v>
+                        <c:v>11</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>0</c:v>
@@ -2246,7 +2294,7 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>36</c:v>
+                        <c:v>44</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2265,7 +2313,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Summary!$A$12</c:f>
+              <c:f>Summary!$A$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2342,21 +2390,21 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Summary!$B$12:$H$12</c:f>
+              <c:f>Summary!$B$13:$H$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
@@ -2365,7 +2413,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2381,11 +2429,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="244187472"/>
-        <c:axId val="244187080"/>
+        <c:axId val="235155808"/>
+        <c:axId val="235155416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="245300688"/>
+        <c:axId val="235154632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2428,7 +2476,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245301080"/>
+        <c:crossAx val="235155024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2436,7 +2484,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="245301080"/>
+        <c:axId val="235155024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2487,12 +2535,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245300688"/>
+        <c:crossAx val="235154632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="244187080"/>
+        <c:axId val="235155416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2529,12 +2577,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244187472"/>
+        <c:crossAx val="235155808"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="244187472"/>
+        <c:axId val="235155808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2543,7 +2591,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="244187080"/>
+        <c:crossAx val="235155416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2915,16 +2963,16 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.77777777777777779</c:v>
+                  <c:v>0.72727272727272729</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.55555555555555558</c:v>
+                  <c:v>0.63636363636363635</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.77777777777777779</c:v>
+                  <c:v>0.72727272727272729</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.66666666666666663</c:v>
+                  <c:v>0.63636363636363635</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2933,7 +2981,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.69444444444444442</c:v>
+                  <c:v>0.68181818181818177</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -2950,8 +2998,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="244188648"/>
-        <c:axId val="246291448"/>
+        <c:axId val="235156984"/>
+        <c:axId val="235157376"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -3127,16 +3175,16 @@
                       <c:formatCode>0.0%</c:formatCode>
                       <c:ptCount val="7"/>
                       <c:pt idx="0">
-                        <c:v>0.57894736842105265</c:v>
+                        <c:v>0.56521739130434778</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.61111111111111116</c:v>
+                        <c:v>0.68181818181818177</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.63157894736842102</c:v>
+                        <c:v>0.65217391304347827</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0.66666666666666663</c:v>
+                        <c:v>0.63636363636363635</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>0</c:v>
@@ -3145,7 +3193,7 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>0.60526315789473684</c:v>
+                        <c:v>0.61956521739130432</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3325,16 +3373,16 @@
                       <c:formatCode>0.0%</c:formatCode>
                       <c:ptCount val="7"/>
                       <c:pt idx="0">
-                        <c:v>0.4</c:v>
+                        <c:v>0.41666666666666669</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.66666666666666663</c:v>
+                        <c:v>0.72727272727272729</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.5</c:v>
+                        <c:v>0.58333333333333337</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0.66666666666666663</c:v>
+                        <c:v>0.63636363636363635</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>0</c:v>
@@ -3343,7 +3391,7 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>0.52500000000000002</c:v>
+                        <c:v>0.5625</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3359,7 +3407,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Summary!$A$10</c15:sqref>
+                          <c15:sqref>Summary!$A$11</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -3480,7 +3528,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Summary!$B$10:$H$10</c15:sqref>
+                          <c15:sqref>Summary!$B$11:$H$11</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -3488,16 +3536,16 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="7"/>
                       <c:pt idx="0">
-                        <c:v>19</c:v>
+                        <c:v>23</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>18</c:v>
+                        <c:v>22</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>19</c:v>
+                        <c:v>23</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>18</c:v>
+                        <c:v>22</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>1</c:v>
@@ -3506,7 +3554,7 @@
                         <c:v>1</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>76</c:v>
+                        <c:v>92</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3522,7 +3570,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Summary!$A$12</c15:sqref>
+                          <c15:sqref>Summary!$A$13</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -3605,7 +3653,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Summary!$B$12:$H$12</c15:sqref>
+                          <c15:sqref>Summary!$B$13:$H$13</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -3613,16 +3661,16 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="7"/>
                       <c:pt idx="0">
-                        <c:v>10</c:v>
+                        <c:v>12</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>9</c:v>
+                        <c:v>11</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>10</c:v>
+                        <c:v>12</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>9</c:v>
+                        <c:v>11</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>1</c:v>
@@ -3631,7 +3679,7 @@
                         <c:v>1</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>40</c:v>
+                        <c:v>48</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3650,7 +3698,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Summary!$A$14</c:f>
+              <c:f>Summary!$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3728,21 +3776,21 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Summary!$B$14:$H$14</c:f>
+              <c:f>Summary!$B$15:$H$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -3751,7 +3799,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>36</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -3768,11 +3816,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="246292232"/>
-        <c:axId val="246291840"/>
+        <c:axId val="235158160"/>
+        <c:axId val="235157768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="244188648"/>
+        <c:axId val="235156984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3815,7 +3863,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246291448"/>
+        <c:crossAx val="235157376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3823,7 +3871,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="246291448"/>
+        <c:axId val="235157376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3874,12 +3922,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244188648"/>
+        <c:crossAx val="235156984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="246291840"/>
+        <c:axId val="235157768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3918,12 +3966,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246292232"/>
+        <c:crossAx val="235158160"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="246292232"/>
+        <c:axId val="235158160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3932,7 +3980,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="246291840"/>
+        <c:crossAx val="235157768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6054,7 +6102,7 @@
   <dimension ref="A1:O53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7068,40 +7116,205 @@
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
+      <c r="A21">
+        <v>619</v>
+      </c>
+      <c r="B21" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C21" t="s">
+        <v>112</v>
+      </c>
+      <c r="D21" t="s">
+        <v>113</v>
+      </c>
+      <c r="E21" t="s">
+        <v>114</v>
+      </c>
+      <c r="F21" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G21" s="1">
+        <v>3</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J21" s="1">
+        <v>1</v>
+      </c>
+      <c r="K21" s="1">
+        <v>3</v>
+      </c>
+      <c r="L21" s="1">
+        <v>3</v>
+      </c>
+      <c r="M21" s="1">
+        <v>3</v>
+      </c>
+      <c r="N21" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O21" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
+      <c r="A22">
+        <v>620</v>
+      </c>
+      <c r="B22" t="s">
+        <v>111</v>
+      </c>
+      <c r="C22" t="s">
+        <v>107</v>
+      </c>
+      <c r="D22" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22" t="s">
+        <v>109</v>
+      </c>
+      <c r="F22" t="s">
+        <v>110</v>
+      </c>
+      <c r="G22" s="1">
+        <v>1</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J22" s="1">
+        <v>1</v>
+      </c>
+      <c r="K22" s="1">
+        <v>1</v>
+      </c>
+      <c r="L22" s="1">
+        <v>1</v>
+      </c>
+      <c r="M22" s="1">
+        <v>1</v>
+      </c>
+      <c r="N22" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O22" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
+      <c r="A23">
+        <v>621</v>
+      </c>
+      <c r="B23" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C23" t="s">
+        <v>116</v>
+      </c>
+      <c r="D23" t="s">
+        <v>117</v>
+      </c>
+      <c r="E23" t="s">
+        <v>118</v>
+      </c>
+      <c r="F23" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G23" s="1">
+        <v>3</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J23" s="1">
+        <v>3</v>
+      </c>
+      <c r="K23" s="1">
+        <v>3</v>
+      </c>
+      <c r="L23" s="1">
+        <v>2</v>
+      </c>
+      <c r="M23" s="1">
+        <v>2</v>
+      </c>
+      <c r="N23" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O23" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
+      <c r="A24">
+        <v>622</v>
+      </c>
+      <c r="B24" t="s">
+        <v>115</v>
+      </c>
+      <c r="C24" t="s">
+        <v>119</v>
+      </c>
+      <c r="D24" t="s">
+        <v>120</v>
+      </c>
+      <c r="E24" t="s">
+        <v>121</v>
+      </c>
+      <c r="F24" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G24" s="1">
+        <v>3</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J24" s="1">
+        <v>2</v>
+      </c>
+      <c r="K24" s="1">
+        <v>3</v>
+      </c>
+      <c r="L24" s="1">
+        <v>3</v>
+      </c>
+      <c r="M24" s="1">
+        <v>2</v>
+      </c>
+      <c r="N24" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O24" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G25" s="1"/>
@@ -7372,10 +7585,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA21"/>
+  <dimension ref="A1:AA25"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:AA21"/>
+      <selection activeCell="A24" sqref="A24:AA25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9588,6 +9801,446 @@
         <v>1</v>
       </c>
     </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <f>Data!A21</f>
+        <v>619</v>
+      </c>
+      <c r="B22" s="4" t="e">
+        <f>Data!B21</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C22" s="5" t="str">
+        <f>Data!H21</f>
+        <v>Steve</v>
+      </c>
+      <c r="D22" s="2" t="str">
+        <f>Data!I21</f>
+        <v>Bob</v>
+      </c>
+      <c r="E22" s="1">
+        <f>IF(Data!J21=Data!$G21,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="1">
+        <f>IF(Data!K21=Data!$G21,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G22" s="1">
+        <f>IF(Data!L21=Data!$G21,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H22" s="1">
+        <f>IF(Data!M21=Data!$G21,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="I22" s="1" t="e">
+        <f>IF(Data!N21=Data!$G21,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J22" s="1" t="e">
+        <f>IF(Data!O21=Data!$G21,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K22" s="1">
+        <f t="shared" ref="K22:K23" si="270">COUNTIF(E22:J22,"&lt;&gt;#N/A")</f>
+        <v>4</v>
+      </c>
+      <c r="L22" s="1">
+        <f t="shared" ref="L22:L23" si="271">SUMIF(E22:J22,"&lt;&gt;#N/A")</f>
+        <v>3</v>
+      </c>
+      <c r="M22" s="1">
+        <f t="shared" ref="M22:M23" si="272">IF(SUMIF(E22:J22,"&lt;&gt;#N/A")=0, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="N22" s="1">
+        <f t="shared" ref="N22:N23" si="273">IF(K22=L22,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O22" s="1" t="e">
+        <f t="shared" ref="O22:O23" si="274">IF(L22=1,INDEX($E$2:$J$2,1,MATCH(1,E22:J22,0)),NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P22" s="8">
+        <f t="shared" ref="P22:P23" si="275">IF(ISNA(E22),P21,IF(E22=1,P21+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="Q22" s="8">
+        <f t="shared" ref="Q22:Q23" si="276">IF(ISNA(F22),Q21,IF(F22=1,Q21+1,0))</f>
+        <v>2</v>
+      </c>
+      <c r="R22" s="8">
+        <f t="shared" ref="R22:R23" si="277">IF(ISNA(G22),R21,IF(G22=1,R21+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="S22" s="8">
+        <f t="shared" ref="S22:S23" si="278">IF(ISNA(H22),S21,IF(H22=1,S21+1,0))</f>
+        <v>4</v>
+      </c>
+      <c r="T22" s="8">
+        <f t="shared" ref="T22:T23" si="279">IF(ISNA(I22),T21,IF(I22=1,T21+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="U22" s="8">
+        <f t="shared" ref="U22:U23" si="280">IF(ISNA(J22),U21,IF(J22=1,U21+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="V22" s="10">
+        <f t="shared" ref="V22:V23" si="281">IF(ISNA(E22),V21,IF(E22=0,V21+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="W22" s="10">
+        <f t="shared" ref="W22:W23" si="282">IF(ISNA(F22),W21,IF(F22=0,W21+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="X22" s="10">
+        <f t="shared" ref="X22:X23" si="283">IF(ISNA(G22),X21,IF(G22=0,X21+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="Y22" s="10">
+        <f t="shared" ref="Y22:Y23" si="284">IF(ISNA(H22),Y21,IF(H22=0,Y21+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="Z22" s="10">
+        <f t="shared" ref="Z22:Z23" si="285">IF(ISNA(I22),Z21,IF(I22=0,Z21+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AA22" s="10">
+        <f t="shared" ref="AA22:AA23" si="286">IF(ISNA(J22),AA21,IF(J22=0,AA21+1,0))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <f>Data!A22</f>
+        <v>620</v>
+      </c>
+      <c r="B23" s="4" t="str">
+        <f>Data!B22</f>
+        <v>Goats</v>
+      </c>
+      <c r="C23" s="5" t="str">
+        <f>Data!H22</f>
+        <v>Steve</v>
+      </c>
+      <c r="D23" s="2" t="str">
+        <f>Data!I22</f>
+        <v>Evan</v>
+      </c>
+      <c r="E23" s="1">
+        <f>IF(Data!J22=Data!$G22,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F23" s="1">
+        <f>IF(Data!K22=Data!$G22,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G23" s="1">
+        <f>IF(Data!L22=Data!$G22,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H23" s="1">
+        <f>IF(Data!M22=Data!$G22,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="I23" s="1" t="e">
+        <f>IF(Data!N22=Data!$G22,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J23" s="1" t="e">
+        <f>IF(Data!O22=Data!$G22,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K23" s="1">
+        <f t="shared" si="270"/>
+        <v>4</v>
+      </c>
+      <c r="L23" s="1">
+        <f t="shared" si="271"/>
+        <v>4</v>
+      </c>
+      <c r="M23" s="1">
+        <f t="shared" si="272"/>
+        <v>0</v>
+      </c>
+      <c r="N23" s="1">
+        <f t="shared" si="273"/>
+        <v>1</v>
+      </c>
+      <c r="O23" s="1" t="e">
+        <f t="shared" si="274"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P23" s="8">
+        <f t="shared" si="275"/>
+        <v>1</v>
+      </c>
+      <c r="Q23" s="8">
+        <f t="shared" si="276"/>
+        <v>3</v>
+      </c>
+      <c r="R23" s="8">
+        <f t="shared" si="277"/>
+        <v>2</v>
+      </c>
+      <c r="S23" s="8">
+        <f t="shared" si="278"/>
+        <v>5</v>
+      </c>
+      <c r="T23" s="8">
+        <f t="shared" si="279"/>
+        <v>0</v>
+      </c>
+      <c r="U23" s="8">
+        <f t="shared" si="280"/>
+        <v>0</v>
+      </c>
+      <c r="V23" s="10">
+        <f t="shared" si="281"/>
+        <v>0</v>
+      </c>
+      <c r="W23" s="10">
+        <f t="shared" si="282"/>
+        <v>0</v>
+      </c>
+      <c r="X23" s="10">
+        <f t="shared" si="283"/>
+        <v>0</v>
+      </c>
+      <c r="Y23" s="10">
+        <f t="shared" si="284"/>
+        <v>0</v>
+      </c>
+      <c r="Z23" s="10">
+        <f t="shared" si="285"/>
+        <v>1</v>
+      </c>
+      <c r="AA23" s="10">
+        <f t="shared" si="286"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <f>Data!A23</f>
+        <v>621</v>
+      </c>
+      <c r="B24" s="4" t="e">
+        <f>Data!B23</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C24" s="5" t="str">
+        <f>Data!H23</f>
+        <v>Steve</v>
+      </c>
+      <c r="D24" s="2" t="str">
+        <f>Data!I23</f>
+        <v>Cara</v>
+      </c>
+      <c r="E24" s="1">
+        <f>IF(Data!J23=Data!$G23,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F24" s="1">
+        <f>IF(Data!K23=Data!$G23,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G24" s="1">
+        <f>IF(Data!L23=Data!$G23,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H24" s="1">
+        <f>IF(Data!M23=Data!$G23,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I24" s="1" t="e">
+        <f>IF(Data!N23=Data!$G23,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J24" s="1" t="e">
+        <f>IF(Data!O23=Data!$G23,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K24" s="1">
+        <f t="shared" ref="K24:K25" si="287">COUNTIF(E24:J24,"&lt;&gt;#N/A")</f>
+        <v>4</v>
+      </c>
+      <c r="L24" s="1">
+        <f t="shared" ref="L24:L25" si="288">SUMIF(E24:J24,"&lt;&gt;#N/A")</f>
+        <v>2</v>
+      </c>
+      <c r="M24" s="1">
+        <f t="shared" ref="M24:M25" si="289">IF(SUMIF(E24:J24,"&lt;&gt;#N/A")=0, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="N24" s="1">
+        <f t="shared" ref="N24:N25" si="290">IF(K24=L24,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O24" s="1" t="e">
+        <f t="shared" ref="O24:O25" si="291">IF(L24=1,INDEX($E$2:$J$2,1,MATCH(1,E24:J24,0)),NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P24" s="8">
+        <f t="shared" ref="P24:P25" si="292">IF(ISNA(E24),P23,IF(E24=1,P23+1,0))</f>
+        <v>2</v>
+      </c>
+      <c r="Q24" s="8">
+        <f t="shared" ref="Q24:Q25" si="293">IF(ISNA(F24),Q23,IF(F24=1,Q23+1,0))</f>
+        <v>4</v>
+      </c>
+      <c r="R24" s="8">
+        <f t="shared" ref="R24:R25" si="294">IF(ISNA(G24),R23,IF(G24=1,R23+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="S24" s="8">
+        <f t="shared" ref="S24:S25" si="295">IF(ISNA(H24),S23,IF(H24=1,S23+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="T24" s="8">
+        <f t="shared" ref="T24:T25" si="296">IF(ISNA(I24),T23,IF(I24=1,T23+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="U24" s="8">
+        <f t="shared" ref="U24:U25" si="297">IF(ISNA(J24),U23,IF(J24=1,U23+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="V24" s="10">
+        <f t="shared" ref="V24:V25" si="298">IF(ISNA(E24),V23,IF(E24=0,V23+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="W24" s="10">
+        <f t="shared" ref="W24:W25" si="299">IF(ISNA(F24),W23,IF(F24=0,W23+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="X24" s="10">
+        <f t="shared" ref="X24:X25" si="300">IF(ISNA(G24),X23,IF(G24=0,X23+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="Y24" s="10">
+        <f t="shared" ref="Y24:Y25" si="301">IF(ISNA(H24),Y23,IF(H24=0,Y23+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="Z24" s="10">
+        <f t="shared" ref="Z24:Z25" si="302">IF(ISNA(I24),Z23,IF(I24=0,Z23+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AA24" s="10">
+        <f t="shared" ref="AA24:AA25" si="303">IF(ISNA(J24),AA23,IF(J24=0,AA23+1,0))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <f>Data!A24</f>
+        <v>622</v>
+      </c>
+      <c r="B25" s="4" t="str">
+        <f>Data!B24</f>
+        <v>Trees</v>
+      </c>
+      <c r="C25" s="5" t="str">
+        <f>Data!H24</f>
+        <v>Steve</v>
+      </c>
+      <c r="D25" s="2" t="str">
+        <f>Data!I24</f>
+        <v>Evan</v>
+      </c>
+      <c r="E25" s="1">
+        <f>IF(Data!J24=Data!$G24,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F25" s="1">
+        <f>IF(Data!K24=Data!$G24,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G25" s="1">
+        <f>IF(Data!L24=Data!$G24,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H25" s="1">
+        <f>IF(Data!M24=Data!$G24,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I25" s="1" t="e">
+        <f>IF(Data!N24=Data!$G24,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J25" s="1" t="e">
+        <f>IF(Data!O24=Data!$G24,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K25" s="1">
+        <f t="shared" si="287"/>
+        <v>4</v>
+      </c>
+      <c r="L25" s="1">
+        <f t="shared" si="288"/>
+        <v>2</v>
+      </c>
+      <c r="M25" s="1">
+        <f t="shared" si="289"/>
+        <v>0</v>
+      </c>
+      <c r="N25" s="1">
+        <f t="shared" si="290"/>
+        <v>0</v>
+      </c>
+      <c r="O25" s="1" t="e">
+        <f t="shared" si="291"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P25" s="8">
+        <f t="shared" si="292"/>
+        <v>0</v>
+      </c>
+      <c r="Q25" s="8">
+        <f t="shared" si="293"/>
+        <v>5</v>
+      </c>
+      <c r="R25" s="8">
+        <f t="shared" si="294"/>
+        <v>1</v>
+      </c>
+      <c r="S25" s="8">
+        <f t="shared" si="295"/>
+        <v>0</v>
+      </c>
+      <c r="T25" s="8">
+        <f t="shared" si="296"/>
+        <v>0</v>
+      </c>
+      <c r="U25" s="8">
+        <f t="shared" si="297"/>
+        <v>0</v>
+      </c>
+      <c r="V25" s="10">
+        <f t="shared" si="298"/>
+        <v>1</v>
+      </c>
+      <c r="W25" s="10">
+        <f t="shared" si="299"/>
+        <v>0</v>
+      </c>
+      <c r="X25" s="10">
+        <f t="shared" si="300"/>
+        <v>0</v>
+      </c>
+      <c r="Y25" s="10">
+        <f t="shared" si="301"/>
+        <v>2</v>
+      </c>
+      <c r="Z25" s="10">
+        <f t="shared" si="302"/>
+        <v>1</v>
+      </c>
+      <c r="AA25" s="10">
+        <f t="shared" si="303"/>
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="P1:U1"/>
@@ -9600,10 +10253,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9646,19 +10299,19 @@
       </c>
       <c r="B2" s="6">
         <f>SUMIF(Results!E3:E53,"&lt;&gt;#N/A")/COUNTIFS(Results!E3:E53,"&lt;&gt;#N/A",Results!E3:E53,"&lt;&gt;")</f>
-        <v>0.57894736842105265</v>
+        <v>0.56521739130434778</v>
       </c>
       <c r="C2" s="6">
         <f>SUMIF(Results!F3:F53,"&lt;&gt;#N/A")/COUNTIFS(Results!F3:F53,"&lt;&gt;#N/A",Results!F3:F53,"&lt;&gt;")</f>
-        <v>0.61111111111111116</v>
+        <v>0.68181818181818177</v>
       </c>
       <c r="D2" s="6">
         <f>SUMIF(Results!G3:G53,"&lt;&gt;#N/A")/COUNTIFS(Results!G3:G53,"&lt;&gt;#N/A",Results!G3:G53,"&lt;&gt;")</f>
-        <v>0.63157894736842102</v>
+        <v>0.65217391304347827</v>
       </c>
       <c r="E2" s="6">
         <f>SUMIF(Results!H3:H53,"&lt;&gt;#N/A")/COUNTIFS(Results!H3:H53,"&lt;&gt;#N/A",Results!H3:H53,"&lt;&gt;")</f>
-        <v>0.66666666666666663</v>
+        <v>0.63636363636363635</v>
       </c>
       <c r="F2" s="6">
         <f>SUMIF(Results!I3:I53,"&lt;&gt;#N/A")/COUNTIFS(Results!I3:I53,"&lt;&gt;#N/A",Results!I3:I53,"&lt;&gt;")</f>
@@ -9670,7 +10323,7 @@
       </c>
       <c r="H2" s="6">
         <f>SUM(Results!L3:L53)/SUM(Results!K3:K53)</f>
-        <v>0.60526315789473684</v>
+        <v>0.61956521739130432</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -9679,19 +10332,19 @@
       </c>
       <c r="B3" s="6">
         <f>SUMIFS(Results!E3:E53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!E3:E53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!E3:E53, "&lt;&gt;#N/A", Results!E3:E53, "&lt;&gt;")</f>
-        <v>0.4</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="C3" s="6">
         <f>SUMIFS(Results!F3:F53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!F3:F53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!F3:F53, "&lt;&gt;#N/A", Results!F3:F53, "&lt;&gt;")</f>
-        <v>0.66666666666666663</v>
+        <v>0.72727272727272729</v>
       </c>
       <c r="D3" s="6">
         <f>SUMIFS(Results!G3:G53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!G3:G53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!G3:G53, "&lt;&gt;#N/A", Results!G3:G53, "&lt;&gt;")</f>
-        <v>0.5</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="E3" s="6">
         <f>SUMIFS(Results!H3:H53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!H3:H53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!H3:H53, "&lt;&gt;#N/A", Results!H3:H53, "&lt;&gt;")</f>
-        <v>0.66666666666666663</v>
+        <v>0.63636363636363635</v>
       </c>
       <c r="F3" s="6">
         <f>SUMIFS(Results!I3:I53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!I3:I53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!I3:I53, "&lt;&gt;#N/A", Results!I3:I53, "&lt;&gt;")</f>
@@ -9703,7 +10356,7 @@
       </c>
       <c r="H3" s="6">
         <f>SUMIF(Results!B3:B53,"&lt;&gt;#N/A",Results!L3:L53)/SUMIF(Results!B3:B53,"&lt;&gt;#N/A",Results!K3:K53)</f>
-        <v>0.52500000000000002</v>
+        <v>0.5625</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -9712,19 +10365,19 @@
       </c>
       <c r="B4" s="6">
         <f>SUMIFS(Results!E3:E53,Results!$B$3:$B$53,"=#N/A",Results!E3:E53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!E3:E53, "&lt;&gt;#N/A", Results!E3:E53, "&lt;&gt;")</f>
-        <v>0.77777777777777779</v>
+        <v>0.72727272727272729</v>
       </c>
       <c r="C4" s="6">
         <f>SUMIFS(Results!F3:F53,Results!$B$3:$B$53,"=#N/A",Results!F3:F53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!F3:F53, "&lt;&gt;#N/A", Results!F3:F53, "&lt;&gt;")</f>
-        <v>0.55555555555555558</v>
+        <v>0.63636363636363635</v>
       </c>
       <c r="D4" s="6">
         <f>SUMIFS(Results!G3:G53,Results!$B$3:$B$53,"=#N/A",Results!G3:G53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!G3:G53, "&lt;&gt;#N/A", Results!G3:G53, "&lt;&gt;")</f>
-        <v>0.77777777777777779</v>
+        <v>0.72727272727272729</v>
       </c>
       <c r="E4" s="6">
         <f>SUMIFS(Results!H3:H53,Results!$B$3:$B$53,"=#N/A",Results!H3:H53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!H3:H53, "&lt;&gt;#N/A", Results!H3:H53, "&lt;&gt;")</f>
-        <v>0.66666666666666663</v>
+        <v>0.63636363636363635</v>
       </c>
       <c r="F4" s="6" t="e">
         <f>SUMIFS(Results!I3:I53,Results!$B$3:$B$53,"=#N/A",Results!I3:I53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!I3:I53, "&lt;&gt;#N/A", Results!I3:I53, "&lt;&gt;")</f>
@@ -9736,7 +10389,7 @@
       </c>
       <c r="H4" s="6">
         <f>SUMIF(Results!B3:B53,"=#N/A",Results!L3:L53)/SUMIF(Results!B3:B53,"=#N/A",Results!K3:K53)</f>
-        <v>0.69444444444444442</v>
+        <v>0.68181818181818177</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -9749,7 +10402,7 @@
       </c>
       <c r="C5" s="1">
         <f>MAX(Results!Q3:Q53)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D5" s="1">
         <f>MAX(Results!R3:R53)</f>
@@ -9757,7 +10410,7 @@
       </c>
       <c r="E5" s="1">
         <f>MAX(Results!S3:S53)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F5" s="1">
         <f>MAX(Results!T3:T53)</f>
@@ -9769,7 +10422,7 @@
       </c>
       <c r="H5" s="1">
         <f>MAX(B5:G5)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -9790,7 +10443,7 @@
       </c>
       <c r="E6" s="1">
         <f>MAX(Results!Y3:Y53)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6" s="1">
         <f>MAX(Results!Z3:Z53)</f>
@@ -9844,11 +10497,11 @@
       </c>
       <c r="B8" s="7">
         <f>SUMIF(Results!$D$3:$D$53,B1,Results!$L$3:$L$53)/SUMIF(Results!$D$3:$D$53,B1,Results!$K$3:$K$53)</f>
-        <v>0.6875</v>
+        <v>0.7</v>
       </c>
       <c r="C8" s="7">
         <f>SUMIF(Results!$D$3:$D$53,C1,Results!$L$3:$L$53)/SUMIF(Results!$D$3:$D$53,C1,Results!$K$3:$K$53)</f>
-        <v>0.58333333333333337</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="D8" s="7">
         <f>SUMIF(Results!$D$3:$D$53,D1,Results!$L$3:$L$53)/SUMIF(Results!$D$3:$D$53,D1,Results!$K$3:$K$53)</f>
@@ -9873,266 +10526,299 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>122</v>
       </c>
       <c r="B9" s="1">
-        <f>SUMIF(Results!E3:E53,"&lt;&gt;#N/A")</f>
-        <v>11</v>
+        <f>COUNTIF(Data!$I$2:$I$53,Summary!B1)</f>
+        <v>5</v>
       </c>
       <c r="C9" s="1">
-        <f>SUMIF(Results!F3:F53,"&lt;&gt;#N/A")</f>
-        <v>11</v>
+        <f>COUNTIF(Data!$I$2:$I$53,Summary!C1)</f>
+        <v>7</v>
       </c>
       <c r="D9" s="1">
-        <f>SUMIF(Results!G3:G53,"&lt;&gt;#N/A")</f>
-        <v>12</v>
+        <f>COUNTIF(Data!$I$2:$I$53,Summary!D1)</f>
+        <v>6</v>
       </c>
       <c r="E9" s="1">
-        <f>SUMIF(Results!H3:H53,"&lt;&gt;#N/A")</f>
-        <v>12</v>
+        <f>COUNTIF(Data!$I$2:$I$53,Summary!E1)</f>
+        <v>5</v>
       </c>
       <c r="F9" s="1">
-        <f>SUMIF(Results!I3:I53,"&lt;&gt;#N/A")</f>
+        <f>COUNTIF(Data!$I$2:$I$53,Summary!F1)</f>
         <v>0</v>
       </c>
       <c r="G9" s="1">
-        <f>SUMIF(Results!J3:J53,"&lt;&gt;#N/A")</f>
+        <f>COUNTIF(Data!$I$2:$I$53,Summary!G1)</f>
         <v>0</v>
       </c>
       <c r="H9" s="1">
         <f>SUM(B9:G9)</f>
-        <v>46</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>56</v>
+      <c r="A10" t="s">
+        <v>55</v>
       </c>
       <c r="B10" s="1">
-        <f>COUNTIFS(Results!E3:E53,"&lt;&gt;#N/A",Results!E3:E53,"&lt;&gt;")</f>
-        <v>19</v>
+        <f>SUMIF(Results!E3:E53,"&lt;&gt;#N/A")</f>
+        <v>13</v>
       </c>
       <c r="C10" s="1">
-        <f>COUNTIFS(Results!F3:F53,"&lt;&gt;#N/A",Results!F3:F53,"&lt;&gt;")</f>
-        <v>18</v>
+        <f>SUMIF(Results!F3:F53,"&lt;&gt;#N/A")</f>
+        <v>15</v>
       </c>
       <c r="D10" s="1">
-        <f>COUNTIFS(Results!G3:G53,"&lt;&gt;#N/A",Results!G3:G53,"&lt;&gt;")</f>
-        <v>19</v>
+        <f>SUMIF(Results!G3:G53,"&lt;&gt;#N/A")</f>
+        <v>15</v>
       </c>
       <c r="E10" s="1">
-        <f>COUNTIFS(Results!H3:H53,"&lt;&gt;#N/A",Results!H3:H53,"&lt;&gt;")</f>
-        <v>18</v>
+        <f>SUMIF(Results!H3:H53,"&lt;&gt;#N/A")</f>
+        <v>14</v>
       </c>
       <c r="F10" s="1">
-        <f>COUNTIFS(Results!I3:I53,"&lt;&gt;#N/A",Results!I3:I53,"&lt;&gt;")</f>
-        <v>1</v>
+        <f>SUMIF(Results!I3:I53,"&lt;&gt;#N/A")</f>
+        <v>0</v>
       </c>
       <c r="G10" s="1">
-        <f>COUNTIFS(Results!J3:J53,"&lt;&gt;#N/A",Results!J3:J53,"&lt;&gt;")</f>
-        <v>1</v>
+        <f>SUMIF(Results!J3:J53,"&lt;&gt;#N/A")</f>
+        <v>0</v>
       </c>
       <c r="H10" s="1">
-        <f t="shared" ref="H10:H14" si="0">SUM(B10:G10)</f>
-        <v>76</v>
+        <f>SUM(B10:G10)</f>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B11" s="1">
-        <f>SUMIFS(Results!E3:E53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!E3:E53, "&lt;&gt;#N/A")</f>
-        <v>4</v>
+        <f>COUNTIFS(Results!E3:E53,"&lt;&gt;#N/A",Results!E3:E53,"&lt;&gt;")</f>
+        <v>23</v>
       </c>
       <c r="C11" s="1">
-        <f>SUMIFS(Results!F3:F53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!F3:F53, "&lt;&gt;#N/A")</f>
-        <v>6</v>
+        <f>COUNTIFS(Results!F3:F53,"&lt;&gt;#N/A",Results!F3:F53,"&lt;&gt;")</f>
+        <v>22</v>
       </c>
       <c r="D11" s="1">
-        <f>SUMIFS(Results!G3:G53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!G3:G53, "&lt;&gt;#N/A")</f>
-        <v>5</v>
+        <f>COUNTIFS(Results!G3:G53,"&lt;&gt;#N/A",Results!G3:G53,"&lt;&gt;")</f>
+        <v>23</v>
       </c>
       <c r="E11" s="1">
-        <f>SUMIFS(Results!H3:H53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!H3:H53, "&lt;&gt;#N/A")</f>
-        <v>6</v>
+        <f>COUNTIFS(Results!H3:H53,"&lt;&gt;#N/A",Results!H3:H53,"&lt;&gt;")</f>
+        <v>22</v>
       </c>
       <c r="F11" s="1">
-        <f>SUMIFS(Results!I3:I53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!I3:I53, "&lt;&gt;#N/A")</f>
-        <v>0</v>
+        <f>COUNTIFS(Results!I3:I53,"&lt;&gt;#N/A",Results!I3:I53,"&lt;&gt;")</f>
+        <v>1</v>
       </c>
       <c r="G11" s="1">
-        <f>SUMIFS(Results!J3:J53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!J3:J53, "&lt;&gt;#N/A")</f>
-        <v>0</v>
+        <f>COUNTIFS(Results!J3:J53,"&lt;&gt;#N/A",Results!J3:J53,"&lt;&gt;")</f>
+        <v>1</v>
       </c>
       <c r="H11" s="1">
-        <f t="shared" si="0"/>
-        <v>21</v>
+        <f t="shared" ref="H11:H15" si="0">SUM(B11:G11)</f>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B12" s="1">
-        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!E3:E53, "&lt;&gt;#N/A", Results!E3:E53, "&lt;&gt;")</f>
-        <v>10</v>
+        <f>SUMIFS(Results!E3:E53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!E3:E53, "&lt;&gt;#N/A")</f>
+        <v>5</v>
       </c>
       <c r="C12" s="1">
-        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!F3:F53, "&lt;&gt;#N/A", Results!F3:F53, "&lt;&gt;")</f>
-        <v>9</v>
+        <f>SUMIFS(Results!F3:F53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!F3:F53, "&lt;&gt;#N/A")</f>
+        <v>8</v>
       </c>
       <c r="D12" s="1">
-        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!G3:G53, "&lt;&gt;#N/A", Results!G3:G53, "&lt;&gt;")</f>
-        <v>10</v>
+        <f>SUMIFS(Results!G3:G53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!G3:G53, "&lt;&gt;#N/A")</f>
+        <v>7</v>
       </c>
       <c r="E12" s="1">
-        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!H3:H53, "&lt;&gt;#N/A", Results!H3:H53, "&lt;&gt;")</f>
-        <v>9</v>
+        <f>SUMIFS(Results!H3:H53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!H3:H53, "&lt;&gt;#N/A")</f>
+        <v>7</v>
       </c>
       <c r="F12" s="1">
-        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!I3:I53, "&lt;&gt;#N/A", Results!I3:I53, "&lt;&gt;")</f>
-        <v>1</v>
+        <f>SUMIFS(Results!I3:I53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!I3:I53, "&lt;&gt;#N/A")</f>
+        <v>0</v>
       </c>
       <c r="G12" s="1">
-        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!J3:J53, "&lt;&gt;#N/A", Results!J3:J53, "&lt;&gt;")</f>
-        <v>1</v>
+        <f>SUMIFS(Results!J3:J53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!J3:J53, "&lt;&gt;#N/A")</f>
+        <v>0</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13" s="1">
-        <f>SUMIFS(Results!E3:E53,Results!$B$3:$B$53,"=#N/A",Results!E3:E53, "&lt;&gt;#N/A")</f>
-        <v>7</v>
+        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!E3:E53, "&lt;&gt;#N/A", Results!E3:E53, "&lt;&gt;")</f>
+        <v>12</v>
       </c>
       <c r="C13" s="1">
-        <f>SUMIFS(Results!F3:F53,Results!$B$3:$B$53,"=#N/A",Results!F3:F53, "&lt;&gt;#N/A")</f>
-        <v>5</v>
+        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!F3:F53, "&lt;&gt;#N/A", Results!F3:F53, "&lt;&gt;")</f>
+        <v>11</v>
       </c>
       <c r="D13" s="1">
-        <f>SUMIFS(Results!G3:G53,Results!$B$3:$B$53,"=#N/A",Results!G3:G53, "&lt;&gt;#N/A")</f>
-        <v>7</v>
+        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!G3:G53, "&lt;&gt;#N/A", Results!G3:G53, "&lt;&gt;")</f>
+        <v>12</v>
       </c>
       <c r="E13" s="1">
-        <f>SUMIFS(Results!H3:H53,Results!$B$3:$B$53,"=#N/A",Results!H3:H53, "&lt;&gt;#N/A")</f>
-        <v>6</v>
+        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!H3:H53, "&lt;&gt;#N/A", Results!H3:H53, "&lt;&gt;")</f>
+        <v>11</v>
       </c>
       <c r="F13" s="1">
-        <f>SUMIFS(Results!I3:I53,Results!$B$3:$B$53,"=#N/A",Results!I3:I53, "&lt;&gt;#N/A")</f>
-        <v>0</v>
+        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!I3:I53, "&lt;&gt;#N/A", Results!I3:I53, "&lt;&gt;")</f>
+        <v>1</v>
       </c>
       <c r="G13" s="1">
-        <f>SUMIFS(Results!J3:J53,Results!$B$3:$B$53,"=#N/A",Results!J3:J53, "&lt;&gt;#N/A")</f>
-        <v>0</v>
+        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!J3:J53, "&lt;&gt;#N/A", Results!J3:J53, "&lt;&gt;")</f>
+        <v>1</v>
       </c>
       <c r="H13" s="1">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B14" s="1">
-        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!E3:E53, "&lt;&gt;#N/A", Results!E3:E53, "&lt;&gt;")</f>
-        <v>9</v>
+        <f>SUMIFS(Results!E3:E53,Results!$B$3:$B$53,"=#N/A",Results!E3:E53, "&lt;&gt;#N/A")</f>
+        <v>8</v>
       </c>
       <c r="C14" s="1">
-        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!F3:F53, "&lt;&gt;#N/A", Results!F3:F53, "&lt;&gt;")</f>
-        <v>9</v>
+        <f>SUMIFS(Results!F3:F53,Results!$B$3:$B$53,"=#N/A",Results!F3:F53, "&lt;&gt;#N/A")</f>
+        <v>7</v>
       </c>
       <c r="D14" s="1">
-        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!G3:G53, "&lt;&gt;#N/A", Results!G3:G53, "&lt;&gt;")</f>
-        <v>9</v>
+        <f>SUMIFS(Results!G3:G53,Results!$B$3:$B$53,"=#N/A",Results!G3:G53, "&lt;&gt;#N/A")</f>
+        <v>8</v>
       </c>
       <c r="E14" s="1">
-        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!H3:H53, "&lt;&gt;#N/A", Results!H3:H53, "&lt;&gt;")</f>
-        <v>9</v>
+        <f>SUMIFS(Results!H3:H53,Results!$B$3:$B$53,"=#N/A",Results!H3:H53, "&lt;&gt;#N/A")</f>
+        <v>7</v>
       </c>
       <c r="F14" s="1">
-        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!I3:I53, "&lt;&gt;#N/A", Results!I3:I53, "&lt;&gt;")</f>
+        <f>SUMIFS(Results!I3:I53,Results!$B$3:$B$53,"=#N/A",Results!I3:I53, "&lt;&gt;#N/A")</f>
         <v>0</v>
       </c>
       <c r="G14" s="1">
-        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!J3:J53, "&lt;&gt;#N/A", Results!J3:J53, "&lt;&gt;")</f>
+        <f>SUMIFS(Results!J3:J53,Results!$B$3:$B$53,"=#N/A",Results!J3:J53, "&lt;&gt;#N/A")</f>
         <v>0</v>
       </c>
       <c r="H14" s="1">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="B15" s="1">
-        <f>SUMIF(Results!$C$3:$C$53,Summary!B1,Results!$M$3:$M$53)</f>
-        <v>0</v>
+        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!E3:E53, "&lt;&gt;#N/A", Results!E3:E53, "&lt;&gt;")</f>
+        <v>11</v>
       </c>
       <c r="C15" s="1">
-        <f>SUMIF(Results!$C$3:$C$53,Summary!C1,Results!$M$3:$M$53)</f>
-        <v>0</v>
+        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!F3:F53, "&lt;&gt;#N/A", Results!F3:F53, "&lt;&gt;")</f>
+        <v>11</v>
       </c>
       <c r="D15" s="1">
-        <f>SUMIF(Results!$C$3:$C$53,Summary!D1,Results!$M$3:$M$53)</f>
-        <v>0</v>
+        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!G3:G53, "&lt;&gt;#N/A", Results!G3:G53, "&lt;&gt;")</f>
+        <v>11</v>
       </c>
       <c r="E15" s="1">
-        <f>SUMIF(Results!$C$3:$C$53,Summary!E1,Results!$M$3:$M$53)</f>
-        <v>0</v>
+        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!H3:H53, "&lt;&gt;#N/A", Results!H3:H53, "&lt;&gt;")</f>
+        <v>11</v>
       </c>
       <c r="F15" s="1">
-        <f>SUMIF(Results!$C$3:$C$53,Summary!F1,Results!$M$3:$M$53)</f>
+        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!I3:I53, "&lt;&gt;#N/A", Results!I3:I53, "&lt;&gt;")</f>
         <v>0</v>
       </c>
       <c r="G15" s="1">
-        <f>SUMIF(Results!$C$3:$C$53,Summary!G1,Results!$M$3:$M$53)</f>
-        <v>1</v>
+        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!J3:J53, "&lt;&gt;#N/A", Results!J3:J53, "&lt;&gt;")</f>
+        <v>0</v>
       </c>
       <c r="H15" s="1">
-        <f>SUM(B15:G15)</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="1">
+        <f>SUMIF(Results!$C$3:$C$53,Summary!B1,Results!$M$3:$M$53)</f>
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
+        <f>SUMIF(Results!$C$3:$C$53,Summary!C1,Results!$M$3:$M$53)</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="1">
+        <f>SUMIF(Results!$C$3:$C$53,Summary!D1,Results!$M$3:$M$53)</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <f>SUMIF(Results!$C$3:$C$53,Summary!E1,Results!$M$3:$M$53)</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="1">
+        <f>SUMIF(Results!$C$3:$C$53,Summary!F1,Results!$M$3:$M$53)</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <f>SUMIF(Results!$C$3:$C$53,Summary!G1,Results!$M$3:$M$53)</f>
+        <v>1</v>
+      </c>
+      <c r="H16" s="1">
+        <f>SUM(B16:G16)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B17" s="1">
         <f>SUMIF(Results!E3:E53,"&lt;&gt;#N/A",Results!$N$3:$N$53)</f>
-        <v>3</v>
-      </c>
-      <c r="C16" s="1">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1">
         <f>SUMIF(Results!F3:F53,"&lt;&gt;#N/A",Results!$N$3:$N$53)</f>
-        <v>3</v>
-      </c>
-      <c r="D16" s="1">
+        <v>4</v>
+      </c>
+      <c r="D17" s="1">
         <f>SUMIF(Results!G3:G53,"&lt;&gt;#N/A",Results!$N$3:$N$53)</f>
-        <v>3</v>
-      </c>
-      <c r="E16" s="1">
+        <v>4</v>
+      </c>
+      <c r="E17" s="1">
         <f>SUMIF(Results!H3:H53,"&lt;&gt;#N/A",Results!$N$3:$N$53)</f>
-        <v>3</v>
-      </c>
-      <c r="F16" s="1">
+        <v>4</v>
+      </c>
+      <c r="F17" s="1">
         <f>SUMIF(Results!I3:I53,"&lt;&gt;#N/A",Results!$N$3:$N$53)</f>
         <v>0</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G17" s="1">
         <f>SUMIF(Results!J3:J53,"&lt;&gt;#N/A",Results!$N$3:$N$53)</f>
         <v>0</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H17" s="1">
         <f>SUM(Results!N3:N53)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated through episode 649, found 1 error in record keeping for episode 635, added new statistic for panelist performance when answering first
</commit_message>
<xml_diff>
--- a/SGU_Science_or_Fiction.xlsx
+++ b/SGU_Science_or_Fiction.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6135" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6135"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,9 @@
     <sheet name="Summary" sheetId="3" r:id="rId3"/>
     <sheet name="Visuals" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$U$50</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="223">
   <si>
     <t>Episode</t>
   </si>
@@ -673,6 +676,30 @@
   </si>
   <si>
     <t>How Smart are Carnivores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Researchers find that viruses share some of their genes across all kingdoms of life, not just the ones they infect. </t>
+  </si>
+  <si>
+    <t>A new study finds that playing 3D video games increased gray matter in the memory forming parts of the brain.</t>
+  </si>
+  <si>
+    <t>Researchers have demonstrated a new technique for 3D printing entire organs made out of a host’s own stem cells</t>
+  </si>
+  <si>
+    <t>Scientists report a breakthrough with hydrogen-boron fusion using lasers and predict a working prototype within 10 years.</t>
+  </si>
+  <si>
+    <t>plants, and bioengineered a tree that, when mature, several together can produce enough electricity to power a small home.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Researchers demonstrate a method they claim can be used to convert 850 million tons of atmospheric CO2 into a mineral each year, using seawater and scrap metal, and producing hydrogen as a side product. </t>
+  </si>
+  <si>
+    <t>Panelist Performance When Answering First</t>
+  </si>
+  <si>
+    <t>Correct Guesses When Answring First</t>
   </si>
 </sst>
 </file>
@@ -775,7 +802,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -834,6 +861,15 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -841,7 +877,437 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="51">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1209,16 +1675,16 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>0.5</c:v>
+                  <c:v>0.52083333333333337</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.63414634146341464</c:v>
+                  <c:v>0.62790697674418605</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.53333333333333333</c:v>
+                  <c:v>0.55319148936170215</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.59090909090909094</c:v>
+                  <c:v>0.58695652173913049</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.33333333333333331</c:v>
@@ -1245,7 +1711,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.55555555555555558</c:v>
+                  <c:v>0.56345177664974622</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1261,8 +1727,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="185988776"/>
-        <c:axId val="185993256"/>
+        <c:axId val="127263760"/>
+        <c:axId val="127264152"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -1389,7 +1855,7 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>0</c:v>
+                        <c:v>1</c:v>
                       </c:pt>
                       <c:pt idx="10">
                         <c:v>0</c:v>
@@ -1398,7 +1864,7 @@
                         <c:v>1</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>0.54</c:v>
+                        <c:v>0.54455445544554459</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1502,16 +1968,16 @@
                       <c:formatCode>0.0%</c:formatCode>
                       <c:ptCount val="13"/>
                       <c:pt idx="0">
-                        <c:v>0.59090909090909094</c:v>
+                        <c:v>0.625</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.55000000000000004</c:v>
+                        <c:v>0.54545454545454541</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.47619047619047616</c:v>
+                        <c:v>0.52173913043478259</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0.68181818181818177</c:v>
+                        <c:v>0.66666666666666663</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>0</c:v>
@@ -1529,7 +1995,7 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>1</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="10">
                         <c:v>0</c:v>
@@ -1538,7 +2004,7 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>0.5730337078651685</c:v>
+                        <c:v>0.58333333333333337</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1557,7 +2023,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Summary!$A$11</c:f>
+              <c:f>Summary!$A$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1677,21 +2143,21 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Summary!$B$11:$N$11</c:f>
+              <c:f>Summary!$B$13:$N$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>46</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>3</c:v>
@@ -1718,7 +2184,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>183</c:v>
+                  <c:v>197</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1734,11 +2200,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="186002216"/>
-        <c:axId val="186001832"/>
+        <c:axId val="127264936"/>
+        <c:axId val="127264544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="185988776"/>
+        <c:axId val="127263760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1781,7 +2247,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="185993256"/>
+        <c:crossAx val="127264152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1789,7 +2255,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="185993256"/>
+        <c:axId val="127264152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1840,12 +2306,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="185988776"/>
+        <c:crossAx val="127263760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="186001832"/>
+        <c:axId val="127264544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1882,12 +2348,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="186002216"/>
+        <c:crossAx val="127264936"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="186002216"/>
+        <c:axId val="127264936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1896,7 +2362,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186001832"/>
+        <c:crossAx val="127264544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2320,7 +2786,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -2329,7 +2795,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.54</c:v>
+                  <c:v>0.54455445544554459</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -2346,8 +2812,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="185732320"/>
-        <c:axId val="185736800"/>
+        <c:axId val="177541528"/>
+        <c:axId val="177541920"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -2541,16 +3007,16 @@
                       <c:formatCode>0.0%</c:formatCode>
                       <c:ptCount val="13"/>
                       <c:pt idx="0">
-                        <c:v>0.5</c:v>
+                        <c:v>0.52083333333333337</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.63414634146341464</c:v>
+                        <c:v>0.62790697674418605</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.53333333333333333</c:v>
+                        <c:v>0.55319148936170215</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0.59090909090909094</c:v>
+                        <c:v>0.58695652173913049</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>0.33333333333333331</c:v>
@@ -2577,7 +3043,7 @@
                         <c:v>1</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>0.55555555555555558</c:v>
+                        <c:v>0.56345177664974622</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2681,16 +3147,16 @@
                       <c:formatCode>0.0%</c:formatCode>
                       <c:ptCount val="13"/>
                       <c:pt idx="0">
-                        <c:v>0.59090909090909094</c:v>
+                        <c:v>0.625</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.55000000000000004</c:v>
+                        <c:v>0.54545454545454541</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.47619047619047616</c:v>
+                        <c:v>0.52173913043478259</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0.68181818181818177</c:v>
+                        <c:v>0.66666666666666663</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>0</c:v>
@@ -2708,7 +3174,7 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>1</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="10">
                         <c:v>0</c:v>
@@ -2717,7 +3183,7 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>0.5730337078651685</c:v>
+                        <c:v>0.58333333333333337</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2733,7 +3199,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Summary!$A$11</c15:sqref>
+                          <c15:sqref>Summary!$A$13</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -2854,7 +3320,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Summary!$B$11:$N$11</c15:sqref>
+                          <c15:sqref>Summary!$B$13:$N$13</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -2862,16 +3328,16 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="13"/>
                       <c:pt idx="0">
+                        <c:v>48</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>43</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>47</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
                         <c:v>46</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>41</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>45</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>44</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>3</c:v>
@@ -2898,7 +3364,7 @@
                         <c:v>1</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>183</c:v>
+                        <c:v>197</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2914,7 +3380,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Summary!$A$15</c15:sqref>
+                          <c15:sqref>Summary!$A$17</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -2941,7 +3407,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Summary!$B$15:$N$15</c15:sqref>
+                          <c15:sqref>Summary!$B$17:$N$17</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -2949,16 +3415,16 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="13"/>
                       <c:pt idx="0">
+                        <c:v>24</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
                         <c:v>22</c:v>
                       </c:pt>
-                      <c:pt idx="1">
-                        <c:v>20</c:v>
-                      </c:pt>
                       <c:pt idx="2">
-                        <c:v>21</c:v>
+                        <c:v>23</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>22</c:v>
+                        <c:v>24</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>0</c:v>
@@ -2976,7 +3442,7 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>1</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="10">
                         <c:v>1</c:v>
@@ -2985,7 +3451,7 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>85</c:v>
+                        <c:v>96</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3004,7 +3470,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Summary!$A$13</c:f>
+              <c:f>Summary!$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3082,7 +3548,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Summary!$B$13:$N$13</c:f>
+              <c:f>Summary!$B$15:$N$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -3114,7 +3580,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -3123,7 +3589,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>98</c:v>
+                  <c:v>101</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3139,11 +3605,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="185739616"/>
-        <c:axId val="185739232"/>
+        <c:axId val="177542704"/>
+        <c:axId val="177542312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="185732320"/>
+        <c:axId val="177541528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3186,7 +3652,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="185736800"/>
+        <c:crossAx val="177541920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3194,7 +3660,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="185736800"/>
+        <c:axId val="177541920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3245,12 +3711,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="185732320"/>
+        <c:crossAx val="177541528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="185739232"/>
+        <c:axId val="177542312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3287,12 +3753,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="185739616"/>
+        <c:crossAx val="177542704"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="185739616"/>
+        <c:axId val="177542704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3301,7 +3767,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185739232"/>
+        <c:crossAx val="177542312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3698,16 +4164,16 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>0.59090909090909094</c:v>
+                  <c:v>0.625</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.55000000000000004</c:v>
+                  <c:v>0.54545454545454541</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.47619047619047616</c:v>
+                  <c:v>0.52173913043478259</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.68181818181818177</c:v>
+                  <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -3725,7 +4191,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -3734,7 +4200,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.5730337078651685</c:v>
+                  <c:v>0.58333333333333337</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -3751,8 +4217,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="185822624"/>
-        <c:axId val="186432480"/>
+        <c:axId val="177543880"/>
+        <c:axId val="177544272"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -3946,16 +4412,16 @@
                       <c:formatCode>0.0%</c:formatCode>
                       <c:ptCount val="13"/>
                       <c:pt idx="0">
-                        <c:v>0.5</c:v>
+                        <c:v>0.52083333333333337</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.63414634146341464</c:v>
+                        <c:v>0.62790697674418605</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.53333333333333333</c:v>
+                        <c:v>0.55319148936170215</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0.59090909090909094</c:v>
+                        <c:v>0.58695652173913049</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>0.33333333333333331</c:v>
@@ -3982,7 +4448,7 @@
                         <c:v>1</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>0.55555555555555558</c:v>
+                        <c:v>0.56345177664974622</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4207,7 +4673,7 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>0</c:v>
+                        <c:v>1</c:v>
                       </c:pt>
                       <c:pt idx="10">
                         <c:v>0</c:v>
@@ -4216,7 +4682,7 @@
                         <c:v>1</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>0.54</c:v>
+                        <c:v>0.54455445544554459</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4232,7 +4698,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Summary!$A$11</c15:sqref>
+                          <c15:sqref>Summary!$A$13</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -4353,7 +4819,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Summary!$B$11:$N$11</c15:sqref>
+                          <c15:sqref>Summary!$B$13:$N$13</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -4361,16 +4827,16 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="13"/>
                       <c:pt idx="0">
+                        <c:v>48</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>43</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>47</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
                         <c:v>46</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>41</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>45</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>44</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>3</c:v>
@@ -4397,7 +4863,7 @@
                         <c:v>1</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>183</c:v>
+                        <c:v>197</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4413,7 +4879,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Summary!$A$13</c15:sqref>
+                          <c15:sqref>Summary!$A$15</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -4496,7 +4962,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Summary!$B$13:$N$13</c15:sqref>
+                          <c15:sqref>Summary!$B$15:$N$15</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -4531,7 +4997,7 @@
                         <c:v>1</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>0</c:v>
+                        <c:v>1</c:v>
                       </c:pt>
                       <c:pt idx="10">
                         <c:v>0</c:v>
@@ -4540,7 +5006,7 @@
                         <c:v>1</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>98</c:v>
+                        <c:v>101</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4559,7 +5025,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Summary!$A$15</c:f>
+              <c:f>Summary!$A$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4638,21 +5104,21 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Summary!$B$15:$N$15</c:f>
+              <c:f>Summary!$B$17:$N$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>22</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>20</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>21</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4670,7 +5136,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1</c:v>
@@ -4679,7 +5145,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>85</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -4696,11 +5162,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="136723800"/>
-        <c:axId val="136723408"/>
+        <c:axId val="177778616"/>
+        <c:axId val="177544664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="185822624"/>
+        <c:axId val="177543880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4743,7 +5209,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="186432480"/>
+        <c:crossAx val="177544272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4751,7 +5217,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="186432480"/>
+        <c:axId val="177544272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4802,12 +5268,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="185822624"/>
+        <c:crossAx val="177543880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="136723408"/>
+        <c:axId val="177544664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4846,12 +5312,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="136723800"/>
+        <c:crossAx val="177778616"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="136723800"/>
+        <c:axId val="177778616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4860,7 +5326,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136723408"/>
+        <c:crossAx val="177544664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6982,9 +7448,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J52" sqref="J52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9562,8 +10028,9 @@
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="S35" s="1">
-        <v>2</v>
+      <c r="S35" s="1" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
       </c>
       <c r="T35" s="1" t="e">
         <f>NA()</f>
@@ -9634,9 +10101,8 @@
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="S36" s="1" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="S36" s="1">
+        <v>2</v>
       </c>
       <c r="T36" s="1" t="e">
         <f>NA()</f>
@@ -10450,25 +10916,141 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="49" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
-      <c r="J49" s="1"/>
-      <c r="K49" s="1"/>
-      <c r="L49" s="1"/>
-      <c r="M49" s="1"/>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>648</v>
+      </c>
+      <c r="B49" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C49" t="s">
+        <v>215</v>
+      </c>
+      <c r="D49" t="s">
+        <v>216</v>
+      </c>
+      <c r="E49" t="s">
+        <v>217</v>
+      </c>
+      <c r="F49" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G49" s="1">
+        <v>3</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J49" s="1">
+        <v>3</v>
+      </c>
+      <c r="K49" s="1">
+        <v>2</v>
+      </c>
+      <c r="L49" s="1">
+        <v>3</v>
+      </c>
+      <c r="M49" s="1">
+        <v>2</v>
+      </c>
+      <c r="N49" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="O49" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="P49" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Q49" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="R49" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S49" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T49" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U49" t="e">
+        <v>#N/A</v>
+      </c>
     </row>
-    <row r="50" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
-      <c r="I50" s="1"/>
-      <c r="J50" s="1"/>
-      <c r="K50" s="1"/>
-      <c r="L50" s="1"/>
-      <c r="M50" s="1"/>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>649</v>
+      </c>
+      <c r="B50" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C50" t="s">
+        <v>218</v>
+      </c>
+      <c r="D50" t="s">
+        <v>219</v>
+      </c>
+      <c r="E50" t="s">
+        <v>220</v>
+      </c>
+      <c r="F50" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G50" s="1">
+        <v>2</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J50" s="1">
+        <v>2</v>
+      </c>
+      <c r="K50" s="1">
+        <v>2</v>
+      </c>
+      <c r="L50" s="1">
+        <v>2</v>
+      </c>
+      <c r="M50" s="1">
+        <v>2</v>
+      </c>
+      <c r="N50" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="O50" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="P50" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Q50" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="R50" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S50" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T50" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U50" t="e">
+        <v>#N/A</v>
+      </c>
     </row>
-    <row r="51" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
@@ -10477,7 +11059,7 @@
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
     </row>
-    <row r="52" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
@@ -10486,7 +11068,7 @@
       <c r="L52" s="1"/>
       <c r="M52" s="1"/>
     </row>
-    <row r="53" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
@@ -10496,6 +11078,7 @@
       <c r="M53" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:U50"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
@@ -10503,13 +11086,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AS49"/>
+  <dimension ref="A1:AS51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="U25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="W25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AJ27" sqref="AJ27:AJ33"/>
+      <selection pane="bottomRight" activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16763,9 +17346,9 @@
         <f>IF(Data!R35=Data!$G35,1,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="N36" s="1">
+      <c r="N36" s="1" t="e">
         <f>IF(Data!S35=Data!$G35,1,0)</f>
-        <v>1</v>
+        <v>#N/A</v>
       </c>
       <c r="O36" s="1" t="e">
         <f>IF(Data!T35=Data!$G35,1,0)</f>
@@ -16777,11 +17360,11 @@
       </c>
       <c r="Q36" s="1">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R36" s="1">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S36" s="1">
         <f t="shared" si="7"/>
@@ -16833,7 +17416,7 @@
       </c>
       <c r="AE36" s="8">
         <f t="shared" ref="AE36:AE39" si="64">IF(ISNA(N36),AE35,IF(N36=1,AE35+1,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF36" s="8">
         <f t="shared" si="20"/>
@@ -16945,9 +17528,9 @@
         <f>IF(Data!R36=Data!$G36,1,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="N37" s="1" t="e">
+      <c r="N37" s="1">
         <f>IF(Data!S36=Data!$G36,1,0)</f>
-        <v>#N/A</v>
+        <v>1</v>
       </c>
       <c r="O37" s="1" t="e">
         <f>IF(Data!T36=Data!$G36,1,0)</f>
@@ -16959,11 +17542,11 @@
       </c>
       <c r="Q37" s="1">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R37" s="1">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S37" s="1">
         <f t="shared" si="7"/>
@@ -19256,6 +19839,370 @@
       </c>
       <c r="AS49" s="10">
         <f t="shared" si="148"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A50" s="3">
+        <f>Data!A49</f>
+        <v>648</v>
+      </c>
+      <c r="B50" s="4" t="e">
+        <f>Data!B49</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C50" s="5" t="str">
+        <f>Data!H49</f>
+        <v>Steve</v>
+      </c>
+      <c r="D50" s="2" t="str">
+        <f>Data!I49</f>
+        <v>Cara</v>
+      </c>
+      <c r="E50" s="1">
+        <f>IF(Data!J49=Data!$G49,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F50" s="1">
+        <f>IF(Data!K49=Data!$G49,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G50" s="1">
+        <f>IF(Data!L49=Data!$G49,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H50" s="1">
+        <f>IF(Data!M49=Data!$G49,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I50" s="1" t="e">
+        <f>IF(Data!N49=Data!$G49,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J50" s="1" t="e">
+        <f>IF(Data!O49=Data!$G49,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K50" s="1" t="e">
+        <f>IF(Data!P49=Data!$G49,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="L50" s="1" t="e">
+        <f>IF(Data!Q49=Data!$G49,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M50" s="1" t="e">
+        <f>IF(Data!R49=Data!$G49,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N50" s="1" t="e">
+        <f>IF(Data!S49=Data!$G49,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O50" s="1" t="e">
+        <f>IF(Data!T49=Data!$G49,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P50" s="1" t="e">
+        <f>IF(Data!U49=Data!$G49,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q50" s="1">
+        <f t="shared" ref="Q50:Q51" si="149">COUNTIF(E50:P50,"&lt;&gt;#N/A")</f>
+        <v>4</v>
+      </c>
+      <c r="R50" s="1">
+        <f t="shared" ref="R50:R51" si="150">SUMIF(E50:P50,"&lt;&gt;#N/A")</f>
+        <v>2</v>
+      </c>
+      <c r="S50" s="1">
+        <f t="shared" ref="S50:S51" si="151">IF(R50=0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="T50" s="1">
+        <f t="shared" ref="T50:T51" si="152">IF(Q50=R50,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="U50" s="1" t="e">
+        <f t="shared" ref="U50:U51" si="153">IF(R50=1,INDEX($E$2:$P$2,1,MATCH(1,E50:P50,0)),NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="V50" s="8">
+        <f t="shared" ref="V50:V51" si="154">IF(ISNA(E50),V49,IF(E50=1,V49+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="W50" s="8">
+        <f t="shared" ref="W50:W51" si="155">IF(ISNA(F50),W49,IF(F50=1,W49+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="X50" s="8">
+        <f t="shared" ref="X50:X51" si="156">IF(ISNA(G50),X49,IF(G50=1,X49+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="Y50" s="8">
+        <f t="shared" ref="Y50:Y51" si="157">IF(ISNA(H50),Y49,IF(H50=1,Y49+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="Z50" s="8">
+        <f t="shared" ref="Z50:Z51" si="158">IF(ISNA(I50),Z49,IF(I50=1,Z49+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AA50" s="8">
+        <f t="shared" ref="AA50:AA51" si="159">IF(ISNA(J50),AA49,IF(J50=1,AA49+1,0))</f>
+        <v>2</v>
+      </c>
+      <c r="AB50" s="8">
+        <f t="shared" ref="AB50:AB51" si="160">IF(ISNA(K50),AB49,IF(K50=1,AB49+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AC50" s="8">
+        <f t="shared" ref="AC50:AC51" si="161">IF(ISNA(L50),AC49,IF(L50=1,AC49+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AD50" s="8">
+        <f t="shared" ref="AD50:AD51" si="162">IF(ISNA(M50),AD49,IF(M50=1,AD49+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AE50" s="8">
+        <f t="shared" ref="AE50:AE51" si="163">IF(ISNA(N50),AE49,IF(N50=1,AE49+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AF50" s="8">
+        <f t="shared" ref="AF50:AF51" si="164">IF(ISNA(O50),AF49,IF(O50=1,AF49+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AG50" s="8">
+        <f t="shared" ref="AG50:AG51" si="165">IF(ISNA(P50),AG49,IF(P50=1,AG49+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AH50" s="10">
+        <f t="shared" ref="AH50:AH51" si="166">IF(ISNA(E50),AH49,IF(E50=0,AH49+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AI50" s="10">
+        <f t="shared" ref="AI50:AI51" si="167">IF(ISNA(F50),AI49,IF(F50=0,AI49+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AJ50" s="10">
+        <f t="shared" ref="AJ50:AJ51" si="168">IF(ISNA(G50),AJ49,IF(G50=0,AJ49+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AK50" s="10">
+        <f t="shared" ref="AK50:AK51" si="169">IF(ISNA(H50),AK49,IF(H50=0,AK49+1,0))</f>
+        <v>3</v>
+      </c>
+      <c r="AL50" s="10">
+        <f t="shared" ref="AL50:AL51" si="170">IF(ISNA(I50),AL49,IF(I50=0,AL49+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AM50" s="10">
+        <f t="shared" ref="AM50:AM51" si="171">IF(ISNA(J50),AM49,IF(J50=0,AM49+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AN50" s="10">
+        <f t="shared" ref="AN50:AN51" si="172">IF(ISNA(K50),AN49,IF(K50=0,AN49+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AO50" s="10">
+        <f t="shared" ref="AO50:AO51" si="173">IF(ISNA(L50),AO49,IF(L50=0,AO49+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AP50" s="10">
+        <f t="shared" ref="AP50:AP51" si="174">IF(ISNA(M50),AP49,IF(M50=0,AP49+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AQ50" s="10">
+        <f t="shared" ref="AQ50:AQ51" si="175">IF(ISNA(N50),AQ49,IF(N50=0,AQ49+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AR50" s="10">
+        <f t="shared" ref="AR50:AR51" si="176">IF(ISNA(O50),AR49,IF(O50=0,AR49+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AS50" s="10">
+        <f t="shared" ref="AS50:AS51" si="177">IF(ISNA(P50),AS49,IF(P50=0,AS49+1,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A51" s="3">
+        <f>Data!A50</f>
+        <v>649</v>
+      </c>
+      <c r="B51" s="4" t="e">
+        <f>Data!B50</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C51" s="5" t="str">
+        <f>Data!H50</f>
+        <v>Steve</v>
+      </c>
+      <c r="D51" s="2" t="str">
+        <f>Data!I50</f>
+        <v>Bob</v>
+      </c>
+      <c r="E51" s="1">
+        <f>IF(Data!J50=Data!$G50,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F51" s="1">
+        <f>IF(Data!K50=Data!$G50,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G51" s="1">
+        <f>IF(Data!L50=Data!$G50,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H51" s="1">
+        <f>IF(Data!M50=Data!$G50,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="I51" s="1" t="e">
+        <f>IF(Data!N50=Data!$G50,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J51" s="1" t="e">
+        <f>IF(Data!O50=Data!$G50,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K51" s="1" t="e">
+        <f>IF(Data!P50=Data!$G50,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="L51" s="1" t="e">
+        <f>IF(Data!Q50=Data!$G50,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M51" s="1" t="e">
+        <f>IF(Data!R50=Data!$G50,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N51" s="1" t="e">
+        <f>IF(Data!S50=Data!$G50,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O51" s="1" t="e">
+        <f>IF(Data!T50=Data!$G50,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P51" s="1" t="e">
+        <f>IF(Data!U50=Data!$G50,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q51" s="1">
+        <f t="shared" si="149"/>
+        <v>4</v>
+      </c>
+      <c r="R51" s="1">
+        <f t="shared" si="150"/>
+        <v>4</v>
+      </c>
+      <c r="S51" s="1">
+        <f t="shared" si="151"/>
+        <v>0</v>
+      </c>
+      <c r="T51" s="1">
+        <f t="shared" si="152"/>
+        <v>1</v>
+      </c>
+      <c r="U51" s="1" t="e">
+        <f t="shared" si="153"/>
+        <v>#N/A</v>
+      </c>
+      <c r="V51" s="8">
+        <f t="shared" si="154"/>
+        <v>2</v>
+      </c>
+      <c r="W51" s="8">
+        <f t="shared" si="155"/>
+        <v>1</v>
+      </c>
+      <c r="X51" s="8">
+        <f t="shared" si="156"/>
+        <v>2</v>
+      </c>
+      <c r="Y51" s="8">
+        <f t="shared" si="157"/>
+        <v>1</v>
+      </c>
+      <c r="Z51" s="8">
+        <f t="shared" si="158"/>
+        <v>1</v>
+      </c>
+      <c r="AA51" s="8">
+        <f t="shared" si="159"/>
+        <v>2</v>
+      </c>
+      <c r="AB51" s="8">
+        <f t="shared" si="160"/>
+        <v>0</v>
+      </c>
+      <c r="AC51" s="8">
+        <f t="shared" si="161"/>
+        <v>1</v>
+      </c>
+      <c r="AD51" s="8">
+        <f t="shared" si="162"/>
+        <v>0</v>
+      </c>
+      <c r="AE51" s="8">
+        <f t="shared" si="163"/>
+        <v>1</v>
+      </c>
+      <c r="AF51" s="8">
+        <f t="shared" si="164"/>
+        <v>0</v>
+      </c>
+      <c r="AG51" s="8">
+        <f t="shared" si="165"/>
+        <v>1</v>
+      </c>
+      <c r="AH51" s="10">
+        <f t="shared" si="166"/>
+        <v>0</v>
+      </c>
+      <c r="AI51" s="10">
+        <f t="shared" si="167"/>
+        <v>0</v>
+      </c>
+      <c r="AJ51" s="10">
+        <f t="shared" si="168"/>
+        <v>0</v>
+      </c>
+      <c r="AK51" s="10">
+        <f t="shared" si="169"/>
+        <v>0</v>
+      </c>
+      <c r="AL51" s="10">
+        <f t="shared" si="170"/>
+        <v>0</v>
+      </c>
+      <c r="AM51" s="10">
+        <f t="shared" si="171"/>
+        <v>0</v>
+      </c>
+      <c r="AN51" s="10">
+        <f t="shared" si="172"/>
+        <v>1</v>
+      </c>
+      <c r="AO51" s="10">
+        <f t="shared" si="173"/>
+        <v>0</v>
+      </c>
+      <c r="AP51" s="10">
+        <f t="shared" si="174"/>
+        <v>1</v>
+      </c>
+      <c r="AQ51" s="10">
+        <f t="shared" si="175"/>
+        <v>0</v>
+      </c>
+      <c r="AR51" s="10">
+        <f t="shared" si="176"/>
+        <v>1</v>
+      </c>
+      <c r="AS51" s="10">
+        <f t="shared" si="177"/>
         <v>0</v>
       </c>
     </row>
@@ -19271,9 +20218,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -19342,19 +20291,19 @@
       </c>
       <c r="B2" s="6">
         <f>SUMIF(Results!E3:E53,"&lt;&gt;#N/A")/COUNTIFS(Results!E3:E53,"&lt;&gt;#N/A",Results!E3:E53,"&lt;&gt;")</f>
-        <v>0.5</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="C2" s="6">
         <f>SUMIF(Results!F3:F53,"&lt;&gt;#N/A")/COUNTIFS(Results!F3:F53,"&lt;&gt;#N/A",Results!F3:F53,"&lt;&gt;")</f>
-        <v>0.63414634146341464</v>
+        <v>0.62790697674418605</v>
       </c>
       <c r="D2" s="6">
         <f>SUMIF(Results!G3:G53,"&lt;&gt;#N/A")/COUNTIFS(Results!G3:G53,"&lt;&gt;#N/A",Results!G3:G53,"&lt;&gt;")</f>
-        <v>0.53333333333333333</v>
+        <v>0.55319148936170215</v>
       </c>
       <c r="E2" s="6">
         <f>SUMIF(Results!H3:H53,"&lt;&gt;#N/A")/COUNTIFS(Results!H3:H53,"&lt;&gt;#N/A",Results!H3:H53,"&lt;&gt;")</f>
-        <v>0.59090909090909094</v>
+        <v>0.58695652173913049</v>
       </c>
       <c r="F2" s="6">
         <f>SUMIF(Results!I3:I53,"&lt;&gt;#N/A")/COUNTIFS(Results!I3:I53,"&lt;&gt;#N/A",Results!I3:I53,"&lt;&gt;")</f>
@@ -19390,7 +20339,7 @@
       </c>
       <c r="N2" s="6">
         <f>SUM(Results!R3:R53)/SUM(Results!Q3:Q53)</f>
-        <v>0.55555555555555558</v>
+        <v>0.56345177664974622</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -19433,9 +20382,9 @@
         <f>SUMIFS(Results!M3:M53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!M3:M53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!M3:M53, "&lt;&gt;#N/A", Results!M3:M53, "&lt;&gt;")</f>
         <v>0</v>
       </c>
-      <c r="K3" s="6" t="e">
+      <c r="K3" s="6">
         <f>SUMIFS(Results!N3:N53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!N3:N53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!N3:N53, "&lt;&gt;#N/A", Results!N3:N53, "&lt;&gt;")</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="L3" s="6" t="e">
         <f>SUMIFS(Results!O3:O53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!O3:O53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!O3:O53, "&lt;&gt;#N/A", Results!O3:O53, "&lt;&gt;")</f>
@@ -19447,7 +20396,7 @@
       </c>
       <c r="N3" s="6">
         <f>SUMIF(Results!B3:B53,"&lt;&gt;#N/A",Results!R3:R53)/SUMIF(Results!B3:B53,"&lt;&gt;#N/A",Results!Q3:Q53)</f>
-        <v>0.54</v>
+        <v>0.54455445544554459</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -19456,19 +20405,19 @@
       </c>
       <c r="B4" s="6">
         <f>SUMIFS(Results!E3:E53,Results!$B$3:$B$53,"=#N/A",Results!E3:E53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!E3:E53, "&lt;&gt;#N/A", Results!E3:E53, "&lt;&gt;")</f>
-        <v>0.59090909090909094</v>
+        <v>0.625</v>
       </c>
       <c r="C4" s="6">
         <f>SUMIFS(Results!F3:F53,Results!$B$3:$B$53,"=#N/A",Results!F3:F53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!F3:F53, "&lt;&gt;#N/A", Results!F3:F53, "&lt;&gt;")</f>
-        <v>0.55000000000000004</v>
+        <v>0.54545454545454541</v>
       </c>
       <c r="D4" s="6">
         <f>SUMIFS(Results!G3:G53,Results!$B$3:$B$53,"=#N/A",Results!G3:G53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!G3:G53, "&lt;&gt;#N/A", Results!G3:G53, "&lt;&gt;")</f>
-        <v>0.47619047619047616</v>
+        <v>0.52173913043478259</v>
       </c>
       <c r="E4" s="6">
         <f>SUMIFS(Results!H3:H53,Results!$B$3:$B$53,"=#N/A",Results!H3:H53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!H3:H53, "&lt;&gt;#N/A", Results!H3:H53, "&lt;&gt;")</f>
-        <v>0.68181818181818177</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F4" s="6" t="e">
         <f>SUMIFS(Results!I3:I53,Results!$B$3:$B$53,"=#N/A",Results!I3:I53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!I3:I53, "&lt;&gt;#N/A", Results!I3:I53, "&lt;&gt;")</f>
@@ -19490,9 +20439,9 @@
         <f>SUMIFS(Results!M3:M53,Results!$B$3:$B$53,"=#N/A",Results!M3:M53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!M3:M53, "&lt;&gt;#N/A", Results!M3:M53, "&lt;&gt;")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="6" t="e">
         <f>SUMIFS(Results!N3:N53,Results!$B$3:$B$53,"=#N/A",Results!N3:N53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!N3:N53, "&lt;&gt;#N/A", Results!N3:N53, "&lt;&gt;")</f>
-        <v>1</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="L4" s="6">
         <f>SUMIFS(Results!O3:O53,Results!$B$3:$B$53,"=#N/A",Results!O3:O53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!O3:O53, "&lt;&gt;#N/A", Results!O3:O53, "&lt;&gt;")</f>
@@ -19504,7 +20453,7 @@
       </c>
       <c r="N4" s="6">
         <f>SUMIF(Results!B3:B53,"=#N/A",Results!R3:R53)/SUMIF(Results!B3:B53,"=#N/A",Results!Q3:Q53)</f>
-        <v>0.5730337078651685</v>
+        <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -19560,7 +20509,7 @@
         <v>1</v>
       </c>
       <c r="N5" s="1">
-        <f>MAX(B5:G5)</f>
+        <f>MAX(B5:M5)</f>
         <v>6</v>
       </c>
     </row>
@@ -19617,7 +20566,7 @@
         <v>0</v>
       </c>
       <c r="N6" s="1">
-        <f>MAX(B6:G6)</f>
+        <f>MAX(B6:M6)</f>
         <v>5</v>
       </c>
     </row>
@@ -19674,7 +20623,7 @@
         <v>0</v>
       </c>
       <c r="N7" s="1">
-        <f>MAX(B7:G7)</f>
+        <f>MAX(B7:M7)</f>
         <v>4</v>
       </c>
     </row>
@@ -19684,11 +20633,11 @@
       </c>
       <c r="B8" s="7">
         <f>SUMIF(Results!$D$3:$D$53,B1,Results!$R$3:$R$53)/SUMIF(Results!$D$3:$D$53,B1,Results!$Q$3:$Q$53)</f>
-        <v>0.56818181818181823</v>
+        <v>0.5957446808510638</v>
       </c>
       <c r="C8" s="7">
         <f>SUMIF(Results!$D$3:$D$53,C1,Results!$R$3:$R$53)/SUMIF(Results!$D$3:$D$53,C1,Results!$Q$3:$Q$53)</f>
-        <v>0.53488372093023251</v>
+        <v>0.53191489361702127</v>
       </c>
       <c r="D8" s="7">
         <f>SUMIF(Results!$D$3:$D$53,D1,Results!$R$3:$R$53)/SUMIF(Results!$D$3:$D$53,D1,Results!$Q$3:$Q$53)</f>
@@ -19730,548 +20679,668 @@
         <f>SUMIF(Results!$D$3:$D$53,M1,Results!$R$3:$R$53)/SUMIF(Results!$D$3:$D$53,M1,Results!$Q$3:$Q$53)</f>
         <v>0.8</v>
       </c>
-      <c r="N8" s="1" t="e">
-        <f>MAX(B8:G8)</f>
+      <c r="N8" s="22" t="e">
+        <f>MAX(B8:M8)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>122</v>
-      </c>
-      <c r="B9" s="1">
-        <f>COUNTIF(Data!$I$2:$I$53,Summary!B1)</f>
-        <v>11</v>
-      </c>
-      <c r="C9" s="1">
-        <f>COUNTIF(Data!$I$2:$I$53,Summary!C1)</f>
-        <v>11</v>
-      </c>
-      <c r="D9" s="1">
-        <f>COUNTIF(Data!$I$2:$I$53,Summary!D1)</f>
-        <v>10</v>
-      </c>
-      <c r="E9" s="1">
-        <f>COUNTIF(Data!$I$2:$I$53,Summary!E1)</f>
-        <v>9</v>
-      </c>
-      <c r="F9" s="1">
-        <f>COUNTIF(Data!$I$2:$I$53,Summary!F1)</f>
-        <v>0</v>
-      </c>
-      <c r="G9" s="1">
-        <f>COUNTIF(Data!$I$2:$I$53,Summary!G1)</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="1">
-        <f>COUNTIF(Data!$I$2:$I$53,Summary!H1)</f>
-        <v>1</v>
-      </c>
-      <c r="I9" s="1">
-        <f>COUNTIF(Data!$I$2:$I$53,Summary!I1)</f>
-        <v>1</v>
-      </c>
-      <c r="J9" s="1">
-        <f>COUNTIF(Data!$I$2:$I$53,Summary!J1)</f>
-        <v>1</v>
-      </c>
-      <c r="K9" s="1">
-        <f>COUNTIF(Data!$I$2:$I$53,Summary!K1)</f>
-        <v>1</v>
-      </c>
-      <c r="L9" s="1">
-        <f>COUNTIF(Data!$I$2:$I$53,Summary!L1)</f>
-        <v>1</v>
-      </c>
-      <c r="M9" s="1">
-        <f>COUNTIF(Data!$I$2:$I$53,Summary!M1)</f>
-        <v>1</v>
-      </c>
-      <c r="N9" s="1">
-        <f t="shared" ref="N9:N16" si="0">SUM(B9:G9)</f>
-        <v>41</v>
+        <v>222</v>
+      </c>
+      <c r="B9" s="23">
+        <f>SUMIF(Results!$D$3:$D$53,B1,Results!E$3:E$53)</f>
+        <v>2</v>
+      </c>
+      <c r="C9" s="23">
+        <f>SUMIF(Results!$D$3:$D$53,C1,Results!F$3:F$53)</f>
+        <v>3</v>
+      </c>
+      <c r="D9" s="23">
+        <f>SUMIF(Results!$D$3:$D$53,D1,Results!G$3:G$53)</f>
+        <v>2</v>
+      </c>
+      <c r="E9" s="23">
+        <f>SUMIF(Results!$D$3:$D$53,E1,Results!H$3:H$53)</f>
+        <v>3</v>
+      </c>
+      <c r="F9" s="23">
+        <f>SUMIF(Results!$D$3:$D$53,F1,Results!I$3:I$53)</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="23">
+        <f>SUMIF(Results!$D$3:$D$53,G1,Results!J$3:J$53)</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="23">
+        <f>SUMIF(Results!$D$3:$D$53,H1,Results!K$3:K$53)</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="23">
+        <f>SUMIF(Results!$D$3:$D$53,I1,Results!L$3:L$53)</f>
+        <v>1</v>
+      </c>
+      <c r="J9" s="23">
+        <f>SUMIF(Results!$D$3:$D$53,J1,Results!M$3:M$53)</f>
+        <v>0</v>
+      </c>
+      <c r="K9" s="23">
+        <f>SUMIF(Results!$D$3:$D$53,K1,Results!N$3:N$53)</f>
+        <v>1</v>
+      </c>
+      <c r="L9" s="23">
+        <f>SUMIF(Results!$D$3:$D$53,L1,Results!O$3:O$53)</f>
+        <v>0</v>
+      </c>
+      <c r="M9" s="23">
+        <f>SUMIF(Results!$D$3:$D$53,M1,Results!P$3:P$53)</f>
+        <v>1</v>
+      </c>
+      <c r="N9" s="24">
+        <f>SUM(B9:M9)</f>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B10" s="1">
+        <f>COUNTIF(Data!$I$2:$I$53,Summary!B1)</f>
+        <v>12</v>
+      </c>
+      <c r="C10" s="1">
+        <f>COUNTIF(Data!$I$2:$I$53,Summary!C1)</f>
+        <v>12</v>
+      </c>
+      <c r="D10" s="1">
+        <f>COUNTIF(Data!$I$2:$I$53,Summary!D1)</f>
+        <v>10</v>
+      </c>
+      <c r="E10" s="1">
+        <f>COUNTIF(Data!$I$2:$I$53,Summary!E1)</f>
+        <v>9</v>
+      </c>
+      <c r="F10" s="1">
+        <f>COUNTIF(Data!$I$2:$I$53,Summary!F1)</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <f>COUNTIF(Data!$I$2:$I$53,Summary!G1)</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <f>COUNTIF(Data!$I$2:$I$53,Summary!H1)</f>
+        <v>1</v>
+      </c>
+      <c r="I10" s="1">
+        <f>COUNTIF(Data!$I$2:$I$53,Summary!I1)</f>
+        <v>1</v>
+      </c>
+      <c r="J10" s="1">
+        <f>COUNTIF(Data!$I$2:$I$53,Summary!J1)</f>
+        <v>1</v>
+      </c>
+      <c r="K10" s="1">
+        <f>COUNTIF(Data!$I$2:$I$53,Summary!K1)</f>
+        <v>1</v>
+      </c>
+      <c r="L10" s="1">
+        <f>COUNTIF(Data!$I$2:$I$53,Summary!L1)</f>
+        <v>1</v>
+      </c>
+      <c r="M10" s="1">
+        <f>COUNTIF(Data!$I$2:$I$53,Summary!M1)</f>
+        <v>1</v>
+      </c>
+      <c r="N10" s="1">
+        <f>SUM(B10:M10)</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>221</v>
+      </c>
+      <c r="B11" s="7">
+        <f>SUMIF(Results!$D$3:$D$53,B1,Results!E$3:E$53)/COUNTIF(Results!$D$3:$D$53,B1)</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="C11" s="7">
+        <f>SUMIF(Results!$D$3:$D$53,C1,Results!F$3:F$53)/COUNTIF(Results!$D$3:$D$53,C1)</f>
+        <v>0.25</v>
+      </c>
+      <c r="D11" s="7">
+        <f>SUMIF(Results!$D$3:$D$53,D1,Results!G$3:G$53)/COUNTIF(Results!$D$3:$D$53,D1)</f>
+        <v>0.2</v>
+      </c>
+      <c r="E11" s="7">
+        <f>SUMIF(Results!$D$3:$D$53,E1,Results!H$3:H$53)/COUNTIF(Results!$D$3:$D$53,E1)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F11" s="7" t="e">
+        <f>SUMIF(Results!$D$3:$D$53,F1,Results!I$3:I$53)/COUNTIF(Results!$D$3:$D$53,F1)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G11" s="7" t="e">
+        <f>SUMIF(Results!$D$3:$D$53,G1,Results!J$3:J$53)/COUNTIF(Results!$D$3:$D$53,G1)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H11" s="7">
+        <f>SUMIF(Results!$D$3:$D$53,H1,Results!K$3:K$53)/COUNTIF(Results!$D$3:$D$53,H1)</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="7">
+        <f>SUMIF(Results!$D$3:$D$53,I1,Results!L$3:L$53)/COUNTIF(Results!$D$3:$D$53,I1)</f>
+        <v>1</v>
+      </c>
+      <c r="J11" s="7">
+        <f>SUMIF(Results!$D$3:$D$53,J1,Results!M$3:M$53)/COUNTIF(Results!$D$3:$D$53,J1)</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="7">
+        <f>SUMIF(Results!$D$3:$D$53,K1,Results!N$3:N$53)/COUNTIF(Results!$D$3:$D$53,K1)</f>
+        <v>1</v>
+      </c>
+      <c r="L11" s="7">
+        <f>SUMIF(Results!$D$3:$D$53,L1,Results!O$3:O$53)/COUNTIF(Results!$D$3:$D$53,L1)</f>
+        <v>0</v>
+      </c>
+      <c r="M11" s="7">
+        <f>SUMIF(Results!$D$3:$D$53,M1,Results!P$3:P$53)/COUNTIF(Results!$D$3:$D$53,M1)</f>
+        <v>1</v>
+      </c>
+      <c r="N11" s="6">
+        <f>N9/N10</f>
+        <v>0.26530612244897961</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B12" s="1">
         <f>SUMIF(Results!E3:E53,"&lt;&gt;#N/A")</f>
-        <v>23</v>
-      </c>
-      <c r="C10" s="1">
+        <v>25</v>
+      </c>
+      <c r="C12" s="1">
         <f>SUMIF(Results!F3:F53,"&lt;&gt;#N/A")</f>
+        <v>27</v>
+      </c>
+      <c r="D12" s="1">
+        <f>SUMIF(Results!G3:G53,"&lt;&gt;#N/A")</f>
         <v>26</v>
       </c>
-      <c r="D10" s="1">
-        <f>SUMIF(Results!G3:G53,"&lt;&gt;#N/A")</f>
-        <v>24</v>
-      </c>
-      <c r="E10" s="1">
+      <c r="E12" s="1">
         <f>SUMIF(Results!H3:H53,"&lt;&gt;#N/A")</f>
-        <v>26</v>
-      </c>
-      <c r="F10" s="1">
+        <v>27</v>
+      </c>
+      <c r="F12" s="1">
         <f>SUMIF(Results!I3:I53,"&lt;&gt;#N/A")</f>
         <v>1</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G12" s="1">
         <f>SUMIF(Results!J3:J53,"&lt;&gt;#N/A")</f>
         <v>2</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H12" s="1">
         <f>SUMIF(Results!K3:K53,"&lt;&gt;#N/A")</f>
         <v>0</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I12" s="1">
         <f>SUMIF(Results!L3:L53,"&lt;&gt;#N/A")</f>
         <v>1</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J12" s="1">
         <f>SUMIF(Results!M3:M53,"&lt;&gt;#N/A")</f>
         <v>0</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K12" s="1">
         <f>SUMIF(Results!N3:N53,"&lt;&gt;#N/A")</f>
         <v>1</v>
       </c>
-      <c r="L10" s="1">
+      <c r="L12" s="1">
         <f>SUMIF(Results!O3:O53,"&lt;&gt;#N/A")</f>
         <v>0</v>
       </c>
-      <c r="M10" s="1">
+      <c r="M12" s="1">
         <f>SUMIF(Results!P3:P53,"&lt;&gt;#N/A")</f>
         <v>1</v>
       </c>
-      <c r="N10" s="1">
-        <f t="shared" si="0"/>
-        <v>102</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B11" s="1">
-        <f>COUNTIFS(Results!E3:E53,"&lt;&gt;#N/A",Results!E3:E53,"&lt;&gt;")</f>
-        <v>46</v>
-      </c>
-      <c r="C11" s="1">
-        <f>COUNTIFS(Results!F3:F53,"&lt;&gt;#N/A",Results!F3:F53,"&lt;&gt;")</f>
-        <v>41</v>
-      </c>
-      <c r="D11" s="1">
-        <f>COUNTIFS(Results!G3:G53,"&lt;&gt;#N/A",Results!G3:G53,"&lt;&gt;")</f>
-        <v>45</v>
-      </c>
-      <c r="E11" s="1">
-        <f>COUNTIFS(Results!H3:H53,"&lt;&gt;#N/A",Results!H3:H53,"&lt;&gt;")</f>
-        <v>44</v>
-      </c>
-      <c r="F11" s="1">
-        <f>COUNTIFS(Results!I3:I53,"&lt;&gt;#N/A",Results!I3:I53,"&lt;&gt;")</f>
-        <v>3</v>
-      </c>
-      <c r="G11" s="1">
-        <f>COUNTIFS(Results!J3:J53,"&lt;&gt;#N/A",Results!J3:J53,"&lt;&gt;")</f>
-        <v>4</v>
-      </c>
-      <c r="H11" s="1">
-        <f>COUNTIFS(Results!K3:K53,"&lt;&gt;#N/A",Results!K3:K53,"&lt;&gt;")</f>
-        <v>1</v>
-      </c>
-      <c r="I11" s="1">
-        <f>COUNTIFS(Results!L3:L53,"&lt;&gt;#N/A",Results!L3:L53,"&lt;&gt;")</f>
-        <v>1</v>
-      </c>
-      <c r="J11" s="1">
-        <f>COUNTIFS(Results!M3:M53,"&lt;&gt;#N/A",Results!M3:M53,"&lt;&gt;")</f>
-        <v>1</v>
-      </c>
-      <c r="K11" s="1">
-        <f>COUNTIFS(Results!N3:N53,"&lt;&gt;#N/A",Results!N3:N53,"&lt;&gt;")</f>
-        <v>1</v>
-      </c>
-      <c r="L11" s="1">
-        <f>COUNTIFS(Results!O3:O53,"&lt;&gt;#N/A",Results!O3:O53,"&lt;&gt;")</f>
-        <v>1</v>
-      </c>
-      <c r="M11" s="1">
-        <f>COUNTIFS(Results!P3:P53,"&lt;&gt;#N/A",Results!P3:P53,"&lt;&gt;")</f>
-        <v>1</v>
-      </c>
-      <c r="N11" s="1">
-        <f t="shared" si="0"/>
-        <v>183</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12" s="1">
-        <f>SUMIFS(Results!E3:E53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!E3:E53, "&lt;&gt;#N/A")</f>
-        <v>10</v>
-      </c>
-      <c r="C12" s="1">
-        <f>SUMIFS(Results!F3:F53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!F3:F53, "&lt;&gt;#N/A")</f>
-        <v>15</v>
-      </c>
-      <c r="D12" s="1">
-        <f>SUMIFS(Results!G3:G53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!G3:G53, "&lt;&gt;#N/A")</f>
-        <v>14</v>
-      </c>
-      <c r="E12" s="1">
-        <f>SUMIFS(Results!H3:H53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!H3:H53, "&lt;&gt;#N/A")</f>
-        <v>11</v>
-      </c>
-      <c r="F12" s="1">
-        <f>SUMIFS(Results!I3:I53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!I3:I53, "&lt;&gt;#N/A")</f>
-        <v>1</v>
-      </c>
-      <c r="G12" s="1">
-        <f>SUMIFS(Results!J3:J53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!J3:J53, "&lt;&gt;#N/A")</f>
-        <v>2</v>
-      </c>
-      <c r="H12" s="1">
-        <f>SUMIFS(Results!K3:K53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!K3:K53, "&lt;&gt;#N/A")</f>
-        <v>0</v>
-      </c>
-      <c r="I12" s="1">
-        <f>SUMIFS(Results!L3:L53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!L3:L53, "&lt;&gt;#N/A")</f>
-        <v>0</v>
-      </c>
-      <c r="J12" s="1">
-        <f>SUMIFS(Results!M3:M53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!M3:M53, "&lt;&gt;#N/A")</f>
-        <v>0</v>
-      </c>
-      <c r="K12" s="1">
-        <f>SUMIFS(Results!N3:N53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!N3:N53, "&lt;&gt;#N/A")</f>
-        <v>0</v>
-      </c>
-      <c r="L12" s="1">
-        <f>SUMIFS(Results!O3:O53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!O3:O53, "&lt;&gt;#N/A")</f>
-        <v>0</v>
-      </c>
-      <c r="M12" s="1">
-        <f>SUMIFS(Results!P3:P53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!P3:P53, "&lt;&gt;#N/A")</f>
-        <v>1</v>
-      </c>
       <c r="N12" s="1">
-        <f t="shared" si="0"/>
-        <v>53</v>
+        <f>SUM(B12:M12)</f>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B13" s="1">
-        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!E3:E53, "&lt;&gt;#N/A", Results!E3:E53, "&lt;&gt;")</f>
-        <v>24</v>
+        <f>COUNTIFS(Results!E3:E53,"&lt;&gt;#N/A",Results!E3:E53,"&lt;&gt;")</f>
+        <v>48</v>
       </c>
       <c r="C13" s="1">
-        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!F3:F53, "&lt;&gt;#N/A", Results!F3:F53, "&lt;&gt;")</f>
-        <v>21</v>
+        <f>COUNTIFS(Results!F3:F53,"&lt;&gt;#N/A",Results!F3:F53,"&lt;&gt;")</f>
+        <v>43</v>
       </c>
       <c r="D13" s="1">
-        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!G3:G53, "&lt;&gt;#N/A", Results!G3:G53, "&lt;&gt;")</f>
-        <v>24</v>
+        <f>COUNTIFS(Results!G3:G53,"&lt;&gt;#N/A",Results!G3:G53,"&lt;&gt;")</f>
+        <v>47</v>
       </c>
       <c r="E13" s="1">
-        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!H3:H53, "&lt;&gt;#N/A", Results!H3:H53, "&lt;&gt;")</f>
-        <v>22</v>
+        <f>COUNTIFS(Results!H3:H53,"&lt;&gt;#N/A",Results!H3:H53,"&lt;&gt;")</f>
+        <v>46</v>
       </c>
       <c r="F13" s="1">
-        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!I3:I53, "&lt;&gt;#N/A", Results!I3:I53, "&lt;&gt;")</f>
+        <f>COUNTIFS(Results!I3:I53,"&lt;&gt;#N/A",Results!I3:I53,"&lt;&gt;")</f>
         <v>3</v>
       </c>
       <c r="G13" s="1">
-        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!J3:J53, "&lt;&gt;#N/A", Results!J3:J53, "&lt;&gt;")</f>
+        <f>COUNTIFS(Results!J3:J53,"&lt;&gt;#N/A",Results!J3:J53,"&lt;&gt;")</f>
         <v>4</v>
       </c>
       <c r="H13" s="1">
-        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!K3:K53, "&lt;&gt;#N/A", Results!K3:K53, "&lt;&gt;")</f>
-        <v>0</v>
+        <f>COUNTIFS(Results!K3:K53,"&lt;&gt;#N/A",Results!K3:K53,"&lt;&gt;")</f>
+        <v>1</v>
       </c>
       <c r="I13" s="1">
-        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!L3:L53, "&lt;&gt;#N/A", Results!L3:L53, "&lt;&gt;")</f>
-        <v>0</v>
+        <f>COUNTIFS(Results!L3:L53,"&lt;&gt;#N/A",Results!L3:L53,"&lt;&gt;")</f>
+        <v>1</v>
       </c>
       <c r="J13" s="1">
-        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!M3:M53, "&lt;&gt;#N/A", Results!M3:M53, "&lt;&gt;")</f>
+        <f>COUNTIFS(Results!M3:M53,"&lt;&gt;#N/A",Results!M3:M53,"&lt;&gt;")</f>
         <v>1</v>
       </c>
       <c r="K13" s="1">
-        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!N3:N53, "&lt;&gt;#N/A", Results!N3:N53, "&lt;&gt;")</f>
-        <v>0</v>
+        <f>COUNTIFS(Results!N3:N53,"&lt;&gt;#N/A",Results!N3:N53,"&lt;&gt;")</f>
+        <v>1</v>
       </c>
       <c r="L13" s="1">
-        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!O3:O53, "&lt;&gt;#N/A", Results!O3:O53, "&lt;&gt;")</f>
-        <v>0</v>
+        <f>COUNTIFS(Results!O3:O53,"&lt;&gt;#N/A",Results!O3:O53,"&lt;&gt;")</f>
+        <v>1</v>
       </c>
       <c r="M13" s="1">
-        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!P3:P53, "&lt;&gt;#N/A", Results!P3:P53, "&lt;&gt;")</f>
+        <f>COUNTIFS(Results!P3:P53,"&lt;&gt;#N/A",Results!P3:P53,"&lt;&gt;")</f>
         <v>1</v>
       </c>
       <c r="N13" s="1">
-        <f t="shared" si="0"/>
-        <v>98</v>
+        <f>SUM(B13:M13)</f>
+        <v>197</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B14" s="1">
-        <f>SUMIFS(Results!E3:E53,Results!$B$3:$B$53,"=#N/A",Results!E3:E53, "&lt;&gt;#N/A")</f>
-        <v>13</v>
+        <f>SUMIFS(Results!E3:E53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!E3:E53, "&lt;&gt;#N/A")</f>
+        <v>10</v>
       </c>
       <c r="C14" s="1">
-        <f>SUMIFS(Results!F3:F53,Results!$B$3:$B$53,"=#N/A",Results!F3:F53, "&lt;&gt;#N/A")</f>
+        <f>SUMIFS(Results!F3:F53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!F3:F53, "&lt;&gt;#N/A")</f>
+        <v>15</v>
+      </c>
+      <c r="D14" s="1">
+        <f>SUMIFS(Results!G3:G53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!G3:G53, "&lt;&gt;#N/A")</f>
+        <v>14</v>
+      </c>
+      <c r="E14" s="1">
+        <f>SUMIFS(Results!H3:H53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!H3:H53, "&lt;&gt;#N/A")</f>
         <v>11</v>
       </c>
-      <c r="D14" s="1">
-        <f>SUMIFS(Results!G3:G53,Results!$B$3:$B$53,"=#N/A",Results!G3:G53, "&lt;&gt;#N/A")</f>
-        <v>10</v>
-      </c>
-      <c r="E14" s="1">
-        <f>SUMIFS(Results!H3:H53,Results!$B$3:$B$53,"=#N/A",Results!H3:H53, "&lt;&gt;#N/A")</f>
-        <v>15</v>
-      </c>
       <c r="F14" s="1">
-        <f>SUMIFS(Results!I3:I53,Results!$B$3:$B$53,"=#N/A",Results!I3:I53, "&lt;&gt;#N/A")</f>
-        <v>0</v>
+        <f>SUMIFS(Results!I3:I53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!I3:I53, "&lt;&gt;#N/A")</f>
+        <v>1</v>
       </c>
       <c r="G14" s="1">
-        <f>SUMIFS(Results!J3:J53,Results!$B$3:$B$53,"=#N/A",Results!J3:J53, "&lt;&gt;#N/A")</f>
-        <v>0</v>
+        <f>SUMIFS(Results!J3:J53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!J3:J53, "&lt;&gt;#N/A")</f>
+        <v>2</v>
       </c>
       <c r="H14" s="1">
-        <f>SUMIFS(Results!K3:K53,Results!$B$3:$B$53,"=#N/A",Results!K3:K53, "&lt;&gt;#N/A")</f>
+        <f>SUMIFS(Results!K3:K53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!K3:K53, "&lt;&gt;#N/A")</f>
         <v>0</v>
       </c>
       <c r="I14" s="1">
-        <f>SUMIFS(Results!L3:L53,Results!$B$3:$B$53,"=#N/A",Results!L3:L53, "&lt;&gt;#N/A")</f>
-        <v>1</v>
+        <f>SUMIFS(Results!L3:L53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!L3:L53, "&lt;&gt;#N/A")</f>
+        <v>0</v>
       </c>
       <c r="J14" s="1">
-        <f>SUMIFS(Results!M3:M53,Results!$B$3:$B$53,"=#N/A",Results!M3:M53, "&lt;&gt;#N/A")</f>
+        <f>SUMIFS(Results!M3:M53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!M3:M53, "&lt;&gt;#N/A")</f>
         <v>0</v>
       </c>
       <c r="K14" s="1">
-        <f>SUMIFS(Results!N3:N53,Results!$B$3:$B$53,"=#N/A",Results!N3:N53, "&lt;&gt;#N/A")</f>
+        <f>SUMIFS(Results!N3:N53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!N3:N53, "&lt;&gt;#N/A")</f>
         <v>1</v>
       </c>
       <c r="L14" s="1">
-        <f>SUMIFS(Results!O3:O53,Results!$B$3:$B$53,"=#N/A",Results!O3:O53, "&lt;&gt;#N/A")</f>
+        <f>SUMIFS(Results!O3:O53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!O3:O53, "&lt;&gt;#N/A")</f>
         <v>0</v>
       </c>
       <c r="M14" s="1">
-        <f>SUMIFS(Results!P3:P53,Results!$B$3:$B$53,"=#N/A",Results!P3:P53, "&lt;&gt;#N/A")</f>
-        <v>0</v>
+        <f>SUMIFS(Results!P3:P53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!P3:P53, "&lt;&gt;#N/A")</f>
+        <v>1</v>
       </c>
       <c r="N14" s="1">
-        <f t="shared" si="0"/>
-        <v>49</v>
+        <f>SUM(B14:M14)</f>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B15" s="1">
-        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!E3:E53, "&lt;&gt;#N/A", Results!E3:E53, "&lt;&gt;")</f>
+        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!E3:E53, "&lt;&gt;#N/A", Results!E3:E53, "&lt;&gt;")</f>
+        <v>24</v>
+      </c>
+      <c r="C15" s="1">
+        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!F3:F53, "&lt;&gt;#N/A", Results!F3:F53, "&lt;&gt;")</f>
+        <v>21</v>
+      </c>
+      <c r="D15" s="1">
+        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!G3:G53, "&lt;&gt;#N/A", Results!G3:G53, "&lt;&gt;")</f>
+        <v>24</v>
+      </c>
+      <c r="E15" s="1">
+        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!H3:H53, "&lt;&gt;#N/A", Results!H3:H53, "&lt;&gt;")</f>
         <v>22</v>
       </c>
-      <c r="C15" s="1">
-        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!F3:F53, "&lt;&gt;#N/A", Results!F3:F53, "&lt;&gt;")</f>
-        <v>20</v>
-      </c>
-      <c r="D15" s="1">
-        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!G3:G53, "&lt;&gt;#N/A", Results!G3:G53, "&lt;&gt;")</f>
-        <v>21</v>
-      </c>
-      <c r="E15" s="1">
-        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!H3:H53, "&lt;&gt;#N/A", Results!H3:H53, "&lt;&gt;")</f>
-        <v>22</v>
-      </c>
       <c r="F15" s="1">
-        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!I3:I53, "&lt;&gt;#N/A", Results!I3:I53, "&lt;&gt;")</f>
-        <v>0</v>
+        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!I3:I53, "&lt;&gt;#N/A", Results!I3:I53, "&lt;&gt;")</f>
+        <v>3</v>
       </c>
       <c r="G15" s="1">
-        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!J3:J53, "&lt;&gt;#N/A", Results!J3:J53, "&lt;&gt;")</f>
-        <v>0</v>
+        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!J3:J53, "&lt;&gt;#N/A", Results!J3:J53, "&lt;&gt;")</f>
+        <v>4</v>
       </c>
       <c r="H15" s="1">
-        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!K3:K53, "&lt;&gt;#N/A", Results!K3:K53, "&lt;&gt;")</f>
-        <v>1</v>
+        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!K3:K53, "&lt;&gt;#N/A", Results!K3:K53, "&lt;&gt;")</f>
+        <v>0</v>
       </c>
       <c r="I15" s="1">
-        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!L3:L53, "&lt;&gt;#N/A", Results!L3:L53, "&lt;&gt;")</f>
-        <v>1</v>
+        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!L3:L53, "&lt;&gt;#N/A", Results!L3:L53, "&lt;&gt;")</f>
+        <v>0</v>
       </c>
       <c r="J15" s="1">
-        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!M3:M53, "&lt;&gt;#N/A", Results!M3:M53, "&lt;&gt;")</f>
-        <v>0</v>
+        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!M3:M53, "&lt;&gt;#N/A", Results!M3:M53, "&lt;&gt;")</f>
+        <v>1</v>
       </c>
       <c r="K15" s="1">
-        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!N3:N53, "&lt;&gt;#N/A", Results!N3:N53, "&lt;&gt;")</f>
+        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!N3:N53, "&lt;&gt;#N/A", Results!N3:N53, "&lt;&gt;")</f>
         <v>1</v>
       </c>
       <c r="L15" s="1">
-        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!O3:O53, "&lt;&gt;#N/A", Results!O3:O53, "&lt;&gt;")</f>
-        <v>1</v>
+        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!O3:O53, "&lt;&gt;#N/A", Results!O3:O53, "&lt;&gt;")</f>
+        <v>0</v>
       </c>
       <c r="M15" s="1">
-        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!P3:P53, "&lt;&gt;#N/A", Results!P3:P53, "&lt;&gt;")</f>
-        <v>0</v>
+        <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!P3:P53, "&lt;&gt;#N/A", Results!P3:P53, "&lt;&gt;")</f>
+        <v>1</v>
       </c>
       <c r="N15" s="1">
-        <f t="shared" si="0"/>
-        <v>85</v>
+        <f>SUM(B15:M15)</f>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="B16" s="1">
-        <f>SUMIF(Results!$C$3:$C$53,Summary!B1,Results!$S$3:$S$53)</f>
-        <v>0</v>
+        <f>SUMIFS(Results!E3:E53,Results!$B$3:$B$53,"=#N/A",Results!E3:E53, "&lt;&gt;#N/A")</f>
+        <v>15</v>
       </c>
       <c r="C16" s="1">
-        <f>SUMIF(Results!$C$3:$C$53,Summary!C1,Results!$S$3:$S$53)</f>
-        <v>0</v>
+        <f>SUMIFS(Results!F3:F53,Results!$B$3:$B$53,"=#N/A",Results!F3:F53, "&lt;&gt;#N/A")</f>
+        <v>12</v>
       </c>
       <c r="D16" s="1">
-        <f>SUMIF(Results!$C$3:$C$53,Summary!D1,Results!$S$3:$S$53)</f>
-        <v>0</v>
+        <f>SUMIFS(Results!G3:G53,Results!$B$3:$B$53,"=#N/A",Results!G3:G53, "&lt;&gt;#N/A")</f>
+        <v>12</v>
       </c>
       <c r="E16" s="1">
-        <f>SUMIF(Results!$C$3:$C$53,Summary!E1,Results!$S$3:$S$53)</f>
-        <v>1</v>
+        <f>SUMIFS(Results!H3:H53,Results!$B$3:$B$53,"=#N/A",Results!H3:H53, "&lt;&gt;#N/A")</f>
+        <v>16</v>
       </c>
       <c r="F16" s="1">
-        <f>SUMIF(Results!$C$3:$C$53,Summary!F1,Results!$S$3:$S$53)</f>
+        <f>SUMIFS(Results!I3:I53,Results!$B$3:$B$53,"=#N/A",Results!I3:I53, "&lt;&gt;#N/A")</f>
         <v>0</v>
       </c>
       <c r="G16" s="1">
-        <f>SUMIF(Results!$C$3:$C$53,Summary!G1,Results!$S$3:$S$53)</f>
-        <v>5</v>
+        <f>SUMIFS(Results!J3:J53,Results!$B$3:$B$53,"=#N/A",Results!J3:J53, "&lt;&gt;#N/A")</f>
+        <v>0</v>
       </c>
       <c r="H16" s="1">
-        <f>SUMIF(Results!$C$3:$C$53,Summary!H1,Results!$S$3:$S$53)</f>
+        <f>SUMIFS(Results!K3:K53,Results!$B$3:$B$53,"=#N/A",Results!K3:K53, "&lt;&gt;#N/A")</f>
         <v>0</v>
       </c>
       <c r="I16" s="1">
-        <f>SUMIF(Results!$C$3:$C$53,Summary!I1,Results!$S$3:$S$53)</f>
-        <v>0</v>
+        <f>SUMIFS(Results!L3:L53,Results!$B$3:$B$53,"=#N/A",Results!L3:L53, "&lt;&gt;#N/A")</f>
+        <v>1</v>
       </c>
       <c r="J16" s="1">
-        <f>SUMIF(Results!$C$3:$C$53,Summary!J1,Results!$S$3:$S$53)</f>
+        <f>SUMIFS(Results!M3:M53,Results!$B$3:$B$53,"=#N/A",Results!M3:M53, "&lt;&gt;#N/A")</f>
         <v>0</v>
       </c>
       <c r="K16" s="1">
-        <f>SUMIF(Results!$C$3:$C$53,Summary!K1,Results!$S$3:$S$53)</f>
+        <f>SUMIFS(Results!N3:N53,Results!$B$3:$B$53,"=#N/A",Results!N3:N53, "&lt;&gt;#N/A")</f>
         <v>0</v>
       </c>
       <c r="L16" s="1">
-        <f>SUMIF(Results!$C$3:$C$53,Summary!L1,Results!$S$3:$S$53)</f>
+        <f>SUMIFS(Results!O3:O53,Results!$B$3:$B$53,"=#N/A",Results!O3:O53, "&lt;&gt;#N/A")</f>
         <v>0</v>
       </c>
       <c r="M16" s="1">
-        <f>SUMIF(Results!$C$3:$C$53,Summary!M1,Results!$S$3:$S$53)</f>
-        <v>0</v>
-      </c>
-      <c r="N16" s="19">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f>SUMIFS(Results!P3:P53,Results!$B$3:$B$53,"=#N/A",Results!P3:P53, "&lt;&gt;#N/A")</f>
+        <v>0</v>
+      </c>
+      <c r="N16" s="1">
+        <f>SUM(B16:M16)</f>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="1">
+        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!E3:E53, "&lt;&gt;#N/A", Results!E3:E53, "&lt;&gt;")</f>
+        <v>24</v>
+      </c>
+      <c r="C17" s="1">
+        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!F3:F53, "&lt;&gt;#N/A", Results!F3:F53, "&lt;&gt;")</f>
+        <v>22</v>
+      </c>
+      <c r="D17" s="1">
+        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!G3:G53, "&lt;&gt;#N/A", Results!G3:G53, "&lt;&gt;")</f>
+        <v>23</v>
+      </c>
+      <c r="E17" s="1">
+        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!H3:H53, "&lt;&gt;#N/A", Results!H3:H53, "&lt;&gt;")</f>
+        <v>24</v>
+      </c>
+      <c r="F17" s="1">
+        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!I3:I53, "&lt;&gt;#N/A", Results!I3:I53, "&lt;&gt;")</f>
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!J3:J53, "&lt;&gt;#N/A", Results!J3:J53, "&lt;&gt;")</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="1">
+        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!K3:K53, "&lt;&gt;#N/A", Results!K3:K53, "&lt;&gt;")</f>
+        <v>1</v>
+      </c>
+      <c r="I17" s="1">
+        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!L3:L53, "&lt;&gt;#N/A", Results!L3:L53, "&lt;&gt;")</f>
+        <v>1</v>
+      </c>
+      <c r="J17" s="1">
+        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!M3:M53, "&lt;&gt;#N/A", Results!M3:M53, "&lt;&gt;")</f>
+        <v>0</v>
+      </c>
+      <c r="K17" s="1">
+        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!N3:N53, "&lt;&gt;#N/A", Results!N3:N53, "&lt;&gt;")</f>
+        <v>0</v>
+      </c>
+      <c r="L17" s="1">
+        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!O3:O53, "&lt;&gt;#N/A", Results!O3:O53, "&lt;&gt;")</f>
+        <v>1</v>
+      </c>
+      <c r="M17" s="1">
+        <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!P3:P53, "&lt;&gt;#N/A", Results!P3:P53, "&lt;&gt;")</f>
+        <v>0</v>
+      </c>
+      <c r="N17" s="1">
+        <f>SUM(B17:M17)</f>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="1">
+        <f>SUMIF(Results!$C$3:$C$53,Summary!B1,Results!$S$3:$S$53)</f>
+        <v>0</v>
+      </c>
+      <c r="C18" s="1">
+        <f>SUMIF(Results!$C$3:$C$53,Summary!C1,Results!$S$3:$S$53)</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="1">
+        <f>SUMIF(Results!$C$3:$C$53,Summary!D1,Results!$S$3:$S$53)</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
+        <f>SUMIF(Results!$C$3:$C$53,Summary!E1,Results!$S$3:$S$53)</f>
+        <v>1</v>
+      </c>
+      <c r="F18" s="1">
+        <f>SUMIF(Results!$C$3:$C$53,Summary!F1,Results!$S$3:$S$53)</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
+        <f>SUMIF(Results!$C$3:$C$53,Summary!G1,Results!$S$3:$S$53)</f>
+        <v>5</v>
+      </c>
+      <c r="H18" s="1">
+        <f>SUMIF(Results!$C$3:$C$53,Summary!H1,Results!$S$3:$S$53)</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="1">
+        <f>SUMIF(Results!$C$3:$C$53,Summary!I1,Results!$S$3:$S$53)</f>
+        <v>0</v>
+      </c>
+      <c r="J18" s="1">
+        <f>SUMIF(Results!$C$3:$C$53,Summary!J1,Results!$S$3:$S$53)</f>
+        <v>0</v>
+      </c>
+      <c r="K18" s="1">
+        <f>SUMIF(Results!$C$3:$C$53,Summary!K1,Results!$S$3:$S$53)</f>
+        <v>0</v>
+      </c>
+      <c r="L18" s="1">
+        <f>SUMIF(Results!$C$3:$C$53,Summary!L1,Results!$S$3:$S$53)</f>
+        <v>0</v>
+      </c>
+      <c r="M18" s="1">
+        <f>SUMIF(Results!$C$3:$C$53,Summary!M1,Results!$S$3:$S$53)</f>
+        <v>0</v>
+      </c>
+      <c r="N18" s="19">
+        <f>SUM(Results!S3:S53)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B19" s="1">
         <f>SUMIF(Results!E3:E53,"&lt;&gt;#N/A",Results!$T$3:$T$53)</f>
-        <v>6</v>
-      </c>
-      <c r="C17" s="1">
+        <v>7</v>
+      </c>
+      <c r="C19" s="1">
         <f>SUMIF(Results!F3:F53,"&lt;&gt;#N/A",Results!$T$3:$T$53)</f>
-        <v>6</v>
-      </c>
-      <c r="D17" s="1">
+        <v>7</v>
+      </c>
+      <c r="D19" s="1">
         <f>SUMIF(Results!G3:G53,"&lt;&gt;#N/A",Results!$T$3:$T$53)</f>
-        <v>6</v>
-      </c>
-      <c r="E17" s="1">
+        <v>7</v>
+      </c>
+      <c r="E19" s="1">
         <f>SUMIF(Results!H3:H53,"&lt;&gt;#N/A",Results!$T$3:$T$53)</f>
-        <v>6</v>
-      </c>
-      <c r="F17" s="1">
+        <v>7</v>
+      </c>
+      <c r="F19" s="1">
         <f>SUMIF(Results!I3:I53,"&lt;&gt;#N/A",Results!$T$3:$T$53)</f>
         <v>0</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G19" s="1">
         <f>SUMIF(Results!J3:J53,"&lt;&gt;#N/A",Results!$T$3:$T$53)</f>
         <v>0</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H19" s="1">
         <f>SUMIF(Results!K3:K53,"&lt;&gt;#N/A",Results!$T$3:$T$53)</f>
         <v>0</v>
       </c>
-      <c r="I17" s="1">
+      <c r="I19" s="1">
         <f>SUMIF(Results!L3:L53,"&lt;&gt;#N/A",Results!$T$3:$T$53)</f>
         <v>0</v>
       </c>
-      <c r="J17" s="1">
+      <c r="J19" s="1">
         <f>SUMIF(Results!M3:M53,"&lt;&gt;#N/A",Results!$T$3:$T$53)</f>
         <v>0</v>
       </c>
-      <c r="K17" s="1">
+      <c r="K19" s="1">
         <f>SUMIF(Results!N3:N53,"&lt;&gt;#N/A",Results!$T$3:$T$53)</f>
-        <v>0</v>
-      </c>
-      <c r="L17" s="1">
+        <v>1</v>
+      </c>
+      <c r="L19" s="1">
         <f>SUMIF(Results!O3:O53,"&lt;&gt;#N/A",Results!$T$3:$T$53)</f>
         <v>0</v>
       </c>
-      <c r="M17" s="1">
+      <c r="M19" s="1">
         <f>SUMIF(Results!P3:P53,"&lt;&gt;#N/A",Results!$T$3:$T$53)</f>
         <v>0</v>
       </c>
-      <c r="N17" s="19">
+      <c r="N19" s="19">
         <f>SUM(Results!T3:T53)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B9:M9">
-    <cfRule type="top10" dxfId="7" priority="8" rank="1"/>
+  <conditionalFormatting sqref="B10:M10">
+    <cfRule type="top10" dxfId="19" priority="10" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8:G8 N11">
+    <cfRule type="top10" dxfId="18" priority="9" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:G7">
+    <cfRule type="top10" dxfId="17" priority="8" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6:G6">
+    <cfRule type="top10" dxfId="16" priority="7" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:G5">
+    <cfRule type="top10" dxfId="15" priority="6" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:G4">
+    <cfRule type="top10" dxfId="14" priority="5" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:G3">
+    <cfRule type="top10" dxfId="13" priority="4" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:G2">
+    <cfRule type="top10" dxfId="12" priority="3" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:G8">
-    <cfRule type="top10" dxfId="6" priority="7" rank="1"/>
+    <cfRule type="top10" dxfId="11" priority="2" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7:G7">
-    <cfRule type="top10" dxfId="5" priority="6" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B6:G6">
-    <cfRule type="top10" dxfId="4" priority="5" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B5:G5">
-    <cfRule type="top10" dxfId="3" priority="4" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B4:G4">
-    <cfRule type="top10" dxfId="2" priority="3" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3:G3">
-    <cfRule type="top10" dxfId="1" priority="2" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:G2">
-    <cfRule type="top10" dxfId="0" priority="1" rank="1"/>
+  <conditionalFormatting sqref="B11:G11">
+    <cfRule type="top10" dxfId="10" priority="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -20282,8 +21351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+    <sheetView topLeftCell="A29" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="N62" sqref="N62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated through episode 651 which is the very last episode of 2017
</commit_message>
<xml_diff>
--- a/SGU_Science_or_Fiction.xlsx
+++ b/SGU_Science_or_Fiction.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="227">
   <si>
     <t>Episode</t>
   </si>
@@ -700,6 +700,18 @@
   </si>
   <si>
     <t>Correct Guesses When Answring First</t>
+  </si>
+  <si>
+    <t>New research on medieval cathedral glass finds that it flows 16 orders of magnitude faster than previously estimated.</t>
+  </si>
+  <si>
+    <t>New flu vaccine practice guidelines increase precautions for patients with egg allergies due to an increase in reported allergic reactions.</t>
+  </si>
+  <si>
+    <t>Researchers have successfully harnessed sperm to deliver chemotherapy directly to cervical cancer cells.</t>
+  </si>
+  <si>
+    <t>Science News Stories You May Have Missed</t>
   </si>
 </sst>
 </file>
@@ -855,12 +867,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -870,6 +876,12 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -877,417 +889,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="51">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1675,16 +1277,16 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>0.52083333333333337</c:v>
+                  <c:v>0.52</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.62790697674418605</c:v>
+                  <c:v>0.62222222222222223</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.55319148936170215</c:v>
+                  <c:v>0.53061224489795922</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.58695652173913049</c:v>
+                  <c:v>0.58333333333333337</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.33333333333333331</c:v>
@@ -1711,7 +1313,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.56345177664974622</c:v>
+                  <c:v>0.55609756097560981</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1727,8 +1329,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="127263760"/>
-        <c:axId val="127264152"/>
+        <c:axId val="190107168"/>
+        <c:axId val="190038032"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -1828,16 +1430,16 @@
                       <c:formatCode>0.0%</c:formatCode>
                       <c:ptCount val="13"/>
                       <c:pt idx="0">
-                        <c:v>0.41666666666666669</c:v>
+                        <c:v>0.44</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.7142857142857143</c:v>
+                        <c:v>0.68181818181818177</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.58333333333333337</c:v>
+                        <c:v>0.56000000000000005</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0.5</c:v>
+                        <c:v>0.47826086956521741</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>0.33333333333333331</c:v>
@@ -1864,7 +1466,7 @@
                         <c:v>1</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>0.54455445544554459</c:v>
+                        <c:v>0.53333333333333333</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1968,16 +1570,16 @@
                       <c:formatCode>0.0%</c:formatCode>
                       <c:ptCount val="13"/>
                       <c:pt idx="0">
-                        <c:v>0.625</c:v>
+                        <c:v>0.6</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.54545454545454541</c:v>
+                        <c:v>0.56521739130434778</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.52173913043478259</c:v>
+                        <c:v>0.5</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0.66666666666666663</c:v>
+                        <c:v>0.68</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>0</c:v>
@@ -2004,7 +1606,7 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>0.58333333333333337</c:v>
+                        <c:v>0.57999999999999996</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2148,16 +1750,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>48</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>47</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>46</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>3</c:v>
@@ -2184,7 +1786,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>197</c:v>
+                  <c:v>205</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2200,11 +1802,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="127264936"/>
-        <c:axId val="127264544"/>
+        <c:axId val="190352856"/>
+        <c:axId val="190164472"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="127263760"/>
+        <c:axId val="190107168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2247,7 +1849,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="127264152"/>
+        <c:crossAx val="190038032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2255,7 +1857,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="127264152"/>
+        <c:axId val="190038032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2306,12 +1908,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="127263760"/>
+        <c:crossAx val="190107168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="127264544"/>
+        <c:axId val="190164472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2348,12 +1950,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="127264936"/>
+        <c:crossAx val="190352856"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="127264936"/>
+        <c:axId val="190352856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2362,7 +1964,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127264544"/>
+        <c:crossAx val="190164472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2759,16 +2361,16 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>0.41666666666666669</c:v>
+                  <c:v>0.44</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.7142857142857143</c:v>
+                  <c:v>0.68181818181818177</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.58333333333333337</c:v>
+                  <c:v>0.56000000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5</c:v>
+                  <c:v>0.47826086956521741</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.33333333333333331</c:v>
@@ -2795,7 +2397,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.54455445544554459</c:v>
+                  <c:v>0.53333333333333333</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -2812,8 +2414,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="177541528"/>
-        <c:axId val="177541920"/>
+        <c:axId val="189827904"/>
+        <c:axId val="189828288"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -3007,16 +2609,16 @@
                       <c:formatCode>0.0%</c:formatCode>
                       <c:ptCount val="13"/>
                       <c:pt idx="0">
-                        <c:v>0.52083333333333337</c:v>
+                        <c:v>0.52</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.62790697674418605</c:v>
+                        <c:v>0.62222222222222223</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.55319148936170215</c:v>
+                        <c:v>0.53061224489795922</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0.58695652173913049</c:v>
+                        <c:v>0.58333333333333337</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>0.33333333333333331</c:v>
@@ -3043,7 +2645,7 @@
                         <c:v>1</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>0.56345177664974622</c:v>
+                        <c:v>0.55609756097560981</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3147,16 +2749,16 @@
                       <c:formatCode>0.0%</c:formatCode>
                       <c:ptCount val="13"/>
                       <c:pt idx="0">
-                        <c:v>0.625</c:v>
+                        <c:v>0.6</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.54545454545454541</c:v>
+                        <c:v>0.56521739130434778</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.52173913043478259</c:v>
+                        <c:v>0.5</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0.66666666666666663</c:v>
+                        <c:v>0.68</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>0</c:v>
@@ -3183,7 +2785,7 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>0.58333333333333337</c:v>
+                        <c:v>0.57999999999999996</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3328,16 +2930,16 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="13"/>
                       <c:pt idx="0">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>45</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>49</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
                         <c:v>48</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>43</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>47</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>46</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>3</c:v>
@@ -3364,7 +2966,7 @@
                         <c:v>1</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>197</c:v>
+                        <c:v>205</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3415,16 +3017,16 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="13"/>
                       <c:pt idx="0">
+                        <c:v>25</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>23</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
                         <c:v>24</c:v>
                       </c:pt>
-                      <c:pt idx="1">
-                        <c:v>22</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>23</c:v>
-                      </c:pt>
                       <c:pt idx="3">
-                        <c:v>24</c:v>
+                        <c:v>25</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>0</c:v>
@@ -3451,7 +3053,7 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>96</c:v>
+                        <c:v>100</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3553,16 +3155,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>3</c:v>
@@ -3589,7 +3191,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>101</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3605,11 +3207,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="177542704"/>
-        <c:axId val="177542312"/>
+        <c:axId val="189942952"/>
+        <c:axId val="189928232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="177541528"/>
+        <c:axId val="189827904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3652,7 +3254,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="177541920"/>
+        <c:crossAx val="189828288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3660,7 +3262,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="177541920"/>
+        <c:axId val="189828288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3711,12 +3313,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="177541528"/>
+        <c:crossAx val="189827904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="177542312"/>
+        <c:axId val="189928232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3753,12 +3355,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="177542704"/>
+        <c:crossAx val="189942952"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="177542704"/>
+        <c:axId val="189942952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3767,7 +3369,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="177542312"/>
+        <c:crossAx val="189928232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4164,16 +3766,16 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>0.625</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.54545454545454541</c:v>
+                  <c:v>0.56521739130434778</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.52173913043478259</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.66666666666666663</c:v>
+                  <c:v>0.68</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4200,7 +3802,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.58333333333333337</c:v>
+                  <c:v>0.57999999999999996</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -4217,8 +3819,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="177543880"/>
-        <c:axId val="177544272"/>
+        <c:axId val="189989744"/>
+        <c:axId val="190008440"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -4412,16 +4014,16 @@
                       <c:formatCode>0.0%</c:formatCode>
                       <c:ptCount val="13"/>
                       <c:pt idx="0">
-                        <c:v>0.52083333333333337</c:v>
+                        <c:v>0.52</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.62790697674418605</c:v>
+                        <c:v>0.62222222222222223</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.55319148936170215</c:v>
+                        <c:v>0.53061224489795922</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0.58695652173913049</c:v>
+                        <c:v>0.58333333333333337</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>0.33333333333333331</c:v>
@@ -4448,7 +4050,7 @@
                         <c:v>1</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>0.56345177664974622</c:v>
+                        <c:v>0.55609756097560981</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4646,16 +4248,16 @@
                       <c:formatCode>0.0%</c:formatCode>
                       <c:ptCount val="13"/>
                       <c:pt idx="0">
-                        <c:v>0.41666666666666669</c:v>
+                        <c:v>0.44</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.7142857142857143</c:v>
+                        <c:v>0.68181818181818177</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.58333333333333337</c:v>
+                        <c:v>0.56000000000000005</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0.5</c:v>
+                        <c:v>0.47826086956521741</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>0.33333333333333331</c:v>
@@ -4682,7 +4284,7 @@
                         <c:v>1</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>0.54455445544554459</c:v>
+                        <c:v>0.53333333333333333</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4827,16 +4429,16 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="13"/>
                       <c:pt idx="0">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>45</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>49</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
                         <c:v>48</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>43</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>47</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>46</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>3</c:v>
@@ -4863,7 +4465,7 @@
                         <c:v>1</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>197</c:v>
+                        <c:v>205</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4970,16 +4572,16 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="13"/>
                       <c:pt idx="0">
-                        <c:v>24</c:v>
+                        <c:v>25</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>21</c:v>
+                        <c:v>22</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>24</c:v>
+                        <c:v>25</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>22</c:v>
+                        <c:v>23</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>3</c:v>
@@ -5006,7 +4608,7 @@
                         <c:v>1</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>101</c:v>
+                        <c:v>105</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -5109,16 +4711,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>24</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>23</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>24</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -5145,7 +4747,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>96</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -5162,11 +4764,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="177778616"/>
-        <c:axId val="177544664"/>
+        <c:axId val="190392168"/>
+        <c:axId val="190008824"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="177543880"/>
+        <c:axId val="189989744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5209,7 +4811,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="177544272"/>
+        <c:crossAx val="190008440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5217,7 +4819,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="177544272"/>
+        <c:axId val="190008440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5268,12 +4870,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="177543880"/>
+        <c:crossAx val="189989744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="177544664"/>
+        <c:axId val="190008824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5312,12 +4914,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="177778616"/>
+        <c:crossAx val="190392168"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="177778616"/>
+        <c:axId val="190392168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5326,7 +4928,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="177544664"/>
+        <c:crossAx val="190008824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7449,8 +7051,8 @@
   <dimension ref="A1:U53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J52" sqref="J52"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N52" sqref="N52:U52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11051,22 +10653,128 @@
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
-      <c r="I51" s="1"/>
-      <c r="J51" s="1"/>
-      <c r="K51" s="1"/>
-      <c r="L51" s="1"/>
-      <c r="M51" s="1"/>
+      <c r="A51">
+        <v>650</v>
+      </c>
+      <c r="B51" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C51" t="s">
+        <v>223</v>
+      </c>
+      <c r="D51" t="s">
+        <v>224</v>
+      </c>
+      <c r="E51" t="s">
+        <v>225</v>
+      </c>
+      <c r="F51" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G51" s="1">
+        <v>2</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J51" s="1">
+        <v>1</v>
+      </c>
+      <c r="K51" s="1">
+        <v>2</v>
+      </c>
+      <c r="L51" s="1">
+        <v>1</v>
+      </c>
+      <c r="M51" s="1">
+        <v>2</v>
+      </c>
+      <c r="N51" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="O51" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="P51" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Q51" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="R51" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S51" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T51" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U51" t="e">
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-      <c r="I52" s="1"/>
-      <c r="J52" s="1"/>
-      <c r="K52" s="1"/>
-      <c r="L52" s="1"/>
-      <c r="M52" s="1"/>
+      <c r="A52">
+        <v>651</v>
+      </c>
+      <c r="B52" t="s">
+        <v>226</v>
+      </c>
+      <c r="F52" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G52" s="1">
+        <v>1</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J52" s="1">
+        <v>1</v>
+      </c>
+      <c r="K52" s="1">
+        <v>3</v>
+      </c>
+      <c r="L52" s="1">
+        <v>2</v>
+      </c>
+      <c r="M52" s="1">
+        <v>2</v>
+      </c>
+      <c r="N52" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="O52" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="P52" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Q52" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="R52" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S52" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T52" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U52" t="e">
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="G53" s="1"/>
@@ -11086,13 +10794,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AS51"/>
+  <dimension ref="A1:AS53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="W25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A45" sqref="A45"/>
+      <selection pane="bottomRight" activeCell="A52" sqref="A52:XFD53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11105,34 +10813,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="V1" s="20" t="s">
+      <c r="V1" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="W1" s="20"/>
-      <c r="X1" s="20"/>
-      <c r="Y1" s="20"/>
-      <c r="Z1" s="20"/>
-      <c r="AA1" s="20"/>
-      <c r="AB1" s="20"/>
-      <c r="AC1" s="20"/>
-      <c r="AD1" s="20"/>
-      <c r="AE1" s="20"/>
-      <c r="AF1" s="20"/>
-      <c r="AG1" s="20"/>
-      <c r="AH1" s="21" t="s">
+      <c r="W1" s="23"/>
+      <c r="X1" s="23"/>
+      <c r="Y1" s="23"/>
+      <c r="Z1" s="23"/>
+      <c r="AA1" s="23"/>
+      <c r="AB1" s="23"/>
+      <c r="AC1" s="23"/>
+      <c r="AD1" s="23"/>
+      <c r="AE1" s="23"/>
+      <c r="AF1" s="23"/>
+      <c r="AG1" s="23"/>
+      <c r="AH1" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="AI1" s="21"/>
-      <c r="AJ1" s="21"/>
-      <c r="AK1" s="21"/>
-      <c r="AL1" s="21"/>
-      <c r="AM1" s="21"/>
-      <c r="AN1" s="21"/>
-      <c r="AO1" s="21"/>
-      <c r="AP1" s="21"/>
-      <c r="AQ1" s="21"/>
-      <c r="AR1" s="21"/>
-      <c r="AS1" s="21"/>
+      <c r="AI1" s="24"/>
+      <c r="AJ1" s="24"/>
+      <c r="AK1" s="24"/>
+      <c r="AL1" s="24"/>
+      <c r="AM1" s="24"/>
+      <c r="AN1" s="24"/>
+      <c r="AO1" s="24"/>
+      <c r="AP1" s="24"/>
+      <c r="AQ1" s="24"/>
+      <c r="AR1" s="24"/>
+      <c r="AS1" s="24"/>
     </row>
     <row r="2" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="str">
@@ -20203,6 +19911,370 @@
       </c>
       <c r="AS51" s="10">
         <f t="shared" si="177"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A52" s="3">
+        <f>Data!A51</f>
+        <v>650</v>
+      </c>
+      <c r="B52" s="4" t="e">
+        <f>Data!B51</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C52" s="5" t="str">
+        <f>Data!H51</f>
+        <v>Steve</v>
+      </c>
+      <c r="D52" s="2" t="str">
+        <f>Data!I51</f>
+        <v>Evan</v>
+      </c>
+      <c r="E52" s="1">
+        <f>IF(Data!J51=Data!$G51,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F52" s="1">
+        <f>IF(Data!K51=Data!$G51,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G52" s="1">
+        <f>IF(Data!L51=Data!$G51,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H52" s="1">
+        <f>IF(Data!M51=Data!$G51,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="I52" s="1" t="e">
+        <f>IF(Data!N51=Data!$G51,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J52" s="1" t="e">
+        <f>IF(Data!O51=Data!$G51,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K52" s="1" t="e">
+        <f>IF(Data!P51=Data!$G51,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="L52" s="1" t="e">
+        <f>IF(Data!Q51=Data!$G51,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M52" s="1" t="e">
+        <f>IF(Data!R51=Data!$G51,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N52" s="1" t="e">
+        <f>IF(Data!S51=Data!$G51,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O52" s="1" t="e">
+        <f>IF(Data!T51=Data!$G51,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P52" s="1" t="e">
+        <f>IF(Data!U51=Data!$G51,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q52" s="1">
+        <f t="shared" ref="Q52:Q53" si="178">COUNTIF(E52:P52,"&lt;&gt;#N/A")</f>
+        <v>4</v>
+      </c>
+      <c r="R52" s="1">
+        <f t="shared" ref="R52:R53" si="179">SUMIF(E52:P52,"&lt;&gt;#N/A")</f>
+        <v>2</v>
+      </c>
+      <c r="S52" s="1">
+        <f t="shared" ref="S52:S53" si="180">IF(R52=0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="T52" s="1">
+        <f t="shared" ref="T52:T53" si="181">IF(Q52=R52,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="U52" s="1" t="e">
+        <f t="shared" ref="U52:U53" si="182">IF(R52=1,INDEX($E$2:$P$2,1,MATCH(1,E52:P52,0)),NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="V52" s="8">
+        <f t="shared" ref="V52:V53" si="183">IF(ISNA(E52),V51,IF(E52=1,V51+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="W52" s="8">
+        <f t="shared" ref="W52:W53" si="184">IF(ISNA(F52),W51,IF(F52=1,W51+1,0))</f>
+        <v>2</v>
+      </c>
+      <c r="X52" s="8">
+        <f t="shared" ref="X52:X53" si="185">IF(ISNA(G52),X51,IF(G52=1,X51+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="Y52" s="8">
+        <f t="shared" ref="Y52:Y53" si="186">IF(ISNA(H52),Y51,IF(H52=1,Y51+1,0))</f>
+        <v>2</v>
+      </c>
+      <c r="Z52" s="8">
+        <f t="shared" ref="Z52:Z53" si="187">IF(ISNA(I52),Z51,IF(I52=1,Z51+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AA52" s="8">
+        <f t="shared" ref="AA52:AA53" si="188">IF(ISNA(J52),AA51,IF(J52=1,AA51+1,0))</f>
+        <v>2</v>
+      </c>
+      <c r="AB52" s="8">
+        <f t="shared" ref="AB52:AB53" si="189">IF(ISNA(K52),AB51,IF(K52=1,AB51+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AC52" s="8">
+        <f t="shared" ref="AC52:AC53" si="190">IF(ISNA(L52),AC51,IF(L52=1,AC51+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AD52" s="8">
+        <f t="shared" ref="AD52:AD53" si="191">IF(ISNA(M52),AD51,IF(M52=1,AD51+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AE52" s="8">
+        <f t="shared" ref="AE52:AE53" si="192">IF(ISNA(N52),AE51,IF(N52=1,AE51+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AF52" s="8">
+        <f t="shared" ref="AF52:AF53" si="193">IF(ISNA(O52),AF51,IF(O52=1,AF51+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AG52" s="8">
+        <f t="shared" ref="AG52:AG53" si="194">IF(ISNA(P52),AG51,IF(P52=1,AG51+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AH52" s="10">
+        <f t="shared" ref="AH52:AH53" si="195">IF(ISNA(E52),AH51,IF(E52=0,AH51+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AI52" s="10">
+        <f t="shared" ref="AI52:AI53" si="196">IF(ISNA(F52),AI51,IF(F52=0,AI51+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AJ52" s="10">
+        <f t="shared" ref="AJ52:AJ53" si="197">IF(ISNA(G52),AJ51,IF(G52=0,AJ51+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AK52" s="10">
+        <f t="shared" ref="AK52:AK53" si="198">IF(ISNA(H52),AK51,IF(H52=0,AK51+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AL52" s="10">
+        <f t="shared" ref="AL52:AL53" si="199">IF(ISNA(I52),AL51,IF(I52=0,AL51+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AM52" s="10">
+        <f t="shared" ref="AM52:AM53" si="200">IF(ISNA(J52),AM51,IF(J52=0,AM51+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AN52" s="10">
+        <f t="shared" ref="AN52:AN53" si="201">IF(ISNA(K52),AN51,IF(K52=0,AN51+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AO52" s="10">
+        <f t="shared" ref="AO52:AO53" si="202">IF(ISNA(L52),AO51,IF(L52=0,AO51+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AP52" s="10">
+        <f t="shared" ref="AP52:AP53" si="203">IF(ISNA(M52),AP51,IF(M52=0,AP51+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AQ52" s="10">
+        <f t="shared" ref="AQ52:AQ53" si="204">IF(ISNA(N52),AQ51,IF(N52=0,AQ51+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AR52" s="10">
+        <f t="shared" ref="AR52:AR53" si="205">IF(ISNA(O52),AR51,IF(O52=0,AR51+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AS52" s="10">
+        <f t="shared" ref="AS52:AS53" si="206">IF(ISNA(P52),AS51,IF(P52=0,AS51+1,0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A53" s="3">
+        <f>Data!A52</f>
+        <v>651</v>
+      </c>
+      <c r="B53" s="4" t="str">
+        <f>Data!B52</f>
+        <v>Science News Stories You May Have Missed</v>
+      </c>
+      <c r="C53" s="5" t="str">
+        <f>Data!H52</f>
+        <v>Steve</v>
+      </c>
+      <c r="D53" s="2" t="str">
+        <f>Data!I52</f>
+        <v>Jay</v>
+      </c>
+      <c r="E53" s="1">
+        <f>IF(Data!J52=Data!$G52,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F53" s="1">
+        <f>IF(Data!K52=Data!$G52,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G53" s="1">
+        <f>IF(Data!L52=Data!$G52,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H53" s="1">
+        <f>IF(Data!M52=Data!$G52,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I53" s="1" t="e">
+        <f>IF(Data!N52=Data!$G52,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J53" s="1" t="e">
+        <f>IF(Data!O52=Data!$G52,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K53" s="1" t="e">
+        <f>IF(Data!P52=Data!$G52,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="L53" s="1" t="e">
+        <f>IF(Data!Q52=Data!$G52,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M53" s="1" t="e">
+        <f>IF(Data!R52=Data!$G52,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N53" s="1" t="e">
+        <f>IF(Data!S52=Data!$G52,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O53" s="1" t="e">
+        <f>IF(Data!T52=Data!$G52,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P53" s="1" t="e">
+        <f>IF(Data!U52=Data!$G52,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q53" s="1">
+        <f t="shared" si="178"/>
+        <v>4</v>
+      </c>
+      <c r="R53" s="1">
+        <f t="shared" si="179"/>
+        <v>1</v>
+      </c>
+      <c r="S53" s="1">
+        <f t="shared" si="180"/>
+        <v>0</v>
+      </c>
+      <c r="T53" s="1">
+        <f t="shared" si="181"/>
+        <v>0</v>
+      </c>
+      <c r="U53" s="1" t="str">
+        <f t="shared" si="182"/>
+        <v>Bob</v>
+      </c>
+      <c r="V53" s="8">
+        <f t="shared" si="183"/>
+        <v>1</v>
+      </c>
+      <c r="W53" s="8">
+        <f t="shared" si="184"/>
+        <v>0</v>
+      </c>
+      <c r="X53" s="8">
+        <f t="shared" si="185"/>
+        <v>0</v>
+      </c>
+      <c r="Y53" s="8">
+        <f t="shared" si="186"/>
+        <v>0</v>
+      </c>
+      <c r="Z53" s="8">
+        <f t="shared" si="187"/>
+        <v>1</v>
+      </c>
+      <c r="AA53" s="8">
+        <f t="shared" si="188"/>
+        <v>2</v>
+      </c>
+      <c r="AB53" s="8">
+        <f t="shared" si="189"/>
+        <v>0</v>
+      </c>
+      <c r="AC53" s="8">
+        <f t="shared" si="190"/>
+        <v>1</v>
+      </c>
+      <c r="AD53" s="8">
+        <f t="shared" si="191"/>
+        <v>0</v>
+      </c>
+      <c r="AE53" s="8">
+        <f t="shared" si="192"/>
+        <v>1</v>
+      </c>
+      <c r="AF53" s="8">
+        <f t="shared" si="193"/>
+        <v>0</v>
+      </c>
+      <c r="AG53" s="8">
+        <f t="shared" si="194"/>
+        <v>1</v>
+      </c>
+      <c r="AH53" s="10">
+        <f t="shared" si="195"/>
+        <v>0</v>
+      </c>
+      <c r="AI53" s="10">
+        <f t="shared" si="196"/>
+        <v>1</v>
+      </c>
+      <c r="AJ53" s="10">
+        <f t="shared" si="197"/>
+        <v>2</v>
+      </c>
+      <c r="AK53" s="10">
+        <f t="shared" si="198"/>
+        <v>1</v>
+      </c>
+      <c r="AL53" s="10">
+        <f t="shared" si="199"/>
+        <v>0</v>
+      </c>
+      <c r="AM53" s="10">
+        <f t="shared" si="200"/>
+        <v>0</v>
+      </c>
+      <c r="AN53" s="10">
+        <f t="shared" si="201"/>
+        <v>1</v>
+      </c>
+      <c r="AO53" s="10">
+        <f t="shared" si="202"/>
+        <v>0</v>
+      </c>
+      <c r="AP53" s="10">
+        <f t="shared" si="203"/>
+        <v>1</v>
+      </c>
+      <c r="AQ53" s="10">
+        <f t="shared" si="204"/>
+        <v>0</v>
+      </c>
+      <c r="AR53" s="10">
+        <f t="shared" si="205"/>
+        <v>1</v>
+      </c>
+      <c r="AS53" s="10">
+        <f t="shared" si="206"/>
         <v>0</v>
       </c>
     </row>
@@ -20221,7 +20293,7 @@
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20291,19 +20363,19 @@
       </c>
       <c r="B2" s="6">
         <f>SUMIF(Results!E3:E53,"&lt;&gt;#N/A")/COUNTIFS(Results!E3:E53,"&lt;&gt;#N/A",Results!E3:E53,"&lt;&gt;")</f>
-        <v>0.52083333333333337</v>
+        <v>0.52</v>
       </c>
       <c r="C2" s="6">
         <f>SUMIF(Results!F3:F53,"&lt;&gt;#N/A")/COUNTIFS(Results!F3:F53,"&lt;&gt;#N/A",Results!F3:F53,"&lt;&gt;")</f>
-        <v>0.62790697674418605</v>
+        <v>0.62222222222222223</v>
       </c>
       <c r="D2" s="6">
         <f>SUMIF(Results!G3:G53,"&lt;&gt;#N/A")/COUNTIFS(Results!G3:G53,"&lt;&gt;#N/A",Results!G3:G53,"&lt;&gt;")</f>
-        <v>0.55319148936170215</v>
+        <v>0.53061224489795922</v>
       </c>
       <c r="E2" s="6">
         <f>SUMIF(Results!H3:H53,"&lt;&gt;#N/A")/COUNTIFS(Results!H3:H53,"&lt;&gt;#N/A",Results!H3:H53,"&lt;&gt;")</f>
-        <v>0.58695652173913049</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="F2" s="6">
         <f>SUMIF(Results!I3:I53,"&lt;&gt;#N/A")/COUNTIFS(Results!I3:I53,"&lt;&gt;#N/A",Results!I3:I53,"&lt;&gt;")</f>
@@ -20339,7 +20411,7 @@
       </c>
       <c r="N2" s="6">
         <f>SUM(Results!R3:R53)/SUM(Results!Q3:Q53)</f>
-        <v>0.56345177664974622</v>
+        <v>0.55609756097560981</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -20348,19 +20420,19 @@
       </c>
       <c r="B3" s="6">
         <f>SUMIFS(Results!E3:E53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!E3:E53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!E3:E53, "&lt;&gt;#N/A", Results!E3:E53, "&lt;&gt;")</f>
-        <v>0.41666666666666669</v>
+        <v>0.44</v>
       </c>
       <c r="C3" s="6">
         <f>SUMIFS(Results!F3:F53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!F3:F53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!F3:F53, "&lt;&gt;#N/A", Results!F3:F53, "&lt;&gt;")</f>
-        <v>0.7142857142857143</v>
+        <v>0.68181818181818177</v>
       </c>
       <c r="D3" s="6">
         <f>SUMIFS(Results!G3:G53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!G3:G53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!G3:G53, "&lt;&gt;#N/A", Results!G3:G53, "&lt;&gt;")</f>
-        <v>0.58333333333333337</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="E3" s="6">
         <f>SUMIFS(Results!H3:H53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!H3:H53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!H3:H53, "&lt;&gt;#N/A", Results!H3:H53, "&lt;&gt;")</f>
-        <v>0.5</v>
+        <v>0.47826086956521741</v>
       </c>
       <c r="F3" s="6">
         <f>SUMIFS(Results!I3:I53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!I3:I53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!I3:I53, "&lt;&gt;#N/A", Results!I3:I53, "&lt;&gt;")</f>
@@ -20396,7 +20468,7 @@
       </c>
       <c r="N3" s="6">
         <f>SUMIF(Results!B3:B53,"&lt;&gt;#N/A",Results!R3:R53)/SUMIF(Results!B3:B53,"&lt;&gt;#N/A",Results!Q3:Q53)</f>
-        <v>0.54455445544554459</v>
+        <v>0.53333333333333333</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -20405,19 +20477,19 @@
       </c>
       <c r="B4" s="6">
         <f>SUMIFS(Results!E3:E53,Results!$B$3:$B$53,"=#N/A",Results!E3:E53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!E3:E53, "&lt;&gt;#N/A", Results!E3:E53, "&lt;&gt;")</f>
-        <v>0.625</v>
+        <v>0.6</v>
       </c>
       <c r="C4" s="6">
         <f>SUMIFS(Results!F3:F53,Results!$B$3:$B$53,"=#N/A",Results!F3:F53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!F3:F53, "&lt;&gt;#N/A", Results!F3:F53, "&lt;&gt;")</f>
-        <v>0.54545454545454541</v>
+        <v>0.56521739130434778</v>
       </c>
       <c r="D4" s="6">
         <f>SUMIFS(Results!G3:G53,Results!$B$3:$B$53,"=#N/A",Results!G3:G53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!G3:G53, "&lt;&gt;#N/A", Results!G3:G53, "&lt;&gt;")</f>
-        <v>0.52173913043478259</v>
+        <v>0.5</v>
       </c>
       <c r="E4" s="6">
         <f>SUMIFS(Results!H3:H53,Results!$B$3:$B$53,"=#N/A",Results!H3:H53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!H3:H53, "&lt;&gt;#N/A", Results!H3:H53, "&lt;&gt;")</f>
-        <v>0.66666666666666663</v>
+        <v>0.68</v>
       </c>
       <c r="F4" s="6" t="e">
         <f>SUMIFS(Results!I3:I53,Results!$B$3:$B$53,"=#N/A",Results!I3:I53, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!I3:I53, "&lt;&gt;#N/A", Results!I3:I53, "&lt;&gt;")</f>
@@ -20453,7 +20525,7 @@
       </c>
       <c r="N4" s="6">
         <f>SUMIF(Results!B3:B53,"=#N/A",Results!R3:R53)/SUMIF(Results!B3:B53,"=#N/A",Results!Q3:Q53)</f>
-        <v>0.58333333333333337</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -20576,7 +20648,7 @@
       </c>
       <c r="B7" s="1">
         <f>COUNTIF(Results!$U$3:$U$53,Summary!B1)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C7" s="1">
         <f>COUNTIF(Results!$U$3:$U$53,Summary!C1)</f>
@@ -20623,8 +20695,8 @@
         <v>0</v>
       </c>
       <c r="N7" s="1">
-        <f>MAX(B7:M7)</f>
-        <v>4</v>
+        <f>SUM(B7:M7)</f>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -20641,11 +20713,11 @@
       </c>
       <c r="D8" s="7">
         <f>SUMIF(Results!$D$3:$D$53,D1,Results!$R$3:$R$53)/SUMIF(Results!$D$3:$D$53,D1,Results!$Q$3:$Q$53)</f>
-        <v>0.51219512195121952</v>
+        <v>0.48888888888888887</v>
       </c>
       <c r="E8" s="7">
         <f>SUMIF(Results!$D$3:$D$53,E1,Results!$R$3:$R$53)/SUMIF(Results!$D$3:$D$53,E1,Results!$Q$3:$Q$53)</f>
-        <v>0.5714285714285714</v>
+        <v>0.5641025641025641</v>
       </c>
       <c r="F8" s="7" t="e">
         <f>SUMIF(Results!$D$3:$D$53,F1,Results!$R$3:$R$53)/SUMIF(Results!$D$3:$D$53,F1,Results!$Q$3:$Q$53)</f>
@@ -20679,7 +20751,7 @@
         <f>SUMIF(Results!$D$3:$D$53,M1,Results!$R$3:$R$53)/SUMIF(Results!$D$3:$D$53,M1,Results!$Q$3:$Q$53)</f>
         <v>0.8</v>
       </c>
-      <c r="N8" s="22" t="e">
+      <c r="N8" s="20" t="e">
         <f>MAX(B8:M8)</f>
         <v>#DIV/0!</v>
       </c>
@@ -20688,57 +20760,57 @@
       <c r="A9" t="s">
         <v>222</v>
       </c>
-      <c r="B9" s="23">
+      <c r="B9" s="21">
         <f>SUMIF(Results!$D$3:$D$53,B1,Results!E$3:E$53)</f>
         <v>2</v>
       </c>
-      <c r="C9" s="23">
+      <c r="C9" s="21">
         <f>SUMIF(Results!$D$3:$D$53,C1,Results!F$3:F$53)</f>
         <v>3</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="21">
         <f>SUMIF(Results!$D$3:$D$53,D1,Results!G$3:G$53)</f>
         <v>2</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="21">
         <f>SUMIF(Results!$D$3:$D$53,E1,Results!H$3:H$53)</f>
-        <v>3</v>
-      </c>
-      <c r="F9" s="23">
+        <v>4</v>
+      </c>
+      <c r="F9" s="21">
         <f>SUMIF(Results!$D$3:$D$53,F1,Results!I$3:I$53)</f>
         <v>0</v>
       </c>
-      <c r="G9" s="23">
+      <c r="G9" s="21">
         <f>SUMIF(Results!$D$3:$D$53,G1,Results!J$3:J$53)</f>
         <v>0</v>
       </c>
-      <c r="H9" s="23">
+      <c r="H9" s="21">
         <f>SUMIF(Results!$D$3:$D$53,H1,Results!K$3:K$53)</f>
         <v>0</v>
       </c>
-      <c r="I9" s="23">
+      <c r="I9" s="21">
         <f>SUMIF(Results!$D$3:$D$53,I1,Results!L$3:L$53)</f>
         <v>1</v>
       </c>
-      <c r="J9" s="23">
+      <c r="J9" s="21">
         <f>SUMIF(Results!$D$3:$D$53,J1,Results!M$3:M$53)</f>
         <v>0</v>
       </c>
-      <c r="K9" s="23">
+      <c r="K9" s="21">
         <f>SUMIF(Results!$D$3:$D$53,K1,Results!N$3:N$53)</f>
         <v>1</v>
       </c>
-      <c r="L9" s="23">
+      <c r="L9" s="21">
         <f>SUMIF(Results!$D$3:$D$53,L1,Results!O$3:O$53)</f>
         <v>0</v>
       </c>
-      <c r="M9" s="23">
+      <c r="M9" s="21">
         <f>SUMIF(Results!$D$3:$D$53,M1,Results!P$3:P$53)</f>
         <v>1</v>
       </c>
-      <c r="N9" s="24">
+      <c r="N9" s="22">
         <f>SUM(B9:M9)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -20755,11 +20827,11 @@
       </c>
       <c r="D10" s="1">
         <f>COUNTIF(Data!$I$2:$I$53,Summary!D1)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E10" s="1">
         <f>COUNTIF(Data!$I$2:$I$53,Summary!E1)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F10" s="1">
         <f>COUNTIF(Data!$I$2:$I$53,Summary!F1)</f>
@@ -20795,7 +20867,7 @@
       </c>
       <c r="N10" s="1">
         <f>SUM(B10:M10)</f>
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -20812,11 +20884,11 @@
       </c>
       <c r="D11" s="7">
         <f>SUMIF(Results!$D$3:$D$53,D1,Results!G$3:G$53)/COUNTIF(Results!$D$3:$D$53,D1)</f>
-        <v>0.2</v>
+        <v>0.18181818181818182</v>
       </c>
       <c r="E11" s="7">
         <f>SUMIF(Results!$D$3:$D$53,E1,Results!H$3:H$53)/COUNTIF(Results!$D$3:$D$53,E1)</f>
-        <v>0.33333333333333331</v>
+        <v>0.4</v>
       </c>
       <c r="F11" s="7" t="e">
         <f>SUMIF(Results!$D$3:$D$53,F1,Results!I$3:I$53)/COUNTIF(Results!$D$3:$D$53,F1)</f>
@@ -20852,7 +20924,7 @@
       </c>
       <c r="N11" s="6">
         <f>N9/N10</f>
-        <v>0.26530612244897961</v>
+        <v>0.27450980392156865</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -20861,11 +20933,11 @@
       </c>
       <c r="B12" s="1">
         <f>SUMIF(Results!E3:E53,"&lt;&gt;#N/A")</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1">
         <f>SUMIF(Results!F3:F53,"&lt;&gt;#N/A")</f>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D12" s="1">
         <f>SUMIF(Results!G3:G53,"&lt;&gt;#N/A")</f>
@@ -20873,7 +20945,7 @@
       </c>
       <c r="E12" s="1">
         <f>SUMIF(Results!H3:H53,"&lt;&gt;#N/A")</f>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F12" s="1">
         <f>SUMIF(Results!I3:I53,"&lt;&gt;#N/A")</f>
@@ -20908,8 +20980,8 @@
         <v>1</v>
       </c>
       <c r="N12" s="1">
-        <f>SUM(B12:M12)</f>
-        <v>111</v>
+        <f t="shared" ref="N12:N17" si="0">SUM(B12:M12)</f>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -20918,19 +20990,19 @@
       </c>
       <c r="B13" s="1">
         <f>COUNTIFS(Results!E3:E53,"&lt;&gt;#N/A",Results!E3:E53,"&lt;&gt;")</f>
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C13" s="1">
         <f>COUNTIFS(Results!F3:F53,"&lt;&gt;#N/A",Results!F3:F53,"&lt;&gt;")</f>
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D13" s="1">
         <f>COUNTIFS(Results!G3:G53,"&lt;&gt;#N/A",Results!G3:G53,"&lt;&gt;")</f>
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E13" s="1">
         <f>COUNTIFS(Results!H3:H53,"&lt;&gt;#N/A",Results!H3:H53,"&lt;&gt;")</f>
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F13" s="1">
         <f>COUNTIFS(Results!I3:I53,"&lt;&gt;#N/A",Results!I3:I53,"&lt;&gt;")</f>
@@ -20965,8 +21037,8 @@
         <v>1</v>
       </c>
       <c r="N13" s="1">
-        <f>SUM(B13:M13)</f>
-        <v>197</v>
+        <f t="shared" si="0"/>
+        <v>205</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -20975,7 +21047,7 @@
       </c>
       <c r="B14" s="1">
         <f>SUMIFS(Results!E3:E53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!E3:E53, "&lt;&gt;#N/A")</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C14" s="1">
         <f>SUMIFS(Results!F3:F53,Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!F3:F53, "&lt;&gt;#N/A")</f>
@@ -21022,8 +21094,8 @@
         <v>1</v>
       </c>
       <c r="N14" s="1">
-        <f>SUM(B14:M14)</f>
-        <v>55</v>
+        <f t="shared" si="0"/>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -21032,19 +21104,19 @@
       </c>
       <c r="B15" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!E3:E53, "&lt;&gt;#N/A", Results!E3:E53, "&lt;&gt;")</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C15" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!F3:F53, "&lt;&gt;#N/A", Results!F3:F53, "&lt;&gt;")</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D15" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!G3:G53, "&lt;&gt;#N/A", Results!G3:G53, "&lt;&gt;")</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E15" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!H3:H53, "&lt;&gt;#N/A", Results!H3:H53, "&lt;&gt;")</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F15" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"&lt;&gt;#N/A",Results!I3:I53, "&lt;&gt;#N/A", Results!I3:I53, "&lt;&gt;")</f>
@@ -21079,8 +21151,8 @@
         <v>1</v>
       </c>
       <c r="N15" s="1">
-        <f>SUM(B15:M15)</f>
-        <v>101</v>
+        <f t="shared" si="0"/>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -21093,7 +21165,7 @@
       </c>
       <c r="C16" s="1">
         <f>SUMIFS(Results!F3:F53,Results!$B$3:$B$53,"=#N/A",Results!F3:F53, "&lt;&gt;#N/A")</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D16" s="1">
         <f>SUMIFS(Results!G3:G53,Results!$B$3:$B$53,"=#N/A",Results!G3:G53, "&lt;&gt;#N/A")</f>
@@ -21101,7 +21173,7 @@
       </c>
       <c r="E16" s="1">
         <f>SUMIFS(Results!H3:H53,Results!$B$3:$B$53,"=#N/A",Results!H3:H53, "&lt;&gt;#N/A")</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F16" s="1">
         <f>SUMIFS(Results!I3:I53,Results!$B$3:$B$53,"=#N/A",Results!I3:I53, "&lt;&gt;#N/A")</f>
@@ -21136,8 +21208,8 @@
         <v>0</v>
       </c>
       <c r="N16" s="1">
-        <f>SUM(B16:M16)</f>
-        <v>56</v>
+        <f t="shared" si="0"/>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -21146,19 +21218,19 @@
       </c>
       <c r="B17" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!E3:E53, "&lt;&gt;#N/A", Results!E3:E53, "&lt;&gt;")</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C17" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!F3:F53, "&lt;&gt;#N/A", Results!F3:F53, "&lt;&gt;")</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D17" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!G3:G53, "&lt;&gt;#N/A", Results!G3:G53, "&lt;&gt;")</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E17" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!H3:H53, "&lt;&gt;#N/A", Results!H3:H53, "&lt;&gt;")</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F17" s="1">
         <f>COUNTIFS(Results!$B$3:$B$53,"=#N/A",Results!I3:I53, "&lt;&gt;#N/A", Results!I3:I53, "&lt;&gt;")</f>
@@ -21193,8 +21265,8 @@
         <v>0</v>
       </c>
       <c r="N17" s="1">
-        <f>SUM(B17:M17)</f>
-        <v>96</v>
+        <f t="shared" si="0"/>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -21313,34 +21385,34 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B10:M10">
-    <cfRule type="top10" dxfId="19" priority="10" rank="1"/>
+    <cfRule type="top10" dxfId="9" priority="10" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:G8 N11">
-    <cfRule type="top10" dxfId="18" priority="9" rank="1"/>
+    <cfRule type="top10" dxfId="8" priority="9" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:G7">
-    <cfRule type="top10" dxfId="17" priority="8" rank="1"/>
+    <cfRule type="top10" dxfId="7" priority="8" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:G6">
-    <cfRule type="top10" dxfId="16" priority="7" rank="1"/>
+    <cfRule type="top10" dxfId="6" priority="7" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:G5">
-    <cfRule type="top10" dxfId="15" priority="6" rank="1"/>
+    <cfRule type="top10" dxfId="5" priority="6" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:G4">
-    <cfRule type="top10" dxfId="14" priority="5" rank="1"/>
+    <cfRule type="top10" dxfId="4" priority="5" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:G3">
-    <cfRule type="top10" dxfId="13" priority="4" rank="1"/>
+    <cfRule type="top10" dxfId="3" priority="4" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:G2">
-    <cfRule type="top10" dxfId="12" priority="3" rank="1"/>
+    <cfRule type="top10" dxfId="2" priority="3" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:G8">
-    <cfRule type="top10" dxfId="11" priority="2" rank="1"/>
+    <cfRule type="top10" dxfId="1" priority="2" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:G11">
-    <cfRule type="top10" dxfId="10" priority="1" rank="1"/>
+    <cfRule type="top10" dxfId="0" priority="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -21351,7 +21423,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
       <selection activeCell="N62" sqref="N62"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added ability to generate Visuals in R
</commit_message>
<xml_diff>
--- a/SGU_Science_or_Fiction.xlsx
+++ b/SGU_Science_or_Fiction.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6135"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6135" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -12827,7 +12827,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I88" sqref="I88"/>
     </sheetView>
@@ -23143,14 +23143,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AV102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B71" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="P105" sqref="P105"/>
+      <selection pane="bottomRight" activeCell="U16" sqref="U16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23405,7 +23404,7 @@
         <v>Bill</v>
       </c>
     </row>
-    <row r="3" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A3" s="24">
         <f>Data!A2</f>
         <v>600</v>
@@ -23573,7 +23572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A4" s="24">
         <f>Data!A3</f>
         <v>601</v>
@@ -23767,7 +23766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A5" s="24">
         <f>Data!A4</f>
         <v>602</v>
@@ -24155,7 +24154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A7" s="24">
         <f>Data!A6</f>
         <v>604</v>
@@ -24349,7 +24348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A8" s="24">
         <f>Data!A7</f>
         <v>605</v>
@@ -24737,7 +24736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A10" s="24">
         <f>Data!A9</f>
         <v>607</v>
@@ -25125,7 +25124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A12" s="24">
         <f>Data!A11</f>
         <v>609</v>
@@ -25319,7 +25318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A13" s="24">
         <f>Data!A12</f>
         <v>610</v>
@@ -25513,7 +25512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A14" s="24">
         <f>Data!A13</f>
         <v>611</v>
@@ -25707,7 +25706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A15" s="24">
         <f>Data!A14</f>
         <v>612</v>
@@ -26095,7 +26094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A17" s="24">
         <f>Data!A16</f>
         <v>614</v>
@@ -26289,7 +26288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A18" s="24">
         <f>Data!A17</f>
         <v>615</v>
@@ -26483,7 +26482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A19" s="24">
         <f>Data!A18</f>
         <v>616</v>
@@ -26677,7 +26676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A20" s="24">
         <f>Data!A19</f>
         <v>617</v>
@@ -26871,7 +26870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A21" s="24">
         <f>Data!A20</f>
         <v>618</v>
@@ -27259,7 +27258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A23" s="24">
         <f>Data!A22</f>
         <v>620</v>
@@ -27453,7 +27452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A24" s="24">
         <f>Data!A23</f>
         <v>621</v>
@@ -27647,7 +27646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A25" s="24">
         <f>Data!A24</f>
         <v>622</v>
@@ -27841,7 +27840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A26" s="24">
         <f>Data!A25</f>
         <v>623</v>
@@ -28229,7 +28228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A28" s="24">
         <f>Data!A27</f>
         <v>625</v>
@@ -28423,7 +28422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A29" s="24">
         <f>Data!A28</f>
         <v>626</v>
@@ -28617,7 +28616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A30" s="24">
         <f>Data!A29</f>
         <v>627</v>
@@ -28811,7 +28810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A31" s="24">
         <f>Data!A30</f>
         <v>629</v>
@@ -29005,7 +29004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A32" s="24">
         <f>Data!A31</f>
         <v>630</v>
@@ -29199,7 +29198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A33" s="24">
         <f>Data!A32</f>
         <v>631</v>
@@ -29587,7 +29586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A35" s="24">
         <f>Data!A34</f>
         <v>633</v>
@@ -29975,7 +29974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A37" s="24">
         <f>Data!A36</f>
         <v>635</v>
@@ -30169,7 +30168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A38" s="24">
         <f>Data!A37</f>
         <v>636</v>
@@ -30363,7 +30362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A39" s="24">
         <f>Data!A38</f>
         <v>637</v>
@@ -30557,7 +30556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A40" s="24">
         <f>Data!A39</f>
         <v>638</v>
@@ -30752,7 +30751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A41" s="24">
         <f>Data!A40</f>
         <v>639</v>
@@ -30946,7 +30945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A42" s="24">
         <f>Data!A41</f>
         <v>640</v>
@@ -31140,7 +31139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A43" s="24">
         <f>Data!A42</f>
         <v>641</v>
@@ -31334,7 +31333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A44" s="24">
         <f>Data!A43</f>
         <v>642</v>
@@ -31528,7 +31527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A45" s="24">
         <f>Data!A44</f>
         <v>643</v>
@@ -31722,7 +31721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A46" s="24">
         <f>Data!A45</f>
         <v>644</v>
@@ -32498,7 +32497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A50" s="24">
         <f>Data!A49</f>
         <v>648</v>
@@ -32886,7 +32885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A52" s="24">
         <f>Data!A51</f>
         <v>650</v>
@@ -33080,7 +33079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A53" s="24">
         <f>Data!A52</f>
         <v>651</v>
@@ -33274,7 +33273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A54" s="24">
         <f>Data!A53</f>
         <v>652</v>
@@ -33468,7 +33467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A55" s="24">
         <f>Data!A54</f>
         <v>653</v>
@@ -33662,7 +33661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A56" s="24">
         <f>Data!A55</f>
         <v>654</v>
@@ -33856,7 +33855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A57" s="24">
         <f>Data!A56</f>
         <v>655</v>
@@ -34050,7 +34049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A58" s="24">
         <f>Data!A57</f>
         <v>656</v>
@@ -34244,7 +34243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A59" s="24">
         <f>Data!A58</f>
         <v>657</v>
@@ -34438,7 +34437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A60" s="24">
         <f>Data!A59</f>
         <v>658</v>
@@ -34826,7 +34825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A62" s="24">
         <f>Data!A61</f>
         <v>660</v>
@@ -35214,7 +35213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <f>Data!A63</f>
         <v>662</v>
@@ -35602,7 +35601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <f>Data!A65</f>
         <v>664</v>
@@ -35796,7 +35795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <f>Data!A66</f>
         <v>665</v>
@@ -36184,7 +36183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <f>Data!A68</f>
         <v>667</v>
@@ -36378,7 +36377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <f>Data!A69</f>
         <v>668</v>
@@ -36572,7 +36571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <f>Data!A70</f>
         <v>669</v>
@@ -36766,7 +36765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <f>Data!A71</f>
         <v>670</v>
@@ -37154,7 +37153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <f>Data!A73</f>
         <v>672</v>
@@ -37348,7 +37347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <f>Data!A74</f>
         <v>673</v>
@@ -37542,7 +37541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <f>Data!A75</f>
         <v>674</v>
@@ -37736,7 +37735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <f>Data!A76</f>
         <v>675</v>
@@ -37930,7 +37929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <f>Data!A77</f>
         <v>676</v>
@@ -38124,7 +38123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <f>Data!A78</f>
         <v>677</v>
@@ -38318,7 +38317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <f>Data!A79</f>
         <v>678</v>
@@ -38512,7 +38511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <f>Data!A80</f>
         <v>679</v>
@@ -38900,7 +38899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <f>Data!A82</f>
         <v>681</v>
@@ -39094,7 +39093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <f>Data!A83</f>
         <v>682</v>
@@ -39676,7 +39675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <f>Data!A86</f>
         <v>685</v>
@@ -39870,7 +39869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <f>Data!A87</f>
         <v>686</v>
@@ -40258,92 +40257,86 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <f>Data!A89</f>
         <v>688</v>
       </c>
     </row>
-    <row r="91" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <f>Data!A90</f>
         <v>689</v>
       </c>
     </row>
-    <row r="92" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <f>Data!A91</f>
         <v>690</v>
       </c>
     </row>
-    <row r="93" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <f>Data!A92</f>
         <v>691</v>
       </c>
     </row>
-    <row r="94" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <f>Data!A93</f>
         <v>692</v>
       </c>
     </row>
-    <row r="95" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <f>Data!A94</f>
         <v>693</v>
       </c>
     </row>
-    <row r="96" spans="1:48" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <f>Data!A95</f>
         <v>694</v>
       </c>
     </row>
-    <row r="97" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <f>Data!A96</f>
         <v>695</v>
       </c>
     </row>
-    <row r="98" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <f>Data!A97</f>
         <v>696</v>
       </c>
     </row>
-    <row r="99" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <f>Data!A98</f>
         <v>697</v>
       </c>
     </row>
-    <row r="100" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <f>Data!A99</f>
         <v>698</v>
       </c>
     </row>
-    <row r="101" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <f>Data!A100</f>
         <v>699</v>
       </c>
     </row>
-    <row r="102" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <f>Data!A101</f>
         <v>700</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:V102">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="Bob"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A2:V102"/>
   <mergeCells count="2">
     <mergeCell ref="W1:AH1"/>
     <mergeCell ref="AJ1:AV1"/>
@@ -41488,8 +41481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22:C30"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated through episode 750 and updated answering order performance to include number of sweeps
</commit_message>
<xml_diff>
--- a/SGU_Science_or_Fiction.xlsx
+++ b/SGU_Science_or_Fiction.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xwhx\Desktop\SGU_Science_or_Fiction\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xwhx\SourceControl\SGU_Science_or_Fiction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4414A4B-196E-4F4F-A2E9-D4720070B1FC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6440448C-6348-491B-BE18-E082DB7CE512}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="311">
   <si>
     <t>Episode</t>
   </si>
@@ -978,6 +978,9 @@
   </si>
   <si>
     <t>Daylight Savings Time</t>
+  </si>
+  <si>
+    <t>Carl Sagan</t>
   </si>
 </sst>
 </file>
@@ -13306,11 +13309,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z146"/>
+  <dimension ref="A1:Z149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I134" sqref="I134:Z146"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I147" sqref="I147:Z149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -25025,7 +25028,7 @@
         <v>#N/A</v>
       </c>
       <c r="Z131" s="22" t="e">
-        <f t="shared" ref="Z131:Z146" si="24">INDEX(AnsLkUp,MATCH($A131 &amp; "_"&amp;Z$1,LookupName,0),3)</f>
+        <f t="shared" ref="Z131:Z149" si="24">INDEX(AnsLkUp,MATCH($A131 &amp; "_"&amp;Z$1,LookupName,0),3)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -25048,7 +25051,7 @@
         <v>Jay</v>
       </c>
       <c r="J132" s="22">
-        <f t="shared" ref="J132:Y146" si="26">INDEX(AnsLkUp,MATCH($A132 &amp; "_"&amp;J$1,LookupName,0),3)</f>
+        <f t="shared" ref="J132:Y147" si="26">INDEX(AnsLkUp,MATCH($A132 &amp; "_"&amp;J$1,LookupName,0),3)</f>
         <v>1</v>
       </c>
       <c r="K132" s="22">
@@ -26323,6 +26326,266 @@
       <c r="Z146" s="22" t="e">
         <f t="shared" si="24"/>
         <v>#N/A</v>
+      </c>
+    </row>
+    <row r="147" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A147">
+        <v>748</v>
+      </c>
+      <c r="B147" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G147" s="1">
+        <v>1</v>
+      </c>
+      <c r="H147" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I147" s="22" t="str">
+        <f t="shared" ref="I147:I149" si="28">INDEX(AnsLkUp,MATCH(A147 &amp; "_1",LookupOrder,1),2)</f>
+        <v>Cara</v>
+      </c>
+      <c r="J147" s="22">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+      <c r="K147" s="22">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+      <c r="L147" s="22">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+      <c r="M147" s="22">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+      <c r="N147" s="22" t="e">
+        <f t="shared" si="26"/>
+        <v>#N/A</v>
+      </c>
+      <c r="O147" s="22" t="e">
+        <f t="shared" si="26"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P147" s="22" t="e">
+        <f t="shared" si="26"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q147" s="22" t="e">
+        <f t="shared" si="26"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R147" s="22" t="e">
+        <f t="shared" si="26"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S147" s="22" t="e">
+        <f t="shared" si="26"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T147" s="22" t="e">
+        <f t="shared" si="26"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U147" s="22" t="e">
+        <f t="shared" si="26"/>
+        <v>#N/A</v>
+      </c>
+      <c r="V147" s="22" t="e">
+        <f t="shared" si="26"/>
+        <v>#N/A</v>
+      </c>
+      <c r="W147" s="22" t="e">
+        <f t="shared" si="26"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X147" s="22" t="e">
+        <f t="shared" si="26"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y147" s="22" t="e">
+        <f t="shared" ref="J147:Y149" si="29">INDEX(AnsLkUp,MATCH($A147 &amp; "_"&amp;Y$1,LookupName,0),3)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Z147" s="22" t="e">
+        <f t="shared" si="24"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="148" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A148">
+        <v>749</v>
+      </c>
+      <c r="B148" t="s">
+        <v>310</v>
+      </c>
+      <c r="G148" s="1">
+        <v>1</v>
+      </c>
+      <c r="H148" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I148" s="22" t="str">
+        <f t="shared" si="28"/>
+        <v>Evan</v>
+      </c>
+      <c r="J148" s="22">
+        <f t="shared" si="29"/>
+        <v>3</v>
+      </c>
+      <c r="K148" s="22">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="L148" s="22">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="M148" s="22">
+        <f t="shared" si="29"/>
+        <v>3</v>
+      </c>
+      <c r="N148" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="O148" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P148" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q148" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R148" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S148" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T148" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U148" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="V148" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="W148" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X148" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y148" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Z148" s="22" t="e">
+        <f t="shared" si="24"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="149" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A149">
+        <v>750</v>
+      </c>
+      <c r="B149" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G149" s="1">
+        <v>3</v>
+      </c>
+      <c r="H149" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I149" s="22" t="str">
+        <f t="shared" si="28"/>
+        <v>Guest</v>
+      </c>
+      <c r="J149" s="22">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="K149" s="22">
+        <f t="shared" si="29"/>
+        <v>3</v>
+      </c>
+      <c r="L149" s="22">
+        <f t="shared" si="29"/>
+        <v>3</v>
+      </c>
+      <c r="M149" s="22">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="N149" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="O149" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P149" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q149" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R149" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S149" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T149" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U149" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="V149" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="W149" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X149" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y149" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Z149" s="22">
+        <f t="shared" si="24"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -26334,11 +26597,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F368"/>
+  <dimension ref="A1:F381"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A362" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E370" sqref="E370"/>
+      <pane ySplit="1" topLeftCell="A363" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D382" sqref="D382"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -33709,11 +33972,11 @@
         <v>1</v>
       </c>
       <c r="E335" s="23" t="str">
-        <f t="shared" ref="E335:E368" si="20">A335 &amp; "_" &amp; D335</f>
+        <f t="shared" ref="E335:E381" si="20">A335 &amp; "_" &amp; D335</f>
         <v>739_1</v>
       </c>
       <c r="F335" s="23" t="str">
-        <f t="shared" ref="F335:F368" si="21">A335 &amp; "_" &amp; B335</f>
+        <f t="shared" ref="F335:F381" si="21">A335 &amp; "_" &amp; B335</f>
         <v>739_Richard</v>
       </c>
     </row>
@@ -34441,6 +34704,292 @@
       <c r="F368" s="23" t="str">
         <f t="shared" si="21"/>
         <v>747_Evan</v>
+      </c>
+    </row>
+    <row r="369" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A369">
+        <v>748</v>
+      </c>
+      <c r="B369" t="s">
+        <v>23</v>
+      </c>
+      <c r="C369" s="1">
+        <v>1</v>
+      </c>
+      <c r="D369" s="1">
+        <v>1</v>
+      </c>
+      <c r="E369" s="23" t="str">
+        <f t="shared" si="20"/>
+        <v>748_1</v>
+      </c>
+      <c r="F369" s="23" t="str">
+        <f t="shared" si="21"/>
+        <v>748_Cara</v>
+      </c>
+    </row>
+    <row r="370" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A370">
+        <v>748</v>
+      </c>
+      <c r="B370" t="s">
+        <v>7</v>
+      </c>
+      <c r="C370" s="1">
+        <v>1</v>
+      </c>
+      <c r="D370" s="1">
+        <v>2</v>
+      </c>
+      <c r="E370" s="23" t="str">
+        <f t="shared" si="20"/>
+        <v>748_2</v>
+      </c>
+      <c r="F370" s="23" t="str">
+        <f t="shared" si="21"/>
+        <v>748_Evan</v>
+      </c>
+    </row>
+    <row r="371" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A371">
+        <v>748</v>
+      </c>
+      <c r="B371" t="s">
+        <v>6</v>
+      </c>
+      <c r="C371" s="1">
+        <v>1</v>
+      </c>
+      <c r="D371" s="1">
+        <v>3</v>
+      </c>
+      <c r="E371" s="23" t="str">
+        <f t="shared" si="20"/>
+        <v>748_3</v>
+      </c>
+      <c r="F371" s="23" t="str">
+        <f t="shared" si="21"/>
+        <v>748_Jay</v>
+      </c>
+    </row>
+    <row r="372" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A372">
+        <v>748</v>
+      </c>
+      <c r="B372" t="s">
+        <v>5</v>
+      </c>
+      <c r="C372" s="1">
+        <v>1</v>
+      </c>
+      <c r="D372" s="1">
+        <v>4</v>
+      </c>
+      <c r="E372" s="23" t="str">
+        <f t="shared" si="20"/>
+        <v>748_4</v>
+      </c>
+      <c r="F372" s="23" t="str">
+        <f t="shared" si="21"/>
+        <v>748_Bob</v>
+      </c>
+    </row>
+    <row r="373" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A373">
+        <v>749</v>
+      </c>
+      <c r="B373" t="s">
+        <v>7</v>
+      </c>
+      <c r="C373" s="1">
+        <v>3</v>
+      </c>
+      <c r="D373" s="1">
+        <v>1</v>
+      </c>
+      <c r="E373" s="23" t="str">
+        <f t="shared" si="20"/>
+        <v>749_1</v>
+      </c>
+      <c r="F373" s="23" t="str">
+        <f t="shared" si="21"/>
+        <v>749_Evan</v>
+      </c>
+    </row>
+    <row r="374" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A374">
+        <v>749</v>
+      </c>
+      <c r="B374" t="s">
+        <v>5</v>
+      </c>
+      <c r="C374" s="1">
+        <v>3</v>
+      </c>
+      <c r="D374" s="1">
+        <v>2</v>
+      </c>
+      <c r="E374" s="23" t="str">
+        <f t="shared" si="20"/>
+        <v>749_2</v>
+      </c>
+      <c r="F374" s="23" t="str">
+        <f t="shared" si="21"/>
+        <v>749_Bob</v>
+      </c>
+    </row>
+    <row r="375" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A375">
+        <v>749</v>
+      </c>
+      <c r="B375" t="s">
+        <v>23</v>
+      </c>
+      <c r="C375" s="1">
+        <v>1</v>
+      </c>
+      <c r="D375" s="1">
+        <v>3</v>
+      </c>
+      <c r="E375" s="23" t="str">
+        <f t="shared" si="20"/>
+        <v>749_3</v>
+      </c>
+      <c r="F375" s="23" t="str">
+        <f t="shared" si="21"/>
+        <v>749_Cara</v>
+      </c>
+    </row>
+    <row r="376" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A376">
+        <v>749</v>
+      </c>
+      <c r="B376" t="s">
+        <v>6</v>
+      </c>
+      <c r="C376" s="1">
+        <v>1</v>
+      </c>
+      <c r="D376" s="1">
+        <v>4</v>
+      </c>
+      <c r="E376" s="23" t="str">
+        <f t="shared" si="20"/>
+        <v>749_4</v>
+      </c>
+      <c r="F376" s="23" t="str">
+        <f t="shared" si="21"/>
+        <v>749_Jay</v>
+      </c>
+    </row>
+    <row r="377" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A377">
+        <v>750</v>
+      </c>
+      <c r="B377" t="s">
+        <v>298</v>
+      </c>
+      <c r="C377" s="1">
+        <v>1</v>
+      </c>
+      <c r="D377" s="1">
+        <v>1</v>
+      </c>
+      <c r="E377" s="23" t="str">
+        <f t="shared" si="20"/>
+        <v>750_1</v>
+      </c>
+      <c r="F377" s="23" t="str">
+        <f t="shared" si="21"/>
+        <v>750_Guest</v>
+      </c>
+    </row>
+    <row r="378" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A378">
+        <v>750</v>
+      </c>
+      <c r="B378" t="s">
+        <v>7</v>
+      </c>
+      <c r="C378" s="1">
+        <v>1</v>
+      </c>
+      <c r="D378" s="1">
+        <v>2</v>
+      </c>
+      <c r="E378" s="23" t="str">
+        <f t="shared" si="20"/>
+        <v>750_2</v>
+      </c>
+      <c r="F378" s="23" t="str">
+        <f t="shared" si="21"/>
+        <v>750_Evan</v>
+      </c>
+    </row>
+    <row r="379" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A379">
+        <v>750</v>
+      </c>
+      <c r="B379" t="s">
+        <v>5</v>
+      </c>
+      <c r="C379" s="1">
+        <v>1</v>
+      </c>
+      <c r="D379" s="1">
+        <v>3</v>
+      </c>
+      <c r="E379" s="23" t="str">
+        <f t="shared" si="20"/>
+        <v>750_3</v>
+      </c>
+      <c r="F379" s="23" t="str">
+        <f t="shared" si="21"/>
+        <v>750_Bob</v>
+      </c>
+    </row>
+    <row r="380" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A380">
+        <v>750</v>
+      </c>
+      <c r="B380" t="s">
+        <v>23</v>
+      </c>
+      <c r="C380" s="1">
+        <v>3</v>
+      </c>
+      <c r="D380" s="1">
+        <v>4</v>
+      </c>
+      <c r="E380" s="23" t="str">
+        <f t="shared" si="20"/>
+        <v>750_4</v>
+      </c>
+      <c r="F380" s="23" t="str">
+        <f t="shared" si="21"/>
+        <v>750_Cara</v>
+      </c>
+    </row>
+    <row r="381" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A381">
+        <v>750</v>
+      </c>
+      <c r="B381" t="s">
+        <v>6</v>
+      </c>
+      <c r="C381" s="1">
+        <v>3</v>
+      </c>
+      <c r="D381" s="1">
+        <v>5</v>
+      </c>
+      <c r="E381" s="23" t="str">
+        <f t="shared" si="20"/>
+        <v>750_5</v>
+      </c>
+      <c r="F381" s="23" t="str">
+        <f t="shared" si="21"/>
+        <v>750_Jay</v>
       </c>
     </row>
   </sheetData>
@@ -34452,13 +35001,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:BH147"/>
+  <dimension ref="A1:BH150"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B133" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A146" sqref="A146:XFD147"/>
+      <selection pane="bottomRight" activeCell="A148" sqref="A148:XFD150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -69817,6 +70366,732 @@
       <c r="BH147" s="9">
         <f t="shared" si="744"/>
         <v>4</v>
+      </c>
+    </row>
+    <row r="148" spans="1:60" x14ac:dyDescent="0.35">
+      <c r="A148" s="24">
+        <f>Data!A147</f>
+        <v>748</v>
+      </c>
+      <c r="B148" s="26" t="e">
+        <f>Data!B147</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C148" s="27" t="str">
+        <f>Data!H147</f>
+        <v>Steve</v>
+      </c>
+      <c r="D148" s="25" t="str">
+        <f>Data!I147</f>
+        <v>Cara</v>
+      </c>
+      <c r="E148" s="22">
+        <f>IF(Data!J147=Data!$G147,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F148" s="22">
+        <f>IF(Data!K147=Data!$G147,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G148" s="22">
+        <f>IF(Data!L147=Data!$G147,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H148" s="22">
+        <f>IF(Data!M147=Data!$G147,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="I148" s="22" t="e">
+        <f>IF(Data!N147=Data!$G147,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J148" s="22" t="e">
+        <f>IF(Data!O147=Data!$G147,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K148" s="22" t="e">
+        <f>IF(Data!P147=Data!$G147,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="L148" s="22" t="e">
+        <f>IF(Data!Q147=Data!$G147,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M148" s="22" t="e">
+        <f>IF(Data!R147=Data!$G147,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N148" s="22" t="e">
+        <f>IF(Data!S147=Data!$G147,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O148" s="22" t="e">
+        <f>IF(Data!T147=Data!$G147,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P148" s="22" t="e">
+        <f>IF(Data!U147=Data!$G147,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q148" s="22" t="e">
+        <f>IF(Data!V147=Data!$G147,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R148" s="22" t="e">
+        <f>IF(Data!W147=Data!$G147,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="S148" s="22" t="e">
+        <f>IF(Data!X147=Data!$G147,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="T148" s="22" t="e">
+        <f>IF(Data!Y147=Data!$G147,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="U148" s="22" t="e">
+        <f>IF(Data!Z147=Data!$G147,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="V148" s="22">
+        <f t="shared" ref="V148:V150" si="745">COUNTIF(E148:U148,"&lt;&gt;#N/A")</f>
+        <v>4</v>
+      </c>
+      <c r="W148" s="22">
+        <f t="shared" ref="W148:W150" si="746">SUMIF(E148:U148,"&lt;&gt;#N/A")</f>
+        <v>4</v>
+      </c>
+      <c r="X148" s="22">
+        <f t="shared" ref="X148:X150" si="747">IF(W148=0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y148" s="22">
+        <f t="shared" ref="Y148:Y150" si="748">IF(V148=W148,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Z148" s="22" t="e">
+        <f t="shared" ref="Z148:Z150" si="749">IF(W148=1,INDEX($E$2:$U$2,1,MATCH(1,E148:U148,0)),NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AA148" s="7">
+        <f t="shared" ref="AA148:AA150" si="750">IF(ISNA(E148),AA147,IF(E148=1,AA147+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AB148" s="7">
+        <f t="shared" ref="AB148:AB150" si="751">IF(ISNA(F148),AB147,IF(F148=1,AB147+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AC148" s="7">
+        <f t="shared" ref="AC148:AC150" si="752">IF(ISNA(G148),AC147,IF(G148=1,AC147+1,0))</f>
+        <v>4</v>
+      </c>
+      <c r="AD148" s="7">
+        <f t="shared" ref="AD148:AD150" si="753">IF(ISNA(H148),AD147,IF(H148=1,AD147+1,0))</f>
+        <v>2</v>
+      </c>
+      <c r="AE148" s="7">
+        <f t="shared" ref="AE148:AE150" si="754">IF(ISNA(I148),AE147,IF(I148=1,AE147+1,0))</f>
+        <v>3</v>
+      </c>
+      <c r="AF148" s="7">
+        <f t="shared" ref="AF148:AF150" si="755">IF(ISNA(J148),AF147,IF(J148=1,AF147+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AG148" s="7">
+        <f t="shared" ref="AG148:AG150" si="756">IF(ISNA(K148),AG147,IF(K148=1,AG147+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AH148" s="7">
+        <f t="shared" ref="AH148:AH150" si="757">IF(ISNA(L148),AH147,IF(L148=1,AH147+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AI148" s="7">
+        <f t="shared" ref="AI148:AI150" si="758">IF(ISNA(M148),AI147,IF(M148=1,AI147+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AJ148" s="7">
+        <f t="shared" ref="AJ148:AJ150" si="759">IF(ISNA(N148),AJ147,IF(N148=1,AJ147+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AK148" s="7">
+        <f t="shared" ref="AK148:AK150" si="760">IF(ISNA(O148),AK147,IF(O148=1,AK147+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AL148" s="7">
+        <f t="shared" ref="AL148:AL150" si="761">IF(ISNA(P148),AL147,IF(P148=1,AL147+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AM148" s="7">
+        <f t="shared" ref="AM148:AM150" si="762">IF(ISNA(Q148),AM147,IF(Q148=1,AM147+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AN148" s="7">
+        <f t="shared" ref="AN148:AN150" si="763">IF(ISNA(R148),AN147,IF(R148=1,AN147+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AO148" s="7">
+        <f t="shared" ref="AO148:AO150" si="764">IF(ISNA(S148),AO147,IF(S148=1,AO147+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AP148" s="7">
+        <f t="shared" ref="AP148:AP150" si="765">IF(ISNA(T148),AP147,IF(T148=1,AP147+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AQ148" s="7">
+        <f t="shared" ref="AQ148:AQ150" si="766">IF(ISNA(U148),AQ147,IF(U148=1,AQ147+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AR148" s="9">
+        <f t="shared" ref="AR148:AR150" si="767">IF(ISNA(E148),AR147,IF(E148=0,AR147+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AS148" s="9">
+        <f t="shared" ref="AS148:AS150" si="768">IF(ISNA(F148),AS147,IF(F148=0,AS147+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AT148" s="9">
+        <f t="shared" ref="AT148:AT150" si="769">IF(ISNA(G148),AT147,IF(G148=0,AT147+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AU148" s="9">
+        <f t="shared" ref="AU148:AU150" si="770">IF(ISNA(H148),AU147,IF(H148=0,AU147+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AV148" s="9">
+        <f t="shared" ref="AV148:AV150" si="771">IF(ISNA(I148),AV147,IF(I148=0,AV147+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AW148" s="9">
+        <f t="shared" ref="AW148:AW150" si="772">IF(ISNA(J148),AW147,IF(J148=0,AW147+1,0))</f>
+        <v>5</v>
+      </c>
+      <c r="AX148" s="9">
+        <f t="shared" ref="AX148:AX150" si="773">IF(ISNA(K148),AX147,IF(K148=0,AX147+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AY148" s="9">
+        <f t="shared" ref="AY148:AY150" si="774">IF(ISNA(L148),AY147,IF(L148=0,AY147+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AZ148" s="9">
+        <f t="shared" ref="AZ148:AZ150" si="775">IF(ISNA(M148),AZ147,IF(M148=0,AZ147+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="BA148" s="9">
+        <f t="shared" ref="BA148:BA150" si="776">IF(ISNA(N148),BA147,IF(N148=0,BA147+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="BB148" s="9">
+        <f t="shared" ref="BB148:BB150" si="777">IF(ISNA(O148),BB147,IF(O148=0,BB147+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="BC148" s="9">
+        <f t="shared" ref="BC148:BC150" si="778">IF(ISNA(P148),BC147,IF(P148=0,BC147+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="BD148" s="9">
+        <f t="shared" ref="BD148:BD150" si="779">IF(ISNA(Q148),BD147,IF(Q148=0,BD147+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="BE148" s="9">
+        <f t="shared" ref="BE148:BE150" si="780">IF(ISNA(R148),BE147,IF(R148=0,BE147+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="BF148" s="9">
+        <f t="shared" ref="BF148:BF150" si="781">IF(ISNA(S148),BF147,IF(S148=0,BF147+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="BG148" s="9">
+        <f t="shared" ref="BG148:BG150" si="782">IF(ISNA(T148),BG147,IF(T148=0,BG147+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="BH148" s="9">
+        <f t="shared" ref="BH148:BH150" si="783">IF(ISNA(U148),BH147,IF(U148=0,BH147+1,0))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="149" spans="1:60" x14ac:dyDescent="0.35">
+      <c r="A149" s="24">
+        <f>Data!A148</f>
+        <v>749</v>
+      </c>
+      <c r="B149" s="26" t="str">
+        <f>Data!B148</f>
+        <v>Carl Sagan</v>
+      </c>
+      <c r="C149" s="27" t="str">
+        <f>Data!H148</f>
+        <v>Steve</v>
+      </c>
+      <c r="D149" s="25" t="str">
+        <f>Data!I148</f>
+        <v>Evan</v>
+      </c>
+      <c r="E149" s="22">
+        <f>IF(Data!J148=Data!$G148,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F149" s="22">
+        <f>IF(Data!K148=Data!$G148,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G149" s="22">
+        <f>IF(Data!L148=Data!$G148,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H149" s="22">
+        <f>IF(Data!M148=Data!$G148,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I149" s="22" t="e">
+        <f>IF(Data!N148=Data!$G148,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J149" s="22" t="e">
+        <f>IF(Data!O148=Data!$G148,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K149" s="22" t="e">
+        <f>IF(Data!P148=Data!$G148,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="L149" s="22" t="e">
+        <f>IF(Data!Q148=Data!$G148,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M149" s="22" t="e">
+        <f>IF(Data!R148=Data!$G148,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N149" s="22" t="e">
+        <f>IF(Data!S148=Data!$G148,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O149" s="22" t="e">
+        <f>IF(Data!T148=Data!$G148,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P149" s="22" t="e">
+        <f>IF(Data!U148=Data!$G148,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q149" s="22" t="e">
+        <f>IF(Data!V148=Data!$G148,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R149" s="22" t="e">
+        <f>IF(Data!W148=Data!$G148,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="S149" s="22" t="e">
+        <f>IF(Data!X148=Data!$G148,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="T149" s="22" t="e">
+        <f>IF(Data!Y148=Data!$G148,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="U149" s="22" t="e">
+        <f>IF(Data!Z148=Data!$G148,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="V149" s="22">
+        <f t="shared" si="745"/>
+        <v>4</v>
+      </c>
+      <c r="W149" s="22">
+        <f t="shared" si="746"/>
+        <v>2</v>
+      </c>
+      <c r="X149" s="22">
+        <f t="shared" si="747"/>
+        <v>0</v>
+      </c>
+      <c r="Y149" s="22">
+        <f t="shared" si="748"/>
+        <v>0</v>
+      </c>
+      <c r="Z149" s="22" t="e">
+        <f t="shared" si="749"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA149" s="7">
+        <f t="shared" si="750"/>
+        <v>0</v>
+      </c>
+      <c r="AB149" s="7">
+        <f t="shared" si="751"/>
+        <v>2</v>
+      </c>
+      <c r="AC149" s="7">
+        <f t="shared" si="752"/>
+        <v>5</v>
+      </c>
+      <c r="AD149" s="7">
+        <f t="shared" si="753"/>
+        <v>0</v>
+      </c>
+      <c r="AE149" s="7">
+        <f t="shared" si="754"/>
+        <v>3</v>
+      </c>
+      <c r="AF149" s="7">
+        <f t="shared" si="755"/>
+        <v>0</v>
+      </c>
+      <c r="AG149" s="7">
+        <f t="shared" si="756"/>
+        <v>0</v>
+      </c>
+      <c r="AH149" s="7">
+        <f t="shared" si="757"/>
+        <v>1</v>
+      </c>
+      <c r="AI149" s="7">
+        <f t="shared" si="758"/>
+        <v>0</v>
+      </c>
+      <c r="AJ149" s="7">
+        <f t="shared" si="759"/>
+        <v>1</v>
+      </c>
+      <c r="AK149" s="7">
+        <f t="shared" si="760"/>
+        <v>0</v>
+      </c>
+      <c r="AL149" s="7">
+        <f t="shared" si="761"/>
+        <v>0</v>
+      </c>
+      <c r="AM149" s="7">
+        <f t="shared" si="762"/>
+        <v>0</v>
+      </c>
+      <c r="AN149" s="7">
+        <f t="shared" si="763"/>
+        <v>1</v>
+      </c>
+      <c r="AO149" s="7">
+        <f t="shared" si="764"/>
+        <v>0</v>
+      </c>
+      <c r="AP149" s="7">
+        <f t="shared" si="765"/>
+        <v>0</v>
+      </c>
+      <c r="AQ149" s="7">
+        <f t="shared" si="766"/>
+        <v>0</v>
+      </c>
+      <c r="AR149" s="9">
+        <f t="shared" si="767"/>
+        <v>1</v>
+      </c>
+      <c r="AS149" s="9">
+        <f t="shared" si="768"/>
+        <v>0</v>
+      </c>
+      <c r="AT149" s="9">
+        <f t="shared" si="769"/>
+        <v>0</v>
+      </c>
+      <c r="AU149" s="9">
+        <f t="shared" si="770"/>
+        <v>1</v>
+      </c>
+      <c r="AV149" s="9">
+        <f t="shared" si="771"/>
+        <v>0</v>
+      </c>
+      <c r="AW149" s="9">
+        <f t="shared" si="772"/>
+        <v>5</v>
+      </c>
+      <c r="AX149" s="9">
+        <f t="shared" si="773"/>
+        <v>0</v>
+      </c>
+      <c r="AY149" s="9">
+        <f t="shared" si="774"/>
+        <v>0</v>
+      </c>
+      <c r="AZ149" s="9">
+        <f t="shared" si="775"/>
+        <v>0</v>
+      </c>
+      <c r="BA149" s="9">
+        <f t="shared" si="776"/>
+        <v>0</v>
+      </c>
+      <c r="BB149" s="9">
+        <f t="shared" si="777"/>
+        <v>0</v>
+      </c>
+      <c r="BC149" s="9">
+        <f t="shared" si="778"/>
+        <v>0</v>
+      </c>
+      <c r="BD149" s="9">
+        <f t="shared" si="779"/>
+        <v>1</v>
+      </c>
+      <c r="BE149" s="9">
+        <f t="shared" si="780"/>
+        <v>0</v>
+      </c>
+      <c r="BF149" s="9">
+        <f t="shared" si="781"/>
+        <v>1</v>
+      </c>
+      <c r="BG149" s="9">
+        <f t="shared" si="782"/>
+        <v>1</v>
+      </c>
+      <c r="BH149" s="9">
+        <f t="shared" si="783"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="150" spans="1:60" x14ac:dyDescent="0.35">
+      <c r="A150" s="24">
+        <f>Data!A149</f>
+        <v>750</v>
+      </c>
+      <c r="B150" s="26" t="e">
+        <f>Data!B149</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C150" s="27" t="str">
+        <f>Data!H149</f>
+        <v>Steve</v>
+      </c>
+      <c r="D150" s="25" t="str">
+        <f>Data!I149</f>
+        <v>Guest</v>
+      </c>
+      <c r="E150" s="22">
+        <f>IF(Data!J149=Data!$G149,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F150" s="22">
+        <f>IF(Data!K149=Data!$G149,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G150" s="22">
+        <f>IF(Data!L149=Data!$G149,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H150" s="22">
+        <f>IF(Data!M149=Data!$G149,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I150" s="22" t="e">
+        <f>IF(Data!N149=Data!$G149,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J150" s="22" t="e">
+        <f>IF(Data!O149=Data!$G149,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K150" s="22" t="e">
+        <f>IF(Data!P149=Data!$G149,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="L150" s="22" t="e">
+        <f>IF(Data!Q149=Data!$G149,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M150" s="22" t="e">
+        <f>IF(Data!R149=Data!$G149,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N150" s="22" t="e">
+        <f>IF(Data!S149=Data!$G149,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O150" s="22" t="e">
+        <f>IF(Data!T149=Data!$G149,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P150" s="22" t="e">
+        <f>IF(Data!U149=Data!$G149,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q150" s="22" t="e">
+        <f>IF(Data!V149=Data!$G149,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R150" s="22" t="e">
+        <f>IF(Data!W149=Data!$G149,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="S150" s="22" t="e">
+        <f>IF(Data!X149=Data!$G149,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="T150" s="22" t="e">
+        <f>IF(Data!Y149=Data!$G149,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="U150" s="22">
+        <f>IF(Data!Z149=Data!$G149,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V150" s="22">
+        <f t="shared" si="745"/>
+        <v>5</v>
+      </c>
+      <c r="W150" s="22">
+        <f t="shared" si="746"/>
+        <v>2</v>
+      </c>
+      <c r="X150" s="22">
+        <f t="shared" si="747"/>
+        <v>0</v>
+      </c>
+      <c r="Y150" s="22">
+        <f t="shared" si="748"/>
+        <v>0</v>
+      </c>
+      <c r="Z150" s="22" t="e">
+        <f t="shared" si="749"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA150" s="7">
+        <f t="shared" si="750"/>
+        <v>0</v>
+      </c>
+      <c r="AB150" s="7">
+        <f t="shared" si="751"/>
+        <v>3</v>
+      </c>
+      <c r="AC150" s="7">
+        <f t="shared" si="752"/>
+        <v>6</v>
+      </c>
+      <c r="AD150" s="7">
+        <f t="shared" si="753"/>
+        <v>0</v>
+      </c>
+      <c r="AE150" s="7">
+        <f t="shared" si="754"/>
+        <v>3</v>
+      </c>
+      <c r="AF150" s="7">
+        <f t="shared" si="755"/>
+        <v>0</v>
+      </c>
+      <c r="AG150" s="7">
+        <f t="shared" si="756"/>
+        <v>0</v>
+      </c>
+      <c r="AH150" s="7">
+        <f t="shared" si="757"/>
+        <v>1</v>
+      </c>
+      <c r="AI150" s="7">
+        <f t="shared" si="758"/>
+        <v>0</v>
+      </c>
+      <c r="AJ150" s="7">
+        <f t="shared" si="759"/>
+        <v>1</v>
+      </c>
+      <c r="AK150" s="7">
+        <f t="shared" si="760"/>
+        <v>0</v>
+      </c>
+      <c r="AL150" s="7">
+        <f t="shared" si="761"/>
+        <v>0</v>
+      </c>
+      <c r="AM150" s="7">
+        <f t="shared" si="762"/>
+        <v>0</v>
+      </c>
+      <c r="AN150" s="7">
+        <f t="shared" si="763"/>
+        <v>1</v>
+      </c>
+      <c r="AO150" s="7">
+        <f t="shared" si="764"/>
+        <v>0</v>
+      </c>
+      <c r="AP150" s="7">
+        <f t="shared" si="765"/>
+        <v>0</v>
+      </c>
+      <c r="AQ150" s="7">
+        <f t="shared" si="766"/>
+        <v>0</v>
+      </c>
+      <c r="AR150" s="9">
+        <f t="shared" si="767"/>
+        <v>2</v>
+      </c>
+      <c r="AS150" s="9">
+        <f t="shared" si="768"/>
+        <v>0</v>
+      </c>
+      <c r="AT150" s="9">
+        <f t="shared" si="769"/>
+        <v>0</v>
+      </c>
+      <c r="AU150" s="9">
+        <f t="shared" si="770"/>
+        <v>2</v>
+      </c>
+      <c r="AV150" s="9">
+        <f t="shared" si="771"/>
+        <v>0</v>
+      </c>
+      <c r="AW150" s="9">
+        <f t="shared" si="772"/>
+        <v>5</v>
+      </c>
+      <c r="AX150" s="9">
+        <f t="shared" si="773"/>
+        <v>0</v>
+      </c>
+      <c r="AY150" s="9">
+        <f t="shared" si="774"/>
+        <v>0</v>
+      </c>
+      <c r="AZ150" s="9">
+        <f t="shared" si="775"/>
+        <v>0</v>
+      </c>
+      <c r="BA150" s="9">
+        <f t="shared" si="776"/>
+        <v>0</v>
+      </c>
+      <c r="BB150" s="9">
+        <f t="shared" si="777"/>
+        <v>0</v>
+      </c>
+      <c r="BC150" s="9">
+        <f t="shared" si="778"/>
+        <v>0</v>
+      </c>
+      <c r="BD150" s="9">
+        <f t="shared" si="779"/>
+        <v>1</v>
+      </c>
+      <c r="BE150" s="9">
+        <f t="shared" si="780"/>
+        <v>0</v>
+      </c>
+      <c r="BF150" s="9">
+        <f t="shared" si="781"/>
+        <v>1</v>
+      </c>
+      <c r="BG150" s="9">
+        <f t="shared" si="782"/>
+        <v>1</v>
+      </c>
+      <c r="BH150" s="9">
+        <f t="shared" si="783"/>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -72331,7 +73606,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
@@ -72415,19 +73690,19 @@
       </c>
       <c r="B2" s="5">
         <f>SUMIF(Results!E105:E151,"&lt;&gt;#N/A")/COUNTIFS(Results!E105:E151,"&lt;&gt;#N/A",Results!E105:E151,"&lt;&gt;")</f>
-        <v>0.47619047619047616</v>
+        <v>0.46666666666666667</v>
       </c>
       <c r="C2" s="5">
         <f>SUMIF(Results!F105:F151,"&lt;&gt;#N/A")/COUNTIFS(Results!F105:F151,"&lt;&gt;#N/A",Results!F105:F151,"&lt;&gt;")</f>
-        <v>0.69696969696969702</v>
+        <v>0.72222222222222221</v>
       </c>
       <c r="D2" s="5">
         <f>SUMIF(Results!G105:G151,"&lt;&gt;#N/A")/COUNTIFS(Results!G105:G151,"&lt;&gt;#N/A",Results!G105:G151,"&lt;&gt;")</f>
-        <v>0.59523809523809523</v>
+        <v>0.62222222222222223</v>
       </c>
       <c r="E2" s="5">
         <f>SUMIF(Results!H105:H151,"&lt;&gt;#N/A")/COUNTIFS(Results!H105:H151,"&lt;&gt;#N/A",Results!H105:H151,"&lt;&gt;")</f>
-        <v>0.55000000000000004</v>
+        <v>0.53488372093023251</v>
       </c>
       <c r="F2" s="5">
         <f>SUMIF(Results!I105:I151,"&lt;&gt;#N/A")/COUNTIFS(Results!I105:I151,"&lt;&gt;#N/A",Results!I105:I151,"&lt;&gt;")</f>
@@ -72475,7 +73750,7 @@
       </c>
       <c r="Q2" s="5">
         <f>SUM(Results!W105:W151)/SUM(Results!V105:V151)</f>
-        <v>0.56024096385542166</v>
+        <v>0.56424581005586594</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.35">
@@ -72484,19 +73759,19 @@
       </c>
       <c r="B3" s="5">
         <f>SUMIFS(Results!E105:E151,Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!E105:E151, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!E105:E151, "&lt;&gt;#N/A", Results!E105:E151, "&lt;&gt;")</f>
-        <v>0.45454545454545453</v>
+        <v>0.43478260869565216</v>
       </c>
       <c r="C3" s="5">
         <f>SUMIFS(Results!F105:F151,Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!F105:F151, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!F105:F151, "&lt;&gt;#N/A", Results!F105:F151, "&lt;&gt;")</f>
-        <v>0.76470588235294112</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="D3" s="5">
         <f>SUMIFS(Results!G105:G151,Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!G105:G151, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!G105:G151, "&lt;&gt;#N/A", Results!G105:G151, "&lt;&gt;")</f>
-        <v>0.68181818181818177</v>
+        <v>0.69565217391304346</v>
       </c>
       <c r="E3" s="5">
         <f>SUMIFS(Results!H105:H151,Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!H105:H151, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!H105:H151, "&lt;&gt;#N/A", Results!H105:H151, "&lt;&gt;")</f>
-        <v>0.45454545454545453</v>
+        <v>0.43478260869565216</v>
       </c>
       <c r="F3" s="5">
         <f>SUMIFS(Results!I105:I151,Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!I105:I151, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!I105:I151, "&lt;&gt;#N/A", Results!I105:I151, "&lt;&gt;")</f>
@@ -72544,7 +73819,7 @@
       </c>
       <c r="Q3" s="5">
         <f>SUMIF(Results!B105:B151,"&lt;&gt;#N/A",Results!W105:W151)/SUMIF(Results!B105:B151,"&lt;&gt;#N/A",Results!V105:V151)</f>
-        <v>0.56043956043956045</v>
+        <v>0.55789473684210522</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
@@ -72557,15 +73832,15 @@
       </c>
       <c r="C4" s="5">
         <f>SUMIFS(Results!F105:F151,Results!$B$105:$B$151,"=#N/A",Results!F105:F151, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$151,"=#N/A",Results!F105:F151, "&lt;&gt;#N/A", Results!F105:F151, "&lt;&gt;")</f>
-        <v>0.625</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="D4" s="5">
         <f>SUMIFS(Results!G105:G151,Results!$B$105:$B$151,"=#N/A",Results!G105:G151, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$151,"=#N/A",Results!G105:G151, "&lt;&gt;#N/A", Results!G105:G151, "&lt;&gt;")</f>
-        <v>0.5</v>
+        <v>0.54545454545454541</v>
       </c>
       <c r="E4" s="5">
         <f>SUMIFS(Results!H105:H151,Results!$B$105:$B$151,"=#N/A",Results!H105:H151, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$151,"=#N/A",Results!H105:H151, "&lt;&gt;#N/A", Results!H105:H151, "&lt;&gt;")</f>
-        <v>0.66666666666666663</v>
+        <v>0.65</v>
       </c>
       <c r="F4" s="5" t="e">
         <f>SUMIFS(Results!I105:I151,Results!$B$105:$B$151,"=#N/A",Results!I105:I151, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$151,"=#N/A",Results!I105:I151, "&lt;&gt;#N/A", Results!I105:I151, "&lt;&gt;")</f>
@@ -72613,7 +73888,7 @@
       </c>
       <c r="Q4" s="5">
         <f>SUMIF(Results!B105:B151,"=#N/A",Results!W105:W151)/SUMIF(Results!B105:B151,"=#N/A",Results!V105:V151)</f>
-        <v>0.56000000000000005</v>
+        <v>0.5714285714285714</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
@@ -72630,7 +73905,7 @@
       </c>
       <c r="D5" s="1">
         <f>MAX(Results!AC105:AC151)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E5" s="1">
         <f>MAX(Results!AD105:AD151)</f>
@@ -72833,7 +74108,7 @@
       </c>
       <c r="C8" s="6">
         <f>SUMIF(Results!$D$105:$D$151,C1,Results!$W$105:$W$151)/SUMIF(Results!$D$105:$D$151,C1,Results!$V$105:$V$151)</f>
-        <v>0.67741935483870963</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="D8" s="6">
         <f>SUMIF(Results!$D$105:$D$151,D1,Results!$W$105:$W$151)/SUMIF(Results!$D$105:$D$151,D1,Results!$V$105:$V$151)</f>
@@ -72841,7 +74116,7 @@
       </c>
       <c r="E8" s="6">
         <f>SUMIF(Results!$D$105:$D$151,E1,Results!$W$105:$W$151)/SUMIF(Results!$D$105:$D$151,E1,Results!$V$105:$V$151)</f>
-        <v>0.43333333333333335</v>
+        <v>0.44117647058823528</v>
       </c>
       <c r="F8" s="6" t="e">
         <f>SUMIF(Results!$D$105:$D$151,F1,Results!$W$105:$W$151)/SUMIF(Results!$D$105:$D$151,F1,Results!$V$105:$V$151)</f>
@@ -72899,7 +74174,7 @@
       </c>
       <c r="C9" s="20">
         <f>SUMIF(Results!$D$105:$D$151,C1,Results!F$105:F$151)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D9" s="20">
         <f>SUMIF(Results!$D$105:$D$151,D1,Results!G$105:G$151)</f>
@@ -72955,7 +74230,7 @@
       </c>
       <c r="Q9" s="21">
         <f>SUM(B9:P9)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.35">
@@ -72968,7 +74243,7 @@
       </c>
       <c r="C10" s="1">
         <f>COUNTIF(Results!$D$105:$D$151,'Summary 2019'!C1)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D10" s="1">
         <f>COUNTIF(Results!$D$105:$D$151,'Summary 2019'!D1)</f>
@@ -72976,7 +74251,7 @@
       </c>
       <c r="E10" s="1">
         <f>COUNTIF(Results!$D$105:$D$151,'Summary 2019'!E1)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F10" s="1">
         <f>COUNTIF(Results!$D$105:$D$151,'Summary 2019'!F1)</f>
@@ -73024,7 +74299,7 @@
       </c>
       <c r="Q10" s="1">
         <f>SUM(B10:P10)</f>
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.35">
@@ -73037,7 +74312,7 @@
       </c>
       <c r="C11" s="6">
         <f>SUMIF(Results!$D$105:$D$151,C1,Results!F$105:F$151)/COUNTIF(Results!$D$105:$D$151,C1)</f>
-        <v>0.625</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="D11" s="6">
         <f>SUMIF(Results!$D$105:$D$151,D1,Results!G$105:G$151)/COUNTIF(Results!$D$105:$D$151,D1)</f>
@@ -73045,7 +74320,7 @@
       </c>
       <c r="E11" s="6">
         <f>SUMIF(Results!$D$105:$D$151,E1,Results!H$105:H$151)/COUNTIF(Results!$D$105:$D$151,E1)</f>
-        <v>0.375</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F11" s="6" t="e">
         <f>SUMIF(Results!$D$105:$D$151,F1,Results!I$105:I$151)/COUNTIF(Results!$D$105:$D$151,F1)</f>
@@ -73093,7 +74368,7 @@
       </c>
       <c r="Q11" s="5">
         <f>Q9/Q10</f>
-        <v>0.35897435897435898</v>
+        <v>0.36585365853658536</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.35">
@@ -73102,19 +74377,19 @@
       </c>
       <c r="B12" s="1">
         <f>SUMIF(Results!E105:E151,"&lt;&gt;#N/A")</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C12" s="1">
         <f>SUMIF(Results!F105:F151,"&lt;&gt;#N/A")</f>
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D12" s="1">
         <f>SUMIF(Results!G105:G151,"&lt;&gt;#N/A")</f>
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E12" s="1">
         <f>SUMIF(Results!H105:H151,"&lt;&gt;#N/A")</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F12" s="1">
         <f>SUMIF(Results!I105:I151,"&lt;&gt;#N/A")</f>
@@ -73162,7 +74437,7 @@
       </c>
       <c r="Q12" s="1">
         <f t="shared" ref="Q12:Q17" si="0">SUM(B12:P12)</f>
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.35">
@@ -73171,19 +74446,19 @@
       </c>
       <c r="B13" s="1">
         <f>COUNTIFS(Results!E105:E151,"&lt;&gt;#N/A",Results!E105:E151,"&lt;&gt;")</f>
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C13" s="1">
         <f>COUNTIFS(Results!F105:F151,"&lt;&gt;#N/A",Results!F105:F151,"&lt;&gt;")</f>
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D13" s="1">
         <f>COUNTIFS(Results!G105:G151,"&lt;&gt;#N/A",Results!G105:G151,"&lt;&gt;")</f>
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E13" s="1">
         <f>COUNTIFS(Results!H105:H151,"&lt;&gt;#N/A",Results!H105:H151,"&lt;&gt;")</f>
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F13" s="1">
         <f>COUNTIFS(Results!I105:I151,"&lt;&gt;#N/A",Results!I105:I151,"&lt;&gt;")</f>
@@ -73231,7 +74506,7 @@
       </c>
       <c r="Q13" s="1">
         <f t="shared" si="0"/>
-        <v>162</v>
+        <v>174</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.35">
@@ -73244,11 +74519,11 @@
       </c>
       <c r="C14" s="1">
         <f>SUMIFS(Results!F105:F151,Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!F105:F151, "&lt;&gt;#N/A")</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D14" s="1">
         <f>SUMIFS(Results!G105:G151,Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!G105:G151, "&lt;&gt;#N/A")</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E14" s="1">
         <f>SUMIFS(Results!H105:H151,Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!H105:H151, "&lt;&gt;#N/A")</f>
@@ -73300,7 +74575,7 @@
       </c>
       <c r="Q14" s="1">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.35">
@@ -73309,19 +74584,19 @@
       </c>
       <c r="B15" s="1">
         <f>COUNTIFS(Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!E105:E151, "&lt;&gt;#N/A", Results!E105:E151, "&lt;&gt;")</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C15" s="1">
         <f>COUNTIFS(Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!F105:F151, "&lt;&gt;#N/A", Results!F105:F151, "&lt;&gt;")</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D15" s="1">
         <f>COUNTIFS(Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!G105:G151, "&lt;&gt;#N/A", Results!G105:G151, "&lt;&gt;")</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E15" s="1">
         <f>COUNTIFS(Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!H105:H151, "&lt;&gt;#N/A", Results!H105:H151, "&lt;&gt;")</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F15" s="1">
         <f>COUNTIFS(Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!I105:I151, "&lt;&gt;#N/A", Results!I105:I151, "&lt;&gt;")</f>
@@ -73369,7 +74644,7 @@
       </c>
       <c r="Q15" s="1">
         <f t="shared" si="0"/>
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.35">
@@ -73378,19 +74653,19 @@
       </c>
       <c r="B16" s="1">
         <f>SUMIFS(Results!E105:E151,Results!$B$105:$B$151,"=#N/A",Results!E105:E151, "&lt;&gt;#N/A")</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C16" s="1">
         <f>SUMIFS(Results!F105:F151,Results!$B$105:$B$151,"=#N/A",Results!F105:F151, "&lt;&gt;#N/A")</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D16" s="1">
         <f>SUMIFS(Results!G105:G151,Results!$B$105:$B$151,"=#N/A",Results!G105:G151, "&lt;&gt;#N/A")</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E16" s="1">
         <f>SUMIFS(Results!H105:H151,Results!$B$105:$B$151,"=#N/A",Results!H105:H151, "&lt;&gt;#N/A")</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F16" s="1">
         <f>SUMIFS(Results!I105:I151,Results!$B$105:$B$151,"=#N/A",Results!I105:I151, "&lt;&gt;#N/A")</f>
@@ -73438,7 +74713,7 @@
       </c>
       <c r="Q16" s="1">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.35">
@@ -73447,19 +74722,19 @@
       </c>
       <c r="B17" s="1">
         <f>COUNTIFS(Results!$B$105:$B$151,"=#N/A",Results!E105:E151, "&lt;&gt;#N/A", Results!E105:E151, "&lt;&gt;")</f>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C17" s="1">
         <f>COUNTIFS(Results!$B$105:$B$151,"=#N/A",Results!F105:F151, "&lt;&gt;#N/A", Results!F105:F151, "&lt;&gt;")</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D17" s="1">
         <f>COUNTIFS(Results!$B$105:$B$151,"=#N/A",Results!G105:G151, "&lt;&gt;#N/A", Results!G105:G151, "&lt;&gt;")</f>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E17" s="1">
         <f>COUNTIFS(Results!$B$105:$B$151,"=#N/A",Results!H105:H151, "&lt;&gt;#N/A", Results!H105:H151, "&lt;&gt;")</f>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F17" s="1">
         <f>COUNTIFS(Results!$B$105:$B$151,"=#N/A",Results!I105:I151, "&lt;&gt;#N/A", Results!I105:I151, "&lt;&gt;")</f>
@@ -73507,7 +74782,7 @@
       </c>
       <c r="Q17" s="1">
         <f t="shared" si="0"/>
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.35">
@@ -73585,19 +74860,19 @@
       </c>
       <c r="B19" s="1">
         <f>SUMIF(Results!E105:E151,"&lt;&gt;#N/A",Results!$Y$105:$Y$151)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C19" s="1">
         <f>SUMIF(Results!F105:F151,"&lt;&gt;#N/A",Results!$Y$105:$Y$151)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D19" s="1">
         <f>SUMIF(Results!G105:G151,"&lt;&gt;#N/A",Results!$Y$105:$Y$151)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E19" s="1">
         <f>SUMIF(Results!H105:H151,"&lt;&gt;#N/A",Results!$Y$105:$Y$151)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F19" s="1">
         <f>SUMIF(Results!I105:I151,"&lt;&gt;#N/A",Results!$Y$105:$Y$151)</f>
@@ -73645,7 +74920,7 @@
       </c>
       <c r="Q19" s="18">
         <f>SUM(Results!Y105:Y151)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Through Episode 754
</commit_message>
<xml_diff>
--- a/SGU_Science_or_Fiction.xlsx
+++ b/SGU_Science_or_Fiction.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xwhx\SourceControl\SGU_Science_or_Fiction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6440448C-6348-491B-BE18-E082DB7CE512}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121B8629-ED15-496F-B5A5-874BB743E718}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="317">
   <si>
     <t>Episode</t>
   </si>
@@ -981,6 +981,24 @@
   </si>
   <si>
     <t>Carl Sagan</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>RichardS</t>
+  </si>
+  <si>
+    <t>Scotland</t>
+  </si>
+  <si>
+    <t>Scott</t>
+  </si>
+  <si>
+    <t>Hybrids</t>
+  </si>
+  <si>
+    <t>Coffee</t>
   </si>
 </sst>
 </file>
@@ -13309,11 +13327,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z149"/>
+  <dimension ref="A1:Z153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I147" sqref="I147:Z149"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A135" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I153" sqref="I153:Z153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -25028,7 +25046,7 @@
         <v>#N/A</v>
       </c>
       <c r="Z131" s="22" t="e">
-        <f t="shared" ref="Z131:Z149" si="24">INDEX(AnsLkUp,MATCH($A131 &amp; "_"&amp;Z$1,LookupName,0),3)</f>
+        <f t="shared" ref="Z131:Z153" si="24">INDEX(AnsLkUp,MATCH($A131 &amp; "_"&amp;Z$1,LookupName,0),3)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -26407,7 +26425,7 @@
         <v>#N/A</v>
       </c>
       <c r="Y147" s="22" t="e">
-        <f t="shared" ref="J147:Y149" si="29">INDEX(AnsLkUp,MATCH($A147 &amp; "_"&amp;Y$1,LookupName,0),3)</f>
+        <f t="shared" ref="J147:Y153" si="29">INDEX(AnsLkUp,MATCH($A147 &amp; "_"&amp;Y$1,LookupName,0),3)</f>
         <v>#N/A</v>
       </c>
       <c r="Z147" s="22" t="e">
@@ -26586,6 +26604,350 @@
       <c r="Z149" s="22">
         <f t="shared" si="24"/>
         <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A150">
+        <v>751</v>
+      </c>
+      <c r="B150" t="s">
+        <v>311</v>
+      </c>
+      <c r="G150" s="1">
+        <v>2</v>
+      </c>
+      <c r="H150" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="I150" s="22" t="str">
+        <f t="shared" ref="I150:I152" si="30">INDEX(AnsLkUp,MATCH(A150 &amp; "_1",LookupOrder,1),2)</f>
+        <v>Jay</v>
+      </c>
+      <c r="J150" s="22">
+        <f t="shared" si="29"/>
+        <v>3</v>
+      </c>
+      <c r="K150" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="L150" s="22">
+        <f t="shared" si="29"/>
+        <v>4</v>
+      </c>
+      <c r="M150" s="22">
+        <f t="shared" si="29"/>
+        <v>4</v>
+      </c>
+      <c r="N150" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="O150" s="22">
+        <f t="shared" si="29"/>
+        <v>3</v>
+      </c>
+      <c r="P150" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q150" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R150" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S150" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T150" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U150" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="V150" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="W150" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X150" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y150" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Z150" s="22" t="e">
+        <f t="shared" si="24"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="151" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A151">
+        <v>752</v>
+      </c>
+      <c r="B151" t="s">
+        <v>313</v>
+      </c>
+      <c r="G151" s="1">
+        <v>3</v>
+      </c>
+      <c r="H151" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="I151" s="22" t="str">
+        <f t="shared" si="30"/>
+        <v>George</v>
+      </c>
+      <c r="J151" s="22">
+        <f t="shared" si="29"/>
+        <v>2</v>
+      </c>
+      <c r="K151" s="22">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="L151" s="22">
+        <f t="shared" si="29"/>
+        <v>2</v>
+      </c>
+      <c r="M151" s="22">
+        <f t="shared" si="29"/>
+        <v>3</v>
+      </c>
+      <c r="N151" s="22">
+        <f t="shared" si="29"/>
+        <v>2</v>
+      </c>
+      <c r="O151" s="22">
+        <f t="shared" si="29"/>
+        <v>3</v>
+      </c>
+      <c r="P151" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q151" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R151" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S151" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T151" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U151" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="V151" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="W151" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X151" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y151" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Z151" s="22" t="e">
+        <f t="shared" si="24"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="152" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A152">
+        <v>753</v>
+      </c>
+      <c r="B152" t="s">
+        <v>315</v>
+      </c>
+      <c r="G152" s="1">
+        <v>2</v>
+      </c>
+      <c r="H152" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I152" s="22" t="str">
+        <f t="shared" si="30"/>
+        <v>Evan</v>
+      </c>
+      <c r="J152" s="22">
+        <f t="shared" si="29"/>
+        <v>2</v>
+      </c>
+      <c r="K152" s="22">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="L152" s="22">
+        <f t="shared" si="29"/>
+        <v>2</v>
+      </c>
+      <c r="M152" s="22">
+        <f t="shared" si="29"/>
+        <v>3</v>
+      </c>
+      <c r="N152" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="O152" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P152" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q152" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R152" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S152" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T152" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U152" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="V152" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="W152" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X152" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y152" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Z152" s="22" t="e">
+        <f t="shared" si="24"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="153" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A153">
+        <v>754</v>
+      </c>
+      <c r="B153" t="s">
+        <v>316</v>
+      </c>
+      <c r="G153" s="1">
+        <v>3</v>
+      </c>
+      <c r="H153" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I153" s="22" t="str">
+        <f t="shared" ref="I153" si="31">INDEX(AnsLkUp,MATCH(A153 &amp; "_1",LookupOrder,1),2)</f>
+        <v>Evan</v>
+      </c>
+      <c r="J153" s="22">
+        <f t="shared" si="29"/>
+        <v>3</v>
+      </c>
+      <c r="K153" s="22">
+        <f t="shared" si="29"/>
+        <v>3</v>
+      </c>
+      <c r="L153" s="22">
+        <f t="shared" si="29"/>
+        <v>3</v>
+      </c>
+      <c r="M153" s="22">
+        <f t="shared" si="29"/>
+        <v>3</v>
+      </c>
+      <c r="N153" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="O153" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P153" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q153" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R153" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S153" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T153" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U153" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="V153" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="W153" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X153" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y153" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Z153" s="22" t="e">
+        <f t="shared" si="24"/>
+        <v>#N/A</v>
       </c>
     </row>
   </sheetData>
@@ -26597,11 +26959,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F381"/>
+  <dimension ref="A1:F399"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A363" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D382" sqref="D382"/>
+      <pane ySplit="1" topLeftCell="A381" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F397" sqref="F397:F399"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -33972,11 +34334,11 @@
         <v>1</v>
       </c>
       <c r="E335" s="23" t="str">
-        <f t="shared" ref="E335:E381" si="20">A335 &amp; "_" &amp; D335</f>
+        <f t="shared" ref="E335:E399" si="20">A335 &amp; "_" &amp; D335</f>
         <v>739_1</v>
       </c>
       <c r="F335" s="23" t="str">
-        <f t="shared" ref="F335:F381" si="21">A335 &amp; "_" &amp; B335</f>
+        <f t="shared" ref="F335:F398" si="21">A335 &amp; "_" &amp; B335</f>
         <v>739_Richard</v>
       </c>
     </row>
@@ -34990,6 +35352,402 @@
       <c r="F381" s="23" t="str">
         <f t="shared" si="21"/>
         <v>750_Jay</v>
+      </c>
+    </row>
+    <row r="382" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A382">
+        <v>751</v>
+      </c>
+      <c r="B382" t="s">
+        <v>6</v>
+      </c>
+      <c r="C382" s="1">
+        <v>4</v>
+      </c>
+      <c r="D382" s="1">
+        <v>1</v>
+      </c>
+      <c r="E382" s="23" t="str">
+        <f t="shared" si="20"/>
+        <v>751_1</v>
+      </c>
+      <c r="F382" s="23" t="str">
+        <f t="shared" si="21"/>
+        <v>751_Jay</v>
+      </c>
+    </row>
+    <row r="383" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A383">
+        <v>751</v>
+      </c>
+      <c r="B383" t="s">
+        <v>7</v>
+      </c>
+      <c r="C383" s="1">
+        <v>4</v>
+      </c>
+      <c r="D383" s="1">
+        <v>2</v>
+      </c>
+      <c r="E383" s="23" t="str">
+        <f t="shared" si="20"/>
+        <v>751_2</v>
+      </c>
+      <c r="F383" s="23" t="str">
+        <f t="shared" si="21"/>
+        <v>751_Evan</v>
+      </c>
+    </row>
+    <row r="384" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A384">
+        <v>751</v>
+      </c>
+      <c r="B384" t="s">
+        <v>12</v>
+      </c>
+      <c r="C384" s="1">
+        <v>3</v>
+      </c>
+      <c r="D384" s="1">
+        <v>3</v>
+      </c>
+      <c r="E384" s="23" t="str">
+        <f t="shared" si="20"/>
+        <v>751_3</v>
+      </c>
+      <c r="F384" s="23" t="str">
+        <f t="shared" si="21"/>
+        <v>751_Steve</v>
+      </c>
+    </row>
+    <row r="385" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A385">
+        <v>751</v>
+      </c>
+      <c r="B385" t="s">
+        <v>5</v>
+      </c>
+      <c r="C385" s="1">
+        <v>3</v>
+      </c>
+      <c r="D385" s="1">
+        <v>4</v>
+      </c>
+      <c r="E385" s="23" t="str">
+        <f t="shared" si="20"/>
+        <v>751_4</v>
+      </c>
+      <c r="F385" s="23" t="str">
+        <f t="shared" si="21"/>
+        <v>751_Bob</v>
+      </c>
+    </row>
+    <row r="386" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A386">
+        <v>752</v>
+      </c>
+      <c r="B386" t="s">
+        <v>8</v>
+      </c>
+      <c r="C386" s="1">
+        <v>2</v>
+      </c>
+      <c r="D386" s="1">
+        <v>1</v>
+      </c>
+      <c r="E386" s="23" t="str">
+        <f t="shared" si="20"/>
+        <v>752_1</v>
+      </c>
+      <c r="F386" s="23" t="str">
+        <f t="shared" si="21"/>
+        <v>752_George</v>
+      </c>
+    </row>
+    <row r="387" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A387">
+        <v>752</v>
+      </c>
+      <c r="B387" t="s">
+        <v>5</v>
+      </c>
+      <c r="C387" s="1">
+        <v>2</v>
+      </c>
+      <c r="D387" s="1">
+        <v>2</v>
+      </c>
+      <c r="E387" s="23" t="str">
+        <f t="shared" si="20"/>
+        <v>752_2</v>
+      </c>
+      <c r="F387" s="23" t="str">
+        <f t="shared" si="21"/>
+        <v>752_Bob</v>
+      </c>
+    </row>
+    <row r="388" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A388">
+        <v>752</v>
+      </c>
+      <c r="B388" t="s">
+        <v>12</v>
+      </c>
+      <c r="C388" s="1">
+        <v>3</v>
+      </c>
+      <c r="D388" s="1">
+        <v>3</v>
+      </c>
+      <c r="E388" s="23" t="str">
+        <f t="shared" si="20"/>
+        <v>752_3</v>
+      </c>
+      <c r="F388" s="23" t="str">
+        <f t="shared" si="21"/>
+        <v>752_Steve</v>
+      </c>
+    </row>
+    <row r="389" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A389">
+        <v>752</v>
+      </c>
+      <c r="B389" t="s">
+        <v>23</v>
+      </c>
+      <c r="C389" s="1">
+        <v>1</v>
+      </c>
+      <c r="D389" s="1">
+        <v>4</v>
+      </c>
+      <c r="E389" s="23" t="str">
+        <f t="shared" si="20"/>
+        <v>752_4</v>
+      </c>
+      <c r="F389" s="23" t="str">
+        <f t="shared" si="21"/>
+        <v>752_Cara</v>
+      </c>
+    </row>
+    <row r="390" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A390">
+        <v>752</v>
+      </c>
+      <c r="B390" t="s">
+        <v>6</v>
+      </c>
+      <c r="C390" s="1">
+        <v>2</v>
+      </c>
+      <c r="D390" s="1">
+        <v>5</v>
+      </c>
+      <c r="E390" s="23" t="str">
+        <f t="shared" si="20"/>
+        <v>752_5</v>
+      </c>
+      <c r="F390" s="23" t="str">
+        <f t="shared" si="21"/>
+        <v>752_Jay</v>
+      </c>
+    </row>
+    <row r="391" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A391">
+        <v>752</v>
+      </c>
+      <c r="B391" t="s">
+        <v>7</v>
+      </c>
+      <c r="C391" s="1">
+        <v>3</v>
+      </c>
+      <c r="D391" s="1">
+        <v>6</v>
+      </c>
+      <c r="E391" s="23" t="str">
+        <f t="shared" si="20"/>
+        <v>752_6</v>
+      </c>
+      <c r="F391" s="23" t="str">
+        <f t="shared" si="21"/>
+        <v>752_Evan</v>
+      </c>
+    </row>
+    <row r="392" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A392">
+        <v>753</v>
+      </c>
+      <c r="B392" t="s">
+        <v>7</v>
+      </c>
+      <c r="C392" s="1">
+        <v>3</v>
+      </c>
+      <c r="D392" s="1">
+        <v>1</v>
+      </c>
+      <c r="E392" s="23" t="str">
+        <f t="shared" si="20"/>
+        <v>753_1</v>
+      </c>
+      <c r="F392" s="23" t="str">
+        <f t="shared" si="21"/>
+        <v>753_Evan</v>
+      </c>
+    </row>
+    <row r="393" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A393">
+        <v>753</v>
+      </c>
+      <c r="B393" t="s">
+        <v>23</v>
+      </c>
+      <c r="C393" s="1">
+        <v>1</v>
+      </c>
+      <c r="D393" s="1">
+        <v>2</v>
+      </c>
+      <c r="E393" s="23" t="str">
+        <f t="shared" si="20"/>
+        <v>753_2</v>
+      </c>
+      <c r="F393" s="23" t="str">
+        <f t="shared" si="21"/>
+        <v>753_Cara</v>
+      </c>
+    </row>
+    <row r="394" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A394">
+        <v>753</v>
+      </c>
+      <c r="B394" t="s">
+        <v>6</v>
+      </c>
+      <c r="C394" s="1">
+        <v>2</v>
+      </c>
+      <c r="D394" s="1">
+        <v>3</v>
+      </c>
+      <c r="E394" s="23" t="str">
+        <f t="shared" si="20"/>
+        <v>753_3</v>
+      </c>
+      <c r="F394" s="23" t="str">
+        <f t="shared" si="21"/>
+        <v>753_Jay</v>
+      </c>
+    </row>
+    <row r="395" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A395">
+        <v>753</v>
+      </c>
+      <c r="B395" t="s">
+        <v>5</v>
+      </c>
+      <c r="C395" s="1">
+        <v>2</v>
+      </c>
+      <c r="D395" s="1">
+        <v>4</v>
+      </c>
+      <c r="E395" s="23" t="str">
+        <f t="shared" si="20"/>
+        <v>753_4</v>
+      </c>
+      <c r="F395" s="23" t="str">
+        <f t="shared" si="21"/>
+        <v>753_Bob</v>
+      </c>
+    </row>
+    <row r="396" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A396">
+        <v>754</v>
+      </c>
+      <c r="B396" t="s">
+        <v>7</v>
+      </c>
+      <c r="C396" s="1">
+        <v>3</v>
+      </c>
+      <c r="D396" s="1">
+        <v>1</v>
+      </c>
+      <c r="E396" s="23" t="str">
+        <f t="shared" si="20"/>
+        <v>754_1</v>
+      </c>
+      <c r="F396" s="23" t="str">
+        <f t="shared" si="21"/>
+        <v>754_Evan</v>
+      </c>
+    </row>
+    <row r="397" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A397">
+        <v>754</v>
+      </c>
+      <c r="B397" t="s">
+        <v>5</v>
+      </c>
+      <c r="C397" s="1">
+        <v>3</v>
+      </c>
+      <c r="D397" s="1">
+        <v>2</v>
+      </c>
+      <c r="E397" s="23" t="str">
+        <f t="shared" si="20"/>
+        <v>754_2</v>
+      </c>
+      <c r="F397" s="23" t="str">
+        <f t="shared" si="21"/>
+        <v>754_Bob</v>
+      </c>
+    </row>
+    <row r="398" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A398">
+        <v>754</v>
+      </c>
+      <c r="B398" t="s">
+        <v>6</v>
+      </c>
+      <c r="C398" s="1">
+        <v>3</v>
+      </c>
+      <c r="D398" s="1">
+        <v>3</v>
+      </c>
+      <c r="E398" s="23" t="str">
+        <f t="shared" si="20"/>
+        <v>754_3</v>
+      </c>
+      <c r="F398" s="23" t="str">
+        <f t="shared" si="21"/>
+        <v>754_Jay</v>
+      </c>
+    </row>
+    <row r="399" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A399">
+        <v>754</v>
+      </c>
+      <c r="B399" t="s">
+        <v>23</v>
+      </c>
+      <c r="C399" s="1">
+        <v>3</v>
+      </c>
+      <c r="D399" s="1">
+        <v>4</v>
+      </c>
+      <c r="E399" s="23" t="str">
+        <f t="shared" si="20"/>
+        <v>754_4</v>
+      </c>
+      <c r="F399" s="23" t="str">
+        <f t="shared" ref="F399" si="22">A399 &amp; "_" &amp; B399</f>
+        <v>754_Cara</v>
       </c>
     </row>
   </sheetData>
@@ -35001,13 +35759,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:BH150"/>
+  <dimension ref="A1:BH154"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B133" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B136" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A148" sqref="A148:XFD150"/>
+      <selection pane="bottomRight" activeCell="A154" sqref="A154:XFD154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -71091,6 +71849,974 @@
       </c>
       <c r="BH150" s="9">
         <f t="shared" si="783"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="151" spans="1:60" x14ac:dyDescent="0.35">
+      <c r="A151" s="24">
+        <f>Data!A150</f>
+        <v>751</v>
+      </c>
+      <c r="B151" s="26" t="str">
+        <f>Data!B150</f>
+        <v>Australia</v>
+      </c>
+      <c r="C151" s="27" t="str">
+        <f>Data!H150</f>
+        <v>RichardS</v>
+      </c>
+      <c r="D151" s="25" t="str">
+        <f>Data!I150</f>
+        <v>Jay</v>
+      </c>
+      <c r="E151" s="22">
+        <f>IF(Data!J150=Data!$G150,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F151" s="22" t="e">
+        <f>IF(Data!K150=Data!$G150,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G151" s="22">
+        <f>IF(Data!L150=Data!$G150,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H151" s="22">
+        <f>IF(Data!M150=Data!$G150,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I151" s="22" t="e">
+        <f>IF(Data!N150=Data!$G150,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J151" s="22">
+        <f>IF(Data!O150=Data!$G150,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="K151" s="22" t="e">
+        <f>IF(Data!P150=Data!$G150,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="L151" s="22" t="e">
+        <f>IF(Data!Q150=Data!$G150,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M151" s="22" t="e">
+        <f>IF(Data!R150=Data!$G150,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N151" s="22" t="e">
+        <f>IF(Data!S150=Data!$G150,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O151" s="22" t="e">
+        <f>IF(Data!T150=Data!$G150,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P151" s="22" t="e">
+        <f>IF(Data!U150=Data!$G150,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q151" s="22" t="e">
+        <f>IF(Data!V150=Data!$G150,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R151" s="22" t="e">
+        <f>IF(Data!W150=Data!$G150,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="S151" s="22" t="e">
+        <f>IF(Data!X150=Data!$G150,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="T151" s="22" t="e">
+        <f>IF(Data!Y150=Data!$G150,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="U151" s="22" t="e">
+        <f>IF(Data!Z150=Data!$G150,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="V151" s="22">
+        <f t="shared" ref="V151:V153" si="784">COUNTIF(E151:U151,"&lt;&gt;#N/A")</f>
+        <v>4</v>
+      </c>
+      <c r="W151" s="22">
+        <f t="shared" ref="W151:W153" si="785">SUMIF(E151:U151,"&lt;&gt;#N/A")</f>
+        <v>0</v>
+      </c>
+      <c r="X151" s="22">
+        <f t="shared" ref="X151:X153" si="786">IF(W151=0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Y151" s="22">
+        <f t="shared" ref="Y151:Y153" si="787">IF(V151=W151,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z151" s="22" t="e">
+        <f t="shared" ref="Z151:Z153" si="788">IF(W151=1,INDEX($E$2:$U$2,1,MATCH(1,E151:U151,0)),NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AA151" s="7">
+        <f t="shared" ref="AA151:AA153" si="789">IF(ISNA(E151),AA150,IF(E151=1,AA150+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AB151" s="7">
+        <f t="shared" ref="AB151:AB153" si="790">IF(ISNA(F151),AB150,IF(F151=1,AB150+1,0))</f>
+        <v>3</v>
+      </c>
+      <c r="AC151" s="7">
+        <f t="shared" ref="AC151:AC153" si="791">IF(ISNA(G151),AC150,IF(G151=1,AC150+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AD151" s="7">
+        <f t="shared" ref="AD151:AD153" si="792">IF(ISNA(H151),AD150,IF(H151=1,AD150+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AE151" s="7">
+        <f t="shared" ref="AE151:AE153" si="793">IF(ISNA(I151),AE150,IF(I151=1,AE150+1,0))</f>
+        <v>3</v>
+      </c>
+      <c r="AF151" s="7">
+        <f t="shared" ref="AF151:AF153" si="794">IF(ISNA(J151),AF150,IF(J151=1,AF150+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AG151" s="7">
+        <f t="shared" ref="AG151:AG153" si="795">IF(ISNA(K151),AG150,IF(K151=1,AG150+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AH151" s="7">
+        <f t="shared" ref="AH151:AH153" si="796">IF(ISNA(L151),AH150,IF(L151=1,AH150+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AI151" s="7">
+        <f t="shared" ref="AI151:AI153" si="797">IF(ISNA(M151),AI150,IF(M151=1,AI150+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AJ151" s="7">
+        <f t="shared" ref="AJ151:AJ153" si="798">IF(ISNA(N151),AJ150,IF(N151=1,AJ150+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AK151" s="7">
+        <f t="shared" ref="AK151:AK153" si="799">IF(ISNA(O151),AK150,IF(O151=1,AK150+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AL151" s="7">
+        <f t="shared" ref="AL151:AL153" si="800">IF(ISNA(P151),AL150,IF(P151=1,AL150+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AM151" s="7">
+        <f t="shared" ref="AM151:AM153" si="801">IF(ISNA(Q151),AM150,IF(Q151=1,AM150+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AN151" s="7">
+        <f t="shared" ref="AN151:AN153" si="802">IF(ISNA(R151),AN150,IF(R151=1,AN150+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AO151" s="7">
+        <f t="shared" ref="AO151:AO153" si="803">IF(ISNA(S151),AO150,IF(S151=1,AO150+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AP151" s="7">
+        <f t="shared" ref="AP151:AP153" si="804">IF(ISNA(T151),AP150,IF(T151=1,AP150+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AQ151" s="7">
+        <f t="shared" ref="AQ151:AQ153" si="805">IF(ISNA(U151),AQ150,IF(U151=1,AQ150+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AR151" s="9">
+        <f t="shared" ref="AR151:AR153" si="806">IF(ISNA(E151),AR150,IF(E151=0,AR150+1,0))</f>
+        <v>3</v>
+      </c>
+      <c r="AS151" s="9">
+        <f t="shared" ref="AS151:AS153" si="807">IF(ISNA(F151),AS150,IF(F151=0,AS150+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AT151" s="9">
+        <f t="shared" ref="AT151:AT153" si="808">IF(ISNA(G151),AT150,IF(G151=0,AT150+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AU151" s="9">
+        <f t="shared" ref="AU151:AU153" si="809">IF(ISNA(H151),AU150,IF(H151=0,AU150+1,0))</f>
+        <v>3</v>
+      </c>
+      <c r="AV151" s="9">
+        <f t="shared" ref="AV151:AV153" si="810">IF(ISNA(I151),AV150,IF(I151=0,AV150+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AW151" s="9">
+        <f t="shared" ref="AW151:AW153" si="811">IF(ISNA(J151),AW150,IF(J151=0,AW150+1,0))</f>
+        <v>6</v>
+      </c>
+      <c r="AX151" s="9">
+        <f t="shared" ref="AX151:AX153" si="812">IF(ISNA(K151),AX150,IF(K151=0,AX150+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AY151" s="9">
+        <f t="shared" ref="AY151:AY153" si="813">IF(ISNA(L151),AY150,IF(L151=0,AY150+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AZ151" s="9">
+        <f t="shared" ref="AZ151:AZ153" si="814">IF(ISNA(M151),AZ150,IF(M151=0,AZ150+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="BA151" s="9">
+        <f t="shared" ref="BA151:BA153" si="815">IF(ISNA(N151),BA150,IF(N151=0,BA150+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="BB151" s="9">
+        <f t="shared" ref="BB151:BB153" si="816">IF(ISNA(O151),BB150,IF(O151=0,BB150+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="BC151" s="9">
+        <f t="shared" ref="BC151:BC153" si="817">IF(ISNA(P151),BC150,IF(P151=0,BC150+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="BD151" s="9">
+        <f t="shared" ref="BD151:BD153" si="818">IF(ISNA(Q151),BD150,IF(Q151=0,BD150+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="BE151" s="9">
+        <f t="shared" ref="BE151:BE153" si="819">IF(ISNA(R151),BE150,IF(R151=0,BE150+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="BF151" s="9">
+        <f t="shared" ref="BF151:BF153" si="820">IF(ISNA(S151),BF150,IF(S151=0,BF150+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="BG151" s="9">
+        <f t="shared" ref="BG151:BG153" si="821">IF(ISNA(T151),BG150,IF(T151=0,BG150+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="BH151" s="9">
+        <f t="shared" ref="BH151:BH153" si="822">IF(ISNA(U151),BH150,IF(U151=0,BH150+1,0))</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="152" spans="1:60" x14ac:dyDescent="0.35">
+      <c r="A152" s="24">
+        <f>Data!A151</f>
+        <v>752</v>
+      </c>
+      <c r="B152" s="26" t="str">
+        <f>Data!B151</f>
+        <v>Scotland</v>
+      </c>
+      <c r="C152" s="27" t="str">
+        <f>Data!H151</f>
+        <v>Scott</v>
+      </c>
+      <c r="D152" s="25" t="str">
+        <f>Data!I151</f>
+        <v>George</v>
+      </c>
+      <c r="E152" s="22">
+        <f>IF(Data!J151=Data!$G151,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F152" s="22">
+        <f>IF(Data!K151=Data!$G151,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G152" s="22">
+        <f>IF(Data!L151=Data!$G151,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H152" s="22">
+        <f>IF(Data!M151=Data!$G151,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="I152" s="22">
+        <f>IF(Data!N151=Data!$G151,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J152" s="22">
+        <f>IF(Data!O151=Data!$G151,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="K152" s="22" t="e">
+        <f>IF(Data!P151=Data!$G151,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="L152" s="22" t="e">
+        <f>IF(Data!Q151=Data!$G151,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M152" s="22" t="e">
+        <f>IF(Data!R151=Data!$G151,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N152" s="22" t="e">
+        <f>IF(Data!S151=Data!$G151,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O152" s="22" t="e">
+        <f>IF(Data!T151=Data!$G151,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P152" s="22" t="e">
+        <f>IF(Data!U151=Data!$G151,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q152" s="22" t="e">
+        <f>IF(Data!V151=Data!$G151,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R152" s="22" t="e">
+        <f>IF(Data!W151=Data!$G151,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="S152" s="22" t="e">
+        <f>IF(Data!X151=Data!$G151,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="T152" s="22" t="e">
+        <f>IF(Data!Y151=Data!$G151,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="U152" s="22" t="e">
+        <f>IF(Data!Z151=Data!$G151,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="V152" s="22">
+        <f t="shared" si="784"/>
+        <v>6</v>
+      </c>
+      <c r="W152" s="22">
+        <f t="shared" si="785"/>
+        <v>2</v>
+      </c>
+      <c r="X152" s="22">
+        <f t="shared" si="786"/>
+        <v>0</v>
+      </c>
+      <c r="Y152" s="22">
+        <f t="shared" si="787"/>
+        <v>0</v>
+      </c>
+      <c r="Z152" s="22" t="e">
+        <f t="shared" si="788"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA152" s="7">
+        <f t="shared" si="789"/>
+        <v>0</v>
+      </c>
+      <c r="AB152" s="7">
+        <f t="shared" si="790"/>
+        <v>0</v>
+      </c>
+      <c r="AC152" s="7">
+        <f t="shared" si="791"/>
+        <v>0</v>
+      </c>
+      <c r="AD152" s="7">
+        <f t="shared" si="792"/>
+        <v>1</v>
+      </c>
+      <c r="AE152" s="7">
+        <f t="shared" si="793"/>
+        <v>0</v>
+      </c>
+      <c r="AF152" s="7">
+        <f t="shared" si="794"/>
+        <v>1</v>
+      </c>
+      <c r="AG152" s="7">
+        <f t="shared" si="795"/>
+        <v>0</v>
+      </c>
+      <c r="AH152" s="7">
+        <f t="shared" si="796"/>
+        <v>1</v>
+      </c>
+      <c r="AI152" s="7">
+        <f t="shared" si="797"/>
+        <v>0</v>
+      </c>
+      <c r="AJ152" s="7">
+        <f t="shared" si="798"/>
+        <v>1</v>
+      </c>
+      <c r="AK152" s="7">
+        <f t="shared" si="799"/>
+        <v>0</v>
+      </c>
+      <c r="AL152" s="7">
+        <f t="shared" si="800"/>
+        <v>0</v>
+      </c>
+      <c r="AM152" s="7">
+        <f t="shared" si="801"/>
+        <v>0</v>
+      </c>
+      <c r="AN152" s="7">
+        <f t="shared" si="802"/>
+        <v>1</v>
+      </c>
+      <c r="AO152" s="7">
+        <f t="shared" si="803"/>
+        <v>0</v>
+      </c>
+      <c r="AP152" s="7">
+        <f t="shared" si="804"/>
+        <v>0</v>
+      </c>
+      <c r="AQ152" s="7">
+        <f t="shared" si="805"/>
+        <v>0</v>
+      </c>
+      <c r="AR152" s="9">
+        <f t="shared" si="806"/>
+        <v>4</v>
+      </c>
+      <c r="AS152" s="9">
+        <f t="shared" si="807"/>
+        <v>1</v>
+      </c>
+      <c r="AT152" s="9">
+        <f t="shared" si="808"/>
+        <v>2</v>
+      </c>
+      <c r="AU152" s="9">
+        <f t="shared" si="809"/>
+        <v>0</v>
+      </c>
+      <c r="AV152" s="9">
+        <f t="shared" si="810"/>
+        <v>1</v>
+      </c>
+      <c r="AW152" s="9">
+        <f t="shared" si="811"/>
+        <v>0</v>
+      </c>
+      <c r="AX152" s="9">
+        <f t="shared" si="812"/>
+        <v>0</v>
+      </c>
+      <c r="AY152" s="9">
+        <f t="shared" si="813"/>
+        <v>0</v>
+      </c>
+      <c r="AZ152" s="9">
+        <f t="shared" si="814"/>
+        <v>0</v>
+      </c>
+      <c r="BA152" s="9">
+        <f t="shared" si="815"/>
+        <v>0</v>
+      </c>
+      <c r="BB152" s="9">
+        <f t="shared" si="816"/>
+        <v>0</v>
+      </c>
+      <c r="BC152" s="9">
+        <f t="shared" si="817"/>
+        <v>0</v>
+      </c>
+      <c r="BD152" s="9">
+        <f t="shared" si="818"/>
+        <v>1</v>
+      </c>
+      <c r="BE152" s="9">
+        <f t="shared" si="819"/>
+        <v>0</v>
+      </c>
+      <c r="BF152" s="9">
+        <f t="shared" si="820"/>
+        <v>1</v>
+      </c>
+      <c r="BG152" s="9">
+        <f t="shared" si="821"/>
+        <v>1</v>
+      </c>
+      <c r="BH152" s="9">
+        <f t="shared" si="822"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="153" spans="1:60" x14ac:dyDescent="0.35">
+      <c r="A153" s="24">
+        <f>Data!A152</f>
+        <v>753</v>
+      </c>
+      <c r="B153" s="26" t="str">
+        <f>Data!B152</f>
+        <v>Hybrids</v>
+      </c>
+      <c r="C153" s="27" t="str">
+        <f>Data!H152</f>
+        <v>Steve</v>
+      </c>
+      <c r="D153" s="25" t="str">
+        <f>Data!I152</f>
+        <v>Evan</v>
+      </c>
+      <c r="E153" s="22">
+        <f>IF(Data!J152=Data!$G152,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F153" s="22">
+        <f>IF(Data!K152=Data!$G152,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G153" s="22">
+        <f>IF(Data!L152=Data!$G152,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H153" s="22">
+        <f>IF(Data!M152=Data!$G152,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I153" s="22" t="e">
+        <f>IF(Data!N152=Data!$G152,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J153" s="22" t="e">
+        <f>IF(Data!O152=Data!$G152,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K153" s="22" t="e">
+        <f>IF(Data!P152=Data!$G152,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="L153" s="22" t="e">
+        <f>IF(Data!Q152=Data!$G152,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M153" s="22" t="e">
+        <f>IF(Data!R152=Data!$G152,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N153" s="22" t="e">
+        <f>IF(Data!S152=Data!$G152,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O153" s="22" t="e">
+        <f>IF(Data!T152=Data!$G152,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P153" s="22" t="e">
+        <f>IF(Data!U152=Data!$G152,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q153" s="22" t="e">
+        <f>IF(Data!V152=Data!$G152,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R153" s="22" t="e">
+        <f>IF(Data!W152=Data!$G152,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="S153" s="22" t="e">
+        <f>IF(Data!X152=Data!$G152,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="T153" s="22" t="e">
+        <f>IF(Data!Y152=Data!$G152,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="U153" s="22" t="e">
+        <f>IF(Data!Z152=Data!$G152,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="V153" s="22">
+        <f t="shared" si="784"/>
+        <v>4</v>
+      </c>
+      <c r="W153" s="22">
+        <f t="shared" si="785"/>
+        <v>2</v>
+      </c>
+      <c r="X153" s="22">
+        <f t="shared" si="786"/>
+        <v>0</v>
+      </c>
+      <c r="Y153" s="22">
+        <f t="shared" si="787"/>
+        <v>0</v>
+      </c>
+      <c r="Z153" s="22" t="e">
+        <f t="shared" si="788"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA153" s="7">
+        <f t="shared" si="789"/>
+        <v>1</v>
+      </c>
+      <c r="AB153" s="7">
+        <f t="shared" si="790"/>
+        <v>0</v>
+      </c>
+      <c r="AC153" s="7">
+        <f t="shared" si="791"/>
+        <v>1</v>
+      </c>
+      <c r="AD153" s="7">
+        <f t="shared" si="792"/>
+        <v>0</v>
+      </c>
+      <c r="AE153" s="7">
+        <f t="shared" si="793"/>
+        <v>0</v>
+      </c>
+      <c r="AF153" s="7">
+        <f t="shared" si="794"/>
+        <v>1</v>
+      </c>
+      <c r="AG153" s="7">
+        <f t="shared" si="795"/>
+        <v>0</v>
+      </c>
+      <c r="AH153" s="7">
+        <f t="shared" si="796"/>
+        <v>1</v>
+      </c>
+      <c r="AI153" s="7">
+        <f t="shared" si="797"/>
+        <v>0</v>
+      </c>
+      <c r="AJ153" s="7">
+        <f t="shared" si="798"/>
+        <v>1</v>
+      </c>
+      <c r="AK153" s="7">
+        <f t="shared" si="799"/>
+        <v>0</v>
+      </c>
+      <c r="AL153" s="7">
+        <f t="shared" si="800"/>
+        <v>0</v>
+      </c>
+      <c r="AM153" s="7">
+        <f t="shared" si="801"/>
+        <v>0</v>
+      </c>
+      <c r="AN153" s="7">
+        <f t="shared" si="802"/>
+        <v>1</v>
+      </c>
+      <c r="AO153" s="7">
+        <f t="shared" si="803"/>
+        <v>0</v>
+      </c>
+      <c r="AP153" s="7">
+        <f t="shared" si="804"/>
+        <v>0</v>
+      </c>
+      <c r="AQ153" s="7">
+        <f t="shared" si="805"/>
+        <v>0</v>
+      </c>
+      <c r="AR153" s="9">
+        <f t="shared" si="806"/>
+        <v>0</v>
+      </c>
+      <c r="AS153" s="9">
+        <f t="shared" si="807"/>
+        <v>2</v>
+      </c>
+      <c r="AT153" s="9">
+        <f t="shared" si="808"/>
+        <v>0</v>
+      </c>
+      <c r="AU153" s="9">
+        <f t="shared" si="809"/>
+        <v>1</v>
+      </c>
+      <c r="AV153" s="9">
+        <f t="shared" si="810"/>
+        <v>1</v>
+      </c>
+      <c r="AW153" s="9">
+        <f t="shared" si="811"/>
+        <v>0</v>
+      </c>
+      <c r="AX153" s="9">
+        <f t="shared" si="812"/>
+        <v>0</v>
+      </c>
+      <c r="AY153" s="9">
+        <f t="shared" si="813"/>
+        <v>0</v>
+      </c>
+      <c r="AZ153" s="9">
+        <f t="shared" si="814"/>
+        <v>0</v>
+      </c>
+      <c r="BA153" s="9">
+        <f t="shared" si="815"/>
+        <v>0</v>
+      </c>
+      <c r="BB153" s="9">
+        <f t="shared" si="816"/>
+        <v>0</v>
+      </c>
+      <c r="BC153" s="9">
+        <f t="shared" si="817"/>
+        <v>0</v>
+      </c>
+      <c r="BD153" s="9">
+        <f t="shared" si="818"/>
+        <v>1</v>
+      </c>
+      <c r="BE153" s="9">
+        <f t="shared" si="819"/>
+        <v>0</v>
+      </c>
+      <c r="BF153" s="9">
+        <f t="shared" si="820"/>
+        <v>1</v>
+      </c>
+      <c r="BG153" s="9">
+        <f t="shared" si="821"/>
+        <v>1</v>
+      </c>
+      <c r="BH153" s="9">
+        <f t="shared" si="822"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="154" spans="1:60" x14ac:dyDescent="0.35">
+      <c r="A154" s="24">
+        <f>Data!A153</f>
+        <v>754</v>
+      </c>
+      <c r="B154" s="26" t="str">
+        <f>Data!B153</f>
+        <v>Coffee</v>
+      </c>
+      <c r="C154" s="27" t="str">
+        <f>Data!H153</f>
+        <v>Steve</v>
+      </c>
+      <c r="D154" s="25" t="str">
+        <f>Data!I153</f>
+        <v>Evan</v>
+      </c>
+      <c r="E154" s="22">
+        <f>IF(Data!J153=Data!$G153,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F154" s="22">
+        <f>IF(Data!K153=Data!$G153,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G154" s="22">
+        <f>IF(Data!L153=Data!$G153,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H154" s="22">
+        <f>IF(Data!M153=Data!$G153,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="I154" s="22" t="e">
+        <f>IF(Data!N153=Data!$G153,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J154" s="22" t="e">
+        <f>IF(Data!O153=Data!$G153,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K154" s="22" t="e">
+        <f>IF(Data!P153=Data!$G153,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="L154" s="22" t="e">
+        <f>IF(Data!Q153=Data!$G153,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M154" s="22" t="e">
+        <f>IF(Data!R153=Data!$G153,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N154" s="22" t="e">
+        <f>IF(Data!S153=Data!$G153,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O154" s="22" t="e">
+        <f>IF(Data!T153=Data!$G153,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P154" s="22" t="e">
+        <f>IF(Data!U153=Data!$G153,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q154" s="22" t="e">
+        <f>IF(Data!V153=Data!$G153,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R154" s="22" t="e">
+        <f>IF(Data!W153=Data!$G153,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="S154" s="22" t="e">
+        <f>IF(Data!X153=Data!$G153,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="T154" s="22" t="e">
+        <f>IF(Data!Y153=Data!$G153,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="U154" s="22" t="e">
+        <f>IF(Data!Z153=Data!$G153,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="V154" s="22">
+        <f t="shared" ref="V154" si="823">COUNTIF(E154:U154,"&lt;&gt;#N/A")</f>
+        <v>4</v>
+      </c>
+      <c r="W154" s="22">
+        <f t="shared" ref="W154" si="824">SUMIF(E154:U154,"&lt;&gt;#N/A")</f>
+        <v>4</v>
+      </c>
+      <c r="X154" s="22">
+        <f t="shared" ref="X154" si="825">IF(W154=0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y154" s="22">
+        <f t="shared" ref="Y154" si="826">IF(V154=W154,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Z154" s="22" t="e">
+        <f t="shared" ref="Z154" si="827">IF(W154=1,INDEX($E$2:$U$2,1,MATCH(1,E154:U154,0)),NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AA154" s="7">
+        <f t="shared" ref="AA154" si="828">IF(ISNA(E154),AA153,IF(E154=1,AA153+1,0))</f>
+        <v>2</v>
+      </c>
+      <c r="AB154" s="7">
+        <f t="shared" ref="AB154" si="829">IF(ISNA(F154),AB153,IF(F154=1,AB153+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AC154" s="7">
+        <f t="shared" ref="AC154" si="830">IF(ISNA(G154),AC153,IF(G154=1,AC153+1,0))</f>
+        <v>2</v>
+      </c>
+      <c r="AD154" s="7">
+        <f t="shared" ref="AD154" si="831">IF(ISNA(H154),AD153,IF(H154=1,AD153+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AE154" s="7">
+        <f t="shared" ref="AE154" si="832">IF(ISNA(I154),AE153,IF(I154=1,AE153+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AF154" s="7">
+        <f t="shared" ref="AF154" si="833">IF(ISNA(J154),AF153,IF(J154=1,AF153+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AG154" s="7">
+        <f t="shared" ref="AG154" si="834">IF(ISNA(K154),AG153,IF(K154=1,AG153+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AH154" s="7">
+        <f t="shared" ref="AH154" si="835">IF(ISNA(L154),AH153,IF(L154=1,AH153+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AI154" s="7">
+        <f t="shared" ref="AI154" si="836">IF(ISNA(M154),AI153,IF(M154=1,AI153+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AJ154" s="7">
+        <f t="shared" ref="AJ154" si="837">IF(ISNA(N154),AJ153,IF(N154=1,AJ153+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AK154" s="7">
+        <f t="shared" ref="AK154" si="838">IF(ISNA(O154),AK153,IF(O154=1,AK153+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AL154" s="7">
+        <f t="shared" ref="AL154" si="839">IF(ISNA(P154),AL153,IF(P154=1,AL153+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AM154" s="7">
+        <f t="shared" ref="AM154" si="840">IF(ISNA(Q154),AM153,IF(Q154=1,AM153+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AN154" s="7">
+        <f t="shared" ref="AN154" si="841">IF(ISNA(R154),AN153,IF(R154=1,AN153+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AO154" s="7">
+        <f t="shared" ref="AO154" si="842">IF(ISNA(S154),AO153,IF(S154=1,AO153+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AP154" s="7">
+        <f t="shared" ref="AP154" si="843">IF(ISNA(T154),AP153,IF(T154=1,AP153+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AQ154" s="7">
+        <f t="shared" ref="AQ154" si="844">IF(ISNA(U154),AQ153,IF(U154=1,AQ153+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AR154" s="9">
+        <f t="shared" ref="AR154" si="845">IF(ISNA(E154),AR153,IF(E154=0,AR153+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AS154" s="9">
+        <f t="shared" ref="AS154" si="846">IF(ISNA(F154),AS153,IF(F154=0,AS153+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AT154" s="9">
+        <f t="shared" ref="AT154" si="847">IF(ISNA(G154),AT153,IF(G154=0,AT153+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AU154" s="9">
+        <f t="shared" ref="AU154" si="848">IF(ISNA(H154),AU153,IF(H154=0,AU153+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AV154" s="9">
+        <f t="shared" ref="AV154" si="849">IF(ISNA(I154),AV153,IF(I154=0,AV153+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AW154" s="9">
+        <f t="shared" ref="AW154" si="850">IF(ISNA(J154),AW153,IF(J154=0,AW153+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AX154" s="9">
+        <f t="shared" ref="AX154" si="851">IF(ISNA(K154),AX153,IF(K154=0,AX153+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AY154" s="9">
+        <f t="shared" ref="AY154" si="852">IF(ISNA(L154),AY153,IF(L154=0,AY153+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AZ154" s="9">
+        <f t="shared" ref="AZ154" si="853">IF(ISNA(M154),AZ153,IF(M154=0,AZ153+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="BA154" s="9">
+        <f t="shared" ref="BA154" si="854">IF(ISNA(N154),BA153,IF(N154=0,BA153+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="BB154" s="9">
+        <f t="shared" ref="BB154" si="855">IF(ISNA(O154),BB153,IF(O154=0,BB153+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="BC154" s="9">
+        <f t="shared" ref="BC154" si="856">IF(ISNA(P154),BC153,IF(P154=0,BC153+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="BD154" s="9">
+        <f t="shared" ref="BD154" si="857">IF(ISNA(Q154),BD153,IF(Q154=0,BD153+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="BE154" s="9">
+        <f t="shared" ref="BE154" si="858">IF(ISNA(R154),BE153,IF(R154=0,BE153+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="BF154" s="9">
+        <f t="shared" ref="BF154" si="859">IF(ISNA(S154),BF153,IF(S154=0,BF153+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="BG154" s="9">
+        <f t="shared" ref="BG154" si="860">IF(ISNA(T154),BG153,IF(T154=0,BG153+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="BH154" s="9">
+        <f t="shared" ref="BH154" si="861">IF(ISNA(U154),BH153,IF(U154=0,BH153+1,0))</f>
         <v>5</v>
       </c>
     </row>
@@ -72241,7 +73967,7 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -73606,8 +75332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B19" sqref="B2:Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -73689,68 +75415,68 @@
         <v>24</v>
       </c>
       <c r="B2" s="5">
-        <f>SUMIF(Results!E105:E151,"&lt;&gt;#N/A")/COUNTIFS(Results!E105:E151,"&lt;&gt;#N/A",Results!E105:E151,"&lt;&gt;")</f>
-        <v>0.46666666666666667</v>
+        <f>SUMIF(Results!E105:E154,"&lt;&gt;#N/A")/COUNTIFS(Results!E105:E154,"&lt;&gt;#N/A",Results!E105:E154,"&lt;&gt;")</f>
+        <v>0.46938775510204084</v>
       </c>
       <c r="C2" s="5">
-        <f>SUMIF(Results!F105:F151,"&lt;&gt;#N/A")/COUNTIFS(Results!F105:F151,"&lt;&gt;#N/A",Results!F105:F151,"&lt;&gt;")</f>
-        <v>0.72222222222222221</v>
+        <f>SUMIF(Results!F105:F154,"&lt;&gt;#N/A")/COUNTIFS(Results!F105:F154,"&lt;&gt;#N/A",Results!F105:F154,"&lt;&gt;")</f>
+        <v>0.69230769230769229</v>
       </c>
       <c r="D2" s="5">
-        <f>SUMIF(Results!G105:G151,"&lt;&gt;#N/A")/COUNTIFS(Results!G105:G151,"&lt;&gt;#N/A",Results!G105:G151,"&lt;&gt;")</f>
-        <v>0.62222222222222223</v>
+        <f>SUMIF(Results!G105:G154,"&lt;&gt;#N/A")/COUNTIFS(Results!G105:G154,"&lt;&gt;#N/A",Results!G105:G154,"&lt;&gt;")</f>
+        <v>0.61224489795918369</v>
       </c>
       <c r="E2" s="5">
-        <f>SUMIF(Results!H105:H151,"&lt;&gt;#N/A")/COUNTIFS(Results!H105:H151,"&lt;&gt;#N/A",Results!H105:H151,"&lt;&gt;")</f>
-        <v>0.53488372093023251</v>
+        <f>SUMIF(Results!H105:H154,"&lt;&gt;#N/A")/COUNTIFS(Results!H105:H154,"&lt;&gt;#N/A",Results!H105:H154,"&lt;&gt;")</f>
+        <v>0.53191489361702127</v>
       </c>
       <c r="F2" s="5">
-        <f>SUMIF(Results!I105:I151,"&lt;&gt;#N/A")/COUNTIFS(Results!I105:I151,"&lt;&gt;#N/A",Results!I105:I151,"&lt;&gt;")</f>
-        <v>1</v>
+        <f>SUMIF(Results!I105:I154,"&lt;&gt;#N/A")/COUNTIFS(Results!I105:I154,"&lt;&gt;#N/A",Results!I105:I154,"&lt;&gt;")</f>
+        <v>0.66666666666666663</v>
       </c>
       <c r="G2" s="5">
-        <f>SUMIF(Results!J105:J151,"&lt;&gt;#N/A")/COUNTIFS(Results!J105:J151,"&lt;&gt;#N/A",Results!J105:J151,"&lt;&gt;")</f>
-        <v>0</v>
+        <f>SUMIF(Results!J105:J154,"&lt;&gt;#N/A")/COUNTIFS(Results!J105:J154,"&lt;&gt;#N/A",Results!J105:J154,"&lt;&gt;")</f>
+        <v>0.25</v>
       </c>
       <c r="H2" s="5" t="e">
-        <f>SUMIF(Results!K105:K151,"&lt;&gt;#N/A")/COUNTIFS(Results!K105:K151,"&lt;&gt;#N/A",Results!K105:K151,"&lt;&gt;")</f>
+        <f>SUMIF(Results!K105:K154,"&lt;&gt;#N/A")/COUNTIFS(Results!K105:K154,"&lt;&gt;#N/A",Results!K105:K154,"&lt;&gt;")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I2" s="5">
-        <f>SUMIF(Results!L105:L151,"&lt;&gt;#N/A")/COUNTIFS(Results!L105:L151,"&lt;&gt;#N/A",Results!L105:L151,"&lt;&gt;")</f>
+        <f>SUMIF(Results!L105:L154,"&lt;&gt;#N/A")/COUNTIFS(Results!L105:L154,"&lt;&gt;#N/A",Results!L105:L154,"&lt;&gt;")</f>
         <v>1</v>
       </c>
       <c r="J2" s="5" t="e">
-        <f>SUMIF(Results!M105:M151,"&lt;&gt;#N/A")/COUNTIFS(Results!M105:M151,"&lt;&gt;#N/A",Results!M105:M151,"&lt;&gt;")</f>
+        <f>SUMIF(Results!M105:M154,"&lt;&gt;#N/A")/COUNTIFS(Results!M105:M154,"&lt;&gt;#N/A",Results!M105:M154,"&lt;&gt;")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K2" s="5" t="e">
-        <f>SUMIF(Results!N105:N151,"&lt;&gt;#N/A")/COUNTIFS(Results!N105:N151,"&lt;&gt;#N/A",Results!N105:N151,"&lt;&gt;")</f>
+        <f>SUMIF(Results!N105:N154,"&lt;&gt;#N/A")/COUNTIFS(Results!N105:N154,"&lt;&gt;#N/A",Results!N105:N154,"&lt;&gt;")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L2" s="5" t="e">
-        <f>SUMIF(Results!O105:O151,"&lt;&gt;#N/A")/COUNTIFS(Results!O105:O151,"&lt;&gt;#N/A",Results!O105:O151,"&lt;&gt;")</f>
+        <f>SUMIF(Results!O105:O154,"&lt;&gt;#N/A")/COUNTIFS(Results!O105:O154,"&lt;&gt;#N/A",Results!O105:O154,"&lt;&gt;")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M2" s="5" t="e">
-        <f>SUMIF(Results!P105:P151,"&lt;&gt;#N/A")/COUNTIFS(Results!P105:P151,"&lt;&gt;#N/A",Results!P105:P151,"&lt;&gt;")</f>
+        <f>SUMIF(Results!P105:P154,"&lt;&gt;#N/A")/COUNTIFS(Results!P105:P154,"&lt;&gt;#N/A",Results!P105:P154,"&lt;&gt;")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="N2" s="5" t="e">
-        <f>SUMIF(Results!Q105:Q151,"&lt;&gt;#N/A")/COUNTIFS(Results!Q105:Q151,"&lt;&gt;#N/A",Results!Q105:Q151,"&lt;&gt;")</f>
+        <f>SUMIF(Results!Q105:Q154,"&lt;&gt;#N/A")/COUNTIFS(Results!Q105:Q154,"&lt;&gt;#N/A",Results!Q105:Q154,"&lt;&gt;")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="O2" s="5" t="e">
-        <f>SUMIF(Results!R105:R151,"&lt;&gt;#N/A")/COUNTIFS(Results!R105:R151,"&lt;&gt;#N/A",Results!R105:R151,"&lt;&gt;")</f>
+        <f>SUMIF(Results!R105:R154,"&lt;&gt;#N/A")/COUNTIFS(Results!R105:R154,"&lt;&gt;#N/A",Results!R105:R154,"&lt;&gt;")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="P2" s="5" t="e">
-        <f>SUMIF(Results!S105:S151,"&lt;&gt;#N/A")/COUNTIFS(Results!S105:S151,"&lt;&gt;#N/A",Results!S105:S151,"&lt;&gt;")</f>
+        <f>SUMIF(Results!S105:S154,"&lt;&gt;#N/A")/COUNTIFS(Results!S105:S154,"&lt;&gt;#N/A",Results!S105:S154,"&lt;&gt;")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q2" s="5">
-        <f>SUM(Results!W105:W151)/SUM(Results!V105:V151)</f>
-        <v>0.56424581005586594</v>
+        <f>SUM(Results!W105:W154)/SUM(Results!V105:V154)</f>
+        <v>0.5532994923857868</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.35">
@@ -73758,68 +75484,68 @@
         <v>25</v>
       </c>
       <c r="B3" s="5">
-        <f>SUMIFS(Results!E105:E151,Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!E105:E151, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!E105:E151, "&lt;&gt;#N/A", Results!E105:E151, "&lt;&gt;")</f>
-        <v>0.43478260869565216</v>
+        <f>SUMIFS(Results!E105:E154,Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!E105:E154, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!E105:E154, "&lt;&gt;#N/A", Results!E105:E154, "&lt;&gt;")</f>
+        <v>0.44444444444444442</v>
       </c>
       <c r="C3" s="5">
-        <f>SUMIFS(Results!F105:F151,Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!F105:F151, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!F105:F151, "&lt;&gt;#N/A", Results!F105:F151, "&lt;&gt;")</f>
-        <v>0.77777777777777779</v>
+        <f>SUMIFS(Results!F105:F154,Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!F105:F154, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!F105:F154, "&lt;&gt;#N/A", Results!F105:F154, "&lt;&gt;")</f>
+        <v>0.7142857142857143</v>
       </c>
       <c r="D3" s="5">
-        <f>SUMIFS(Results!G105:G151,Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!G105:G151, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!G105:G151, "&lt;&gt;#N/A", Results!G105:G151, "&lt;&gt;")</f>
-        <v>0.69565217391304346</v>
+        <f>SUMIFS(Results!G105:G154,Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!G105:G154, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!G105:G154, "&lt;&gt;#N/A", Results!G105:G154, "&lt;&gt;")</f>
+        <v>0.66666666666666663</v>
       </c>
       <c r="E3" s="5">
-        <f>SUMIFS(Results!H105:H151,Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!H105:H151, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!H105:H151, "&lt;&gt;#N/A", Results!H105:H151, "&lt;&gt;")</f>
-        <v>0.43478260869565216</v>
+        <f>SUMIFS(Results!H105:H154,Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!H105:H154, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!H105:H154, "&lt;&gt;#N/A", Results!H105:H154, "&lt;&gt;")</f>
+        <v>0.44444444444444442</v>
       </c>
       <c r="F3" s="5">
-        <f>SUMIFS(Results!I105:I151,Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!I105:I151, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!I105:I151, "&lt;&gt;#N/A", Results!I105:I151, "&lt;&gt;")</f>
-        <v>1</v>
+        <f>SUMIFS(Results!I105:I154,Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!I105:I154, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!I105:I154, "&lt;&gt;#N/A", Results!I105:I154, "&lt;&gt;")</f>
+        <v>0.66666666666666663</v>
       </c>
       <c r="G3" s="5">
-        <f>SUMIFS(Results!J105:J151,Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!J105:J151, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!J105:J151, "&lt;&gt;#N/A", Results!J105:J151, "&lt;&gt;")</f>
-        <v>0</v>
+        <f>SUMIFS(Results!J105:J154,Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!J105:J154, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!J105:J154, "&lt;&gt;#N/A", Results!J105:J154, "&lt;&gt;")</f>
+        <v>0.25</v>
       </c>
       <c r="H3" s="5" t="e">
-        <f>SUMIFS(Results!K105:K151,Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!K105:K151, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!K105:K151, "&lt;&gt;#N/A", Results!K105:K151, "&lt;&gt;")</f>
+        <f>SUMIFS(Results!K105:K154,Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!K105:K154, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!K105:K154, "&lt;&gt;#N/A", Results!K105:K154, "&lt;&gt;")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I3" s="5">
-        <f>SUMIFS(Results!L105:L151,Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!L105:L151, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!L105:L151, "&lt;&gt;#N/A", Results!L105:L151, "&lt;&gt;")</f>
+        <f>SUMIFS(Results!L105:L154,Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!L105:L154, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!L105:L154, "&lt;&gt;#N/A", Results!L105:L154, "&lt;&gt;")</f>
         <v>1</v>
       </c>
       <c r="J3" s="5" t="e">
-        <f>SUMIFS(Results!M105:M151,Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!M105:M151, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!M105:M151, "&lt;&gt;#N/A", Results!M105:M151, "&lt;&gt;")</f>
+        <f>SUMIFS(Results!M105:M154,Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!M105:M154, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!M105:M154, "&lt;&gt;#N/A", Results!M105:M154, "&lt;&gt;")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K3" s="5" t="e">
-        <f>SUMIFS(Results!N105:N151,Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!N105:N151, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!N105:N151, "&lt;&gt;#N/A", Results!N105:N151, "&lt;&gt;")</f>
+        <f>SUMIFS(Results!N105:N154,Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!N105:N154, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!N105:N154, "&lt;&gt;#N/A", Results!N105:N154, "&lt;&gt;")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L3" s="5" t="e">
-        <f>SUMIFS(Results!O105:O151,Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!O105:O151, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!O105:O151, "&lt;&gt;#N/A", Results!O105:O151, "&lt;&gt;")</f>
+        <f>SUMIFS(Results!O105:O154,Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!O105:O154, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!O105:O154, "&lt;&gt;#N/A", Results!O105:O154, "&lt;&gt;")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M3" s="5" t="e">
-        <f>SUMIFS(Results!P105:P151,Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!P105:P151, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!P105:P151, "&lt;&gt;#N/A", Results!P105:P151, "&lt;&gt;")</f>
+        <f>SUMIFS(Results!P105:P154,Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!P105:P154, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!P105:P154, "&lt;&gt;#N/A", Results!P105:P154, "&lt;&gt;")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="N3" s="5" t="e">
-        <f>SUMIFS(Results!Q105:Q151,Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!Q105:Q151, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!Q105:Q151, "&lt;&gt;#N/A", Results!Q105:Q151, "&lt;&gt;")</f>
+        <f>SUMIFS(Results!Q105:Q154,Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!Q105:Q154, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!Q105:Q154, "&lt;&gt;#N/A", Results!Q105:Q154, "&lt;&gt;")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="O3" s="5" t="e">
-        <f>SUMIFS(Results!R105:R151,Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!R105:R151, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!R105:R151, "&lt;&gt;#N/A", Results!R105:R151, "&lt;&gt;")</f>
+        <f>SUMIFS(Results!R105:R154,Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!R105:R154, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!R105:R154, "&lt;&gt;#N/A", Results!R105:R154, "&lt;&gt;")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="P3" s="5" t="e">
-        <f>SUMIFS(Results!S105:S151,Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!S105:S151, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!S105:S151, "&lt;&gt;#N/A", Results!S105:S151, "&lt;&gt;")</f>
+        <f>SUMIFS(Results!S105:S154,Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!S105:S154, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!S105:S154, "&lt;&gt;#N/A", Results!S105:S154, "&lt;&gt;")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q3" s="5">
-        <f>SUMIF(Results!B105:B151,"&lt;&gt;#N/A",Results!W105:W151)/SUMIF(Results!B105:B151,"&lt;&gt;#N/A",Results!V105:V151)</f>
-        <v>0.55789473684210522</v>
+        <f>SUMIF(Results!B105:B154,"&lt;&gt;#N/A",Results!W105:W154)/SUMIF(Results!B105:B154,"&lt;&gt;#N/A",Results!V105:V154)</f>
+        <v>0.53982300884955747</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
@@ -73827,67 +75553,67 @@
         <v>26</v>
       </c>
       <c r="B4" s="5">
-        <f>SUMIFS(Results!E105:E151,Results!$B$105:$B$151,"=#N/A",Results!E105:E151, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$151,"=#N/A",Results!E105:E151, "&lt;&gt;#N/A", Results!E105:E151, "&lt;&gt;")</f>
+        <f>SUMIFS(Results!E105:E154,Results!$B$105:$B$154,"=#N/A",Results!E105:E154, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$154,"=#N/A",Results!E105:E154, "&lt;&gt;#N/A", Results!E105:E154, "&lt;&gt;")</f>
         <v>0.5</v>
       </c>
       <c r="C4" s="5">
-        <f>SUMIFS(Results!F105:F151,Results!$B$105:$B$151,"=#N/A",Results!F105:F151, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$151,"=#N/A",Results!F105:F151, "&lt;&gt;#N/A", Results!F105:F151, "&lt;&gt;")</f>
+        <f>SUMIFS(Results!F105:F154,Results!$B$105:$B$154,"=#N/A",Results!F105:F154, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$154,"=#N/A",Results!F105:F154, "&lt;&gt;#N/A", Results!F105:F154, "&lt;&gt;")</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="D4" s="5">
-        <f>SUMIFS(Results!G105:G151,Results!$B$105:$B$151,"=#N/A",Results!G105:G151, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$151,"=#N/A",Results!G105:G151, "&lt;&gt;#N/A", Results!G105:G151, "&lt;&gt;")</f>
+        <f>SUMIFS(Results!G105:G154,Results!$B$105:$B$154,"=#N/A",Results!G105:G154, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$154,"=#N/A",Results!G105:G154, "&lt;&gt;#N/A", Results!G105:G154, "&lt;&gt;")</f>
         <v>0.54545454545454541</v>
       </c>
       <c r="E4" s="5">
-        <f>SUMIFS(Results!H105:H151,Results!$B$105:$B$151,"=#N/A",Results!H105:H151, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$151,"=#N/A",Results!H105:H151, "&lt;&gt;#N/A", Results!H105:H151, "&lt;&gt;")</f>
+        <f>SUMIFS(Results!H105:H154,Results!$B$105:$B$154,"=#N/A",Results!H105:H154, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$154,"=#N/A",Results!H105:H154, "&lt;&gt;#N/A", Results!H105:H154, "&lt;&gt;")</f>
         <v>0.65</v>
       </c>
       <c r="F4" s="5" t="e">
-        <f>SUMIFS(Results!I105:I151,Results!$B$105:$B$151,"=#N/A",Results!I105:I151, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$151,"=#N/A",Results!I105:I151, "&lt;&gt;#N/A", Results!I105:I151, "&lt;&gt;")</f>
+        <f>SUMIFS(Results!I105:I154,Results!$B$105:$B$154,"=#N/A",Results!I105:I154, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$154,"=#N/A",Results!I105:I154, "&lt;&gt;#N/A", Results!I105:I154, "&lt;&gt;")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G4" s="5" t="e">
-        <f>SUMIFS(Results!J105:J151,Results!$B$105:$B$151,"=#N/A",Results!J105:J151, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$151,"=#N/A",Results!J105:J151, "&lt;&gt;#N/A", Results!J105:J151, "&lt;&gt;")</f>
+        <f>SUMIFS(Results!J105:J154,Results!$B$105:$B$154,"=#N/A",Results!J105:J154, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$154,"=#N/A",Results!J105:J154, "&lt;&gt;#N/A", Results!J105:J154, "&lt;&gt;")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H4" s="5" t="e">
-        <f>SUMIFS(Results!K105:K151,Results!$B$105:$B$151,"=#N/A",Results!K105:K151, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$151,"=#N/A",Results!K105:K151, "&lt;&gt;#N/A", Results!K105:K151, "&lt;&gt;")</f>
+        <f>SUMIFS(Results!K105:K154,Results!$B$105:$B$154,"=#N/A",Results!K105:K154, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$154,"=#N/A",Results!K105:K154, "&lt;&gt;#N/A", Results!K105:K154, "&lt;&gt;")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I4" s="5" t="e">
-        <f>SUMIFS(Results!L105:L151,Results!$B$105:$B$151,"=#N/A",Results!L105:L151, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$151,"=#N/A",Results!L105:L151, "&lt;&gt;#N/A", Results!L105:L151, "&lt;&gt;")</f>
+        <f>SUMIFS(Results!L105:L154,Results!$B$105:$B$154,"=#N/A",Results!L105:L154, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$154,"=#N/A",Results!L105:L154, "&lt;&gt;#N/A", Results!L105:L154, "&lt;&gt;")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="J4" s="5" t="e">
-        <f>SUMIFS(Results!M105:M151,Results!$B$105:$B$151,"=#N/A",Results!M105:M151, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$151,"=#N/A",Results!M105:M151, "&lt;&gt;#N/A", Results!M105:M151, "&lt;&gt;")</f>
+        <f>SUMIFS(Results!M105:M154,Results!$B$105:$B$154,"=#N/A",Results!M105:M154, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$154,"=#N/A",Results!M105:M154, "&lt;&gt;#N/A", Results!M105:M154, "&lt;&gt;")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K4" s="5" t="e">
-        <f>SUMIFS(Results!N105:N151,Results!$B$105:$B$151,"=#N/A",Results!N105:N151, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$151,"=#N/A",Results!N105:N151, "&lt;&gt;#N/A", Results!N105:N151, "&lt;&gt;")</f>
+        <f>SUMIFS(Results!N105:N154,Results!$B$105:$B$154,"=#N/A",Results!N105:N154, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$154,"=#N/A",Results!N105:N154, "&lt;&gt;#N/A", Results!N105:N154, "&lt;&gt;")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L4" s="5" t="e">
-        <f>SUMIFS(Results!O105:O151,Results!$B$105:$B$151,"=#N/A",Results!O105:O151, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$151,"=#N/A",Results!O105:O151, "&lt;&gt;#N/A", Results!O105:O151, "&lt;&gt;")</f>
+        <f>SUMIFS(Results!O105:O154,Results!$B$105:$B$154,"=#N/A",Results!O105:O154, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$154,"=#N/A",Results!O105:O154, "&lt;&gt;#N/A", Results!O105:O154, "&lt;&gt;")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M4" s="5" t="e">
-        <f>SUMIFS(Results!P105:P151,Results!$B$105:$B$151,"=#N/A",Results!P105:P151, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$151,"=#N/A",Results!P105:P151, "&lt;&gt;#N/A", Results!P105:P151, "&lt;&gt;")</f>
+        <f>SUMIFS(Results!P105:P154,Results!$B$105:$B$154,"=#N/A",Results!P105:P154, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$154,"=#N/A",Results!P105:P154, "&lt;&gt;#N/A", Results!P105:P154, "&lt;&gt;")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="N4" s="5" t="e">
-        <f>SUMIFS(Results!Q105:Q151,Results!$B$105:$B$151,"=#N/A",Results!Q105:Q151, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$151,"=#N/A",Results!Q105:Q151, "&lt;&gt;#N/A", Results!Q105:Q151, "&lt;&gt;")</f>
+        <f>SUMIFS(Results!Q105:Q154,Results!$B$105:$B$154,"=#N/A",Results!Q105:Q154, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$154,"=#N/A",Results!Q105:Q154, "&lt;&gt;#N/A", Results!Q105:Q154, "&lt;&gt;")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="O4" s="5" t="e">
-        <f>SUMIFS(Results!R105:R151,Results!$B$105:$B$151,"=#N/A",Results!R105:R151, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$151,"=#N/A",Results!R105:R151, "&lt;&gt;#N/A", Results!R105:R151, "&lt;&gt;")</f>
+        <f>SUMIFS(Results!R105:R154,Results!$B$105:$B$154,"=#N/A",Results!R105:R154, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$154,"=#N/A",Results!R105:R154, "&lt;&gt;#N/A", Results!R105:R154, "&lt;&gt;")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="P4" s="5" t="e">
-        <f>SUMIFS(Results!S105:S151,Results!$B$105:$B$151,"=#N/A",Results!S105:S151, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$151,"=#N/A",Results!S105:S151, "&lt;&gt;#N/A", Results!S105:S151, "&lt;&gt;")</f>
+        <f>SUMIFS(Results!S105:S154,Results!$B$105:$B$154,"=#N/A",Results!S105:S154, "&lt;&gt;#N/A")/COUNTIFS(Results!$B$105:$B$154,"=#N/A",Results!S105:S154, "&lt;&gt;#N/A", Results!S105:S154, "&lt;&gt;")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q4" s="5">
-        <f>SUMIF(Results!B105:B151,"=#N/A",Results!W105:W151)/SUMIF(Results!B105:B151,"=#N/A",Results!V105:V151)</f>
+        <f>SUMIF(Results!B105:B154,"=#N/A",Results!W105:W154)/SUMIF(Results!B105:B154,"=#N/A",Results!V105:V154)</f>
         <v>0.5714285714285714</v>
       </c>
     </row>
@@ -73896,63 +75622,63 @@
         <v>27</v>
       </c>
       <c r="B5" s="1">
-        <f>MAX(Results!AA105:AA151)</f>
+        <f>MAX(Results!AA105:AA154)</f>
         <v>3</v>
       </c>
       <c r="C5" s="1">
-        <f>MAX(Results!AB105:AB151)</f>
+        <f>MAX(Results!AB105:AB154)</f>
         <v>7</v>
       </c>
       <c r="D5" s="1">
-        <f>MAX(Results!AC105:AC151)</f>
+        <f>MAX(Results!AC105:AC154)</f>
         <v>6</v>
       </c>
       <c r="E5" s="1">
-        <f>MAX(Results!AD105:AD151)</f>
+        <f>MAX(Results!AD105:AD154)</f>
         <v>3</v>
       </c>
       <c r="F5" s="1">
-        <f>MAX(Results!AE105:AE151)</f>
+        <f>MAX(Results!AE105:AE154)</f>
         <v>3</v>
       </c>
       <c r="G5" s="1">
-        <f>MAX(Results!AF105:AF151)</f>
-        <v>0</v>
+        <f>MAX(Results!AF105:AF154)</f>
+        <v>1</v>
       </c>
       <c r="H5" s="1">
-        <f>MAX(Results!AG105:AG151)</f>
+        <f>MAX(Results!AG105:AG154)</f>
         <v>0</v>
       </c>
       <c r="I5" s="1">
-        <f>MAX(Results!AH105:AH151)</f>
+        <f>MAX(Results!AH105:AH154)</f>
         <v>1</v>
       </c>
       <c r="J5" s="1">
-        <f>MAX(Results!AI105:AI151)</f>
+        <f>MAX(Results!AI105:AI154)</f>
         <v>0</v>
       </c>
       <c r="K5" s="1">
-        <f>MAX(Results!AJ105:AJ151)</f>
+        <f>MAX(Results!AJ105:AJ154)</f>
         <v>1</v>
       </c>
       <c r="L5" s="1">
-        <f>MAX(Results!AK105:AK151)</f>
+        <f>MAX(Results!AK105:AK154)</f>
         <v>0</v>
       </c>
       <c r="M5" s="1">
-        <f>MAX(Results!AL105:AL151)</f>
+        <f>MAX(Results!AL105:AL154)</f>
         <v>0</v>
       </c>
       <c r="N5" s="1">
-        <f>MAX(Results!AM105:AM151)</f>
+        <f>MAX(Results!AM105:AM154)</f>
         <v>0</v>
       </c>
       <c r="O5" s="1">
-        <f>MAX(Results!AN105:AN151)</f>
+        <f>MAX(Results!AN105:AN154)</f>
         <v>1</v>
       </c>
       <c r="P5" s="1">
-        <f>MAX(Results!AO105:AO151)</f>
+        <f>MAX(Results!AO105:AO154)</f>
         <v>0</v>
       </c>
       <c r="Q5" s="1">
@@ -73965,68 +75691,68 @@
         <v>28</v>
       </c>
       <c r="B6" s="1">
-        <f>MAX(Results!AR105:AR151)</f>
+        <f>MAX(Results!AR105:AR154)</f>
         <v>5</v>
       </c>
       <c r="C6" s="1">
-        <f>MAX(Results!AS105:AS151)</f>
+        <f>MAX(Results!AS105:AS154)</f>
         <v>2</v>
       </c>
       <c r="D6" s="1">
-        <f>MAX(Results!AT105:AT151)</f>
+        <f>MAX(Results!AT105:AT154)</f>
         <v>4</v>
       </c>
       <c r="E6" s="1">
-        <f>MAX(Results!AU105:AU151)</f>
+        <f>MAX(Results!AU105:AU154)</f>
         <v>3</v>
       </c>
       <c r="F6" s="1">
-        <f>MAX(Results!AV105:AV151)</f>
-        <v>0</v>
+        <f>MAX(Results!AV105:AV154)</f>
+        <v>1</v>
       </c>
       <c r="G6" s="1">
-        <f>MAX(Results!AW105:AW151)</f>
-        <v>5</v>
+        <f>MAX(Results!AW105:AW154)</f>
+        <v>6</v>
       </c>
       <c r="H6" s="1">
-        <f>MAX(Results!AX105:AX151)</f>
+        <f>MAX(Results!AX105:AX154)</f>
         <v>0</v>
       </c>
       <c r="I6" s="1">
-        <f>MAX(Results!AY105:AY151)</f>
+        <f>MAX(Results!AY105:AY154)</f>
         <v>0</v>
       </c>
       <c r="J6" s="1">
-        <f>MAX(Results!AZ105:AZ151)</f>
+        <f>MAX(Results!AZ105:AZ154)</f>
         <v>0</v>
       </c>
       <c r="K6" s="1">
-        <f>MAX(Results!BA105:BA151)</f>
+        <f>MAX(Results!BA105:BA154)</f>
         <v>0</v>
       </c>
       <c r="L6" s="1">
-        <f>MAX(Results!BB105:BB151)</f>
+        <f>MAX(Results!BB105:BB154)</f>
         <v>0</v>
       </c>
       <c r="M6" s="1">
-        <f>MAX(Results!BC105:BC151)</f>
+        <f>MAX(Results!BC105:BC154)</f>
         <v>0</v>
       </c>
       <c r="N6" s="1">
-        <f>MAX(Results!BD105:BD151)</f>
+        <f>MAX(Results!BD105:BD154)</f>
         <v>1</v>
       </c>
       <c r="O6" s="1">
-        <f>MAX(Results!BE105:BE151)</f>
+        <f>MAX(Results!BE105:BE154)</f>
         <v>0</v>
       </c>
       <c r="P6" s="1">
-        <f>MAX(Results!BF105:BF151)</f>
+        <f>MAX(Results!BF105:BF154)</f>
         <v>1</v>
       </c>
       <c r="Q6" s="1">
         <f>MAX(B6:P6)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.35">
@@ -74034,63 +75760,63 @@
         <v>53</v>
       </c>
       <c r="B7" s="1">
-        <f>COUNTIF(Results!$Z$105:$Z$151,'Summary 2019'!B1)</f>
+        <f>COUNTIF(Results!$Z$105:$Z$154,'Summary 2019'!B1)</f>
         <v>2</v>
       </c>
       <c r="C7" s="1">
-        <f>COUNTIF(Results!$Z$105:$Z$151,'Summary 2019'!C1)</f>
+        <f>COUNTIF(Results!$Z$105:$Z$154,'Summary 2019'!C1)</f>
         <v>3</v>
       </c>
       <c r="D7" s="1">
-        <f>COUNTIF(Results!$Z$105:$Z$151,'Summary 2019'!D1)</f>
+        <f>COUNTIF(Results!$Z$105:$Z$154,'Summary 2019'!D1)</f>
         <v>2</v>
       </c>
       <c r="E7" s="1">
-        <f>COUNTIF(Results!$Z$105:$Z$151,'Summary 2019'!E1)</f>
+        <f>COUNTIF(Results!$Z$105:$Z$154,'Summary 2019'!E1)</f>
         <v>3</v>
       </c>
       <c r="F7" s="1">
-        <f>COUNTIF(Results!$Z$105:$Z$151,'Summary 2019'!F1)</f>
+        <f>COUNTIF(Results!$Z$105:$Z$154,'Summary 2019'!F1)</f>
         <v>1</v>
       </c>
       <c r="G7" s="1">
-        <f>COUNTIF(Results!$Z$105:$Z$151,'Summary 2019'!G1)</f>
+        <f>COUNTIF(Results!$Z$105:$Z$154,'Summary 2019'!G1)</f>
         <v>0</v>
       </c>
       <c r="H7" s="1">
-        <f>COUNTIF(Results!$Z$105:$Z$151,'Summary 2019'!H1)</f>
+        <f>COUNTIF(Results!$Z$105:$Z$154,'Summary 2019'!H1)</f>
         <v>0</v>
       </c>
       <c r="I7" s="1">
-        <f>COUNTIF(Results!$Z$105:$Z$151,'Summary 2019'!I1)</f>
+        <f>COUNTIF(Results!$Z$105:$Z$154,'Summary 2019'!I1)</f>
         <v>0</v>
       </c>
       <c r="J7" s="1">
-        <f>COUNTIF(Results!$Z$105:$Z$151,'Summary 2019'!J1)</f>
+        <f>COUNTIF(Results!$Z$105:$Z$154,'Summary 2019'!J1)</f>
         <v>0</v>
       </c>
       <c r="K7" s="1">
-        <f>COUNTIF(Results!$Z$105:$Z$151,'Summary 2019'!K1)</f>
+        <f>COUNTIF(Results!$Z$105:$Z$154,'Summary 2019'!K1)</f>
         <v>0</v>
       </c>
       <c r="L7" s="1">
-        <f>COUNTIF(Results!$Z$105:$Z$151,'Summary 2019'!L1)</f>
+        <f>COUNTIF(Results!$Z$105:$Z$154,'Summary 2019'!L1)</f>
         <v>0</v>
       </c>
       <c r="M7" s="1">
-        <f>COUNTIF(Results!$Z$105:$Z$151,'Summary 2019'!M1)</f>
+        <f>COUNTIF(Results!$Z$105:$Z$154,'Summary 2019'!M1)</f>
         <v>0</v>
       </c>
       <c r="N7" s="1">
-        <f>COUNTIF(Results!$Z$105:$Z$151,'Summary 2019'!N1)</f>
+        <f>COUNTIF(Results!$Z$105:$Z$154,'Summary 2019'!N1)</f>
         <v>0</v>
       </c>
       <c r="O7" s="1">
-        <f>COUNTIF(Results!$Z$105:$Z$151,'Summary 2019'!O1)</f>
+        <f>COUNTIF(Results!$Z$105:$Z$154,'Summary 2019'!O1)</f>
         <v>0</v>
       </c>
       <c r="P7" s="1">
-        <f>COUNTIF(Results!$Z$105:$Z$151,'Summary 2019'!P1)</f>
+        <f>COUNTIF(Results!$Z$105:$Z$154,'Summary 2019'!P1)</f>
         <v>0</v>
       </c>
       <c r="Q7" s="1">
@@ -74103,63 +75829,63 @@
         <v>45</v>
       </c>
       <c r="B8" s="6">
-        <f>SUMIF(Results!$D$105:$D$151,B1,Results!$W$105:$W$151)/SUMIF(Results!$D$105:$D$151,B1,Results!$V$105:$V$151)</f>
+        <f>SUMIF(Results!$D$105:$D$154,B1,Results!$W$105:$W$154)/SUMIF(Results!$D$105:$D$154,B1,Results!$V$105:$V$154)</f>
         <v>0.70588235294117652</v>
       </c>
       <c r="C8" s="6">
-        <f>SUMIF(Results!$D$105:$D$151,C1,Results!$W$105:$W$151)/SUMIF(Results!$D$105:$D$151,C1,Results!$V$105:$V$151)</f>
+        <f>SUMIF(Results!$D$105:$D$154,C1,Results!$W$105:$W$154)/SUMIF(Results!$D$105:$D$154,C1,Results!$V$105:$V$154)</f>
         <v>0.7142857142857143</v>
       </c>
       <c r="D8" s="6">
-        <f>SUMIF(Results!$D$105:$D$151,D1,Results!$W$105:$W$151)/SUMIF(Results!$D$105:$D$151,D1,Results!$V$105:$V$151)</f>
-        <v>0.44444444444444442</v>
+        <f>SUMIF(Results!$D$105:$D$154,D1,Results!$W$105:$W$154)/SUMIF(Results!$D$105:$D$154,D1,Results!$V$105:$V$154)</f>
+        <v>0.40816326530612246</v>
       </c>
       <c r="E8" s="6">
-        <f>SUMIF(Results!$D$105:$D$151,E1,Results!$W$105:$W$151)/SUMIF(Results!$D$105:$D$151,E1,Results!$V$105:$V$151)</f>
-        <v>0.44117647058823528</v>
-      </c>
-      <c r="F8" s="6" t="e">
-        <f>SUMIF(Results!$D$105:$D$151,F1,Results!$W$105:$W$151)/SUMIF(Results!$D$105:$D$151,F1,Results!$V$105:$V$151)</f>
+        <f>SUMIF(Results!$D$105:$D$154,E1,Results!$W$105:$W$154)/SUMIF(Results!$D$105:$D$154,E1,Results!$V$105:$V$154)</f>
+        <v>0.5</v>
+      </c>
+      <c r="F8" s="6">
+        <f>SUMIF(Results!$D$105:$D$154,F1,Results!$W$105:$W$154)/SUMIF(Results!$D$105:$D$154,F1,Results!$V$105:$V$154)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G8" s="6">
+        <f>SUMIF(Results!$D$105:$D$154,G1,Results!$W$105:$W$154)/SUMIF(Results!$D$105:$D$154,G1,Results!$V$105:$V$154)</f>
+        <v>0.5</v>
+      </c>
+      <c r="H8" s="6" t="e">
+        <f>SUMIF(Results!$D$105:$D$154,H1,Results!$W$105:$W$154)/SUMIF(Results!$D$105:$D$154,H1,Results!$V$105:$V$154)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G8" s="6">
-        <f>SUMIF(Results!$D$105:$D$151,G1,Results!$W$105:$W$151)/SUMIF(Results!$D$105:$D$151,G1,Results!$V$105:$V$151)</f>
-        <v>0.5</v>
-      </c>
-      <c r="H8" s="6" t="e">
-        <f>SUMIF(Results!$D$105:$D$151,H1,Results!$W$105:$W$151)/SUMIF(Results!$D$105:$D$151,H1,Results!$V$105:$V$151)</f>
+      <c r="I8" s="6">
+        <f>SUMIF(Results!$D$105:$D$154,I1,Results!$W$105:$W$154)/SUMIF(Results!$D$105:$D$154,I1,Results!$V$105:$V$154)</f>
+        <v>0.75</v>
+      </c>
+      <c r="J8" s="6" t="e">
+        <f>SUMIF(Results!$D$105:$D$154,J1,Results!$W$105:$W$154)/SUMIF(Results!$D$105:$D$154,J1,Results!$V$105:$V$154)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I8" s="6">
-        <f>SUMIF(Results!$D$105:$D$151,I1,Results!$W$105:$W$151)/SUMIF(Results!$D$105:$D$151,I1,Results!$V$105:$V$151)</f>
-        <v>0.75</v>
-      </c>
-      <c r="J8" s="6" t="e">
-        <f>SUMIF(Results!$D$105:$D$151,J1,Results!$W$105:$W$151)/SUMIF(Results!$D$105:$D$151,J1,Results!$V$105:$V$151)</f>
+      <c r="K8" s="6" t="e">
+        <f>SUMIF(Results!$D$105:$D$154,K1,Results!$W$105:$W$154)/SUMIF(Results!$D$105:$D$154,K1,Results!$V$105:$V$154)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K8" s="6" t="e">
-        <f>SUMIF(Results!$D$105:$D$151,K1,Results!$W$105:$W$151)/SUMIF(Results!$D$105:$D$151,K1,Results!$V$105:$V$151)</f>
+      <c r="L8" s="6" t="e">
+        <f>SUMIF(Results!$D$105:$D$154,L1,Results!$W$105:$W$154)/SUMIF(Results!$D$105:$D$154,L1,Results!$V$105:$V$154)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L8" s="6" t="e">
-        <f>SUMIF(Results!$D$105:$D$151,L1,Results!$W$105:$W$151)/SUMIF(Results!$D$105:$D$151,L1,Results!$V$105:$V$151)</f>
+      <c r="M8" s="6" t="e">
+        <f>SUMIF(Results!$D$105:$D$154,M1,Results!$W$105:$W$154)/SUMIF(Results!$D$105:$D$154,M1,Results!$V$105:$V$154)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M8" s="6" t="e">
-        <f>SUMIF(Results!$D$105:$D$151,M1,Results!$W$105:$W$151)/SUMIF(Results!$D$105:$D$151,M1,Results!$V$105:$V$151)</f>
+      <c r="N8" s="6" t="e">
+        <f>SUMIF(Results!$D$105:$D$154,N1,Results!$W$105:$W$154)/SUMIF(Results!$D$105:$D$154,N1,Results!$V$105:$V$154)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N8" s="6" t="e">
-        <f>SUMIF(Results!$D$105:$D$151,N1,Results!$W$105:$W$151)/SUMIF(Results!$D$105:$D$151,N1,Results!$V$105:$V$151)</f>
+      <c r="O8" s="6" t="e">
+        <f>SUMIF(Results!$D$105:$D$154,O1,Results!$W$105:$W$154)/SUMIF(Results!$D$105:$D$154,O1,Results!$V$105:$V$154)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="O8" s="6" t="e">
-        <f>SUMIF(Results!$D$105:$D$151,O1,Results!$W$105:$W$151)/SUMIF(Results!$D$105:$D$151,O1,Results!$V$105:$V$151)</f>
-        <v>#DIV/0!</v>
-      </c>
       <c r="P8" s="6" t="e">
-        <f>SUMIF(Results!$D$105:$D$151,P1,Results!$W$105:$W$151)/SUMIF(Results!$D$105:$D$151,P1,Results!$V$105:$V$151)</f>
+        <f>SUMIF(Results!$D$105:$D$154,P1,Results!$W$105:$W$154)/SUMIF(Results!$D$105:$D$154,P1,Results!$V$105:$V$154)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q8" s="19"/>
@@ -74169,68 +75895,68 @@
         <v>222</v>
       </c>
       <c r="B9" s="20">
-        <f>SUMIF(Results!$D$105:$D$151,B1,Results!E$105:E$151)</f>
+        <f>SUMIF(Results!$D$105:$D$154,B1,Results!E$105:E$154)</f>
         <v>2</v>
       </c>
       <c r="C9" s="20">
-        <f>SUMIF(Results!$D$105:$D$151,C1,Results!F$105:F$151)</f>
+        <f>SUMIF(Results!$D$105:$D$154,C1,Results!F$105:F$154)</f>
         <v>6</v>
       </c>
       <c r="D9" s="20">
-        <f>SUMIF(Results!$D$105:$D$151,D1,Results!G$105:G$151)</f>
+        <f>SUMIF(Results!$D$105:$D$154,D1,Results!G$105:G$154)</f>
         <v>3</v>
       </c>
       <c r="E9" s="20">
-        <f>SUMIF(Results!$D$105:$D$151,E1,Results!H$105:H$151)</f>
-        <v>3</v>
+        <f>SUMIF(Results!$D$105:$D$154,E1,Results!H$105:H$154)</f>
+        <v>4</v>
       </c>
       <c r="F9" s="20">
-        <f>SUMIF(Results!$D$105:$D$151,F1,Results!I$105:I$151)</f>
+        <f>SUMIF(Results!$D$105:$D$154,F1,Results!I$105:I$154)</f>
         <v>0</v>
       </c>
       <c r="G9" s="20">
-        <f>SUMIF(Results!$D$105:$D$151,G1,Results!J$105:J$151)</f>
+        <f>SUMIF(Results!$D$105:$D$154,G1,Results!J$105:J$154)</f>
         <v>0</v>
       </c>
       <c r="H9" s="20">
-        <f>SUMIF(Results!$D$105:$D$151,H1,Results!K$105:K$151)</f>
+        <f>SUMIF(Results!$D$105:$D$154,H1,Results!K$105:K$154)</f>
         <v>0</v>
       </c>
       <c r="I9" s="20">
-        <f>SUMIF(Results!$D$105:$D$151,I1,Results!L$105:L$151)</f>
+        <f>SUMIF(Results!$D$105:$D$154,I1,Results!L$105:L$154)</f>
         <v>1</v>
       </c>
       <c r="J9" s="20">
-        <f>SUMIF(Results!$D$105:$D$151,J1,Results!M$105:M$151)</f>
+        <f>SUMIF(Results!$D$105:$D$154,J1,Results!M$105:M$154)</f>
         <v>0</v>
       </c>
       <c r="K9" s="20">
-        <f>SUMIF(Results!$D$105:$D$151,K1,Results!N$105:N$151)</f>
+        <f>SUMIF(Results!$D$105:$D$154,K1,Results!N$105:N$154)</f>
         <v>0</v>
       </c>
       <c r="L9" s="20">
-        <f>SUMIF(Results!$D$105:$D$151,L1,Results!O$105:O$151)</f>
+        <f>SUMIF(Results!$D$105:$D$154,L1,Results!O$105:O$154)</f>
         <v>0</v>
       </c>
       <c r="M9" s="20">
-        <f>SUMIF(Results!$D$105:$D$151,M1,Results!P$105:P$151)</f>
+        <f>SUMIF(Results!$D$105:$D$154,M1,Results!P$105:P$154)</f>
         <v>0</v>
       </c>
       <c r="N9" s="20">
-        <f>SUMIF(Results!$D$105:$D$151,N1,Results!Q$105:Q$151)</f>
+        <f>SUMIF(Results!$D$105:$D$154,N1,Results!Q$105:Q$154)</f>
         <v>0</v>
       </c>
       <c r="O9" s="20">
-        <f>SUMIF(Results!$D$105:$D$151,O1,Results!R$105:R$151)</f>
+        <f>SUMIF(Results!$D$105:$D$154,O1,Results!R$105:R$154)</f>
         <v>0</v>
       </c>
       <c r="P9" s="20">
-        <f>SUMIF(Results!$D$105:$D$151,P1,Results!S$105:S$151)</f>
+        <f>SUMIF(Results!$D$105:$D$154,P1,Results!S$105:S$154)</f>
         <v>0</v>
       </c>
       <c r="Q9" s="21">
         <f>SUM(B9:P9)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.35">
@@ -74238,27 +75964,27 @@
         <v>122</v>
       </c>
       <c r="B10" s="1">
-        <f>COUNTIF(Results!$D$105:$D$151,'Summary 2019'!B1)</f>
+        <f>COUNTIF(Results!$D$105:$D$154,'Summary 2019'!B1)</f>
         <v>9</v>
       </c>
       <c r="C10" s="1">
-        <f>COUNTIF(Results!$D$105:$D$151,'Summary 2019'!C1)</f>
+        <f>COUNTIF(Results!$D$105:$D$154,'Summary 2019'!C1)</f>
         <v>9</v>
       </c>
       <c r="D10" s="1">
-        <f>COUNTIF(Results!$D$105:$D$151,'Summary 2019'!D1)</f>
-        <v>12</v>
+        <f>COUNTIF(Results!$D$105:$D$154,'Summary 2019'!D1)</f>
+        <v>13</v>
       </c>
       <c r="E10" s="1">
-        <f>COUNTIF(Results!$D$105:$D$151,'Summary 2019'!E1)</f>
-        <v>9</v>
+        <f>COUNTIF(Results!$D$105:$D$154,'Summary 2019'!E1)</f>
+        <v>11</v>
       </c>
       <c r="F10" s="1">
-        <f>COUNTIF(Results!$D$105:$D$151,'Summary 2019'!F1)</f>
-        <v>0</v>
+        <f>COUNTIF(Results!$D$105:$D$154,'Summary 2019'!F1)</f>
+        <v>1</v>
       </c>
       <c r="G10" s="1">
-        <f>COUNTIF(Results!$D$105:$D$151,'Summary 2019'!G1)</f>
+        <f>COUNTIF(Results!$D$105:$D$154,'Summary 2019'!G1)</f>
         <v>1</v>
       </c>
       <c r="H10" s="1">
@@ -74299,7 +76025,7 @@
       </c>
       <c r="Q10" s="1">
         <f>SUM(B10:P10)</f>
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.35">
@@ -74307,68 +76033,68 @@
         <v>221</v>
       </c>
       <c r="B11" s="6">
-        <f>SUMIF(Results!$D$105:$D$151,B1,Results!E$105:E$151)/COUNTIF(Results!$D$105:$D$151,B1)</f>
+        <f>SUMIF(Results!$D$105:$D$154,B1,Results!E$105:E$154)/COUNTIF(Results!$D$105:$D$154,B1)</f>
         <v>0.22222222222222221</v>
       </c>
       <c r="C11" s="6">
-        <f>SUMIF(Results!$D$105:$D$151,C1,Results!F$105:F$151)/COUNTIF(Results!$D$105:$D$151,C1)</f>
+        <f>SUMIF(Results!$D$105:$D$154,C1,Results!F$105:F$154)/COUNTIF(Results!$D$105:$D$154,C1)</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="D11" s="6">
-        <f>SUMIF(Results!$D$105:$D$151,D1,Results!G$105:G$151)/COUNTIF(Results!$D$105:$D$151,D1)</f>
-        <v>0.25</v>
+        <f>SUMIF(Results!$D$105:$D$154,D1,Results!G$105:G$154)/COUNTIF(Results!$D$105:$D$154,D1)</f>
+        <v>0.23076923076923078</v>
       </c>
       <c r="E11" s="6">
-        <f>SUMIF(Results!$D$105:$D$151,E1,Results!H$105:H$151)/COUNTIF(Results!$D$105:$D$151,E1)</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="F11" s="6" t="e">
-        <f>SUMIF(Results!$D$105:$D$151,F1,Results!I$105:I$151)/COUNTIF(Results!$D$105:$D$151,F1)</f>
+        <f>SUMIF(Results!$D$105:$D$154,E1,Results!H$105:H$154)/COUNTIF(Results!$D$105:$D$154,E1)</f>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="F11" s="6">
+        <f>SUMIF(Results!$D$105:$D$154,F1,Results!I$105:I$154)/COUNTIF(Results!$D$105:$D$154,F1)</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="6">
+        <f>SUMIF(Results!$D$105:$D$154,G1,Results!J$105:J$154)/COUNTIF(Results!$D$105:$D$154,G1)</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="6" t="e">
+        <f>SUMIF(Results!$D$105:$D$154,H1,Results!K$105:K$154)/COUNTIF(Results!$D$105:$D$154,H1)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G11" s="6">
-        <f>SUMIF(Results!$D$105:$D$151,G1,Results!J$105:J$151)/COUNTIF(Results!$D$105:$D$151,G1)</f>
-        <v>0</v>
-      </c>
-      <c r="H11" s="6" t="e">
-        <f>SUMIF(Results!$D$105:$D$151,H1,Results!K$105:K$151)/COUNTIF(Results!$D$105:$D$151,H1)</f>
+      <c r="I11" s="6">
+        <f>SUMIF(Results!$D$105:$D$154,I1,Results!L$105:L$154)/COUNTIF(Results!$D$105:$D$154,I1)</f>
+        <v>1</v>
+      </c>
+      <c r="J11" s="6" t="e">
+        <f>SUMIF(Results!$D$105:$D$154,J1,Results!M$105:M$154)/COUNTIF(Results!$D$105:$D$154,J1)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I11" s="6">
-        <f>SUMIF(Results!$D$105:$D$151,I1,Results!L$105:L$151)/COUNTIF(Results!$D$105:$D$151,I1)</f>
-        <v>1</v>
-      </c>
-      <c r="J11" s="6" t="e">
-        <f>SUMIF(Results!$D$105:$D$151,J1,Results!M$105:M$151)/COUNTIF(Results!$D$105:$D$151,J1)</f>
+      <c r="K11" s="6" t="e">
+        <f>SUMIF(Results!$D$105:$D$154,K1,Results!N$105:N$154)/COUNTIF(Results!$D$105:$D$154,K1)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K11" s="6" t="e">
-        <f>SUMIF(Results!$D$105:$D$151,K1,Results!N$105:N$151)/COUNTIF(Results!$D$105:$D$151,K1)</f>
+      <c r="L11" s="6" t="e">
+        <f>SUMIF(Results!$D$105:$D$154,L1,Results!O$105:O$154)/COUNTIF(Results!$D$105:$D$154,L1)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L11" s="6" t="e">
-        <f>SUMIF(Results!$D$105:$D$151,L1,Results!O$105:O$151)/COUNTIF(Results!$D$105:$D$151,L1)</f>
+      <c r="M11" s="6" t="e">
+        <f>SUMIF(Results!$D$105:$D$154,M1,Results!P$105:P$154)/COUNTIF(Results!$D$105:$D$154,M1)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M11" s="6" t="e">
-        <f>SUMIF(Results!$D$105:$D$151,M1,Results!P$105:P$151)/COUNTIF(Results!$D$105:$D$151,M1)</f>
+      <c r="N11" s="6" t="e">
+        <f>SUMIF(Results!$D$105:$D$154,N1,Results!Q$105:Q$154)/COUNTIF(Results!$D$105:$D$154,N1)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N11" s="6" t="e">
-        <f>SUMIF(Results!$D$105:$D$151,N1,Results!Q$105:Q$151)/COUNTIF(Results!$D$105:$D$151,N1)</f>
+      <c r="O11" s="6" t="e">
+        <f>SUMIF(Results!$D$105:$D$154,O1,Results!R$105:R$154)/COUNTIF(Results!$D$105:$D$154,O1)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="O11" s="6" t="e">
-        <f>SUMIF(Results!$D$105:$D$151,O1,Results!R$105:R$151)/COUNTIF(Results!$D$105:$D$151,O1)</f>
-        <v>#DIV/0!</v>
-      </c>
       <c r="P11" s="6" t="e">
-        <f>SUMIF(Results!$D$105:$D$151,P1,Results!S$105:S$151)/COUNTIF(Results!$D$105:$D$151,P1)</f>
+        <f>SUMIF(Results!$D$105:$D$154,P1,Results!S$105:S$154)/COUNTIF(Results!$D$105:$D$154,P1)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q11" s="5">
         <f>Q9/Q10</f>
-        <v>0.36585365853658536</v>
+        <v>0.35555555555555557</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.35">
@@ -74376,68 +76102,68 @@
         <v>55</v>
       </c>
       <c r="B12" s="1">
-        <f>SUMIF(Results!E105:E151,"&lt;&gt;#N/A")</f>
-        <v>21</v>
+        <f>SUMIF(Results!E105:E154,"&lt;&gt;#N/A")</f>
+        <v>23</v>
       </c>
       <c r="C12" s="1">
-        <f>SUMIF(Results!F105:F151,"&lt;&gt;#N/A")</f>
-        <v>26</v>
+        <f>SUMIF(Results!F105:F154,"&lt;&gt;#N/A")</f>
+        <v>27</v>
       </c>
       <c r="D12" s="1">
-        <f>SUMIF(Results!G105:G151,"&lt;&gt;#N/A")</f>
-        <v>28</v>
+        <f>SUMIF(Results!G105:G154,"&lt;&gt;#N/A")</f>
+        <v>30</v>
       </c>
       <c r="E12" s="1">
-        <f>SUMIF(Results!H105:H151,"&lt;&gt;#N/A")</f>
-        <v>23</v>
+        <f>SUMIF(Results!H105:H154,"&lt;&gt;#N/A")</f>
+        <v>25</v>
       </c>
       <c r="F12" s="1">
-        <f>SUMIF(Results!I105:I151,"&lt;&gt;#N/A")</f>
+        <f>SUMIF(Results!I105:I154,"&lt;&gt;#N/A")</f>
         <v>2</v>
       </c>
       <c r="G12" s="1">
-        <f>SUMIF(Results!J105:J151,"&lt;&gt;#N/A")</f>
-        <v>0</v>
+        <f>SUMIF(Results!J105:J154,"&lt;&gt;#N/A")</f>
+        <v>1</v>
       </c>
       <c r="H12" s="1">
-        <f>SUMIF(Results!K105:K151,"&lt;&gt;#N/A")</f>
+        <f>SUMIF(Results!K105:K154,"&lt;&gt;#N/A")</f>
         <v>0</v>
       </c>
       <c r="I12" s="1">
-        <f>SUMIF(Results!L105:L151,"&lt;&gt;#N/A")</f>
+        <f>SUMIF(Results!L105:L154,"&lt;&gt;#N/A")</f>
         <v>1</v>
       </c>
       <c r="J12" s="1">
-        <f>SUMIF(Results!M105:M151,"&lt;&gt;#N/A")</f>
+        <f>SUMIF(Results!M105:M154,"&lt;&gt;#N/A")</f>
         <v>0</v>
       </c>
       <c r="K12" s="1">
-        <f>SUMIF(Results!N105:N151,"&lt;&gt;#N/A")</f>
+        <f>SUMIF(Results!N105:N154,"&lt;&gt;#N/A")</f>
         <v>0</v>
       </c>
       <c r="L12" s="1">
-        <f>SUMIF(Results!O105:O151,"&lt;&gt;#N/A")</f>
+        <f>SUMIF(Results!O105:O154,"&lt;&gt;#N/A")</f>
         <v>0</v>
       </c>
       <c r="M12" s="1">
-        <f>SUMIF(Results!P105:P151,"&lt;&gt;#N/A")</f>
+        <f>SUMIF(Results!P105:P154,"&lt;&gt;#N/A")</f>
         <v>0</v>
       </c>
       <c r="N12" s="1">
-        <f>SUMIF(Results!Q105:Q151,"&lt;&gt;#N/A")</f>
+        <f>SUMIF(Results!Q105:Q154,"&lt;&gt;#N/A")</f>
         <v>0</v>
       </c>
       <c r="O12" s="1">
-        <f>SUMIF(Results!R105:R151,"&lt;&gt;#N/A")</f>
+        <f>SUMIF(Results!R105:R154,"&lt;&gt;#N/A")</f>
         <v>0</v>
       </c>
       <c r="P12" s="1">
-        <f>SUMIF(Results!S105:S151,"&lt;&gt;#N/A")</f>
+        <f>SUMIF(Results!S105:S154,"&lt;&gt;#N/A")</f>
         <v>0</v>
       </c>
       <c r="Q12" s="1">
         <f t="shared" ref="Q12:Q17" si="0">SUM(B12:P12)</f>
-        <v>101</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.35">
@@ -74445,68 +76171,68 @@
         <v>56</v>
       </c>
       <c r="B13" s="1">
-        <f>COUNTIFS(Results!E105:E151,"&lt;&gt;#N/A",Results!E105:E151,"&lt;&gt;")</f>
-        <v>45</v>
+        <f>COUNTIFS(Results!E105:E154,"&lt;&gt;#N/A",Results!E105:E154,"&lt;&gt;")</f>
+        <v>49</v>
       </c>
       <c r="C13" s="1">
-        <f>COUNTIFS(Results!F105:F151,"&lt;&gt;#N/A",Results!F105:F151,"&lt;&gt;")</f>
-        <v>36</v>
+        <f>COUNTIFS(Results!F105:F154,"&lt;&gt;#N/A",Results!F105:F154,"&lt;&gt;")</f>
+        <v>39</v>
       </c>
       <c r="D13" s="1">
-        <f>COUNTIFS(Results!G105:G151,"&lt;&gt;#N/A",Results!G105:G151,"&lt;&gt;")</f>
-        <v>45</v>
+        <f>COUNTIFS(Results!G105:G154,"&lt;&gt;#N/A",Results!G105:G154,"&lt;&gt;")</f>
+        <v>49</v>
       </c>
       <c r="E13" s="1">
-        <f>COUNTIFS(Results!H105:H151,"&lt;&gt;#N/A",Results!H105:H151,"&lt;&gt;")</f>
-        <v>43</v>
+        <f>COUNTIFS(Results!H105:H154,"&lt;&gt;#N/A",Results!H105:H154,"&lt;&gt;")</f>
+        <v>47</v>
       </c>
       <c r="F13" s="1">
-        <f>COUNTIFS(Results!I105:I151,"&lt;&gt;#N/A",Results!I105:I151,"&lt;&gt;")</f>
-        <v>2</v>
+        <f>COUNTIFS(Results!I105:I154,"&lt;&gt;#N/A",Results!I105:I154,"&lt;&gt;")</f>
+        <v>3</v>
       </c>
       <c r="G13" s="1">
-        <f>COUNTIFS(Results!J105:J151,"&lt;&gt;#N/A",Results!J105:J151,"&lt;&gt;")</f>
-        <v>2</v>
+        <f>COUNTIFS(Results!J105:J154,"&lt;&gt;#N/A",Results!J105:J154,"&lt;&gt;")</f>
+        <v>4</v>
       </c>
       <c r="H13" s="1">
-        <f>COUNTIFS(Results!K105:K151,"&lt;&gt;#N/A",Results!K105:K151,"&lt;&gt;")</f>
+        <f>COUNTIFS(Results!K105:K154,"&lt;&gt;#N/A",Results!K105:K154,"&lt;&gt;")</f>
         <v>0</v>
       </c>
       <c r="I13" s="1">
-        <f>COUNTIFS(Results!L105:L151,"&lt;&gt;#N/A",Results!L105:L151,"&lt;&gt;")</f>
+        <f>COUNTIFS(Results!L105:L154,"&lt;&gt;#N/A",Results!L105:L154,"&lt;&gt;")</f>
         <v>1</v>
       </c>
       <c r="J13" s="1">
-        <f>COUNTIFS(Results!M105:M151,"&lt;&gt;#N/A",Results!M105:M151,"&lt;&gt;")</f>
+        <f>COUNTIFS(Results!M105:M154,"&lt;&gt;#N/A",Results!M105:M154,"&lt;&gt;")</f>
         <v>0</v>
       </c>
       <c r="K13" s="1">
-        <f>COUNTIFS(Results!N105:N151,"&lt;&gt;#N/A",Results!N105:N151,"&lt;&gt;")</f>
+        <f>COUNTIFS(Results!N105:N154,"&lt;&gt;#N/A",Results!N105:N154,"&lt;&gt;")</f>
         <v>0</v>
       </c>
       <c r="L13" s="1">
-        <f>COUNTIFS(Results!O105:O151,"&lt;&gt;#N/A",Results!O105:O151,"&lt;&gt;")</f>
+        <f>COUNTIFS(Results!O105:O154,"&lt;&gt;#N/A",Results!O105:O154,"&lt;&gt;")</f>
         <v>0</v>
       </c>
       <c r="M13" s="1">
-        <f>COUNTIFS(Results!P105:P151,"&lt;&gt;#N/A",Results!P105:P151,"&lt;&gt;")</f>
+        <f>COUNTIFS(Results!P105:P154,"&lt;&gt;#N/A",Results!P105:P154,"&lt;&gt;")</f>
         <v>0</v>
       </c>
       <c r="N13" s="1">
-        <f>COUNTIFS(Results!Q105:Q151,"&lt;&gt;#N/A",Results!Q105:Q151,"&lt;&gt;")</f>
+        <f>COUNTIFS(Results!Q105:Q154,"&lt;&gt;#N/A",Results!Q105:Q154,"&lt;&gt;")</f>
         <v>0</v>
       </c>
       <c r="O13" s="1">
-        <f>COUNTIFS(Results!R105:R151,"&lt;&gt;#N/A",Results!R105:R151,"&lt;&gt;")</f>
+        <f>COUNTIFS(Results!R105:R154,"&lt;&gt;#N/A",Results!R105:R154,"&lt;&gt;")</f>
         <v>0</v>
       </c>
       <c r="P13" s="1">
-        <f>COUNTIFS(Results!S105:S151,"&lt;&gt;#N/A",Results!S105:S151,"&lt;&gt;")</f>
+        <f>COUNTIFS(Results!S105:S154,"&lt;&gt;#N/A",Results!S105:S154,"&lt;&gt;")</f>
         <v>0</v>
       </c>
       <c r="Q13" s="1">
         <f t="shared" si="0"/>
-        <v>174</v>
+        <v>192</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.35">
@@ -74514,68 +76240,68 @@
         <v>57</v>
       </c>
       <c r="B14" s="1">
-        <f>SUMIFS(Results!E105:E151,Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!E105:E151, "&lt;&gt;#N/A")</f>
-        <v>10</v>
+        <f>SUMIFS(Results!E105:E154,Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!E105:E154, "&lt;&gt;#N/A")</f>
+        <v>12</v>
       </c>
       <c r="C14" s="1">
-        <f>SUMIFS(Results!F105:F151,Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!F105:F151, "&lt;&gt;#N/A")</f>
-        <v>14</v>
+        <f>SUMIFS(Results!F105:F154,Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!F105:F154, "&lt;&gt;#N/A")</f>
+        <v>15</v>
       </c>
       <c r="D14" s="1">
-        <f>SUMIFS(Results!G105:G151,Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!G105:G151, "&lt;&gt;#N/A")</f>
-        <v>16</v>
+        <f>SUMIFS(Results!G105:G154,Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!G105:G154, "&lt;&gt;#N/A")</f>
+        <v>18</v>
       </c>
       <c r="E14" s="1">
-        <f>SUMIFS(Results!H105:H151,Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!H105:H151, "&lt;&gt;#N/A")</f>
-        <v>10</v>
+        <f>SUMIFS(Results!H105:H154,Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!H105:H154, "&lt;&gt;#N/A")</f>
+        <v>12</v>
       </c>
       <c r="F14" s="1">
-        <f>SUMIFS(Results!I105:I151,Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!I105:I151, "&lt;&gt;#N/A")</f>
+        <f>SUMIFS(Results!I105:I154,Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!I105:I154, "&lt;&gt;#N/A")</f>
         <v>2</v>
       </c>
       <c r="G14" s="1">
-        <f>SUMIFS(Results!J105:J151,Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!J105:J151, "&lt;&gt;#N/A")</f>
-        <v>0</v>
+        <f>SUMIFS(Results!J105:J154,Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!J105:J154, "&lt;&gt;#N/A")</f>
+        <v>1</v>
       </c>
       <c r="H14" s="1">
-        <f>SUMIFS(Results!K105:K151,Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!K105:K151, "&lt;&gt;#N/A")</f>
+        <f>SUMIFS(Results!K105:K154,Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!K105:K154, "&lt;&gt;#N/A")</f>
         <v>0</v>
       </c>
       <c r="I14" s="1">
-        <f>SUMIFS(Results!L105:L151,Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!L105:L151, "&lt;&gt;#N/A")</f>
+        <f>SUMIFS(Results!L105:L154,Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!L105:L154, "&lt;&gt;#N/A")</f>
         <v>1</v>
       </c>
       <c r="J14" s="1">
-        <f>SUMIFS(Results!M105:M151,Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!M105:M151, "&lt;&gt;#N/A")</f>
+        <f>SUMIFS(Results!M105:M154,Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!M105:M154, "&lt;&gt;#N/A")</f>
         <v>0</v>
       </c>
       <c r="K14" s="1">
-        <f>SUMIFS(Results!N105:N151,Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!N105:N151, "&lt;&gt;#N/A")</f>
+        <f>SUMIFS(Results!N105:N154,Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!N105:N154, "&lt;&gt;#N/A")</f>
         <v>0</v>
       </c>
       <c r="L14" s="1">
-        <f>SUMIFS(Results!O105:O151,Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!O105:O151, "&lt;&gt;#N/A")</f>
+        <f>SUMIFS(Results!O105:O154,Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!O105:O154, "&lt;&gt;#N/A")</f>
         <v>0</v>
       </c>
       <c r="M14" s="1">
-        <f>SUMIFS(Results!P105:P151,Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!P105:P151, "&lt;&gt;#N/A")</f>
+        <f>SUMIFS(Results!P105:P154,Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!P105:P154, "&lt;&gt;#N/A")</f>
         <v>0</v>
       </c>
       <c r="N14" s="1">
-        <f>SUMIFS(Results!Q105:Q151,Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!Q105:Q151, "&lt;&gt;#N/A")</f>
+        <f>SUMIFS(Results!Q105:Q154,Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!Q105:Q154, "&lt;&gt;#N/A")</f>
         <v>0</v>
       </c>
       <c r="O14" s="1">
-        <f>SUMIFS(Results!R105:R151,Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!R105:R151, "&lt;&gt;#N/A")</f>
+        <f>SUMIFS(Results!R105:R154,Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!R105:R154, "&lt;&gt;#N/A")</f>
         <v>0</v>
       </c>
       <c r="P14" s="1">
-        <f>SUMIFS(Results!S105:S151,Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!S105:S151, "&lt;&gt;#N/A")</f>
+        <f>SUMIFS(Results!S105:S154,Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!S105:S154, "&lt;&gt;#N/A")</f>
         <v>0</v>
       </c>
       <c r="Q14" s="1">
         <f t="shared" si="0"/>
-        <v>53</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.35">
@@ -74583,68 +76309,68 @@
         <v>58</v>
       </c>
       <c r="B15" s="1">
-        <f>COUNTIFS(Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!E105:E151, "&lt;&gt;#N/A", Results!E105:E151, "&lt;&gt;")</f>
-        <v>23</v>
+        <f>COUNTIFS(Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!E105:E154, "&lt;&gt;#N/A", Results!E105:E154, "&lt;&gt;")</f>
+        <v>27</v>
       </c>
       <c r="C15" s="1">
-        <f>COUNTIFS(Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!F105:F151, "&lt;&gt;#N/A", Results!F105:F151, "&lt;&gt;")</f>
-        <v>18</v>
+        <f>COUNTIFS(Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!F105:F154, "&lt;&gt;#N/A", Results!F105:F154, "&lt;&gt;")</f>
+        <v>21</v>
       </c>
       <c r="D15" s="1">
-        <f>COUNTIFS(Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!G105:G151, "&lt;&gt;#N/A", Results!G105:G151, "&lt;&gt;")</f>
-        <v>23</v>
+        <f>COUNTIFS(Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!G105:G154, "&lt;&gt;#N/A", Results!G105:G154, "&lt;&gt;")</f>
+        <v>27</v>
       </c>
       <c r="E15" s="1">
-        <f>COUNTIFS(Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!H105:H151, "&lt;&gt;#N/A", Results!H105:H151, "&lt;&gt;")</f>
-        <v>23</v>
+        <f>COUNTIFS(Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!H105:H154, "&lt;&gt;#N/A", Results!H105:H154, "&lt;&gt;")</f>
+        <v>27</v>
       </c>
       <c r="F15" s="1">
-        <f>COUNTIFS(Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!I105:I151, "&lt;&gt;#N/A", Results!I105:I151, "&lt;&gt;")</f>
-        <v>2</v>
+        <f>COUNTIFS(Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!I105:I154, "&lt;&gt;#N/A", Results!I105:I154, "&lt;&gt;")</f>
+        <v>3</v>
       </c>
       <c r="G15" s="1">
-        <f>COUNTIFS(Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!J105:J151, "&lt;&gt;#N/A", Results!J105:J151, "&lt;&gt;")</f>
-        <v>2</v>
+        <f>COUNTIFS(Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!J105:J154, "&lt;&gt;#N/A", Results!J105:J154, "&lt;&gt;")</f>
+        <v>4</v>
       </c>
       <c r="H15" s="1">
-        <f>COUNTIFS(Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!K105:K151, "&lt;&gt;#N/A", Results!K105:K151, "&lt;&gt;")</f>
+        <f>COUNTIFS(Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!K105:K154, "&lt;&gt;#N/A", Results!K105:K154, "&lt;&gt;")</f>
         <v>0</v>
       </c>
       <c r="I15" s="1">
-        <f>COUNTIFS(Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!L105:L151, "&lt;&gt;#N/A", Results!L105:L151, "&lt;&gt;")</f>
+        <f>COUNTIFS(Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!L105:L154, "&lt;&gt;#N/A", Results!L105:L154, "&lt;&gt;")</f>
         <v>1</v>
       </c>
       <c r="J15" s="1">
-        <f>COUNTIFS(Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!M105:M151, "&lt;&gt;#N/A", Results!M105:M151, "&lt;&gt;")</f>
+        <f>COUNTIFS(Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!M105:M154, "&lt;&gt;#N/A", Results!M105:M154, "&lt;&gt;")</f>
         <v>0</v>
       </c>
       <c r="K15" s="1">
-        <f>COUNTIFS(Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!N105:N151, "&lt;&gt;#N/A", Results!N105:N151, "&lt;&gt;")</f>
+        <f>COUNTIFS(Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!N105:N154, "&lt;&gt;#N/A", Results!N105:N154, "&lt;&gt;")</f>
         <v>0</v>
       </c>
       <c r="L15" s="1">
-        <f>COUNTIFS(Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!O105:O151, "&lt;&gt;#N/A", Results!O105:O151, "&lt;&gt;")</f>
+        <f>COUNTIFS(Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!O105:O154, "&lt;&gt;#N/A", Results!O105:O154, "&lt;&gt;")</f>
         <v>0</v>
       </c>
       <c r="M15" s="1">
-        <f>COUNTIFS(Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!P105:P151, "&lt;&gt;#N/A", Results!P105:P151, "&lt;&gt;")</f>
+        <f>COUNTIFS(Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!P105:P154, "&lt;&gt;#N/A", Results!P105:P154, "&lt;&gt;")</f>
         <v>0</v>
       </c>
       <c r="N15" s="1">
-        <f>COUNTIFS(Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!Q105:Q151, "&lt;&gt;#N/A", Results!Q105:Q151, "&lt;&gt;")</f>
+        <f>COUNTIFS(Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!Q105:Q154, "&lt;&gt;#N/A", Results!Q105:Q154, "&lt;&gt;")</f>
         <v>0</v>
       </c>
       <c r="O15" s="1">
-        <f>COUNTIFS(Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!R105:R151, "&lt;&gt;#N/A", Results!R105:R151, "&lt;&gt;")</f>
+        <f>COUNTIFS(Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!R105:R154, "&lt;&gt;#N/A", Results!R105:R154, "&lt;&gt;")</f>
         <v>0</v>
       </c>
       <c r="P15" s="1">
-        <f>COUNTIFS(Results!$B$105:$B$151,"&lt;&gt;#N/A",Results!S105:S151, "&lt;&gt;#N/A", Results!S105:S151, "&lt;&gt;")</f>
+        <f>COUNTIFS(Results!$B$105:$B$154,"&lt;&gt;#N/A",Results!S105:S154, "&lt;&gt;#N/A", Results!S105:S154, "&lt;&gt;")</f>
         <v>0</v>
       </c>
       <c r="Q15" s="1">
         <f t="shared" si="0"/>
-        <v>92</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.35">
@@ -74652,63 +76378,63 @@
         <v>59</v>
       </c>
       <c r="B16" s="1">
-        <f>SUMIFS(Results!E105:E151,Results!$B$105:$B$151,"=#N/A",Results!E105:E151, "&lt;&gt;#N/A")</f>
+        <f>SUMIFS(Results!E105:E154,Results!$B$105:$B$154,"=#N/A",Results!E105:E154, "&lt;&gt;#N/A")</f>
         <v>11</v>
       </c>
       <c r="C16" s="1">
-        <f>SUMIFS(Results!F105:F151,Results!$B$105:$B$151,"=#N/A",Results!F105:F151, "&lt;&gt;#N/A")</f>
+        <f>SUMIFS(Results!F105:F154,Results!$B$105:$B$154,"=#N/A",Results!F105:F154, "&lt;&gt;#N/A")</f>
         <v>12</v>
       </c>
       <c r="D16" s="1">
-        <f>SUMIFS(Results!G105:G151,Results!$B$105:$B$151,"=#N/A",Results!G105:G151, "&lt;&gt;#N/A")</f>
+        <f>SUMIFS(Results!G105:G154,Results!$B$105:$B$154,"=#N/A",Results!G105:G154, "&lt;&gt;#N/A")</f>
         <v>12</v>
       </c>
       <c r="E16" s="1">
-        <f>SUMIFS(Results!H105:H151,Results!$B$105:$B$151,"=#N/A",Results!H105:H151, "&lt;&gt;#N/A")</f>
+        <f>SUMIFS(Results!H105:H154,Results!$B$105:$B$154,"=#N/A",Results!H105:H154, "&lt;&gt;#N/A")</f>
         <v>13</v>
       </c>
       <c r="F16" s="1">
-        <f>SUMIFS(Results!I105:I151,Results!$B$105:$B$151,"=#N/A",Results!I105:I151, "&lt;&gt;#N/A")</f>
+        <f>SUMIFS(Results!I105:I154,Results!$B$105:$B$154,"=#N/A",Results!I105:I154, "&lt;&gt;#N/A")</f>
         <v>0</v>
       </c>
       <c r="G16" s="1">
-        <f>SUMIFS(Results!J105:J151,Results!$B$105:$B$151,"=#N/A",Results!J105:J151, "&lt;&gt;#N/A")</f>
+        <f>SUMIFS(Results!J105:J154,Results!$B$105:$B$154,"=#N/A",Results!J105:J154, "&lt;&gt;#N/A")</f>
         <v>0</v>
       </c>
       <c r="H16" s="1">
-        <f>SUMIFS(Results!K105:K151,Results!$B$105:$B$151,"=#N/A",Results!K105:K151, "&lt;&gt;#N/A")</f>
+        <f>SUMIFS(Results!K105:K154,Results!$B$105:$B$154,"=#N/A",Results!K105:K154, "&lt;&gt;#N/A")</f>
         <v>0</v>
       </c>
       <c r="I16" s="1">
-        <f>SUMIFS(Results!L105:L151,Results!$B$105:$B$151,"=#N/A",Results!L105:L151, "&lt;&gt;#N/A")</f>
+        <f>SUMIFS(Results!L105:L154,Results!$B$105:$B$154,"=#N/A",Results!L105:L154, "&lt;&gt;#N/A")</f>
         <v>0</v>
       </c>
       <c r="J16" s="1">
-        <f>SUMIFS(Results!M105:M151,Results!$B$105:$B$151,"=#N/A",Results!M105:M151, "&lt;&gt;#N/A")</f>
+        <f>SUMIFS(Results!M105:M154,Results!$B$105:$B$154,"=#N/A",Results!M105:M154, "&lt;&gt;#N/A")</f>
         <v>0</v>
       </c>
       <c r="K16" s="1">
-        <f>SUMIFS(Results!N105:N151,Results!$B$105:$B$151,"=#N/A",Results!N105:N151, "&lt;&gt;#N/A")</f>
+        <f>SUMIFS(Results!N105:N154,Results!$B$105:$B$154,"=#N/A",Results!N105:N154, "&lt;&gt;#N/A")</f>
         <v>0</v>
       </c>
       <c r="L16" s="1">
-        <f>SUMIFS(Results!O105:O151,Results!$B$105:$B$151,"=#N/A",Results!O105:O151, "&lt;&gt;#N/A")</f>
+        <f>SUMIFS(Results!O105:O154,Results!$B$105:$B$154,"=#N/A",Results!O105:O154, "&lt;&gt;#N/A")</f>
         <v>0</v>
       </c>
       <c r="M16" s="1">
-        <f>SUMIFS(Results!P105:P151,Results!$B$105:$B$151,"=#N/A",Results!P105:P151, "&lt;&gt;#N/A")</f>
+        <f>SUMIFS(Results!P105:P154,Results!$B$105:$B$154,"=#N/A",Results!P105:P154, "&lt;&gt;#N/A")</f>
         <v>0</v>
       </c>
       <c r="N16" s="1">
-        <f>SUMIFS(Results!Q105:Q151,Results!$B$105:$B$151,"=#N/A",Results!Q105:Q151, "&lt;&gt;#N/A")</f>
+        <f>SUMIFS(Results!Q105:Q154,Results!$B$105:$B$154,"=#N/A",Results!Q105:Q154, "&lt;&gt;#N/A")</f>
         <v>0</v>
       </c>
       <c r="O16" s="1">
-        <f>SUMIFS(Results!R105:R151,Results!$B$105:$B$151,"=#N/A",Results!R105:R151, "&lt;&gt;#N/A")</f>
+        <f>SUMIFS(Results!R105:R154,Results!$B$105:$B$154,"=#N/A",Results!R105:R154, "&lt;&gt;#N/A")</f>
         <v>0</v>
       </c>
       <c r="P16" s="1">
-        <f>SUMIFS(Results!S105:S151,Results!$B$105:$B$151,"=#N/A",Results!S105:S151, "&lt;&gt;#N/A")</f>
+        <f>SUMIFS(Results!S105:S154,Results!$B$105:$B$154,"=#N/A",Results!S105:S154, "&lt;&gt;#N/A")</f>
         <v>0</v>
       </c>
       <c r="Q16" s="1">
@@ -74721,63 +76447,63 @@
         <v>60</v>
       </c>
       <c r="B17" s="1">
-        <f>COUNTIFS(Results!$B$105:$B$151,"=#N/A",Results!E105:E151, "&lt;&gt;#N/A", Results!E105:E151, "&lt;&gt;")</f>
+        <f>COUNTIFS(Results!$B$105:$B$154,"=#N/A",Results!E105:E154, "&lt;&gt;#N/A", Results!E105:E154, "&lt;&gt;")</f>
         <v>22</v>
       </c>
       <c r="C17" s="1">
-        <f>COUNTIFS(Results!$B$105:$B$151,"=#N/A",Results!F105:F151, "&lt;&gt;#N/A", Results!F105:F151, "&lt;&gt;")</f>
+        <f>COUNTIFS(Results!$B$105:$B$154,"=#N/A",Results!F105:F154, "&lt;&gt;#N/A", Results!F105:F154, "&lt;&gt;")</f>
         <v>18</v>
       </c>
       <c r="D17" s="1">
-        <f>COUNTIFS(Results!$B$105:$B$151,"=#N/A",Results!G105:G151, "&lt;&gt;#N/A", Results!G105:G151, "&lt;&gt;")</f>
+        <f>COUNTIFS(Results!$B$105:$B$154,"=#N/A",Results!G105:G154, "&lt;&gt;#N/A", Results!G105:G154, "&lt;&gt;")</f>
         <v>22</v>
       </c>
       <c r="E17" s="1">
-        <f>COUNTIFS(Results!$B$105:$B$151,"=#N/A",Results!H105:H151, "&lt;&gt;#N/A", Results!H105:H151, "&lt;&gt;")</f>
+        <f>COUNTIFS(Results!$B$105:$B$154,"=#N/A",Results!H105:H154, "&lt;&gt;#N/A", Results!H105:H154, "&lt;&gt;")</f>
         <v>20</v>
       </c>
       <c r="F17" s="1">
-        <f>COUNTIFS(Results!$B$105:$B$151,"=#N/A",Results!I105:I151, "&lt;&gt;#N/A", Results!I105:I151, "&lt;&gt;")</f>
+        <f>COUNTIFS(Results!$B$105:$B$154,"=#N/A",Results!I105:I154, "&lt;&gt;#N/A", Results!I105:I154, "&lt;&gt;")</f>
         <v>0</v>
       </c>
       <c r="G17" s="1">
-        <f>COUNTIFS(Results!$B$105:$B$151,"=#N/A",Results!J105:J151, "&lt;&gt;#N/A", Results!J105:J151, "&lt;&gt;")</f>
+        <f>COUNTIFS(Results!$B$105:$B$154,"=#N/A",Results!J105:J154, "&lt;&gt;#N/A", Results!J105:J154, "&lt;&gt;")</f>
         <v>0</v>
       </c>
       <c r="H17" s="1">
-        <f>COUNTIFS(Results!$B$105:$B$151,"=#N/A",Results!K105:K151, "&lt;&gt;#N/A", Results!K105:K151, "&lt;&gt;")</f>
+        <f>COUNTIFS(Results!$B$105:$B$154,"=#N/A",Results!K105:K154, "&lt;&gt;#N/A", Results!K105:K154, "&lt;&gt;")</f>
         <v>0</v>
       </c>
       <c r="I17" s="1">
-        <f>COUNTIFS(Results!$B$105:$B$151,"=#N/A",Results!L105:L151, "&lt;&gt;#N/A", Results!L105:L151, "&lt;&gt;")</f>
+        <f>COUNTIFS(Results!$B$105:$B$154,"=#N/A",Results!L105:L154, "&lt;&gt;#N/A", Results!L105:L154, "&lt;&gt;")</f>
         <v>0</v>
       </c>
       <c r="J17" s="1">
-        <f>COUNTIFS(Results!$B$105:$B$151,"=#N/A",Results!M105:M151, "&lt;&gt;#N/A", Results!M105:M151, "&lt;&gt;")</f>
+        <f>COUNTIFS(Results!$B$105:$B$154,"=#N/A",Results!M105:M154, "&lt;&gt;#N/A", Results!M105:M154, "&lt;&gt;")</f>
         <v>0</v>
       </c>
       <c r="K17" s="1">
-        <f>COUNTIFS(Results!$B$105:$B$151,"=#N/A",Results!N105:N151, "&lt;&gt;#N/A", Results!N105:N151, "&lt;&gt;")</f>
+        <f>COUNTIFS(Results!$B$105:$B$154,"=#N/A",Results!N105:N154, "&lt;&gt;#N/A", Results!N105:N154, "&lt;&gt;")</f>
         <v>0</v>
       </c>
       <c r="L17" s="1">
-        <f>COUNTIFS(Results!$B$105:$B$151,"=#N/A",Results!O105:O151, "&lt;&gt;#N/A", Results!O105:O151, "&lt;&gt;")</f>
+        <f>COUNTIFS(Results!$B$105:$B$154,"=#N/A",Results!O105:O154, "&lt;&gt;#N/A", Results!O105:O154, "&lt;&gt;")</f>
         <v>0</v>
       </c>
       <c r="M17" s="1">
-        <f>COUNTIFS(Results!$B$105:$B$151,"=#N/A",Results!P105:P151, "&lt;&gt;#N/A", Results!P105:P151, "&lt;&gt;")</f>
+        <f>COUNTIFS(Results!$B$105:$B$154,"=#N/A",Results!P105:P154, "&lt;&gt;#N/A", Results!P105:P154, "&lt;&gt;")</f>
         <v>0</v>
       </c>
       <c r="N17" s="1">
-        <f>COUNTIFS(Results!$B$105:$B$151,"=#N/A",Results!Q105:Q151, "&lt;&gt;#N/A", Results!Q105:Q151, "&lt;&gt;")</f>
+        <f>COUNTIFS(Results!$B$105:$B$154,"=#N/A",Results!Q105:Q154, "&lt;&gt;#N/A", Results!Q105:Q154, "&lt;&gt;")</f>
         <v>0</v>
       </c>
       <c r="O17" s="1">
-        <f>COUNTIFS(Results!$B$105:$B$151,"=#N/A",Results!R105:R151, "&lt;&gt;#N/A", Results!R105:R151, "&lt;&gt;")</f>
+        <f>COUNTIFS(Results!$B$105:$B$154,"=#N/A",Results!R105:R154, "&lt;&gt;#N/A", Results!R105:R154, "&lt;&gt;")</f>
         <v>0</v>
       </c>
       <c r="P17" s="1">
-        <f>COUNTIFS(Results!$B$105:$B$151,"=#N/A",Results!S105:S151, "&lt;&gt;#N/A", Results!S105:S151, "&lt;&gt;")</f>
+        <f>COUNTIFS(Results!$B$105:$B$154,"=#N/A",Results!S105:S154, "&lt;&gt;#N/A", Results!S105:S154, "&lt;&gt;")</f>
         <v>0</v>
       </c>
       <c r="Q17" s="1">
@@ -74790,68 +76516,68 @@
         <v>74</v>
       </c>
       <c r="B18" s="1">
-        <f>SUMIF(Results!$C$105:$C$151,'Summary 2019'!B1,Results!$X$105:$X$151)</f>
+        <f>SUMIF(Results!$C$105:$C$154,'Summary 2019'!B1,Results!$X$105:$X$154)</f>
         <v>0</v>
       </c>
       <c r="C18" s="1">
-        <f>SUMIF(Results!$C$105:$C$151,'Summary 2019'!C1,Results!$X$105:$X$151)</f>
+        <f>SUMIF(Results!$C$105:$C$154,'Summary 2019'!C1,Results!$X$105:$X$154)</f>
         <v>0</v>
       </c>
       <c r="D18" s="1">
-        <f>SUMIF(Results!$C$105:$C$151,'Summary 2019'!D1,Results!$X$105:$X$151)</f>
+        <f>SUMIF(Results!$C$105:$C$154,'Summary 2019'!D1,Results!$X$105:$X$154)</f>
         <v>0</v>
       </c>
       <c r="E18" s="1">
-        <f>SUMIF(Results!$C$105:$C$151,'Summary 2019'!E1,Results!$X$105:$X$151)</f>
+        <f>SUMIF(Results!$C$105:$C$154,'Summary 2019'!E1,Results!$X$105:$X$154)</f>
         <v>0</v>
       </c>
       <c r="F18" s="1">
-        <f>SUMIF(Results!$C$105:$C$151,'Summary 2019'!F1,Results!$X$105:$X$151)</f>
+        <f>SUMIF(Results!$C$105:$C$154,'Summary 2019'!F1,Results!$X$105:$X$154)</f>
         <v>0</v>
       </c>
       <c r="G18" s="1">
-        <f>SUMIF(Results!$C$105:$C$151,'Summary 2019'!G1,Results!$X$105:$X$151)</f>
+        <f>SUMIF(Results!$C$105:$C$154,'Summary 2019'!G1,Results!$X$105:$X$154)</f>
         <v>4</v>
       </c>
       <c r="H18" s="1">
-        <f>SUMIF(Results!$C$105:$C$151,'Summary 2019'!H1,Results!$X$105:$X$151)</f>
+        <f>SUMIF(Results!$C$105:$C$154,'Summary 2019'!H1,Results!$X$105:$X$154)</f>
         <v>0</v>
       </c>
       <c r="I18" s="1">
-        <f>SUMIF(Results!$C$105:$C$151,'Summary 2019'!I1,Results!$X$105:$X$151)</f>
+        <f>SUMIF(Results!$C$105:$C$154,'Summary 2019'!I1,Results!$X$105:$X$154)</f>
         <v>0</v>
       </c>
       <c r="J18" s="1">
-        <f>SUMIF(Results!$C$105:$C$151,'Summary 2019'!J1,Results!$X$105:$X$151)</f>
+        <f>SUMIF(Results!$C$105:$C$154,'Summary 2019'!J1,Results!$X$105:$X$154)</f>
         <v>0</v>
       </c>
       <c r="K18" s="1">
-        <f>SUMIF(Results!$C$105:$C$151,'Summary 2019'!K1,Results!$X$105:$X$151)</f>
+        <f>SUMIF(Results!$C$105:$C$154,'Summary 2019'!K1,Results!$X$105:$X$154)</f>
         <v>0</v>
       </c>
       <c r="L18" s="1">
-        <f>SUMIF(Results!$C$105:$C$151,'Summary 2019'!L1,Results!$X$105:$X$151)</f>
+        <f>SUMIF(Results!$C$105:$C$154,'Summary 2019'!L1,Results!$X$105:$X$154)</f>
         <v>0</v>
       </c>
       <c r="M18" s="1">
-        <f>SUMIF(Results!$C$105:$C$151,'Summary 2019'!M1,Results!$X$105:$X$151)</f>
+        <f>SUMIF(Results!$C$105:$C$154,'Summary 2019'!M1,Results!$X$105:$X$154)</f>
         <v>0</v>
       </c>
       <c r="N18" s="1">
-        <f>SUMIF(Results!$C$105:$C$151,'Summary 2019'!N1,Results!$X$105:$X$151)</f>
+        <f>SUMIF(Results!$C$105:$C$154,'Summary 2019'!N1,Results!$X$105:$X$154)</f>
         <v>0</v>
       </c>
       <c r="O18" s="1">
-        <f>SUMIF(Results!$C$105:$C$151,'Summary 2019'!O1,Results!$X$105:$X$151)</f>
+        <f>SUMIF(Results!$C$105:$C$154,'Summary 2019'!O1,Results!$X$105:$X$154)</f>
         <v>0</v>
       </c>
       <c r="P18" s="1">
-        <f>SUMIF(Results!$C$105:$C$151,'Summary 2019'!P1,Results!$X$105:$X$151)</f>
+        <f>SUMIF(Results!$C$105:$C$154,'Summary 2019'!P1,Results!$X$105:$X$154)</f>
         <v>0</v>
       </c>
       <c r="Q18" s="18">
-        <f>SUM(Results!X105:X151)</f>
-        <v>4</v>
+        <f>SUM(Results!X105:X154)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.35">
@@ -74859,68 +76585,68 @@
         <v>75</v>
       </c>
       <c r="B19" s="1">
-        <f>SUMIF(Results!E105:E151,"&lt;&gt;#N/A",Results!$Y$105:$Y$151)</f>
+        <f>SUMIF(Results!E105:E154,"&lt;&gt;#N/A",Results!$Y$105:$Y$154)</f>
+        <v>9</v>
+      </c>
+      <c r="C19" s="1">
+        <f>SUMIF(Results!F105:F154,"&lt;&gt;#N/A",Results!$Y$105:$Y$154)</f>
         <v>8</v>
       </c>
-      <c r="C19" s="1">
-        <f>SUMIF(Results!F105:F151,"&lt;&gt;#N/A",Results!$Y$105:$Y$151)</f>
-        <v>7</v>
-      </c>
       <c r="D19" s="1">
-        <f>SUMIF(Results!G105:G151,"&lt;&gt;#N/A",Results!$Y$105:$Y$151)</f>
+        <f>SUMIF(Results!G105:G154,"&lt;&gt;#N/A",Results!$Y$105:$Y$154)</f>
+        <v>9</v>
+      </c>
+      <c r="E19" s="1">
+        <f>SUMIF(Results!H105:H154,"&lt;&gt;#N/A",Results!$Y$105:$Y$154)</f>
         <v>8</v>
       </c>
-      <c r="E19" s="1">
-        <f>SUMIF(Results!H105:H151,"&lt;&gt;#N/A",Results!$Y$105:$Y$151)</f>
-        <v>7</v>
-      </c>
       <c r="F19" s="1">
-        <f>SUMIF(Results!I105:I151,"&lt;&gt;#N/A",Results!$Y$105:$Y$151)</f>
+        <f>SUMIF(Results!I105:I154,"&lt;&gt;#N/A",Results!$Y$105:$Y$154)</f>
         <v>1</v>
       </c>
       <c r="G19" s="1">
-        <f>SUMIF(Results!J105:J151,"&lt;&gt;#N/A",Results!$Y$105:$Y$151)</f>
+        <f>SUMIF(Results!J105:J154,"&lt;&gt;#N/A",Results!$Y$105:$Y$154)</f>
         <v>0</v>
       </c>
       <c r="H19" s="1">
-        <f>SUMIF(Results!K105:K151,"&lt;&gt;#N/A",Results!$Y$105:$Y$151)</f>
+        <f>SUMIF(Results!K105:K154,"&lt;&gt;#N/A",Results!$Y$105:$Y$154)</f>
         <v>0</v>
       </c>
       <c r="I19" s="1">
-        <f>SUMIF(Results!L105:L151,"&lt;&gt;#N/A",Results!$Y$105:$Y$151)</f>
+        <f>SUMIF(Results!L105:L154,"&lt;&gt;#N/A",Results!$Y$105:$Y$154)</f>
         <v>0</v>
       </c>
       <c r="J19" s="1">
-        <f>SUMIF(Results!M105:M151,"&lt;&gt;#N/A",Results!$Y$105:$Y$151)</f>
+        <f>SUMIF(Results!M105:M154,"&lt;&gt;#N/A",Results!$Y$105:$Y$154)</f>
         <v>0</v>
       </c>
       <c r="K19" s="1">
-        <f>SUMIF(Results!N105:N151,"&lt;&gt;#N/A",Results!$Y$105:$Y$151)</f>
+        <f>SUMIF(Results!N105:N154,"&lt;&gt;#N/A",Results!$Y$105:$Y$154)</f>
         <v>0</v>
       </c>
       <c r="L19" s="1">
-        <f>SUMIF(Results!O105:O151,"&lt;&gt;#N/A",Results!$Y$105:$Y$151)</f>
+        <f>SUMIF(Results!O105:O154,"&lt;&gt;#N/A",Results!$Y$105:$Y$154)</f>
         <v>0</v>
       </c>
       <c r="M19" s="1">
-        <f>SUMIF(Results!P105:P151,"&lt;&gt;#N/A",Results!$Y$105:$Y$151)</f>
+        <f>SUMIF(Results!P105:P154,"&lt;&gt;#N/A",Results!$Y$105:$Y$154)</f>
         <v>0</v>
       </c>
       <c r="N19" s="1">
-        <f>SUMIF(Results!Q105:Q151,"&lt;&gt;#N/A",Results!$Y$105:$Y$151)</f>
+        <f>SUMIF(Results!Q105:Q154,"&lt;&gt;#N/A",Results!$Y$105:$Y$154)</f>
         <v>0</v>
       </c>
       <c r="O19" s="1">
-        <f>SUMIF(Results!R105:R151,"&lt;&gt;#N/A",Results!$Y$105:$Y$151)</f>
+        <f>SUMIF(Results!R105:R154,"&lt;&gt;#N/A",Results!$Y$105:$Y$154)</f>
         <v>0</v>
       </c>
       <c r="P19" s="1">
-        <f>SUMIF(Results!S105:S151,"&lt;&gt;#N/A",Results!$Y$105:$Y$151)</f>
+        <f>SUMIF(Results!S105:S154,"&lt;&gt;#N/A",Results!$Y$105:$Y$154)</f>
         <v>0</v>
       </c>
       <c r="Q19" s="18">
-        <f>SUM(Results!Y105:Y151)</f>
-        <v>8</v>
+        <f>SUM(Results!Y105:Y154)</f>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated through episode 755
</commit_message>
<xml_diff>
--- a/SGU_Science_or_Fiction.xlsx
+++ b/SGU_Science_or_Fiction.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xwhx\SourceControl\SGU_Science_or_Fiction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121B8629-ED15-496F-B5A5-874BB743E718}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DA9A25-2A58-4C65-89E8-5A479E45FD52}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="317">
   <si>
     <t>Episode</t>
   </si>
@@ -13327,11 +13327,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z153"/>
+  <dimension ref="A1:Z154"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A135" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I153" sqref="I153:Z153"/>
+      <pane ySplit="1" topLeftCell="A136" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I154" sqref="I154:Z154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -25046,7 +25046,7 @@
         <v>#N/A</v>
       </c>
       <c r="Z131" s="22" t="e">
-        <f t="shared" ref="Z131:Z153" si="24">INDEX(AnsLkUp,MATCH($A131 &amp; "_"&amp;Z$1,LookupName,0),3)</f>
+        <f t="shared" ref="Z131:Z154" si="24">INDEX(AnsLkUp,MATCH($A131 &amp; "_"&amp;Z$1,LookupName,0),3)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -26425,7 +26425,7 @@
         <v>#N/A</v>
       </c>
       <c r="Y147" s="22" t="e">
-        <f t="shared" ref="J147:Y153" si="29">INDEX(AnsLkUp,MATCH($A147 &amp; "_"&amp;Y$1,LookupName,0),3)</f>
+        <f t="shared" ref="J147:Y154" si="29">INDEX(AnsLkUp,MATCH($A147 &amp; "_"&amp;Y$1,LookupName,0),3)</f>
         <v>#N/A</v>
       </c>
       <c r="Z147" s="22" t="e">
@@ -26946,6 +26946,92 @@
         <v>#N/A</v>
       </c>
       <c r="Z153" s="22" t="e">
+        <f t="shared" si="24"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="154" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A154">
+        <v>755</v>
+      </c>
+      <c r="B154">
+        <v>2019</v>
+      </c>
+      <c r="G154" s="1">
+        <v>3</v>
+      </c>
+      <c r="H154" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I154" s="22" t="str">
+        <f t="shared" ref="I154" si="32">INDEX(AnsLkUp,MATCH(A154 &amp; "_1",LookupOrder,1),2)</f>
+        <v>Cara</v>
+      </c>
+      <c r="J154" s="22">
+        <f t="shared" si="29"/>
+        <v>3</v>
+      </c>
+      <c r="K154" s="22">
+        <f t="shared" si="29"/>
+        <v>3</v>
+      </c>
+      <c r="L154" s="22">
+        <f t="shared" si="29"/>
+        <v>2</v>
+      </c>
+      <c r="M154" s="22">
+        <f t="shared" si="29"/>
+        <v>3</v>
+      </c>
+      <c r="N154" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="O154" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P154" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q154" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R154" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S154" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T154" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U154" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="V154" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="W154" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X154" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y154" s="22" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Z154" s="22" t="e">
         <f t="shared" si="24"/>
         <v>#N/A</v>
       </c>
@@ -26959,11 +27045,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F399"/>
+  <dimension ref="A1:F403"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A381" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F397" sqref="F397:F399"/>
+      <pane ySplit="1" topLeftCell="A385" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D404" sqref="D404"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -34334,7 +34420,7 @@
         <v>1</v>
       </c>
       <c r="E335" s="23" t="str">
-        <f t="shared" ref="E335:E399" si="20">A335 &amp; "_" &amp; D335</f>
+        <f t="shared" ref="E335:E403" si="20">A335 &amp; "_" &amp; D335</f>
         <v>739_1</v>
       </c>
       <c r="F335" s="23" t="str">
@@ -35746,8 +35832,96 @@
         <v>754_4</v>
       </c>
       <c r="F399" s="23" t="str">
-        <f t="shared" ref="F399" si="22">A399 &amp; "_" &amp; B399</f>
+        <f t="shared" ref="F399:F403" si="22">A399 &amp; "_" &amp; B399</f>
         <v>754_Cara</v>
+      </c>
+    </row>
+    <row r="400" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A400">
+        <v>755</v>
+      </c>
+      <c r="B400" t="s">
+        <v>23</v>
+      </c>
+      <c r="C400" s="1">
+        <v>3</v>
+      </c>
+      <c r="D400" s="1">
+        <v>1</v>
+      </c>
+      <c r="E400" s="23" t="str">
+        <f t="shared" si="20"/>
+        <v>755_1</v>
+      </c>
+      <c r="F400" s="23" t="str">
+        <f t="shared" si="22"/>
+        <v>755_Cara</v>
+      </c>
+    </row>
+    <row r="401" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A401">
+        <v>755</v>
+      </c>
+      <c r="B401" t="s">
+        <v>6</v>
+      </c>
+      <c r="C401" s="1">
+        <v>2</v>
+      </c>
+      <c r="D401" s="1">
+        <v>2</v>
+      </c>
+      <c r="E401" s="23" t="str">
+        <f t="shared" si="20"/>
+        <v>755_2</v>
+      </c>
+      <c r="F401" s="23" t="str">
+        <f t="shared" si="22"/>
+        <v>755_Jay</v>
+      </c>
+    </row>
+    <row r="402" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A402">
+        <v>755</v>
+      </c>
+      <c r="B402" t="s">
+        <v>7</v>
+      </c>
+      <c r="C402" s="1">
+        <v>3</v>
+      </c>
+      <c r="D402" s="1">
+        <v>3</v>
+      </c>
+      <c r="E402" s="23" t="str">
+        <f t="shared" si="20"/>
+        <v>755_3</v>
+      </c>
+      <c r="F402" s="23" t="str">
+        <f t="shared" si="22"/>
+        <v>755_Evan</v>
+      </c>
+    </row>
+    <row r="403" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A403">
+        <v>755</v>
+      </c>
+      <c r="B403" t="s">
+        <v>5</v>
+      </c>
+      <c r="C403" s="1">
+        <v>3</v>
+      </c>
+      <c r="D403" s="1">
+        <v>4</v>
+      </c>
+      <c r="E403" s="23" t="str">
+        <f t="shared" si="20"/>
+        <v>755_4</v>
+      </c>
+      <c r="F403" s="23" t="str">
+        <f t="shared" si="22"/>
+        <v>755_Bob</v>
       </c>
     </row>
   </sheetData>
@@ -35759,13 +35933,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:BH154"/>
+  <dimension ref="A1:BH155"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B136" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B137" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A154" sqref="A154:XFD154"/>
+      <selection pane="bottomRight" activeCell="A155" sqref="A155:XFD155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -72817,6 +72991,248 @@
       </c>
       <c r="BH154" s="9">
         <f t="shared" ref="BH154" si="861">IF(ISNA(U154),BH153,IF(U154=0,BH153+1,0))</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="155" spans="1:60" x14ac:dyDescent="0.35">
+      <c r="A155" s="24">
+        <f>Data!A154</f>
+        <v>755</v>
+      </c>
+      <c r="B155" s="26">
+        <f>Data!B154</f>
+        <v>2019</v>
+      </c>
+      <c r="C155" s="27" t="str">
+        <f>Data!H154</f>
+        <v>Steve</v>
+      </c>
+      <c r="D155" s="25" t="str">
+        <f>Data!I154</f>
+        <v>Cara</v>
+      </c>
+      <c r="E155" s="22">
+        <f>IF(Data!J154=Data!$G154,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F155" s="22">
+        <f>IF(Data!K154=Data!$G154,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="G155" s="22">
+        <f>IF(Data!L154=Data!$G154,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H155" s="22">
+        <f>IF(Data!M154=Data!$G154,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="I155" s="22" t="e">
+        <f>IF(Data!N154=Data!$G154,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J155" s="22" t="e">
+        <f>IF(Data!O154=Data!$G154,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K155" s="22" t="e">
+        <f>IF(Data!P154=Data!$G154,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="L155" s="22" t="e">
+        <f>IF(Data!Q154=Data!$G154,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M155" s="22" t="e">
+        <f>IF(Data!R154=Data!$G154,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N155" s="22" t="e">
+        <f>IF(Data!S154=Data!$G154,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O155" s="22" t="e">
+        <f>IF(Data!T154=Data!$G154,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P155" s="22" t="e">
+        <f>IF(Data!U154=Data!$G154,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q155" s="22" t="e">
+        <f>IF(Data!V154=Data!$G154,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R155" s="22" t="e">
+        <f>IF(Data!W154=Data!$G154,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="S155" s="22" t="e">
+        <f>IF(Data!X154=Data!$G154,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="T155" s="22" t="e">
+        <f>IF(Data!Y154=Data!$G154,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="U155" s="22" t="e">
+        <f>IF(Data!Z154=Data!$G154,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="V155" s="22">
+        <f t="shared" ref="V155" si="862">COUNTIF(E155:U155,"&lt;&gt;#N/A")</f>
+        <v>4</v>
+      </c>
+      <c r="W155" s="22">
+        <f t="shared" ref="W155" si="863">SUMIF(E155:U155,"&lt;&gt;#N/A")</f>
+        <v>3</v>
+      </c>
+      <c r="X155" s="22">
+        <f t="shared" ref="X155" si="864">IF(W155=0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y155" s="22">
+        <f t="shared" ref="Y155" si="865">IF(V155=W155,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z155" s="22" t="e">
+        <f t="shared" ref="Z155" si="866">IF(W155=1,INDEX($E$2:$U$2,1,MATCH(1,E155:U155,0)),NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AA155" s="7">
+        <f t="shared" ref="AA155" si="867">IF(ISNA(E155),AA154,IF(E155=1,AA154+1,0))</f>
+        <v>3</v>
+      </c>
+      <c r="AB155" s="7">
+        <f t="shared" ref="AB155" si="868">IF(ISNA(F155),AB154,IF(F155=1,AB154+1,0))</f>
+        <v>2</v>
+      </c>
+      <c r="AC155" s="7">
+        <f t="shared" ref="AC155" si="869">IF(ISNA(G155),AC154,IF(G155=1,AC154+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AD155" s="7">
+        <f t="shared" ref="AD155" si="870">IF(ISNA(H155),AD154,IF(H155=1,AD154+1,0))</f>
+        <v>2</v>
+      </c>
+      <c r="AE155" s="7">
+        <f t="shared" ref="AE155" si="871">IF(ISNA(I155),AE154,IF(I155=1,AE154+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AF155" s="7">
+        <f t="shared" ref="AF155" si="872">IF(ISNA(J155),AF154,IF(J155=1,AF154+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AG155" s="7">
+        <f t="shared" ref="AG155" si="873">IF(ISNA(K155),AG154,IF(K155=1,AG154+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AH155" s="7">
+        <f t="shared" ref="AH155" si="874">IF(ISNA(L155),AH154,IF(L155=1,AH154+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AI155" s="7">
+        <f t="shared" ref="AI155" si="875">IF(ISNA(M155),AI154,IF(M155=1,AI154+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AJ155" s="7">
+        <f t="shared" ref="AJ155" si="876">IF(ISNA(N155),AJ154,IF(N155=1,AJ154+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AK155" s="7">
+        <f t="shared" ref="AK155" si="877">IF(ISNA(O155),AK154,IF(O155=1,AK154+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AL155" s="7">
+        <f t="shared" ref="AL155" si="878">IF(ISNA(P155),AL154,IF(P155=1,AL154+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AM155" s="7">
+        <f t="shared" ref="AM155" si="879">IF(ISNA(Q155),AM154,IF(Q155=1,AM154+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AN155" s="7">
+        <f t="shared" ref="AN155" si="880">IF(ISNA(R155),AN154,IF(R155=1,AN154+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AO155" s="7">
+        <f t="shared" ref="AO155" si="881">IF(ISNA(S155),AO154,IF(S155=1,AO154+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AP155" s="7">
+        <f t="shared" ref="AP155" si="882">IF(ISNA(T155),AP154,IF(T155=1,AP154+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AQ155" s="7">
+        <f t="shared" ref="AQ155" si="883">IF(ISNA(U155),AQ154,IF(U155=1,AQ154+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AR155" s="9">
+        <f t="shared" ref="AR155" si="884">IF(ISNA(E155),AR154,IF(E155=0,AR154+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AS155" s="9">
+        <f t="shared" ref="AS155" si="885">IF(ISNA(F155),AS154,IF(F155=0,AS154+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AT155" s="9">
+        <f t="shared" ref="AT155" si="886">IF(ISNA(G155),AT154,IF(G155=0,AT154+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AU155" s="9">
+        <f t="shared" ref="AU155" si="887">IF(ISNA(H155),AU154,IF(H155=0,AU154+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AV155" s="9">
+        <f t="shared" ref="AV155" si="888">IF(ISNA(I155),AV154,IF(I155=0,AV154+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AW155" s="9">
+        <f t="shared" ref="AW155" si="889">IF(ISNA(J155),AW154,IF(J155=0,AW154+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AX155" s="9">
+        <f t="shared" ref="AX155" si="890">IF(ISNA(K155),AX154,IF(K155=0,AX154+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AY155" s="9">
+        <f t="shared" ref="AY155" si="891">IF(ISNA(L155),AY154,IF(L155=0,AY154+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AZ155" s="9">
+        <f t="shared" ref="AZ155" si="892">IF(ISNA(M155),AZ154,IF(M155=0,AZ154+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="BA155" s="9">
+        <f t="shared" ref="BA155" si="893">IF(ISNA(N155),BA154,IF(N155=0,BA154+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="BB155" s="9">
+        <f t="shared" ref="BB155" si="894">IF(ISNA(O155),BB154,IF(O155=0,BB154+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="BC155" s="9">
+        <f t="shared" ref="BC155" si="895">IF(ISNA(P155),BC154,IF(P155=0,BC154+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="BD155" s="9">
+        <f t="shared" ref="BD155" si="896">IF(ISNA(Q155),BD154,IF(Q155=0,BD154+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="BE155" s="9">
+        <f t="shared" ref="BE155" si="897">IF(ISNA(R155),BE154,IF(R155=0,BE154+1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="BF155" s="9">
+        <f t="shared" ref="BF155" si="898">IF(ISNA(S155),BF154,IF(S155=0,BF154+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="BG155" s="9">
+        <f t="shared" ref="BG155" si="899">IF(ISNA(T155),BG154,IF(T155=0,BG154+1,0))</f>
+        <v>1</v>
+      </c>
+      <c r="BH155" s="9">
+        <f t="shared" ref="BH155" si="900">IF(ISNA(U155),BH154,IF(U155=0,BH154+1,0))</f>
         <v>5</v>
       </c>
     </row>
@@ -75332,7 +75748,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B19" sqref="B2:Q19"/>
     </sheetView>
   </sheetViews>

</xml_diff>